<commit_message>
Minor update (matchday 21)
- updated code for new FBRef stats;
- updated players list;
- players who changed team handled slightly better
</commit_message>
<xml_diff>
--- a/tmp/playermatchdata.xlsx
+++ b/tmp/playermatchdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="815">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -343,6 +343,18 @@
     <t>dribbles_completed_pct</t>
   </si>
   <si>
+    <t>carries</t>
+  </si>
+  <si>
+    <t>progressive_carries</t>
+  </si>
+  <si>
+    <t>carries_into_final_third</t>
+  </si>
+  <si>
+    <t>carries_into_penalty_area</t>
+  </si>
+  <si>
     <t>passes_received</t>
   </si>
   <si>
@@ -937,6 +949,18 @@
     <t>team_dribbles_completed_pct</t>
   </si>
   <si>
+    <t>team_carries</t>
+  </si>
+  <si>
+    <t>team_progressive_carries</t>
+  </si>
+  <si>
+    <t>team_carries_into_final_third</t>
+  </si>
+  <si>
+    <t>team_carries_into_penalty_area</t>
+  </si>
+  <si>
     <t>team_passes_received</t>
   </si>
   <si>
@@ -1405,6 +1429,18 @@
     <t>vs_team_dribbles_completed_pct</t>
   </si>
   <si>
+    <t>vs_team_carries</t>
+  </si>
+  <si>
+    <t>vs_team_progressive_carries</t>
+  </si>
+  <si>
+    <t>vs_team_carries_into_final_third</t>
+  </si>
+  <si>
+    <t>vs_team_carries_into_penalty_area</t>
+  </si>
+  <si>
     <t>vs_team_passes_received</t>
   </si>
   <si>
@@ -1876,6 +1912,18 @@
     <t>opp_team_dribbles_completed_pct</t>
   </si>
   <si>
+    <t>opp_team_carries</t>
+  </si>
+  <si>
+    <t>opp_team_progressive_carries</t>
+  </si>
+  <si>
+    <t>opp_team_carries_into_final_third</t>
+  </si>
+  <si>
+    <t>opp_team_carries_into_penalty_area</t>
+  </si>
+  <si>
     <t>opp_team_passes_received</t>
   </si>
   <si>
@@ -2344,6 +2392,18 @@
     <t>opp_vs_team_dribbles_completed_pct</t>
   </si>
   <si>
+    <t>opp_vs_team_carries</t>
+  </si>
+  <si>
+    <t>opp_vs_team_progressive_carries</t>
+  </si>
+  <si>
+    <t>opp_vs_team_carries_into_final_third</t>
+  </si>
+  <si>
+    <t>opp_vs_team_carries_into_penalty_area</t>
+  </si>
+  <si>
     <t>opp_vs_team_passes_received</t>
   </si>
   <si>
@@ -2395,7 +2455,7 @@
     <t>Sassuolo</t>
   </si>
   <si>
-    <t>23-098</t>
+    <t>23-105</t>
   </si>
   <si>
     <t>Atalanta</t>
@@ -2756,13 +2816,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ADL2"/>
+  <dimension ref="A1:AEF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:792">
+    <row r="1" spans="1:812">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3259,19 +3319,19 @@
         <v>164</v>
       </c>
       <c r="FK1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="FL1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="FM1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="FN1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="FO1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="FL1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="FM1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="FN1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="FO1" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="FP1" s="1" t="s">
         <v>169</v>
@@ -5136,46 +5196,106 @@
       <c r="ADL1" s="1" t="s">
         <v>789</v>
       </c>
+      <c r="ADM1" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="ADN1" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="ADO1" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="ADP1" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="ADQ1" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="ADR1" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="ADS1" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="ADT1" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="ADU1" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="ADV1" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="ADW1" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="ADX1" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="ADY1" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="ADZ1" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="AEA1" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="AEB1" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="AEC1" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="AED1" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="AEE1" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="AEF1" s="1" t="s">
+        <v>809</v>
+      </c>
     </row>
-    <row r="2" spans="1:792">
+    <row r="2" spans="1:812">
       <c r="A2" s="1" t="s">
-        <v>790</v>
+        <v>810</v>
       </c>
       <c r="B2">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C2">
         <v>2848</v>
       </c>
       <c r="D2" t="s">
-        <v>791</v>
+        <v>811</v>
       </c>
       <c r="E2" t="s">
-        <v>792</v>
+        <v>812</v>
       </c>
       <c r="F2" t="s">
-        <v>790</v>
+        <v>810</v>
       </c>
       <c r="H2">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I2" t="s">
-        <v>793</v>
+        <v>813</v>
       </c>
       <c r="J2">
         <v>1999</v>
       </c>
       <c r="K2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2">
-        <v>1560</v>
+        <v>1636</v>
       </c>
       <c r="N2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -5187,31 +5307,31 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
       <c r="W2">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
       <c r="X2">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
       <c r="Y2">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="Z2">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="AA2">
         <v>0.23</v>
@@ -5223,79 +5343,79 @@
         <v>0</v>
       </c>
       <c r="AD2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>48.6</v>
+        <v>50</v>
       </c>
       <c r="AG2">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="AH2">
-        <v>0.11</v>
+        <v>0.14</v>
       </c>
       <c r="AI2">
-        <v>0.24</v>
+        <v>0.28</v>
       </c>
       <c r="AJ2">
         <v>0.12</v>
       </c>
       <c r="AK2">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AL2">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AM2">
-        <v>422</v>
+        <v>439</v>
       </c>
       <c r="AN2">
-        <v>542</v>
+        <v>565</v>
       </c>
       <c r="AO2">
-        <v>77.90000000000001</v>
+        <v>77.7</v>
       </c>
       <c r="AP2">
-        <v>7242</v>
+        <v>7555</v>
       </c>
       <c r="AQ2">
-        <v>1914</v>
+        <v>2079</v>
       </c>
       <c r="AR2">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="AS2">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="AT2">
-        <v>81.59999999999999</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="AU2">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="AV2">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="AW2">
-        <v>83.5</v>
+        <v>83.2</v>
       </c>
       <c r="AX2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AY2">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AZ2">
-        <v>65.40000000000001</v>
+        <v>64.2</v>
       </c>
       <c r="BA2">
         <v>18</v>
       </c>
       <c r="BB2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="BC2">
         <v>16</v>
@@ -5304,22 +5424,22 @@
         <v>1</v>
       </c>
       <c r="BE2">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="BF2">
-        <v>527</v>
+        <v>549</v>
       </c>
       <c r="BG2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BH2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BI2">
         <v>4</v>
       </c>
       <c r="BJ2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BK2">
         <v>9</v>
@@ -5343,13 +5463,13 @@
         <v>0</v>
       </c>
       <c r="BR2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BS2">
         <v>54</v>
       </c>
       <c r="BT2">
-        <v>3.11</v>
+        <v>2.97</v>
       </c>
       <c r="BU2">
         <v>43</v>
@@ -5370,7 +5490,7 @@
         <v>4</v>
       </c>
       <c r="CA2">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="CB2">
         <v>4</v>
@@ -5391,28 +5511,28 @@
         <v>0</v>
       </c>
       <c r="CH2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="CI2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="CJ2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="CK2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="CL2">
         <v>5</v>
       </c>
       <c r="CM2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="CN2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="CO2">
-        <v>54.5</v>
+        <v>58.3</v>
       </c>
       <c r="CP2">
         <v>10</v>
@@ -5427,7 +5547,7 @@
         <v>13</v>
       </c>
       <c r="CT2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CU2">
         <v>22</v>
@@ -5436,2080 +5556,2140 @@
         <v>0</v>
       </c>
       <c r="CW2">
-        <v>752</v>
+        <v>788</v>
       </c>
       <c r="CX2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="CY2">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="CZ2">
-        <v>371</v>
+        <v>399</v>
       </c>
       <c r="DA2">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="DB2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="DC2">
-        <v>752</v>
+        <v>788</v>
       </c>
       <c r="DD2">
         <v>24</v>
       </c>
       <c r="DE2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="DF2">
-        <v>54.5</v>
+        <v>52.2</v>
       </c>
       <c r="DG2">
-        <v>503</v>
+        <v>444</v>
       </c>
       <c r="DH2">
+        <v>43</v>
+      </c>
+      <c r="DI2">
+        <v>30</v>
+      </c>
+      <c r="DJ2">
+        <v>14</v>
+      </c>
+      <c r="DK2">
+        <v>525</v>
+      </c>
+      <c r="DL2">
+        <v>29</v>
+      </c>
+      <c r="DM2">
+        <v>28</v>
+      </c>
+      <c r="DN2">
+        <v>0</v>
+      </c>
+      <c r="DO2">
         <v>26</v>
       </c>
-      <c r="DI2">
+      <c r="DP2">
+        <v>36</v>
+      </c>
+      <c r="DQ2">
+        <v>0</v>
+      </c>
+      <c r="DR2">
+        <v>0</v>
+      </c>
+      <c r="DS2">
+        <v>0</v>
+      </c>
+      <c r="DT2">
+        <v>0</v>
+      </c>
+      <c r="DU2">
+        <v>91</v>
+      </c>
+      <c r="DV2">
+        <v>16</v>
+      </c>
+      <c r="DW2">
+        <v>12</v>
+      </c>
+      <c r="DX2">
+        <v>57.1</v>
+      </c>
+      <c r="DY2">
+        <v>0</v>
+      </c>
+      <c r="DZ2">
+        <v>0</v>
+      </c>
+      <c r="EA2">
+        <v>0</v>
+      </c>
+      <c r="EB2">
+        <v>0</v>
+      </c>
+      <c r="EC2">
+        <v>0</v>
+      </c>
+      <c r="ED2">
+        <v>0</v>
+      </c>
+      <c r="EE2">
+        <v>0</v>
+      </c>
+      <c r="EF2">
+        <v>0</v>
+      </c>
+      <c r="EG2">
+        <v>0</v>
+      </c>
+      <c r="EH2">
+        <v>0</v>
+      </c>
+      <c r="EI2">
+        <v>0</v>
+      </c>
+      <c r="EJ2">
+        <v>0</v>
+      </c>
+      <c r="EK2">
+        <v>0</v>
+      </c>
+      <c r="EL2">
+        <v>0</v>
+      </c>
+      <c r="EM2">
+        <v>0</v>
+      </c>
+      <c r="EN2">
+        <v>0</v>
+      </c>
+      <c r="EO2">
+        <v>0</v>
+      </c>
+      <c r="EP2">
+        <v>0</v>
+      </c>
+      <c r="EQ2">
+        <v>0</v>
+      </c>
+      <c r="ER2">
+        <v>0</v>
+      </c>
+      <c r="ES2">
+        <v>0</v>
+      </c>
+      <c r="ET2">
+        <v>0</v>
+      </c>
+      <c r="EU2">
+        <v>0</v>
+      </c>
+      <c r="EV2">
+        <v>0</v>
+      </c>
+      <c r="EW2">
+        <v>0</v>
+      </c>
+      <c r="EX2">
+        <v>0</v>
+      </c>
+      <c r="EY2">
+        <v>0</v>
+      </c>
+      <c r="EZ2">
+        <v>0</v>
+      </c>
+      <c r="FA2">
+        <v>0</v>
+      </c>
+      <c r="FB2">
+        <v>0</v>
+      </c>
+      <c r="FC2">
+        <v>0</v>
+      </c>
+      <c r="FD2">
+        <v>0</v>
+      </c>
+      <c r="FE2">
+        <v>0</v>
+      </c>
+      <c r="FF2">
+        <v>0</v>
+      </c>
+      <c r="FG2">
+        <v>0</v>
+      </c>
+      <c r="FH2">
+        <v>0</v>
+      </c>
+      <c r="FI2">
+        <v>0</v>
+      </c>
+      <c r="FJ2">
+        <v>0</v>
+      </c>
+      <c r="FK2">
+        <v>0</v>
+      </c>
+      <c r="FL2">
+        <v>0</v>
+      </c>
+      <c r="FM2">
+        <v>6.275</v>
+      </c>
+      <c r="FN2">
+        <v>0.7154544010627093</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>812</v>
+      </c>
+      <c r="FP2">
         <v>27</v>
       </c>
-      <c r="DJ2">
-        <v>0</v>
-      </c>
-      <c r="DK2">
+      <c r="FQ2">
+        <v>48.3</v>
+      </c>
+      <c r="FR2">
+        <v>20</v>
+      </c>
+      <c r="FS2">
+        <v>220</v>
+      </c>
+      <c r="FT2">
+        <v>1800</v>
+      </c>
+      <c r="FU2">
         <v>23</v>
       </c>
-      <c r="DL2">
-        <v>36</v>
-      </c>
-      <c r="DM2">
-        <v>0</v>
-      </c>
-      <c r="DN2">
-        <v>0</v>
-      </c>
-      <c r="DO2">
-        <v>0</v>
-      </c>
-      <c r="DP2">
-        <v>0</v>
-      </c>
-      <c r="DQ2">
-        <v>86</v>
-      </c>
-      <c r="DR2">
+      <c r="FV2">
+        <v>17</v>
+      </c>
+      <c r="FW2">
+        <v>4</v>
+      </c>
+      <c r="FX2">
+        <v>5</v>
+      </c>
+      <c r="FY2">
+        <v>50</v>
+      </c>
+      <c r="FZ2">
+        <v>2</v>
+      </c>
+      <c r="GA2">
+        <v>1.15</v>
+      </c>
+      <c r="GB2">
+        <v>0.85</v>
+      </c>
+      <c r="GC2">
+        <v>2</v>
+      </c>
+      <c r="GD2">
+        <v>0.95</v>
+      </c>
+      <c r="GE2">
+        <v>1.8</v>
+      </c>
+      <c r="GF2">
+        <v>25.9</v>
+      </c>
+      <c r="GG2">
+        <v>22</v>
+      </c>
+      <c r="GH2">
+        <v>1.29</v>
+      </c>
+      <c r="GI2">
+        <v>1.1</v>
+      </c>
+      <c r="GJ2">
+        <v>20</v>
+      </c>
+      <c r="GK2">
+        <v>20</v>
+      </c>
+      <c r="GL2">
+        <v>1800</v>
+      </c>
+      <c r="GM2">
+        <v>31</v>
+      </c>
+      <c r="GN2">
+        <v>1.55</v>
+      </c>
+      <c r="GO2">
+        <v>64</v>
+      </c>
+      <c r="GP2">
+        <v>33</v>
+      </c>
+      <c r="GQ2">
+        <v>57.8</v>
+      </c>
+      <c r="GR2">
+        <v>5</v>
+      </c>
+      <c r="GS2">
+        <v>5</v>
+      </c>
+      <c r="GT2">
+        <v>10</v>
+      </c>
+      <c r="GU2">
+        <v>5</v>
+      </c>
+      <c r="GV2">
+        <v>25</v>
+      </c>
+      <c r="GW2">
+        <v>4</v>
+      </c>
+      <c r="GX2">
+        <v>4</v>
+      </c>
+      <c r="GY2">
+        <v>0</v>
+      </c>
+      <c r="GZ2">
+        <v>0</v>
+      </c>
+      <c r="HA2">
+        <v>20</v>
+      </c>
+      <c r="HB2">
+        <v>0</v>
+      </c>
+      <c r="HC2">
+        <v>3</v>
+      </c>
+      <c r="HD2">
+        <v>0</v>
+      </c>
+      <c r="HE2">
+        <v>26.1</v>
+      </c>
+      <c r="HF2">
+        <v>0.36</v>
+      </c>
+      <c r="HG2">
+        <v>-4.9</v>
+      </c>
+      <c r="HH2">
+        <v>-0.25</v>
+      </c>
+      <c r="HI2">
+        <v>119</v>
+      </c>
+      <c r="HJ2">
+        <v>279</v>
+      </c>
+      <c r="HK2">
+        <v>42.7</v>
+      </c>
+      <c r="HL2">
+        <v>712</v>
+      </c>
+      <c r="HM2">
+        <v>105</v>
+      </c>
+      <c r="HN2">
+        <v>30.9</v>
+      </c>
+      <c r="HO2">
+        <v>34.2</v>
+      </c>
+      <c r="HP2">
+        <v>183</v>
+      </c>
+      <c r="HQ2">
+        <v>32.2</v>
+      </c>
+      <c r="HR2">
+        <v>32.9</v>
+      </c>
+      <c r="HS2">
+        <v>264</v>
+      </c>
+      <c r="HT2">
         <v>16</v>
       </c>
-      <c r="DS2">
-        <v>11</v>
-      </c>
-      <c r="DT2">
-        <v>59.3</v>
-      </c>
-      <c r="DU2">
-        <v>0</v>
-      </c>
-      <c r="DV2">
-        <v>0</v>
-      </c>
-      <c r="DW2">
-        <v>0</v>
-      </c>
-      <c r="DX2">
-        <v>0</v>
-      </c>
-      <c r="DY2">
-        <v>0</v>
-      </c>
-      <c r="DZ2">
-        <v>0</v>
-      </c>
-      <c r="EA2">
-        <v>0</v>
-      </c>
-      <c r="EB2">
-        <v>0</v>
-      </c>
-      <c r="EC2">
-        <v>0</v>
-      </c>
-      <c r="ED2">
-        <v>0</v>
-      </c>
-      <c r="EE2">
-        <v>0</v>
-      </c>
-      <c r="EF2">
-        <v>0</v>
-      </c>
-      <c r="EG2">
-        <v>0</v>
-      </c>
-      <c r="EH2">
-        <v>0</v>
-      </c>
-      <c r="EI2">
-        <v>0</v>
-      </c>
-      <c r="EJ2">
-        <v>0</v>
-      </c>
-      <c r="EK2">
-        <v>0</v>
-      </c>
-      <c r="EL2">
-        <v>0</v>
-      </c>
-      <c r="EM2">
-        <v>0</v>
-      </c>
-      <c r="EN2">
-        <v>0</v>
-      </c>
-      <c r="EO2">
-        <v>0</v>
-      </c>
-      <c r="EP2">
-        <v>0</v>
-      </c>
-      <c r="EQ2">
-        <v>0</v>
-      </c>
-      <c r="ER2">
-        <v>0</v>
-      </c>
-      <c r="ES2">
-        <v>0</v>
-      </c>
-      <c r="ET2">
-        <v>0</v>
-      </c>
-      <c r="EU2">
-        <v>0</v>
-      </c>
-      <c r="EV2">
-        <v>0</v>
-      </c>
-      <c r="EW2">
-        <v>0</v>
-      </c>
-      <c r="EX2">
-        <v>0</v>
-      </c>
-      <c r="EY2">
-        <v>0</v>
-      </c>
-      <c r="EZ2">
-        <v>0</v>
-      </c>
-      <c r="FA2">
-        <v>0</v>
-      </c>
-      <c r="FB2">
-        <v>0</v>
-      </c>
-      <c r="FC2">
-        <v>0</v>
-      </c>
-      <c r="FD2">
-        <v>0</v>
-      </c>
-      <c r="FE2">
-        <v>0</v>
-      </c>
-      <c r="FF2">
-        <v>0</v>
-      </c>
-      <c r="FG2">
-        <v>0</v>
-      </c>
-      <c r="FH2">
-        <v>0</v>
-      </c>
-      <c r="FI2">
-        <v>6.210526315789473</v>
-      </c>
-      <c r="FJ2">
-        <v>0.6750397546516137</v>
-      </c>
-      <c r="FK2" t="s">
-        <v>792</v>
-      </c>
-      <c r="FL2">
-        <v>27</v>
-      </c>
-      <c r="FM2">
-        <v>48.7</v>
-      </c>
-      <c r="FN2">
+      <c r="HU2">
+        <v>6.1</v>
+      </c>
+      <c r="HV2">
+        <v>15</v>
+      </c>
+      <c r="HW2">
+        <v>0.75</v>
+      </c>
+      <c r="HX2">
+        <v>14</v>
+      </c>
+      <c r="HY2">
+        <v>87</v>
+      </c>
+      <c r="HZ2">
+        <v>10</v>
+      </c>
+      <c r="IA2">
+        <v>34.3</v>
+      </c>
+      <c r="IB2">
+        <v>4.35</v>
+      </c>
+      <c r="IC2">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="ID2">
+        <v>0.22</v>
+      </c>
+      <c r="IE2">
+        <v>0.09</v>
+      </c>
+      <c r="IF2">
+        <v>-2.9</v>
+      </c>
+      <c r="IG2">
+        <v>-3</v>
+      </c>
+      <c r="IH2">
+        <v>7498</v>
+      </c>
+      <c r="II2">
+        <v>9357</v>
+      </c>
+      <c r="IJ2">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="IK2">
+        <v>141620</v>
+      </c>
+      <c r="IL2">
+        <v>52357</v>
+      </c>
+      <c r="IM2">
+        <v>3112</v>
+      </c>
+      <c r="IN2">
+        <v>3536</v>
+      </c>
+      <c r="IO2">
+        <v>88</v>
+      </c>
+      <c r="IP2">
+        <v>3108</v>
+      </c>
+      <c r="IQ2">
+        <v>3609</v>
+      </c>
+      <c r="IR2">
+        <v>86.09999999999999</v>
+      </c>
+      <c r="IS2">
+        <v>1089</v>
+      </c>
+      <c r="IT2">
+        <v>1721</v>
+      </c>
+      <c r="IU2">
+        <v>63.3</v>
+      </c>
+      <c r="IV2">
+        <v>205</v>
+      </c>
+      <c r="IW2">
+        <v>565</v>
+      </c>
+      <c r="IX2">
+        <v>171</v>
+      </c>
+      <c r="IY2">
+        <v>49</v>
+      </c>
+      <c r="IZ2">
+        <v>776</v>
+      </c>
+      <c r="JA2">
+        <v>8237</v>
+      </c>
+      <c r="JB2">
+        <v>1101</v>
+      </c>
+      <c r="JC2">
+        <v>313</v>
+      </c>
+      <c r="JD2">
+        <v>21</v>
+      </c>
+      <c r="JE2">
+        <v>112</v>
+      </c>
+      <c r="JF2">
+        <v>298</v>
+      </c>
+      <c r="JG2">
+        <v>87</v>
+      </c>
+      <c r="JH2">
+        <v>41</v>
+      </c>
+      <c r="JI2">
+        <v>23</v>
+      </c>
+      <c r="JJ2">
+        <v>0</v>
+      </c>
+      <c r="JK2">
+        <v>439</v>
+      </c>
+      <c r="JL2">
         <v>19</v>
       </c>
-      <c r="FO2">
-        <v>209</v>
-      </c>
-      <c r="FP2">
-        <v>1710</v>
-      </c>
-      <c r="FQ2">
-        <v>18</v>
-      </c>
-      <c r="FR2">
-        <v>13</v>
-      </c>
-      <c r="FS2">
-        <v>3</v>
-      </c>
-      <c r="FT2">
-        <v>4</v>
-      </c>
-      <c r="FU2">
-        <v>46</v>
-      </c>
-      <c r="FV2">
-        <v>2</v>
-      </c>
-      <c r="FW2">
-        <v>0.95</v>
-      </c>
-      <c r="FX2">
-        <v>0.68</v>
-      </c>
-      <c r="FY2">
-        <v>1.63</v>
-      </c>
-      <c r="FZ2">
-        <v>0.79</v>
-      </c>
-      <c r="GA2">
-        <v>1.47</v>
-      </c>
-      <c r="GB2">
-        <v>23.7</v>
-      </c>
-      <c r="GC2">
-        <v>20.7</v>
-      </c>
-      <c r="GD2">
-        <v>1.25</v>
-      </c>
-      <c r="GE2">
-        <v>1.09</v>
-      </c>
-      <c r="GF2">
+      <c r="JM2">
+        <v>182</v>
+      </c>
+      <c r="JN2">
+        <v>461</v>
+      </c>
+      <c r="JO2">
+        <v>23.05</v>
+      </c>
+      <c r="JP2">
+        <v>368</v>
+      </c>
+      <c r="JQ2">
+        <v>25</v>
+      </c>
+      <c r="JR2">
         <v>19</v>
-      </c>
-      <c r="GG2">
-        <v>19</v>
-      </c>
-      <c r="GH2">
-        <v>1710</v>
-      </c>
-      <c r="GI2">
-        <v>29</v>
-      </c>
-      <c r="GJ2">
-        <v>1.53</v>
-      </c>
-      <c r="GK2">
-        <v>59</v>
-      </c>
-      <c r="GL2">
-        <v>30</v>
-      </c>
-      <c r="GM2">
-        <v>57.6</v>
-      </c>
-      <c r="GN2">
-        <v>4</v>
-      </c>
-      <c r="GO2">
-        <v>5</v>
-      </c>
-      <c r="GP2">
-        <v>10</v>
-      </c>
-      <c r="GQ2">
-        <v>5</v>
-      </c>
-      <c r="GR2">
-        <v>26.3</v>
-      </c>
-      <c r="GS2">
-        <v>4</v>
-      </c>
-      <c r="GT2">
-        <v>4</v>
-      </c>
-      <c r="GU2">
-        <v>0</v>
-      </c>
-      <c r="GV2">
-        <v>0</v>
-      </c>
-      <c r="GW2">
-        <v>19</v>
-      </c>
-      <c r="GX2">
-        <v>0</v>
-      </c>
-      <c r="GY2">
-        <v>3</v>
-      </c>
-      <c r="GZ2">
-        <v>0</v>
-      </c>
-      <c r="HA2">
-        <v>24.9</v>
-      </c>
-      <c r="HB2">
-        <v>0.37</v>
-      </c>
-      <c r="HC2">
-        <v>-4.1</v>
-      </c>
-      <c r="HD2">
-        <v>-0.22</v>
-      </c>
-      <c r="HE2">
-        <v>109</v>
-      </c>
-      <c r="HF2">
-        <v>260</v>
-      </c>
-      <c r="HG2">
-        <v>41.9</v>
-      </c>
-      <c r="HH2">
-        <v>682</v>
-      </c>
-      <c r="HI2">
-        <v>97</v>
-      </c>
-      <c r="HJ2">
-        <v>30.1</v>
-      </c>
-      <c r="HK2">
-        <v>33.9</v>
-      </c>
-      <c r="HL2">
-        <v>173</v>
-      </c>
-      <c r="HM2">
-        <v>31.8</v>
-      </c>
-      <c r="HN2">
-        <v>32.8</v>
-      </c>
-      <c r="HO2">
-        <v>248</v>
-      </c>
-      <c r="HP2">
-        <v>15</v>
-      </c>
-      <c r="HQ2">
-        <v>6</v>
-      </c>
-      <c r="HR2">
-        <v>15</v>
-      </c>
-      <c r="HS2">
-        <v>0.79</v>
-      </c>
-      <c r="HT2">
-        <v>14</v>
-      </c>
-      <c r="HU2">
-        <v>81</v>
-      </c>
-      <c r="HV2">
-        <v>10</v>
-      </c>
-      <c r="HW2">
-        <v>32.9</v>
-      </c>
-      <c r="HX2">
-        <v>4.26</v>
-      </c>
-      <c r="HY2">
-        <v>0.06</v>
-      </c>
-      <c r="HZ2">
-        <v>0.19</v>
-      </c>
-      <c r="IA2">
-        <v>0.09</v>
-      </c>
-      <c r="IB2">
-        <v>-5.7</v>
-      </c>
-      <c r="IC2">
-        <v>-5.7</v>
-      </c>
-      <c r="ID2">
-        <v>7277</v>
-      </c>
-      <c r="IE2">
-        <v>9046</v>
-      </c>
-      <c r="IF2">
-        <v>80.40000000000001</v>
-      </c>
-      <c r="IG2">
-        <v>137410</v>
-      </c>
-      <c r="IH2">
-        <v>49998</v>
-      </c>
-      <c r="II2">
-        <v>3015</v>
-      </c>
-      <c r="IJ2">
-        <v>3417</v>
-      </c>
-      <c r="IK2">
-        <v>88.2</v>
-      </c>
-      <c r="IL2">
-        <v>3025</v>
-      </c>
-      <c r="IM2">
-        <v>3504</v>
-      </c>
-      <c r="IN2">
-        <v>86.3</v>
-      </c>
-      <c r="IO2">
-        <v>1054</v>
-      </c>
-      <c r="IP2">
-        <v>1655</v>
-      </c>
-      <c r="IQ2">
-        <v>63.7</v>
-      </c>
-      <c r="IR2">
-        <v>198</v>
-      </c>
-      <c r="IS2">
-        <v>546</v>
-      </c>
-      <c r="IT2">
-        <v>166</v>
-      </c>
-      <c r="IU2">
-        <v>48</v>
-      </c>
-      <c r="IV2">
-        <v>550</v>
-      </c>
-      <c r="IW2">
-        <v>7982</v>
-      </c>
-      <c r="IX2">
-        <v>1048</v>
-      </c>
-      <c r="IY2">
-        <v>296</v>
-      </c>
-      <c r="IZ2">
-        <v>20</v>
-      </c>
-      <c r="JA2">
-        <v>109</v>
-      </c>
-      <c r="JB2">
-        <v>288</v>
-      </c>
-      <c r="JC2">
-        <v>84</v>
-      </c>
-      <c r="JD2">
-        <v>40</v>
-      </c>
-      <c r="JE2">
-        <v>21</v>
-      </c>
-      <c r="JF2">
-        <v>0</v>
-      </c>
-      <c r="JG2">
-        <v>419</v>
-      </c>
-      <c r="JH2">
-        <v>16</v>
-      </c>
-      <c r="JI2">
-        <v>173</v>
-      </c>
-      <c r="JJ2">
-        <v>449</v>
-      </c>
-      <c r="JK2">
-        <v>23.63</v>
-      </c>
-      <c r="JL2">
-        <v>358</v>
-      </c>
-      <c r="JM2">
-        <v>24</v>
-      </c>
-      <c r="JN2">
-        <v>19</v>
-      </c>
-      <c r="JO2">
-        <v>24</v>
-      </c>
-      <c r="JP2">
-        <v>17</v>
-      </c>
-      <c r="JQ2">
-        <v>32</v>
-      </c>
-      <c r="JR2">
-        <v>1.68</v>
       </c>
       <c r="JS2">
         <v>24</v>
       </c>
       <c r="JT2">
+        <v>18</v>
+      </c>
+      <c r="JU2">
+        <v>41</v>
+      </c>
+      <c r="JV2">
+        <v>2.05</v>
+      </c>
+      <c r="JW2">
+        <v>31</v>
+      </c>
+      <c r="JX2">
+        <v>2</v>
+      </c>
+      <c r="JY2">
+        <v>2</v>
+      </c>
+      <c r="JZ2">
+        <v>3</v>
+      </c>
+      <c r="KA2">
+        <v>3</v>
+      </c>
+      <c r="KB2">
+        <v>0</v>
+      </c>
+      <c r="KC2">
+        <v>282</v>
+      </c>
+      <c r="KD2">
+        <v>151</v>
+      </c>
+      <c r="KE2">
+        <v>132</v>
+      </c>
+      <c r="KF2">
+        <v>113</v>
+      </c>
+      <c r="KG2">
+        <v>37</v>
+      </c>
+      <c r="KH2">
+        <v>116</v>
+      </c>
+      <c r="KI2">
+        <v>227</v>
+      </c>
+      <c r="KJ2">
+        <v>51.1</v>
+      </c>
+      <c r="KK2">
+        <v>111</v>
+      </c>
+      <c r="KL2">
+        <v>182</v>
+      </c>
+      <c r="KM2">
+        <v>55</v>
+      </c>
+      <c r="KN2">
+        <v>127</v>
+      </c>
+      <c r="KO2">
+        <v>148</v>
+      </c>
+      <c r="KP2">
+        <v>338</v>
+      </c>
+      <c r="KQ2">
+        <v>8</v>
+      </c>
+      <c r="KR2">
+        <v>11358</v>
+      </c>
+      <c r="KS2">
+        <v>1316</v>
+      </c>
+      <c r="KT2">
+        <v>3996</v>
+      </c>
+      <c r="KU2">
+        <v>4881</v>
+      </c>
+      <c r="KV2">
+        <v>2594</v>
+      </c>
+      <c r="KW2">
+        <v>397</v>
+      </c>
+      <c r="KX2">
+        <v>11353</v>
+      </c>
+      <c r="KY2">
+        <v>122</v>
+      </c>
+      <c r="KZ2">
+        <v>299</v>
+      </c>
+      <c r="LA2">
+        <v>40.8</v>
+      </c>
+      <c r="LB2">
+        <v>6477</v>
+      </c>
+      <c r="LC2">
+        <v>378</v>
+      </c>
+      <c r="LD2">
+        <v>244</v>
+      </c>
+      <c r="LE2">
+        <v>106</v>
+      </c>
+      <c r="LF2">
+        <v>7429</v>
+      </c>
+      <c r="LG2">
+        <v>273</v>
+      </c>
+      <c r="LH2">
+        <v>216</v>
+      </c>
+      <c r="LI2">
         <v>1</v>
       </c>
-      <c r="JU2">
+      <c r="LJ2">
+        <v>207</v>
+      </c>
+      <c r="LK2">
+        <v>247</v>
+      </c>
+      <c r="LL2">
+        <v>19</v>
+      </c>
+      <c r="LM2">
+        <v>4</v>
+      </c>
+      <c r="LN2">
+        <v>4</v>
+      </c>
+      <c r="LO2">
+        <v>0</v>
+      </c>
+      <c r="LP2">
+        <v>909</v>
+      </c>
+      <c r="LQ2">
+        <v>183</v>
+      </c>
+      <c r="LR2">
+        <v>229</v>
+      </c>
+      <c r="LS2">
+        <v>44.4</v>
+      </c>
+      <c r="LT2">
+        <v>27</v>
+      </c>
+      <c r="LU2">
+        <v>51.8</v>
+      </c>
+      <c r="LV2">
+        <v>20</v>
+      </c>
+      <c r="LW2">
+        <v>220</v>
+      </c>
+      <c r="LX2">
+        <v>1800</v>
+      </c>
+      <c r="LY2">
+        <v>31</v>
+      </c>
+      <c r="LZ2">
+        <v>22</v>
+      </c>
+      <c r="MA2">
+        <v>4</v>
+      </c>
+      <c r="MB2">
+        <v>4</v>
+      </c>
+      <c r="MC2">
+        <v>46</v>
+      </c>
+      <c r="MD2">
+        <v>1</v>
+      </c>
+      <c r="ME2">
+        <v>1.55</v>
+      </c>
+      <c r="MF2">
+        <v>1.1</v>
+      </c>
+      <c r="MG2">
+        <v>2.65</v>
+      </c>
+      <c r="MH2">
+        <v>1.35</v>
+      </c>
+      <c r="MI2">
+        <v>2.45</v>
+      </c>
+      <c r="MJ2">
+        <v>27.3</v>
+      </c>
+      <c r="MK2">
+        <v>24.7</v>
+      </c>
+      <c r="ML2">
+        <v>1.36</v>
+      </c>
+      <c r="MM2">
+        <v>1.23</v>
+      </c>
+      <c r="MN2">
+        <v>20</v>
+      </c>
+      <c r="MO2">
+        <v>20</v>
+      </c>
+      <c r="MP2">
+        <v>1800</v>
+      </c>
+      <c r="MQ2">
+        <v>23</v>
+      </c>
+      <c r="MR2">
+        <v>1.15</v>
+      </c>
+      <c r="MS2">
+        <v>92</v>
+      </c>
+      <c r="MT2">
+        <v>68</v>
+      </c>
+      <c r="MU2">
+        <v>79.3</v>
+      </c>
+      <c r="MV2">
+        <v>10</v>
+      </c>
+      <c r="MW2">
+        <v>5</v>
+      </c>
+      <c r="MX2">
+        <v>5</v>
+      </c>
+      <c r="MY2">
+        <v>7</v>
+      </c>
+      <c r="MZ2">
+        <v>35</v>
+      </c>
+      <c r="NA2">
+        <v>5</v>
+      </c>
+      <c r="NB2">
+        <v>4</v>
+      </c>
+      <c r="NC2">
+        <v>1</v>
+      </c>
+      <c r="ND2">
+        <v>0</v>
+      </c>
+      <c r="NE2">
+        <v>20</v>
+      </c>
+      <c r="NF2">
+        <v>0</v>
+      </c>
+      <c r="NG2">
+        <v>3</v>
+      </c>
+      <c r="NH2">
+        <v>0</v>
+      </c>
+      <c r="NI2">
+        <v>25.7</v>
+      </c>
+      <c r="NJ2">
+        <v>0.23</v>
+      </c>
+      <c r="NK2">
+        <v>2.7</v>
+      </c>
+      <c r="NL2">
+        <v>0.13</v>
+      </c>
+      <c r="NM2">
+        <v>108</v>
+      </c>
+      <c r="NN2">
+        <v>251</v>
+      </c>
+      <c r="NO2">
+        <v>43</v>
+      </c>
+      <c r="NP2">
+        <v>616</v>
+      </c>
+      <c r="NQ2">
+        <v>105</v>
+      </c>
+      <c r="NR2">
+        <v>31.2</v>
+      </c>
+      <c r="NS2">
+        <v>31</v>
+      </c>
+      <c r="NT2">
+        <v>130</v>
+      </c>
+      <c r="NU2">
+        <v>45.4</v>
+      </c>
+      <c r="NV2">
+        <v>39.3</v>
+      </c>
+      <c r="NW2">
+        <v>234</v>
+      </c>
+      <c r="NX2">
+        <v>7</v>
+      </c>
+      <c r="NY2">
+        <v>3</v>
+      </c>
+      <c r="NZ2">
+        <v>17</v>
+      </c>
+      <c r="OA2">
+        <v>0.85</v>
+      </c>
+      <c r="OB2">
+        <v>15.3</v>
+      </c>
+      <c r="OC2">
+        <v>60</v>
+      </c>
+      <c r="OD2">
+        <v>11</v>
+      </c>
+      <c r="OE2">
+        <v>25.2</v>
+      </c>
+      <c r="OF2">
+        <v>3</v>
+      </c>
+      <c r="OG2">
+        <v>0.11</v>
+      </c>
+      <c r="OH2">
+        <v>0.45</v>
+      </c>
+      <c r="OI2">
+        <v>0.11</v>
+      </c>
+      <c r="OJ2">
+        <v>3.7</v>
+      </c>
+      <c r="OK2">
+        <v>2.3</v>
+      </c>
+      <c r="OL2">
+        <v>8098</v>
+      </c>
+      <c r="OM2">
+        <v>10000</v>
+      </c>
+      <c r="ON2">
+        <v>81</v>
+      </c>
+      <c r="OO2">
+        <v>146437</v>
+      </c>
+      <c r="OP2">
+        <v>52729</v>
+      </c>
+      <c r="OQ2">
+        <v>3434</v>
+      </c>
+      <c r="OR2">
+        <v>3849</v>
+      </c>
+      <c r="OS2">
+        <v>89.2</v>
+      </c>
+      <c r="OT2">
+        <v>3557</v>
+      </c>
+      <c r="OU2">
+        <v>4039</v>
+      </c>
+      <c r="OV2">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="OW2">
+        <v>885</v>
+      </c>
+      <c r="OX2">
+        <v>1542</v>
+      </c>
+      <c r="OY2">
+        <v>57.4</v>
+      </c>
+      <c r="OZ2">
+        <v>188</v>
+      </c>
+      <c r="PA2">
+        <v>586</v>
+      </c>
+      <c r="PB2">
+        <v>192</v>
+      </c>
+      <c r="PC2">
+        <v>58</v>
+      </c>
+      <c r="PD2">
+        <v>762</v>
+      </c>
+      <c r="PE2">
+        <v>9042</v>
+      </c>
+      <c r="PF2">
+        <v>891</v>
+      </c>
+      <c r="PG2">
+        <v>209</v>
+      </c>
+      <c r="PH2">
+        <v>28</v>
+      </c>
+      <c r="PI2">
+        <v>88</v>
+      </c>
+      <c r="PJ2">
+        <v>350</v>
+      </c>
+      <c r="PK2">
+        <v>86</v>
+      </c>
+      <c r="PL2">
+        <v>26</v>
+      </c>
+      <c r="PM2">
+        <v>39</v>
+      </c>
+      <c r="PN2">
+        <v>0</v>
+      </c>
+      <c r="PO2">
+        <v>398</v>
+      </c>
+      <c r="PP2">
+        <v>67</v>
+      </c>
+      <c r="PQ2">
+        <v>159</v>
+      </c>
+      <c r="PR2">
+        <v>433</v>
+      </c>
+      <c r="PS2">
+        <v>21.65</v>
+      </c>
+      <c r="PT2">
+        <v>335</v>
+      </c>
+      <c r="PU2">
+        <v>39</v>
+      </c>
+      <c r="PV2">
+        <v>13</v>
+      </c>
+      <c r="PW2">
+        <v>20</v>
+      </c>
+      <c r="PX2">
+        <v>17</v>
+      </c>
+      <c r="PY2">
+        <v>50</v>
+      </c>
+      <c r="PZ2">
+        <v>2.5</v>
+      </c>
+      <c r="QA2">
+        <v>39</v>
+      </c>
+      <c r="QB2">
+        <v>1</v>
+      </c>
+      <c r="QC2">
+        <v>3</v>
+      </c>
+      <c r="QD2">
+        <v>5</v>
+      </c>
+      <c r="QE2">
         <v>2</v>
       </c>
-      <c r="JV2">
+      <c r="QF2">
+        <v>0</v>
+      </c>
+      <c r="QG2">
+        <v>355</v>
+      </c>
+      <c r="QH2">
+        <v>188</v>
+      </c>
+      <c r="QI2">
+        <v>171</v>
+      </c>
+      <c r="QJ2">
+        <v>141</v>
+      </c>
+      <c r="QK2">
+        <v>43</v>
+      </c>
+      <c r="QL2">
+        <v>139</v>
+      </c>
+      <c r="QM2">
+        <v>261</v>
+      </c>
+      <c r="QN2">
+        <v>53.3</v>
+      </c>
+      <c r="QO2">
+        <v>122</v>
+      </c>
+      <c r="QP2">
+        <v>230</v>
+      </c>
+      <c r="QQ2">
+        <v>71</v>
+      </c>
+      <c r="QR2">
+        <v>159</v>
+      </c>
+      <c r="QS2">
+        <v>175</v>
+      </c>
+      <c r="QT2">
+        <v>312</v>
+      </c>
+      <c r="QU2">
+        <v>6</v>
+      </c>
+      <c r="QV2">
+        <v>12034</v>
+      </c>
+      <c r="QW2">
+        <v>1328</v>
+      </c>
+      <c r="QX2">
+        <v>4127</v>
+      </c>
+      <c r="QY2">
+        <v>5222</v>
+      </c>
+      <c r="QZ2">
+        <v>2797</v>
+      </c>
+      <c r="RA2">
+        <v>440</v>
+      </c>
+      <c r="RB2">
+        <v>12030</v>
+      </c>
+      <c r="RC2">
+        <v>111</v>
+      </c>
+      <c r="RD2">
+        <v>259</v>
+      </c>
+      <c r="RE2">
+        <v>42.9</v>
+      </c>
+      <c r="RF2">
+        <v>6950</v>
+      </c>
+      <c r="RG2">
+        <v>366</v>
+      </c>
+      <c r="RH2">
+        <v>243</v>
+      </c>
+      <c r="RI2">
+        <v>83</v>
+      </c>
+      <c r="RJ2">
+        <v>8024</v>
+      </c>
+      <c r="RK2">
+        <v>272</v>
+      </c>
+      <c r="RL2">
+        <v>166</v>
+      </c>
+      <c r="RM2">
+        <v>1</v>
+      </c>
+      <c r="RN2">
+        <v>262</v>
+      </c>
+      <c r="RO2">
+        <v>190</v>
+      </c>
+      <c r="RP2">
+        <v>67</v>
+      </c>
+      <c r="RQ2">
+        <v>2</v>
+      </c>
+      <c r="RR2">
+        <v>5</v>
+      </c>
+      <c r="RS2">
+        <v>0</v>
+      </c>
+      <c r="RT2">
+        <v>1043</v>
+      </c>
+      <c r="RU2">
+        <v>229</v>
+      </c>
+      <c r="RV2">
+        <v>183</v>
+      </c>
+      <c r="RW2">
+        <v>55.6</v>
+      </c>
+      <c r="RX2" t="s">
+        <v>814</v>
+      </c>
+      <c r="RY2">
+        <v>24</v>
+      </c>
+      <c r="RZ2">
+        <v>49.1</v>
+      </c>
+      <c r="SA2">
+        <v>20</v>
+      </c>
+      <c r="SB2">
+        <v>220</v>
+      </c>
+      <c r="SC2">
+        <v>1800</v>
+      </c>
+      <c r="SD2">
+        <v>38</v>
+      </c>
+      <c r="SE2">
+        <v>27</v>
+      </c>
+      <c r="SF2">
+        <v>6</v>
+      </c>
+      <c r="SG2">
+        <v>8</v>
+      </c>
+      <c r="SH2">
+        <v>51</v>
+      </c>
+      <c r="SI2">
+        <v>1</v>
+      </c>
+      <c r="SJ2">
+        <v>1.9</v>
+      </c>
+      <c r="SK2">
+        <v>1.35</v>
+      </c>
+      <c r="SL2">
+        <v>3.25</v>
+      </c>
+      <c r="SM2">
+        <v>1.6</v>
+      </c>
+      <c r="SN2">
+        <v>2.95</v>
+      </c>
+      <c r="SO2">
+        <v>32.5</v>
+      </c>
+      <c r="SP2">
+        <v>26.1</v>
+      </c>
+      <c r="SQ2">
+        <v>1.62</v>
+      </c>
+      <c r="SR2">
+        <v>1.3</v>
+      </c>
+      <c r="SS2">
+        <v>20</v>
+      </c>
+      <c r="ST2">
+        <v>20</v>
+      </c>
+      <c r="SU2">
+        <v>1800</v>
+      </c>
+      <c r="SV2">
+        <v>23</v>
+      </c>
+      <c r="SW2">
+        <v>1.15</v>
+      </c>
+      <c r="SX2">
+        <v>74</v>
+      </c>
+      <c r="SY2">
+        <v>52</v>
+      </c>
+      <c r="SZ2">
+        <v>70.3</v>
+      </c>
+      <c r="TA2">
+        <v>11</v>
+      </c>
+      <c r="TB2">
+        <v>5</v>
+      </c>
+      <c r="TC2">
+        <v>4</v>
+      </c>
+      <c r="TD2">
+        <v>7</v>
+      </c>
+      <c r="TE2">
+        <v>35</v>
+      </c>
+      <c r="TF2">
+        <v>1</v>
+      </c>
+      <c r="TG2">
+        <v>1</v>
+      </c>
+      <c r="TH2">
+        <v>0</v>
+      </c>
+      <c r="TI2">
+        <v>0</v>
+      </c>
+      <c r="TJ2">
+        <v>20</v>
+      </c>
+      <c r="TK2">
+        <v>1</v>
+      </c>
+      <c r="TL2">
         <v>3</v>
       </c>
-      <c r="JW2">
+      <c r="TM2">
+        <v>1</v>
+      </c>
+      <c r="TN2">
+        <v>18.9</v>
+      </c>
+      <c r="TO2">
+        <v>0.25</v>
+      </c>
+      <c r="TP2">
+        <v>-3.1</v>
+      </c>
+      <c r="TQ2">
+        <v>-0.15</v>
+      </c>
+      <c r="TR2">
+        <v>110</v>
+      </c>
+      <c r="TS2">
+        <v>249</v>
+      </c>
+      <c r="TT2">
+        <v>44.2</v>
+      </c>
+      <c r="TU2">
+        <v>521</v>
+      </c>
+      <c r="TV2">
+        <v>143</v>
+      </c>
+      <c r="TW2">
+        <v>28.8</v>
+      </c>
+      <c r="TX2">
+        <v>31.2</v>
+      </c>
+      <c r="TY2">
+        <v>153</v>
+      </c>
+      <c r="TZ2">
+        <v>64.7</v>
+      </c>
+      <c r="UA2">
+        <v>48.1</v>
+      </c>
+      <c r="UB2">
+        <v>247</v>
+      </c>
+      <c r="UC2">
+        <v>15</v>
+      </c>
+      <c r="UD2">
+        <v>6.1</v>
+      </c>
+      <c r="UE2">
+        <v>26</v>
+      </c>
+      <c r="UF2">
+        <v>1.3</v>
+      </c>
+      <c r="UG2">
+        <v>17.2</v>
+      </c>
+      <c r="UH2">
+        <v>85</v>
+      </c>
+      <c r="UI2">
+        <v>7</v>
+      </c>
+      <c r="UJ2">
+        <v>32.9</v>
+      </c>
+      <c r="UK2">
+        <v>4.25</v>
+      </c>
+      <c r="UL2">
+        <v>0.12</v>
+      </c>
+      <c r="UM2">
+        <v>0.38</v>
+      </c>
+      <c r="UN2">
+        <v>0.1</v>
+      </c>
+      <c r="UO2">
+        <v>5.5</v>
+      </c>
+      <c r="UP2">
+        <v>5.9</v>
+      </c>
+      <c r="UQ2">
+        <v>7683</v>
+      </c>
+      <c r="UR2">
+        <v>9811</v>
+      </c>
+      <c r="US2">
+        <v>78.3</v>
+      </c>
+      <c r="UT2">
+        <v>135397</v>
+      </c>
+      <c r="UU2">
+        <v>52544</v>
+      </c>
+      <c r="UV2">
+        <v>3554</v>
+      </c>
+      <c r="UW2">
+        <v>4090</v>
+      </c>
+      <c r="UX2">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="UY2">
+        <v>3069</v>
+      </c>
+      <c r="UZ2">
+        <v>3670</v>
+      </c>
+      <c r="VA2">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="VB2">
+        <v>829</v>
+      </c>
+      <c r="VC2">
+        <v>1487</v>
+      </c>
+      <c r="VD2">
+        <v>55.7</v>
+      </c>
+      <c r="VE2">
+        <v>219</v>
+      </c>
+      <c r="VF2">
+        <v>582</v>
+      </c>
+      <c r="VG2">
+        <v>213</v>
+      </c>
+      <c r="VH2">
+        <v>44</v>
+      </c>
+      <c r="VI2">
+        <v>858</v>
+      </c>
+      <c r="VJ2">
+        <v>8805</v>
+      </c>
+      <c r="VK2">
+        <v>978</v>
+      </c>
+      <c r="VL2">
+        <v>229</v>
+      </c>
+      <c r="VM2">
+        <v>25</v>
+      </c>
+      <c r="VN2">
+        <v>97</v>
+      </c>
+      <c r="VO2">
+        <v>309</v>
+      </c>
+      <c r="VP2">
+        <v>83</v>
+      </c>
+      <c r="VQ2">
+        <v>33</v>
+      </c>
+      <c r="VR2">
+        <v>31</v>
+      </c>
+      <c r="VS2">
+        <v>0</v>
+      </c>
+      <c r="VT2">
+        <v>437</v>
+      </c>
+      <c r="VU2">
+        <v>28</v>
+      </c>
+      <c r="VV2">
+        <v>163</v>
+      </c>
+      <c r="VW2">
+        <v>481</v>
+      </c>
+      <c r="VX2">
+        <v>24.05</v>
+      </c>
+      <c r="VY2">
+        <v>364</v>
+      </c>
+      <c r="VZ2">
+        <v>39</v>
+      </c>
+      <c r="WA2">
+        <v>23</v>
+      </c>
+      <c r="WB2">
+        <v>27</v>
+      </c>
+      <c r="WC2">
+        <v>21</v>
+      </c>
+      <c r="WD2">
+        <v>69</v>
+      </c>
+      <c r="WE2">
+        <v>3.45</v>
+      </c>
+      <c r="WF2">
+        <v>49</v>
+      </c>
+      <c r="WG2">
+        <v>4</v>
+      </c>
+      <c r="WH2">
+        <v>1</v>
+      </c>
+      <c r="WI2">
+        <v>7</v>
+      </c>
+      <c r="WJ2">
+        <v>7</v>
+      </c>
+      <c r="WK2">
+        <v>1</v>
+      </c>
+      <c r="WL2">
+        <v>348</v>
+      </c>
+      <c r="WM2">
+        <v>197</v>
+      </c>
+      <c r="WN2">
+        <v>157</v>
+      </c>
+      <c r="WO2">
+        <v>147</v>
+      </c>
+      <c r="WP2">
+        <v>44</v>
+      </c>
+      <c r="WQ2">
+        <v>173</v>
+      </c>
+      <c r="WR2">
+        <v>311</v>
+      </c>
+      <c r="WS2">
+        <v>55.6</v>
+      </c>
+      <c r="WT2">
+        <v>138</v>
+      </c>
+      <c r="WU2">
+        <v>222</v>
+      </c>
+      <c r="WV2">
+        <v>45</v>
+      </c>
+      <c r="WW2">
+        <v>177</v>
+      </c>
+      <c r="WX2">
+        <v>230</v>
+      </c>
+      <c r="WY2">
+        <v>330</v>
+      </c>
+      <c r="WZ2">
+        <v>7</v>
+      </c>
+      <c r="XA2">
+        <v>12094</v>
+      </c>
+      <c r="XB2">
+        <v>1254</v>
+      </c>
+      <c r="XC2">
+        <v>3965</v>
+      </c>
+      <c r="XD2">
+        <v>5101</v>
+      </c>
+      <c r="XE2">
+        <v>3139</v>
+      </c>
+      <c r="XF2">
+        <v>497</v>
+      </c>
+      <c r="XG2">
+        <v>12086</v>
+      </c>
+      <c r="XH2">
+        <v>122</v>
+      </c>
+      <c r="XI2">
+        <v>333</v>
+      </c>
+      <c r="XJ2">
+        <v>36.6</v>
+      </c>
+      <c r="XK2">
+        <v>6654</v>
+      </c>
+      <c r="XL2">
+        <v>348</v>
+      </c>
+      <c r="XM2">
+        <v>274</v>
+      </c>
+      <c r="XN2">
+        <v>110</v>
+      </c>
+      <c r="XO2">
+        <v>7625</v>
+      </c>
+      <c r="XP2">
+        <v>326</v>
+      </c>
+      <c r="XQ2">
+        <v>206</v>
+      </c>
+      <c r="XR2">
+        <v>1</v>
+      </c>
+      <c r="XS2">
+        <v>248</v>
+      </c>
+      <c r="XT2">
+        <v>207</v>
+      </c>
+      <c r="XU2">
+        <v>28</v>
+      </c>
+      <c r="XV2">
+        <v>6</v>
+      </c>
+      <c r="XW2">
+        <v>1</v>
+      </c>
+      <c r="XX2">
+        <v>1</v>
+      </c>
+      <c r="XY2">
+        <v>1175</v>
+      </c>
+      <c r="XZ2">
+        <v>303</v>
+      </c>
+      <c r="YA2">
+        <v>248</v>
+      </c>
+      <c r="YB2">
+        <v>55</v>
+      </c>
+      <c r="YC2">
+        <v>24</v>
+      </c>
+      <c r="YD2">
+        <v>51</v>
+      </c>
+      <c r="YE2">
+        <v>20</v>
+      </c>
+      <c r="YF2">
+        <v>220</v>
+      </c>
+      <c r="YG2">
+        <v>1800</v>
+      </c>
+      <c r="YH2">
+        <v>22</v>
+      </c>
+      <c r="YI2">
+        <v>16</v>
+      </c>
+      <c r="YJ2">
+        <v>1</v>
+      </c>
+      <c r="YK2">
+        <v>1</v>
+      </c>
+      <c r="YL2">
+        <v>45</v>
+      </c>
+      <c r="YM2">
+        <v>0</v>
+      </c>
+      <c r="YN2">
+        <v>1.1</v>
+      </c>
+      <c r="YO2">
+        <v>0.8</v>
+      </c>
+      <c r="YP2">
+        <v>1.9</v>
+      </c>
+      <c r="YQ2">
+        <v>1.05</v>
+      </c>
+      <c r="YR2">
+        <v>1.85</v>
+      </c>
+      <c r="YS2">
+        <v>21.3</v>
+      </c>
+      <c r="YT2">
+        <v>20.5</v>
+      </c>
+      <c r="YU2">
+        <v>1.06</v>
+      </c>
+      <c r="YV2">
+        <v>1.02</v>
+      </c>
+      <c r="YW2">
+        <v>20</v>
+      </c>
+      <c r="YX2">
+        <v>20</v>
+      </c>
+      <c r="YY2">
+        <v>1800</v>
+      </c>
+      <c r="YZ2">
+        <v>39</v>
+      </c>
+      <c r="ZA2">
+        <v>1.95</v>
+      </c>
+      <c r="ZB2">
+        <v>93</v>
+      </c>
+      <c r="ZC2">
+        <v>53</v>
+      </c>
+      <c r="ZD2">
+        <v>64.5</v>
+      </c>
+      <c r="ZE2">
+        <v>4</v>
+      </c>
+      <c r="ZF2">
+        <v>5</v>
+      </c>
+      <c r="ZG2">
+        <v>11</v>
+      </c>
+      <c r="ZH2">
+        <v>1</v>
+      </c>
+      <c r="ZI2">
+        <v>5</v>
+      </c>
+      <c r="ZJ2">
+        <v>8</v>
+      </c>
+      <c r="ZK2">
+        <v>6</v>
+      </c>
+      <c r="ZL2">
         <v>2</v>
       </c>
-      <c r="JX2">
-        <v>0</v>
-      </c>
-      <c r="JY2">
-        <v>264</v>
-      </c>
-      <c r="JZ2">
-        <v>140</v>
-      </c>
-      <c r="KA2">
-        <v>124</v>
-      </c>
-      <c r="KB2">
-        <v>105</v>
-      </c>
-      <c r="KC2">
-        <v>35</v>
-      </c>
-      <c r="KD2">
-        <v>106</v>
-      </c>
-      <c r="KE2">
-        <v>211</v>
-      </c>
-      <c r="KF2">
-        <v>50.2</v>
-      </c>
-      <c r="KG2">
-        <v>105</v>
-      </c>
-      <c r="KH2">
-        <v>179</v>
-      </c>
-      <c r="KI2">
-        <v>55</v>
-      </c>
-      <c r="KJ2">
-        <v>124</v>
-      </c>
-      <c r="KK2">
+      <c r="ZM2">
+        <v>0</v>
+      </c>
+      <c r="ZN2">
+        <v>20</v>
+      </c>
+      <c r="ZO2">
+        <v>0</v>
+      </c>
+      <c r="ZP2">
+        <v>2</v>
+      </c>
+      <c r="ZQ2">
+        <v>1</v>
+      </c>
+      <c r="ZR2">
+        <v>33.6</v>
+      </c>
+      <c r="ZS2">
+        <v>0.28</v>
+      </c>
+      <c r="ZT2">
+        <v>-4.4</v>
+      </c>
+      <c r="ZU2">
+        <v>-0.22</v>
+      </c>
+      <c r="ZV2">
+        <v>101</v>
+      </c>
+      <c r="ZW2">
+        <v>312</v>
+      </c>
+      <c r="ZX2">
+        <v>32.4</v>
+      </c>
+      <c r="ZY2">
+        <v>705</v>
+      </c>
+      <c r="ZZ2">
+        <v>96</v>
+      </c>
+      <c r="AAA2">
+        <v>36.5</v>
+      </c>
+      <c r="AAB2">
+        <v>34.9</v>
+      </c>
+      <c r="AAC2">
+        <v>141</v>
+      </c>
+      <c r="AAD2">
+        <v>39</v>
+      </c>
+      <c r="AAE2">
+        <v>37.5</v>
+      </c>
+      <c r="AAF2">
+        <v>239</v>
+      </c>
+      <c r="AAG2">
+        <v>10</v>
+      </c>
+      <c r="AAH2">
+        <v>4.2</v>
+      </c>
+      <c r="AAI2">
+        <v>26</v>
+      </c>
+      <c r="AAJ2">
+        <v>1.3</v>
+      </c>
+      <c r="AAK2">
+        <v>15.5</v>
+      </c>
+      <c r="AAL2">
+        <v>73</v>
+      </c>
+      <c r="AAM2">
+        <v>6</v>
+      </c>
+      <c r="AAN2">
+        <v>30.2</v>
+      </c>
+      <c r="AAO2">
+        <v>3.65</v>
+      </c>
+      <c r="AAP2">
+        <v>0.09</v>
+      </c>
+      <c r="AAQ2">
+        <v>0.29</v>
+      </c>
+      <c r="AAR2">
+        <v>0.09</v>
+      </c>
+      <c r="AAS2">
+        <v>0.7</v>
+      </c>
+      <c r="AAT2">
+        <v>0.5</v>
+      </c>
+      <c r="AAU2">
+        <v>7944</v>
+      </c>
+      <c r="AAV2">
+        <v>10147</v>
+      </c>
+      <c r="AAW2">
+        <v>78.3</v>
+      </c>
+      <c r="AAX2">
+        <v>140518</v>
+      </c>
+      <c r="AAY2">
+        <v>52356</v>
+      </c>
+      <c r="AAZ2">
+        <v>3527</v>
+      </c>
+      <c r="ABA2">
+        <v>4009</v>
+      </c>
+      <c r="ABB2">
+        <v>88</v>
+      </c>
+      <c r="ABC2">
+        <v>3258</v>
+      </c>
+      <c r="ABD2">
+        <v>3865</v>
+      </c>
+      <c r="ABE2">
+        <v>84.3</v>
+      </c>
+      <c r="ABF2">
+        <v>884</v>
+      </c>
+      <c r="ABG2">
+        <v>1624</v>
+      </c>
+      <c r="ABH2">
+        <v>54.4</v>
+      </c>
+      <c r="ABI2">
+        <v>182</v>
+      </c>
+      <c r="ABJ2">
+        <v>570</v>
+      </c>
+      <c r="ABK2">
+        <v>152</v>
+      </c>
+      <c r="ABL2">
+        <v>41</v>
+      </c>
+      <c r="ABM2">
+        <v>688</v>
+      </c>
+      <c r="ABN2">
+        <v>9080</v>
+      </c>
+      <c r="ABO2">
+        <v>1041</v>
+      </c>
+      <c r="ABP2">
+        <v>269</v>
+      </c>
+      <c r="ABQ2">
+        <v>16</v>
+      </c>
+      <c r="ABR2">
+        <v>60</v>
+      </c>
+      <c r="ABS2">
+        <v>324</v>
+      </c>
+      <c r="ABT2">
+        <v>87</v>
+      </c>
+      <c r="ABU2">
+        <v>19</v>
+      </c>
+      <c r="ABV2">
+        <v>38</v>
+      </c>
+      <c r="ABW2">
+        <v>0</v>
+      </c>
+      <c r="ABX2">
+        <v>462</v>
+      </c>
+      <c r="ABY2">
+        <v>26</v>
+      </c>
+      <c r="ABZ2">
+        <v>192</v>
+      </c>
+      <c r="ACA2">
+        <v>424</v>
+      </c>
+      <c r="ACB2">
+        <v>21.2</v>
+      </c>
+      <c r="ACC2">
+        <v>325</v>
+      </c>
+      <c r="ACD2">
+        <v>36</v>
+      </c>
+      <c r="ACE2">
+        <v>16</v>
+      </c>
+      <c r="ACF2">
+        <v>21</v>
+      </c>
+      <c r="ACG2">
+        <v>19</v>
+      </c>
+      <c r="ACH2">
+        <v>40</v>
+      </c>
+      <c r="ACI2">
+        <v>2</v>
+      </c>
+      <c r="ACJ2">
+        <v>30</v>
+      </c>
+      <c r="ACK2">
+        <v>2</v>
+      </c>
+      <c r="ACL2">
+        <v>3</v>
+      </c>
+      <c r="ACM2">
+        <v>2</v>
+      </c>
+      <c r="ACN2">
+        <v>3</v>
+      </c>
+      <c r="ACO2">
+        <v>0</v>
+      </c>
+      <c r="ACP2">
+        <v>368</v>
+      </c>
+      <c r="ACQ2">
+        <v>220</v>
+      </c>
+      <c r="ACR2">
+        <v>200</v>
+      </c>
+      <c r="ACS2">
+        <v>126</v>
+      </c>
+      <c r="ACT2">
+        <v>42</v>
+      </c>
+      <c r="ACU2">
+        <v>162</v>
+      </c>
+      <c r="ACV2">
+        <v>284</v>
+      </c>
+      <c r="ACW2">
+        <v>57</v>
+      </c>
+      <c r="ACX2">
+        <v>122</v>
+      </c>
+      <c r="ACY2">
+        <v>222</v>
+      </c>
+      <c r="ACZ2">
+        <v>75</v>
+      </c>
+      <c r="ADA2">
+        <v>147</v>
+      </c>
+      <c r="ADB2">
+        <v>196</v>
+      </c>
+      <c r="ADC2">
+        <v>324</v>
+      </c>
+      <c r="ADD2">
+        <v>4</v>
+      </c>
+      <c r="ADE2">
+        <v>12444</v>
+      </c>
+      <c r="ADF2">
+        <v>1351</v>
+      </c>
+      <c r="ADG2">
+        <v>4299</v>
+      </c>
+      <c r="ADH2">
+        <v>5533</v>
+      </c>
+      <c r="ADI2">
+        <v>2748</v>
+      </c>
+      <c r="ADJ2">
+        <v>397</v>
+      </c>
+      <c r="ADK2">
+        <v>12443</v>
+      </c>
+      <c r="ADL2">
         <v>138</v>
       </c>
-      <c r="KL2">
-        <v>312</v>
-      </c>
-      <c r="KM2">
-        <v>7</v>
-      </c>
-      <c r="KN2">
-        <v>10853</v>
-      </c>
-      <c r="KO2">
-        <v>1253</v>
-      </c>
-      <c r="KP2">
-        <v>3826</v>
-      </c>
-      <c r="KQ2">
-        <v>4668</v>
-      </c>
-      <c r="KR2">
-        <v>2477</v>
-      </c>
-      <c r="KS2">
-        <v>378</v>
-      </c>
-      <c r="KT2">
-        <v>10849</v>
-      </c>
-      <c r="KU2">
-        <v>117</v>
-      </c>
-      <c r="KV2">
-        <v>283</v>
-      </c>
-      <c r="KW2">
-        <v>41.3</v>
-      </c>
-      <c r="KX2">
-        <v>7180</v>
-      </c>
-      <c r="KY2">
-        <v>253</v>
-      </c>
-      <c r="KZ2">
-        <v>202</v>
-      </c>
-      <c r="LA2">
+      <c r="ADM2">
+        <v>350</v>
+      </c>
+      <c r="ADN2">
+        <v>39.4</v>
+      </c>
+      <c r="ADO2">
+        <v>6961</v>
+      </c>
+      <c r="ADP2">
+        <v>317</v>
+      </c>
+      <c r="ADQ2">
+        <v>239</v>
+      </c>
+      <c r="ADR2">
+        <v>81</v>
+      </c>
+      <c r="ADS2">
+        <v>7831</v>
+      </c>
+      <c r="ADT2">
+        <v>356</v>
+      </c>
+      <c r="ADU2">
+        <v>175</v>
+      </c>
+      <c r="ADV2">
+        <v>0</v>
+      </c>
+      <c r="ADW2">
+        <v>220</v>
+      </c>
+      <c r="ADX2">
+        <v>232</v>
+      </c>
+      <c r="ADY2">
+        <v>26</v>
+      </c>
+      <c r="ADZ2">
         <v>1</v>
       </c>
-      <c r="LB2">
-        <v>199</v>
-      </c>
-      <c r="LC2">
-        <v>236</v>
-      </c>
-      <c r="LD2">
-        <v>16</v>
-      </c>
-      <c r="LE2">
-        <v>3</v>
-      </c>
-      <c r="LF2">
-        <v>4</v>
-      </c>
-      <c r="LG2">
-        <v>0</v>
-      </c>
-      <c r="LH2">
-        <v>868</v>
-      </c>
-      <c r="LI2">
-        <v>173</v>
-      </c>
-      <c r="LJ2">
-        <v>216</v>
-      </c>
-      <c r="LK2">
-        <v>44.5</v>
-      </c>
-      <c r="LL2">
-        <v>27</v>
-      </c>
-      <c r="LM2">
-        <v>51.3</v>
-      </c>
-      <c r="LN2">
-        <v>19</v>
-      </c>
-      <c r="LO2">
-        <v>209</v>
-      </c>
-      <c r="LP2">
-        <v>1710</v>
-      </c>
-      <c r="LQ2">
-        <v>29</v>
-      </c>
-      <c r="LR2">
-        <v>20</v>
-      </c>
-      <c r="LS2">
-        <v>4</v>
-      </c>
-      <c r="LT2">
-        <v>4</v>
-      </c>
-      <c r="LU2">
-        <v>39</v>
-      </c>
-      <c r="LV2">
+      <c r="AEA2">
+        <v>8</v>
+      </c>
+      <c r="AEB2">
         <v>1</v>
       </c>
-      <c r="LW2">
-        <v>1.53</v>
-      </c>
-      <c r="LX2">
-        <v>1.05</v>
-      </c>
-      <c r="LY2">
-        <v>2.58</v>
-      </c>
-      <c r="LZ2">
-        <v>1.32</v>
-      </c>
-      <c r="MA2">
-        <v>2.37</v>
-      </c>
-      <c r="MB2">
-        <v>26.7</v>
-      </c>
-      <c r="MC2">
-        <v>24</v>
-      </c>
-      <c r="MD2">
-        <v>1.4</v>
-      </c>
-      <c r="ME2">
-        <v>1.27</v>
-      </c>
-      <c r="MF2">
-        <v>19</v>
-      </c>
-      <c r="MG2">
-        <v>19</v>
-      </c>
-      <c r="MH2">
-        <v>1710</v>
-      </c>
-      <c r="MI2">
-        <v>18</v>
-      </c>
-      <c r="MJ2">
-        <v>0.95</v>
-      </c>
-      <c r="MK2">
-        <v>85</v>
-      </c>
-      <c r="ML2">
-        <v>66</v>
-      </c>
-      <c r="MM2">
-        <v>82.40000000000001</v>
-      </c>
-      <c r="MN2">
-        <v>10</v>
-      </c>
-      <c r="MO2">
-        <v>5</v>
-      </c>
-      <c r="MP2">
-        <v>4</v>
-      </c>
-      <c r="MQ2">
-        <v>7</v>
-      </c>
-      <c r="MR2">
-        <v>36.8</v>
-      </c>
-      <c r="MS2">
-        <v>4</v>
-      </c>
-      <c r="MT2">
-        <v>3</v>
-      </c>
-      <c r="MU2">
-        <v>1</v>
-      </c>
-      <c r="MV2">
-        <v>0</v>
-      </c>
-      <c r="MW2">
-        <v>19</v>
-      </c>
-      <c r="MX2">
-        <v>0</v>
-      </c>
-      <c r="MY2">
-        <v>2</v>
-      </c>
-      <c r="MZ2">
-        <v>0</v>
-      </c>
-      <c r="NA2">
-        <v>23.1</v>
-      </c>
-      <c r="NB2">
-        <v>0.23</v>
-      </c>
-      <c r="NC2">
-        <v>5.1</v>
-      </c>
-      <c r="ND2">
-        <v>0.27</v>
-      </c>
-      <c r="NE2">
-        <v>105</v>
-      </c>
-      <c r="NF2">
-        <v>245</v>
-      </c>
-      <c r="NG2">
-        <v>42.9</v>
-      </c>
-      <c r="NH2">
-        <v>590</v>
-      </c>
-      <c r="NI2">
-        <v>98</v>
-      </c>
-      <c r="NJ2">
-        <v>31.5</v>
-      </c>
-      <c r="NK2">
-        <v>31.1</v>
-      </c>
-      <c r="NL2">
-        <v>129</v>
-      </c>
-      <c r="NM2">
-        <v>45.7</v>
-      </c>
-      <c r="NN2">
-        <v>39.4</v>
-      </c>
-      <c r="NO2">
-        <v>225</v>
-      </c>
-      <c r="NP2">
-        <v>7</v>
-      </c>
-      <c r="NQ2">
-        <v>3.1</v>
-      </c>
-      <c r="NR2">
-        <v>17</v>
-      </c>
-      <c r="NS2">
-        <v>0.89</v>
-      </c>
-      <c r="NT2">
-        <v>15.3</v>
-      </c>
-      <c r="NU2">
-        <v>55</v>
-      </c>
-      <c r="NV2">
-        <v>11</v>
-      </c>
-      <c r="NW2">
-        <v>24</v>
-      </c>
-      <c r="NX2">
-        <v>2.89</v>
-      </c>
-      <c r="NY2">
-        <v>0.11</v>
-      </c>
-      <c r="NZ2">
-        <v>0.45</v>
-      </c>
-      <c r="OA2">
-        <v>0.11</v>
-      </c>
-      <c r="OB2">
-        <v>2.3</v>
-      </c>
-      <c r="OC2">
-        <v>1</v>
-      </c>
-      <c r="OD2">
-        <v>7741</v>
-      </c>
-      <c r="OE2">
-        <v>9524</v>
-      </c>
-      <c r="OF2">
-        <v>81.3</v>
-      </c>
-      <c r="OG2">
-        <v>139385</v>
-      </c>
-      <c r="OH2">
-        <v>50191</v>
-      </c>
-      <c r="OI2">
-        <v>3312</v>
-      </c>
-      <c r="OJ2">
-        <v>3704</v>
-      </c>
-      <c r="OK2">
-        <v>89.40000000000001</v>
-      </c>
-      <c r="OL2">
-        <v>3380</v>
-      </c>
-      <c r="OM2">
-        <v>3829</v>
-      </c>
-      <c r="ON2">
-        <v>88.3</v>
-      </c>
-      <c r="OO2">
-        <v>834</v>
-      </c>
-      <c r="OP2">
-        <v>1448</v>
-      </c>
-      <c r="OQ2">
-        <v>57.6</v>
-      </c>
-      <c r="OR2">
-        <v>180</v>
-      </c>
-      <c r="OS2">
-        <v>557</v>
-      </c>
-      <c r="OT2">
-        <v>182</v>
-      </c>
-      <c r="OU2">
-        <v>54</v>
-      </c>
-      <c r="OV2">
-        <v>527</v>
-      </c>
-      <c r="OW2">
-        <v>8616</v>
-      </c>
-      <c r="OX2">
-        <v>846</v>
-      </c>
-      <c r="OY2">
-        <v>199</v>
-      </c>
-      <c r="OZ2">
-        <v>28</v>
-      </c>
-      <c r="PA2">
-        <v>85</v>
-      </c>
-      <c r="PB2">
-        <v>327</v>
-      </c>
-      <c r="PC2">
-        <v>84</v>
-      </c>
-      <c r="PD2">
-        <v>26</v>
-      </c>
-      <c r="PE2">
-        <v>37</v>
-      </c>
-      <c r="PF2">
-        <v>0</v>
-      </c>
-      <c r="PG2">
-        <v>372</v>
-      </c>
-      <c r="PH2">
-        <v>62</v>
-      </c>
-      <c r="PI2">
-        <v>154</v>
-      </c>
-      <c r="PJ2">
-        <v>415</v>
-      </c>
-      <c r="PK2">
-        <v>21.84</v>
-      </c>
-      <c r="PL2">
-        <v>321</v>
-      </c>
-      <c r="PM2">
-        <v>38</v>
-      </c>
-      <c r="PN2">
-        <v>12</v>
-      </c>
-      <c r="PO2">
-        <v>20</v>
-      </c>
-      <c r="PP2">
-        <v>16</v>
-      </c>
-      <c r="PQ2">
-        <v>46</v>
-      </c>
-      <c r="PR2">
-        <v>2.42</v>
-      </c>
-      <c r="PS2">
-        <v>35</v>
-      </c>
-      <c r="PT2">
-        <v>1</v>
-      </c>
-      <c r="PU2">
-        <v>3</v>
-      </c>
-      <c r="PV2">
-        <v>5</v>
-      </c>
-      <c r="PW2">
-        <v>2</v>
-      </c>
-      <c r="PX2">
-        <v>0</v>
-      </c>
-      <c r="PY2">
-        <v>334</v>
-      </c>
-      <c r="PZ2">
-        <v>177</v>
-      </c>
-      <c r="QA2">
-        <v>162</v>
-      </c>
-      <c r="QB2">
-        <v>131</v>
-      </c>
-      <c r="QC2">
-        <v>41</v>
-      </c>
-      <c r="QD2">
-        <v>132</v>
-      </c>
-      <c r="QE2">
-        <v>249</v>
-      </c>
-      <c r="QF2">
-        <v>53</v>
-      </c>
-      <c r="QG2">
-        <v>117</v>
-      </c>
-      <c r="QH2">
-        <v>219</v>
-      </c>
-      <c r="QI2">
-        <v>69</v>
-      </c>
-      <c r="QJ2">
-        <v>150</v>
-      </c>
-      <c r="QK2">
-        <v>169</v>
-      </c>
-      <c r="QL2">
-        <v>305</v>
-      </c>
-      <c r="QM2">
-        <v>5</v>
-      </c>
-      <c r="QN2">
-        <v>11422</v>
-      </c>
-      <c r="QO2">
-        <v>1285</v>
-      </c>
-      <c r="QP2">
-        <v>3975</v>
-      </c>
-      <c r="QQ2">
-        <v>4912</v>
-      </c>
-      <c r="QR2">
-        <v>2648</v>
-      </c>
-      <c r="QS2">
-        <v>413</v>
-      </c>
-      <c r="QT2">
-        <v>11418</v>
-      </c>
-      <c r="QU2">
-        <v>105</v>
-      </c>
-      <c r="QV2">
-        <v>241</v>
-      </c>
-      <c r="QW2">
-        <v>43.6</v>
-      </c>
-      <c r="QX2">
-        <v>7636</v>
-      </c>
-      <c r="QY2">
-        <v>260</v>
-      </c>
-      <c r="QZ2">
-        <v>158</v>
-      </c>
-      <c r="RA2">
-        <v>1</v>
-      </c>
-      <c r="RB2">
-        <v>249</v>
-      </c>
-      <c r="RC2">
-        <v>182</v>
-      </c>
-      <c r="RD2">
-        <v>62</v>
-      </c>
-      <c r="RE2">
-        <v>2</v>
-      </c>
-      <c r="RF2">
-        <v>4</v>
-      </c>
-      <c r="RG2">
-        <v>0</v>
-      </c>
-      <c r="RH2">
-        <v>986</v>
-      </c>
-      <c r="RI2">
-        <v>216</v>
-      </c>
-      <c r="RJ2">
-        <v>173</v>
-      </c>
-      <c r="RK2">
-        <v>55.5</v>
-      </c>
-      <c r="RL2" t="s">
-        <v>794</v>
-      </c>
-      <c r="RM2">
-        <v>24</v>
-      </c>
-      <c r="RN2">
-        <v>48.4</v>
-      </c>
-      <c r="RO2">
-        <v>19</v>
-      </c>
-      <c r="RP2">
-        <v>209</v>
-      </c>
-      <c r="RQ2">
-        <v>1710</v>
-      </c>
-      <c r="RR2">
-        <v>36</v>
-      </c>
-      <c r="RS2">
-        <v>25</v>
-      </c>
-      <c r="RT2">
-        <v>6</v>
-      </c>
-      <c r="RU2">
-        <v>8</v>
-      </c>
-      <c r="RV2">
-        <v>51</v>
-      </c>
-      <c r="RW2">
-        <v>1</v>
-      </c>
-      <c r="RX2">
-        <v>1.89</v>
-      </c>
-      <c r="RY2">
-        <v>1.32</v>
-      </c>
-      <c r="RZ2">
-        <v>3.21</v>
-      </c>
-      <c r="SA2">
-        <v>1.58</v>
-      </c>
-      <c r="SB2">
-        <v>2.89</v>
-      </c>
-      <c r="SC2">
-        <v>30.7</v>
-      </c>
-      <c r="SD2">
-        <v>24.3</v>
-      </c>
-      <c r="SE2">
-        <v>1.62</v>
-      </c>
-      <c r="SF2">
-        <v>1.28</v>
-      </c>
-      <c r="SG2">
-        <v>19</v>
-      </c>
-      <c r="SH2">
-        <v>19</v>
-      </c>
-      <c r="SI2">
-        <v>1710</v>
-      </c>
-      <c r="SJ2">
-        <v>23</v>
-      </c>
-      <c r="SK2">
-        <v>1.21</v>
-      </c>
-      <c r="SL2">
-        <v>69</v>
-      </c>
-      <c r="SM2">
-        <v>47</v>
-      </c>
-      <c r="SN2">
-        <v>68.09999999999999</v>
-      </c>
-      <c r="SO2">
-        <v>9</v>
-      </c>
-      <c r="SP2">
-        <v>5</v>
-      </c>
-      <c r="SQ2">
-        <v>4</v>
-      </c>
-      <c r="SR2">
-        <v>6</v>
-      </c>
-      <c r="SS2">
-        <v>31.6</v>
-      </c>
-      <c r="ST2">
-        <v>1</v>
-      </c>
-      <c r="SU2">
-        <v>1</v>
-      </c>
-      <c r="SV2">
-        <v>0</v>
-      </c>
-      <c r="SW2">
-        <v>0</v>
-      </c>
-      <c r="SX2">
-        <v>19</v>
-      </c>
-      <c r="SY2">
-        <v>1</v>
-      </c>
-      <c r="SZ2">
-        <v>3</v>
-      </c>
-      <c r="TA2">
-        <v>1</v>
-      </c>
-      <c r="TB2">
-        <v>18.2</v>
-      </c>
-      <c r="TC2">
-        <v>0.25</v>
-      </c>
-      <c r="TD2">
-        <v>-3.8</v>
-      </c>
-      <c r="TE2">
-        <v>-0.2</v>
-      </c>
-      <c r="TF2">
-        <v>109</v>
-      </c>
-      <c r="TG2">
-        <v>244</v>
-      </c>
-      <c r="TH2">
-        <v>44.7</v>
-      </c>
-      <c r="TI2">
-        <v>502</v>
-      </c>
-      <c r="TJ2">
-        <v>138</v>
-      </c>
-      <c r="TK2">
-        <v>29.1</v>
-      </c>
-      <c r="TL2">
-        <v>31.4</v>
-      </c>
-      <c r="TM2">
-        <v>147</v>
-      </c>
-      <c r="TN2">
-        <v>66.7</v>
-      </c>
-      <c r="TO2">
-        <v>49.2</v>
-      </c>
-      <c r="TP2">
-        <v>233</v>
-      </c>
-      <c r="TQ2">
-        <v>15</v>
-      </c>
-      <c r="TR2">
-        <v>6.4</v>
-      </c>
-      <c r="TS2">
-        <v>24</v>
-      </c>
-      <c r="TT2">
-        <v>1.26</v>
-      </c>
-      <c r="TU2">
-        <v>17</v>
-      </c>
-      <c r="TV2">
-        <v>80</v>
-      </c>
-      <c r="TW2">
-        <v>6</v>
-      </c>
-      <c r="TX2">
-        <v>33.8</v>
-      </c>
-      <c r="TY2">
-        <v>4.21</v>
-      </c>
-      <c r="TZ2">
-        <v>0.13</v>
-      </c>
-      <c r="UA2">
-        <v>0.38</v>
-      </c>
-      <c r="UB2">
-        <v>0.1</v>
-      </c>
-      <c r="UC2">
-        <v>5.3</v>
-      </c>
-      <c r="UD2">
-        <v>5.7</v>
-      </c>
-      <c r="UE2">
-        <v>7096</v>
-      </c>
-      <c r="UF2">
-        <v>9133</v>
-      </c>
-      <c r="UG2">
-        <v>77.7</v>
-      </c>
-      <c r="UH2">
-        <v>126171</v>
-      </c>
-      <c r="UI2">
-        <v>49246</v>
-      </c>
-      <c r="UJ2">
-        <v>3245</v>
-      </c>
-      <c r="UK2">
-        <v>3751</v>
-      </c>
-      <c r="UL2">
-        <v>86.5</v>
-      </c>
-      <c r="UM2">
-        <v>2837</v>
-      </c>
-      <c r="UN2">
-        <v>3411</v>
-      </c>
-      <c r="UO2">
-        <v>83.2</v>
-      </c>
-      <c r="UP2">
-        <v>797</v>
-      </c>
-      <c r="UQ2">
-        <v>1439</v>
-      </c>
-      <c r="UR2">
-        <v>55.4</v>
-      </c>
-      <c r="US2">
-        <v>200</v>
-      </c>
-      <c r="UT2">
-        <v>534</v>
-      </c>
-      <c r="UU2">
-        <v>194</v>
-      </c>
-      <c r="UV2">
-        <v>40</v>
-      </c>
-      <c r="UW2">
-        <v>586</v>
-      </c>
-      <c r="UX2">
-        <v>8171</v>
-      </c>
-      <c r="UY2">
-        <v>935</v>
-      </c>
-      <c r="UZ2">
-        <v>218</v>
-      </c>
-      <c r="VA2">
-        <v>25</v>
-      </c>
-      <c r="VB2">
-        <v>95</v>
-      </c>
-      <c r="VC2">
-        <v>292</v>
-      </c>
-      <c r="VD2">
-        <v>76</v>
-      </c>
-      <c r="VE2">
-        <v>29</v>
-      </c>
-      <c r="VF2">
-        <v>31</v>
-      </c>
-      <c r="VG2">
-        <v>0</v>
-      </c>
-      <c r="VH2">
-        <v>420</v>
-      </c>
-      <c r="VI2">
-        <v>27</v>
-      </c>
-      <c r="VJ2">
-        <v>156</v>
-      </c>
-      <c r="VK2">
-        <v>443</v>
-      </c>
-      <c r="VL2">
-        <v>23.32</v>
-      </c>
-      <c r="VM2">
-        <v>337</v>
-      </c>
-      <c r="VN2">
-        <v>36</v>
-      </c>
-      <c r="VO2">
-        <v>18</v>
-      </c>
-      <c r="VP2">
-        <v>25</v>
-      </c>
-      <c r="VQ2">
-        <v>20</v>
-      </c>
-      <c r="VR2">
-        <v>65</v>
-      </c>
-      <c r="VS2">
-        <v>3.42</v>
-      </c>
-      <c r="VT2">
-        <v>47</v>
-      </c>
-      <c r="VU2">
-        <v>4</v>
-      </c>
-      <c r="VV2">
-        <v>0</v>
-      </c>
-      <c r="VW2">
-        <v>6</v>
-      </c>
-      <c r="VX2">
-        <v>7</v>
-      </c>
-      <c r="VY2">
-        <v>1</v>
-      </c>
-      <c r="VZ2">
-        <v>333</v>
-      </c>
-      <c r="WA2">
-        <v>186</v>
-      </c>
-      <c r="WB2">
-        <v>146</v>
-      </c>
-      <c r="WC2">
-        <v>145</v>
-      </c>
-      <c r="WD2">
-        <v>42</v>
-      </c>
-      <c r="WE2">
-        <v>166</v>
-      </c>
-      <c r="WF2">
-        <v>295</v>
-      </c>
-      <c r="WG2">
-        <v>56.3</v>
-      </c>
-      <c r="WH2">
-        <v>129</v>
-      </c>
-      <c r="WI2">
-        <v>205</v>
-      </c>
-      <c r="WJ2">
-        <v>43</v>
-      </c>
-      <c r="WK2">
-        <v>162</v>
-      </c>
-      <c r="WL2">
-        <v>221</v>
-      </c>
-      <c r="WM2">
-        <v>309</v>
-      </c>
-      <c r="WN2">
-        <v>7</v>
-      </c>
-      <c r="WO2">
-        <v>11218</v>
-      </c>
-      <c r="WP2">
-        <v>1194</v>
-      </c>
-      <c r="WQ2">
-        <v>3758</v>
-      </c>
-      <c r="WR2">
-        <v>4697</v>
-      </c>
-      <c r="WS2">
-        <v>2876</v>
-      </c>
-      <c r="WT2">
-        <v>448</v>
-      </c>
-      <c r="WU2">
-        <v>11210</v>
-      </c>
-      <c r="WV2">
-        <v>110</v>
-      </c>
-      <c r="WW2">
-        <v>307</v>
-      </c>
-      <c r="WX2">
-        <v>35.8</v>
-      </c>
-      <c r="WY2">
-        <v>7018</v>
-      </c>
-      <c r="WZ2">
-        <v>307</v>
-      </c>
-      <c r="XA2">
-        <v>194</v>
-      </c>
-      <c r="XB2">
-        <v>1</v>
-      </c>
-      <c r="XC2">
-        <v>231</v>
-      </c>
-      <c r="XD2">
-        <v>196</v>
-      </c>
-      <c r="XE2">
-        <v>27</v>
-      </c>
-      <c r="XF2">
-        <v>6</v>
-      </c>
-      <c r="XG2">
-        <v>1</v>
-      </c>
-      <c r="XH2">
-        <v>1</v>
-      </c>
-      <c r="XI2">
-        <v>1117</v>
-      </c>
-      <c r="XJ2">
-        <v>279</v>
-      </c>
-      <c r="XK2">
-        <v>239</v>
-      </c>
-      <c r="XL2">
-        <v>53.9</v>
-      </c>
-      <c r="XM2">
-        <v>24</v>
-      </c>
-      <c r="XN2">
-        <v>51.6</v>
-      </c>
-      <c r="XO2">
-        <v>19</v>
-      </c>
-      <c r="XP2">
-        <v>209</v>
-      </c>
-      <c r="XQ2">
-        <v>1710</v>
-      </c>
-      <c r="XR2">
-        <v>22</v>
-      </c>
-      <c r="XS2">
-        <v>16</v>
-      </c>
-      <c r="XT2">
-        <v>1</v>
-      </c>
-      <c r="XU2">
-        <v>1</v>
-      </c>
-      <c r="XV2">
-        <v>43</v>
-      </c>
-      <c r="XW2">
-        <v>0</v>
-      </c>
-      <c r="XX2">
-        <v>1.16</v>
-      </c>
-      <c r="XY2">
-        <v>0.84</v>
-      </c>
-      <c r="XZ2">
-        <v>2</v>
-      </c>
-      <c r="YA2">
-        <v>1.11</v>
-      </c>
-      <c r="YB2">
-        <v>1.95</v>
-      </c>
-      <c r="YC2">
-        <v>20.5</v>
-      </c>
-      <c r="YD2">
-        <v>19.7</v>
-      </c>
-      <c r="YE2">
-        <v>1.08</v>
-      </c>
-      <c r="YF2">
-        <v>1.04</v>
-      </c>
-      <c r="YG2">
-        <v>19</v>
-      </c>
-      <c r="YH2">
-        <v>19</v>
-      </c>
-      <c r="YI2">
-        <v>1710</v>
-      </c>
-      <c r="YJ2">
-        <v>37</v>
-      </c>
-      <c r="YK2">
-        <v>1.95</v>
-      </c>
-      <c r="YL2">
-        <v>88</v>
-      </c>
-      <c r="YM2">
-        <v>50</v>
-      </c>
-      <c r="YN2">
-        <v>64.8</v>
-      </c>
-      <c r="YO2">
-        <v>4</v>
-      </c>
-      <c r="YP2">
-        <v>5</v>
-      </c>
-      <c r="YQ2">
-        <v>10</v>
-      </c>
-      <c r="YR2">
-        <v>1</v>
-      </c>
-      <c r="YS2">
-        <v>5.3</v>
-      </c>
-      <c r="YT2">
-        <v>8</v>
-      </c>
-      <c r="YU2">
-        <v>6</v>
-      </c>
-      <c r="YV2">
-        <v>2</v>
-      </c>
-      <c r="YW2">
-        <v>0</v>
-      </c>
-      <c r="YX2">
-        <v>19</v>
-      </c>
-      <c r="YY2">
-        <v>0</v>
-      </c>
-      <c r="YZ2">
-        <v>2</v>
-      </c>
-      <c r="ZA2">
-        <v>1</v>
-      </c>
-      <c r="ZB2">
-        <v>32.4</v>
-      </c>
-      <c r="ZC2">
-        <v>0.28</v>
-      </c>
-      <c r="ZD2">
-        <v>-3.6</v>
-      </c>
-      <c r="ZE2">
-        <v>-0.19</v>
-      </c>
-      <c r="ZF2">
-        <v>94</v>
-      </c>
-      <c r="ZG2">
-        <v>289</v>
-      </c>
-      <c r="ZH2">
-        <v>32.5</v>
-      </c>
-      <c r="ZI2">
-        <v>681</v>
-      </c>
-      <c r="ZJ2">
-        <v>96</v>
-      </c>
-      <c r="ZK2">
-        <v>35.5</v>
-      </c>
-      <c r="ZL2">
-        <v>34.7</v>
-      </c>
-      <c r="ZM2">
-        <v>129</v>
-      </c>
-      <c r="ZN2">
-        <v>36.4</v>
-      </c>
-      <c r="ZO2">
-        <v>36.3</v>
-      </c>
-      <c r="ZP2">
-        <v>226</v>
-      </c>
-      <c r="ZQ2">
-        <v>10</v>
-      </c>
-      <c r="ZR2">
-        <v>4.4</v>
-      </c>
-      <c r="ZS2">
-        <v>26</v>
-      </c>
-      <c r="ZT2">
-        <v>1.37</v>
-      </c>
-      <c r="ZU2">
-        <v>15.5</v>
-      </c>
-      <c r="ZV2">
-        <v>68</v>
-      </c>
-      <c r="ZW2">
-        <v>6</v>
-      </c>
-      <c r="ZX2">
-        <v>30</v>
-      </c>
-      <c r="ZY2">
-        <v>3.58</v>
-      </c>
-      <c r="ZZ2">
-        <v>0.09</v>
-      </c>
-      <c r="AAA2">
-        <v>0.31</v>
-      </c>
-      <c r="AAB2">
-        <v>0.09</v>
-      </c>
-      <c r="AAC2">
-        <v>1.5</v>
-      </c>
-      <c r="AAD2">
-        <v>1.3</v>
-      </c>
-      <c r="AAE2">
-        <v>7636</v>
-      </c>
-      <c r="AAF2">
-        <v>9720</v>
-      </c>
-      <c r="AAG2">
-        <v>78.59999999999999</v>
-      </c>
-      <c r="AAH2">
-        <v>135321</v>
-      </c>
-      <c r="AAI2">
-        <v>50211</v>
-      </c>
-      <c r="AAJ2">
-        <v>3381</v>
-      </c>
-      <c r="AAK2">
-        <v>3844</v>
-      </c>
-      <c r="AAL2">
-        <v>88</v>
-      </c>
-      <c r="AAM2">
-        <v>3141</v>
-      </c>
-      <c r="AAN2">
-        <v>3722</v>
-      </c>
-      <c r="AAO2">
-        <v>84.40000000000001</v>
-      </c>
-      <c r="AAP2">
-        <v>848</v>
-      </c>
-      <c r="AAQ2">
-        <v>1546</v>
-      </c>
-      <c r="AAR2">
-        <v>54.9</v>
-      </c>
-      <c r="AAS2">
-        <v>173</v>
-      </c>
-      <c r="AAT2">
-        <v>554</v>
-      </c>
-      <c r="AAU2">
-        <v>147</v>
-      </c>
-      <c r="AAV2">
-        <v>39</v>
-      </c>
-      <c r="AAW2">
-        <v>528</v>
-      </c>
-      <c r="AAX2">
-        <v>8718</v>
-      </c>
-      <c r="AAY2">
-        <v>977</v>
-      </c>
-      <c r="AAZ2">
-        <v>251</v>
-      </c>
-      <c r="ABA2">
-        <v>15</v>
-      </c>
-      <c r="ABB2">
-        <v>60</v>
-      </c>
-      <c r="ABC2">
-        <v>307</v>
-      </c>
-      <c r="ABD2">
-        <v>83</v>
-      </c>
-      <c r="ABE2">
-        <v>18</v>
-      </c>
-      <c r="ABF2">
-        <v>35</v>
-      </c>
-      <c r="ABG2">
-        <v>0</v>
-      </c>
-      <c r="ABH2">
-        <v>435</v>
-      </c>
-      <c r="ABI2">
-        <v>25</v>
-      </c>
-      <c r="ABJ2">
-        <v>176</v>
-      </c>
-      <c r="ABK2">
-        <v>403</v>
-      </c>
-      <c r="ABL2">
-        <v>21.21</v>
-      </c>
-      <c r="ABM2">
-        <v>309</v>
-      </c>
-      <c r="ABN2">
-        <v>34</v>
-      </c>
-      <c r="ABO2">
-        <v>16</v>
-      </c>
-      <c r="ABP2">
-        <v>18</v>
-      </c>
-      <c r="ABQ2">
-        <v>19</v>
-      </c>
-      <c r="ABR2">
-        <v>40</v>
-      </c>
-      <c r="ABS2">
-        <v>2.11</v>
-      </c>
-      <c r="ABT2">
-        <v>30</v>
-      </c>
-      <c r="ABU2">
-        <v>2</v>
-      </c>
-      <c r="ABV2">
-        <v>3</v>
-      </c>
-      <c r="ABW2">
-        <v>2</v>
-      </c>
-      <c r="ABX2">
-        <v>3</v>
-      </c>
-      <c r="ABY2">
-        <v>0</v>
-      </c>
-      <c r="ABZ2">
-        <v>345</v>
-      </c>
-      <c r="ACA2">
-        <v>205</v>
-      </c>
-      <c r="ACB2">
-        <v>186</v>
-      </c>
-      <c r="ACC2">
-        <v>118</v>
-      </c>
-      <c r="ACD2">
-        <v>41</v>
-      </c>
-      <c r="ACE2">
-        <v>151</v>
-      </c>
-      <c r="ACF2">
-        <v>261</v>
-      </c>
-      <c r="ACG2">
-        <v>57.9</v>
-      </c>
-      <c r="ACH2">
-        <v>110</v>
-      </c>
-      <c r="ACI2">
-        <v>211</v>
-      </c>
-      <c r="ACJ2">
-        <v>70</v>
-      </c>
-      <c r="ACK2">
-        <v>141</v>
-      </c>
-      <c r="ACL2">
-        <v>192</v>
-      </c>
-      <c r="ACM2">
-        <v>309</v>
-      </c>
-      <c r="ACN2">
-        <v>4</v>
-      </c>
-      <c r="ACO2">
-        <v>11842</v>
-      </c>
-      <c r="ACP2">
-        <v>1296</v>
-      </c>
-      <c r="ACQ2">
-        <v>4092</v>
-      </c>
-      <c r="ACR2">
-        <v>5295</v>
-      </c>
-      <c r="ACS2">
-        <v>2589</v>
-      </c>
-      <c r="ACT2">
-        <v>375</v>
-      </c>
-      <c r="ACU2">
-        <v>11841</v>
-      </c>
-      <c r="ACV2">
-        <v>129</v>
-      </c>
-      <c r="ACW2">
-        <v>332</v>
-      </c>
-      <c r="ACX2">
-        <v>38.9</v>
-      </c>
-      <c r="ACY2">
-        <v>7497</v>
-      </c>
-      <c r="ACZ2">
-        <v>343</v>
-      </c>
-      <c r="ADA2">
-        <v>167</v>
-      </c>
-      <c r="ADB2">
-        <v>0</v>
-      </c>
-      <c r="ADC2">
-        <v>209</v>
-      </c>
-      <c r="ADD2">
-        <v>218</v>
-      </c>
-      <c r="ADE2">
-        <v>25</v>
-      </c>
-      <c r="ADF2">
-        <v>1</v>
-      </c>
-      <c r="ADG2">
-        <v>8</v>
-      </c>
-      <c r="ADH2">
-        <v>1</v>
-      </c>
-      <c r="ADI2">
-        <v>1165</v>
-      </c>
-      <c r="ADJ2">
-        <v>239</v>
-      </c>
-      <c r="ADK2">
-        <v>279</v>
-      </c>
-      <c r="ADL2">
-        <v>46.1</v>
+      <c r="AEC2">
+        <v>1214</v>
+      </c>
+      <c r="AED2">
+        <v>248</v>
+      </c>
+      <c r="AEE2">
+        <v>303</v>
+      </c>
+      <c r="AEF2">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update matchday 22 + code fixed for new FBRef data and Fantacalcio probable lineups
</commit_message>
<xml_diff>
--- a/tmp/playermatchdata.xlsx
+++ b/tmp/playermatchdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="769">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -235,9 +235,6 @@
     <t>sca_passes_dead</t>
   </si>
   <si>
-    <t>sca_dribbles</t>
-  </si>
-  <si>
     <t>sca_shots</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t>gca_passes_dead</t>
   </si>
   <si>
-    <t>gca_dribbles</t>
-  </si>
-  <si>
     <t>gca_shots</t>
   </si>
   <si>
@@ -283,18 +277,6 @@
     <t>tackles_att_3rd</t>
   </si>
   <si>
-    <t>dribble_tackles</t>
-  </si>
-  <si>
-    <t>dribbles_vs</t>
-  </si>
-  <si>
-    <t>dribble_tackles_pct</t>
-  </si>
-  <si>
-    <t>dribbled_past</t>
-  </si>
-  <si>
     <t>blocks</t>
   </si>
   <si>
@@ -334,15 +316,6 @@
     <t>touches_live_ball</t>
   </si>
   <si>
-    <t>dribbles_completed</t>
-  </si>
-  <si>
-    <t>dribbles</t>
-  </si>
-  <si>
-    <t>dribbles_completed_pct</t>
-  </si>
-  <si>
     <t>carries</t>
   </si>
   <si>
@@ -841,9 +814,6 @@
     <t>team_sca_passes_dead</t>
   </si>
   <si>
-    <t>team_sca_dribbles</t>
-  </si>
-  <si>
     <t>team_sca_shots</t>
   </si>
   <si>
@@ -862,9 +832,6 @@
     <t>team_gca_passes_dead</t>
   </si>
   <si>
-    <t>team_gca_dribbles</t>
-  </si>
-  <si>
     <t>team_gca_shots</t>
   </si>
   <si>
@@ -889,18 +856,6 @@
     <t>team_tackles_att_3rd</t>
   </si>
   <si>
-    <t>team_dribble_tackles</t>
-  </si>
-  <si>
-    <t>team_dribbles_vs</t>
-  </si>
-  <si>
-    <t>team_dribble_tackles_pct</t>
-  </si>
-  <si>
-    <t>team_dribbled_past</t>
-  </si>
-  <si>
     <t>team_blocks</t>
   </si>
   <si>
@@ -940,15 +895,6 @@
     <t>team_touches_live_ball</t>
   </si>
   <si>
-    <t>team_dribbles_completed</t>
-  </si>
-  <si>
-    <t>team_dribbles</t>
-  </si>
-  <si>
-    <t>team_dribbles_completed_pct</t>
-  </si>
-  <si>
     <t>team_carries</t>
   </si>
   <si>
@@ -1321,9 +1267,6 @@
     <t>vs_team_sca_passes_dead</t>
   </si>
   <si>
-    <t>vs_team_sca_dribbles</t>
-  </si>
-  <si>
     <t>vs_team_sca_shots</t>
   </si>
   <si>
@@ -1342,9 +1285,6 @@
     <t>vs_team_gca_passes_dead</t>
   </si>
   <si>
-    <t>vs_team_gca_dribbles</t>
-  </si>
-  <si>
     <t>vs_team_gca_shots</t>
   </si>
   <si>
@@ -1369,18 +1309,6 @@
     <t>vs_team_tackles_att_3rd</t>
   </si>
   <si>
-    <t>vs_team_dribble_tackles</t>
-  </si>
-  <si>
-    <t>vs_team_dribbles_vs</t>
-  </si>
-  <si>
-    <t>vs_team_dribble_tackles_pct</t>
-  </si>
-  <si>
-    <t>vs_team_dribbled_past</t>
-  </si>
-  <si>
     <t>vs_team_blocks</t>
   </si>
   <si>
@@ -1420,15 +1348,6 @@
     <t>vs_team_touches_live_ball</t>
   </si>
   <si>
-    <t>vs_team_dribbles_completed</t>
-  </si>
-  <si>
-    <t>vs_team_dribbles</t>
-  </si>
-  <si>
-    <t>vs_team_dribbles_completed_pct</t>
-  </si>
-  <si>
     <t>vs_team_carries</t>
   </si>
   <si>
@@ -1804,9 +1723,6 @@
     <t>opp_team_sca_passes_dead</t>
   </si>
   <si>
-    <t>opp_team_sca_dribbles</t>
-  </si>
-  <si>
     <t>opp_team_sca_shots</t>
   </si>
   <si>
@@ -1825,9 +1741,6 @@
     <t>opp_team_gca_passes_dead</t>
   </si>
   <si>
-    <t>opp_team_gca_dribbles</t>
-  </si>
-  <si>
     <t>opp_team_gca_shots</t>
   </si>
   <si>
@@ -1852,18 +1765,6 @@
     <t>opp_team_tackles_att_3rd</t>
   </si>
   <si>
-    <t>opp_team_dribble_tackles</t>
-  </si>
-  <si>
-    <t>opp_team_dribbles_vs</t>
-  </si>
-  <si>
-    <t>opp_team_dribble_tackles_pct</t>
-  </si>
-  <si>
-    <t>opp_team_dribbled_past</t>
-  </si>
-  <si>
     <t>opp_team_blocks</t>
   </si>
   <si>
@@ -1903,15 +1804,6 @@
     <t>opp_team_touches_live_ball</t>
   </si>
   <si>
-    <t>opp_team_dribbles_completed</t>
-  </si>
-  <si>
-    <t>opp_team_dribbles</t>
-  </si>
-  <si>
-    <t>opp_team_dribbles_completed_pct</t>
-  </si>
-  <si>
     <t>opp_team_carries</t>
   </si>
   <si>
@@ -2284,9 +2176,6 @@
     <t>opp_vs_team_sca_passes_dead</t>
   </si>
   <si>
-    <t>opp_vs_team_sca_dribbles</t>
-  </si>
-  <si>
     <t>opp_vs_team_sca_shots</t>
   </si>
   <si>
@@ -2305,9 +2194,6 @@
     <t>opp_vs_team_gca_passes_dead</t>
   </si>
   <si>
-    <t>opp_vs_team_gca_dribbles</t>
-  </si>
-  <si>
     <t>opp_vs_team_gca_shots</t>
   </si>
   <si>
@@ -2332,18 +2218,6 @@
     <t>opp_vs_team_tackles_att_3rd</t>
   </si>
   <si>
-    <t>opp_vs_team_dribble_tackles</t>
-  </si>
-  <si>
-    <t>opp_vs_team_dribbles_vs</t>
-  </si>
-  <si>
-    <t>opp_vs_team_dribble_tackles_pct</t>
-  </si>
-  <si>
-    <t>opp_vs_team_dribbled_past</t>
-  </si>
-  <si>
     <t>opp_vs_team_blocks</t>
   </si>
   <si>
@@ -2383,15 +2257,6 @@
     <t>opp_vs_team_touches_live_ball</t>
   </si>
   <si>
-    <t>opp_vs_team_dribbles_completed</t>
-  </si>
-  <si>
-    <t>opp_vs_team_dribbles</t>
-  </si>
-  <si>
-    <t>opp_vs_team_dribbles_completed_pct</t>
-  </si>
-  <si>
     <t>opp_vs_team_carries</t>
   </si>
   <si>
@@ -2446,16 +2311,13 @@
     <t>opp_vs_team_aerials_won_pct</t>
   </si>
   <si>
-    <t>Frattesi</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Sassuolo</t>
-  </si>
-  <si>
-    <t>23-105</t>
+    <t>Immobile</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Lazio</t>
   </si>
   <si>
     <t>Atalanta</t>
@@ -2816,13 +2678,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AEF2"/>
+  <dimension ref="A1:ACM2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:812">
+    <row r="1" spans="1:767">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3304,34 +3166,34 @@
         <v>159</v>
       </c>
       <c r="FF1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="FG1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="FG1" s="1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="FH1" s="1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="FI1" s="1" t="s">
+      <c r="FJ1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="FJ1" s="1" t="s">
+      <c r="FK1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="FK1" s="1" t="s">
+      <c r="FL1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="FL1" s="1" t="s">
+      <c r="FM1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="FM1" s="1" t="s">
+      <c r="FN1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="FN1" s="1" t="s">
+      <c r="FO1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="FO1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="FP1" s="1" t="s">
         <v>169</v>
@@ -5121,499 +4983,364 @@
       <c r="ACM1" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="ACN1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:767">
+      <c r="A2" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="ACO1" s="1" t="s">
+      <c r="B2">
+        <v>452</v>
+      </c>
+      <c r="C2">
+        <v>785</v>
+      </c>
+      <c r="D2" t="s">
         <v>766</v>
       </c>
-      <c r="ACP1" s="1" t="s">
+      <c r="E2" t="s">
         <v>767</v>
       </c>
-      <c r="ACQ1" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="ACR1" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="ACS1" s="1" t="s">
-        <v>770</v>
-      </c>
-      <c r="ACT1" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="ACU1" s="1" t="s">
-        <v>772</v>
-      </c>
-      <c r="ACV1" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="ACW1" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="ACX1" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="ACY1" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="ACZ1" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="ADA1" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="ADB1" s="1" t="s">
-        <v>779</v>
-      </c>
-      <c r="ADC1" s="1" t="s">
-        <v>780</v>
-      </c>
-      <c r="ADD1" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="ADE1" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="ADF1" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="ADG1" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="ADH1" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="ADI1" s="1" t="s">
-        <v>786</v>
-      </c>
-      <c r="ADJ1" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="ADK1" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="ADL1" s="1" t="s">
-        <v>789</v>
-      </c>
-      <c r="ADM1" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="ADN1" s="1" t="s">
-        <v>791</v>
-      </c>
-      <c r="ADO1" s="1" t="s">
-        <v>792</v>
-      </c>
-      <c r="ADP1" s="1" t="s">
-        <v>793</v>
-      </c>
-      <c r="ADQ1" s="1" t="s">
-        <v>794</v>
-      </c>
-      <c r="ADR1" s="1" t="s">
-        <v>795</v>
-      </c>
-      <c r="ADS1" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="ADT1" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="ADU1" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="ADV1" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="ADW1" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="ADX1" s="1" t="s">
-        <v>801</v>
-      </c>
-      <c r="ADY1" s="1" t="s">
-        <v>802</v>
-      </c>
-      <c r="ADZ1" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="AEA1" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="AEB1" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="AEC1" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="AED1" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="AEE1" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="AEF1" s="1" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="2" spans="1:812">
-      <c r="A2" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="B2">
-        <v>274</v>
-      </c>
-      <c r="C2">
-        <v>2848</v>
-      </c>
-      <c r="D2" t="s">
-        <v>811</v>
-      </c>
-      <c r="E2" t="s">
-        <v>812</v>
-      </c>
       <c r="F2" t="s">
-        <v>810</v>
+        <v>765</v>
       </c>
       <c r="H2">
-        <v>187</v>
-      </c>
-      <c r="I2" t="s">
-        <v>813</v>
+        <v>250</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
       </c>
       <c r="J2">
-        <v>1999</v>
+        <v>1990</v>
       </c>
       <c r="K2">
+        <v>35</v>
+      </c>
+      <c r="L2">
+        <v>34</v>
+      </c>
+      <c r="M2">
+        <v>2849</v>
+      </c>
+      <c r="N2">
         <v>20</v>
       </c>
-      <c r="L2">
-        <v>20</v>
-      </c>
-      <c r="M2">
-        <v>1636</v>
-      </c>
-      <c r="N2">
-        <v>5</v>
-      </c>
       <c r="O2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0.28</v>
+        <v>0.63</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="V2">
-        <v>0.28</v>
+        <v>0.82</v>
       </c>
       <c r="W2">
-        <v>0.28</v>
+        <v>0.51</v>
       </c>
       <c r="X2">
-        <v>0.28</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="Y2">
-        <v>4.2</v>
+        <v>19.8</v>
       </c>
       <c r="Z2">
-        <v>4.2</v>
+        <v>13.6</v>
       </c>
       <c r="AA2">
-        <v>0.23</v>
+        <v>0.63</v>
       </c>
       <c r="AB2">
-        <v>0.23</v>
+        <v>0.43</v>
       </c>
       <c r="AC2">
         <v>0</v>
       </c>
       <c r="AD2">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>50</v>
+        <v>39.3</v>
       </c>
       <c r="AG2">
-        <v>0.99</v>
+        <v>1.39</v>
       </c>
       <c r="AH2">
         <v>0.14</v>
       </c>
       <c r="AI2">
-        <v>0.28</v>
+        <v>0.36</v>
       </c>
       <c r="AJ2">
         <v>0.12</v>
       </c>
       <c r="AK2">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="AL2">
-        <v>0.8</v>
+        <v>2.4</v>
       </c>
       <c r="AM2">
-        <v>439</v>
+        <v>651</v>
       </c>
       <c r="AN2">
-        <v>565</v>
+        <v>897</v>
       </c>
       <c r="AO2">
-        <v>77.7</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="AP2">
-        <v>7555</v>
+        <v>8700</v>
       </c>
       <c r="AQ2">
-        <v>2079</v>
+        <v>1781</v>
       </c>
       <c r="AR2">
-        <v>204</v>
+        <v>393</v>
       </c>
       <c r="AS2">
-        <v>249</v>
+        <v>488</v>
       </c>
       <c r="AT2">
-        <v>81.90000000000001</v>
+        <v>80.5</v>
       </c>
       <c r="AU2">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="AV2">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="AW2">
-        <v>83.2</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="AX2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="AY2">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="AZ2">
-        <v>64.2</v>
+        <v>63.1</v>
       </c>
       <c r="BA2">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="BB2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="BC2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="BD2">
         <v>1</v>
       </c>
       <c r="BE2">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="BF2">
-        <v>549</v>
+        <v>867</v>
       </c>
       <c r="BG2">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="BH2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="BI2">
+        <v>3</v>
+      </c>
+      <c r="BJ2">
+        <v>3</v>
+      </c>
+      <c r="BK2">
+        <v>18</v>
+      </c>
+      <c r="BL2">
+        <v>6</v>
+      </c>
+      <c r="BM2">
         <v>4</v>
       </c>
-      <c r="BJ2">
-        <v>13</v>
-      </c>
-      <c r="BK2">
-        <v>9</v>
-      </c>
-      <c r="BL2">
-        <v>0</v>
-      </c>
-      <c r="BM2">
-        <v>0</v>
-      </c>
       <c r="BN2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO2">
         <v>0</v>
       </c>
       <c r="BP2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="BQ2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BR2">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="BS2">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="BT2">
-        <v>2.97</v>
+        <v>3.73</v>
       </c>
       <c r="BU2">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="BV2">
         <v>0</v>
       </c>
       <c r="BW2">
+        <v>14</v>
+      </c>
+      <c r="BX2">
+        <v>8</v>
+      </c>
+      <c r="BY2">
+        <v>15</v>
+      </c>
+      <c r="BZ2">
+        <v>0.47</v>
+      </c>
+      <c r="CA2">
+        <v>8</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>2</v>
+      </c>
+      <c r="CD2">
         <v>4</v>
-      </c>
-      <c r="BX2">
-        <v>4</v>
-      </c>
-      <c r="BY2">
-        <v>2</v>
-      </c>
-      <c r="BZ2">
-        <v>4</v>
-      </c>
-      <c r="CA2">
-        <v>0.22</v>
-      </c>
-      <c r="CB2">
-        <v>4</v>
-      </c>
-      <c r="CC2">
-        <v>0</v>
-      </c>
-      <c r="CD2">
-        <v>0</v>
       </c>
       <c r="CE2">
         <v>0</v>
       </c>
       <c r="CF2">
+        <v>14</v>
+      </c>
+      <c r="CG2">
+        <v>13</v>
+      </c>
+      <c r="CH2">
+        <v>4</v>
+      </c>
+      <c r="CI2">
+        <v>6</v>
+      </c>
+      <c r="CJ2">
+        <v>4</v>
+      </c>
+      <c r="CK2">
+        <v>13</v>
+      </c>
+      <c r="CL2">
+        <v>1</v>
+      </c>
+      <c r="CM2">
+        <v>12</v>
+      </c>
+      <c r="CN2">
+        <v>6</v>
+      </c>
+      <c r="CO2">
+        <v>9</v>
+      </c>
+      <c r="CP2">
         <v>0</v>
       </c>
-      <c r="CG2">
+      <c r="CQ2">
+        <v>1218</v>
+      </c>
+      <c r="CR2">
+        <v>10</v>
+      </c>
+      <c r="CS2">
+        <v>94</v>
+      </c>
+      <c r="CT2">
+        <v>443</v>
+      </c>
+      <c r="CU2">
+        <v>692</v>
+      </c>
+      <c r="CV2">
+        <v>207</v>
+      </c>
+      <c r="CW2">
+        <v>1210</v>
+      </c>
+      <c r="CX2">
+        <v>700</v>
+      </c>
+      <c r="CY2">
+        <v>74</v>
+      </c>
+      <c r="CZ2">
+        <v>43</v>
+      </c>
+      <c r="DA2">
+        <v>38</v>
+      </c>
+      <c r="DB2">
+        <v>968</v>
+      </c>
+      <c r="DC2">
+        <v>71</v>
+      </c>
+      <c r="DD2">
+        <v>34</v>
+      </c>
+      <c r="DE2">
         <v>0</v>
       </c>
-      <c r="CH2">
-        <v>40</v>
-      </c>
-      <c r="CI2">
-        <v>18</v>
-      </c>
-      <c r="CJ2">
-        <v>13</v>
-      </c>
-      <c r="CK2">
-        <v>22</v>
-      </c>
-      <c r="CL2">
-        <v>5</v>
-      </c>
-      <c r="CM2">
-        <v>14</v>
-      </c>
-      <c r="CN2">
-        <v>24</v>
-      </c>
-      <c r="CO2">
-        <v>58.3</v>
-      </c>
-      <c r="CP2">
-        <v>10</v>
-      </c>
-      <c r="CQ2">
-        <v>15</v>
-      </c>
-      <c r="CR2">
-        <v>2</v>
-      </c>
-      <c r="CS2">
-        <v>13</v>
-      </c>
-      <c r="CT2">
-        <v>6</v>
-      </c>
-      <c r="CU2">
-        <v>22</v>
-      </c>
-      <c r="CV2">
+      <c r="DF2">
+        <v>37</v>
+      </c>
+      <c r="DG2">
+        <v>44</v>
+      </c>
+      <c r="DH2">
+        <v>30</v>
+      </c>
+      <c r="DI2">
+        <v>3</v>
+      </c>
+      <c r="DJ2">
         <v>0</v>
       </c>
-      <c r="CW2">
-        <v>788</v>
-      </c>
-      <c r="CX2">
-        <v>35</v>
-      </c>
-      <c r="CY2">
-        <v>157</v>
-      </c>
-      <c r="CZ2">
-        <v>399</v>
-      </c>
-      <c r="DA2">
-        <v>244</v>
-      </c>
-      <c r="DB2">
-        <v>53</v>
-      </c>
-      <c r="DC2">
-        <v>788</v>
-      </c>
-      <c r="DD2">
-        <v>24</v>
-      </c>
-      <c r="DE2">
-        <v>46</v>
-      </c>
-      <c r="DF2">
-        <v>52.2</v>
-      </c>
-      <c r="DG2">
-        <v>444</v>
-      </c>
-      <c r="DH2">
-        <v>43</v>
-      </c>
-      <c r="DI2">
-        <v>30</v>
-      </c>
-      <c r="DJ2">
-        <v>14</v>
-      </c>
       <c r="DK2">
-        <v>525</v>
+        <v>0</v>
       </c>
       <c r="DL2">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="DM2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="DN2">
+        <v>54</v>
+      </c>
+      <c r="DO2">
+        <v>32.5</v>
+      </c>
+      <c r="DP2">
         <v>0</v>
-      </c>
-      <c r="DO2">
-        <v>26</v>
-      </c>
-      <c r="DP2">
-        <v>36</v>
       </c>
       <c r="DQ2">
         <v>0</v>
@@ -5628,16 +5355,16 @@
         <v>0</v>
       </c>
       <c r="DU2">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="DV2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="DW2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="DX2">
-        <v>57.1</v>
+        <v>0</v>
       </c>
       <c r="DY2">
         <v>0</v>
@@ -5733,1963 +5460,1828 @@
         <v>0</v>
       </c>
       <c r="FD2">
+        <v>6.228571428571429</v>
+      </c>
+      <c r="FE2">
+        <v>0.9361231385946214</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>767</v>
+      </c>
+      <c r="FG2">
+        <v>30</v>
+      </c>
+      <c r="FH2">
+        <v>53</v>
+      </c>
+      <c r="FI2">
+        <v>38</v>
+      </c>
+      <c r="FJ2">
+        <v>418</v>
+      </c>
+      <c r="FK2">
+        <v>3420</v>
+      </c>
+      <c r="FL2">
+        <v>59</v>
+      </c>
+      <c r="FM2">
+        <v>40</v>
+      </c>
+      <c r="FN2">
+        <v>6</v>
+      </c>
+      <c r="FO2">
+        <v>10</v>
+      </c>
+      <c r="FP2">
+        <v>107</v>
+      </c>
+      <c r="FQ2">
+        <v>5</v>
+      </c>
+      <c r="FR2">
+        <v>1.55</v>
+      </c>
+      <c r="FS2">
+        <v>1.05</v>
+      </c>
+      <c r="FT2">
+        <v>2.61</v>
+      </c>
+      <c r="FU2">
+        <v>1.39</v>
+      </c>
+      <c r="FV2">
+        <v>2.45</v>
+      </c>
+      <c r="FW2">
+        <v>58.2</v>
+      </c>
+      <c r="FX2">
+        <v>50.7</v>
+      </c>
+      <c r="FY2">
+        <v>1.53</v>
+      </c>
+      <c r="FZ2">
+        <v>1.33</v>
+      </c>
+      <c r="GA2">
+        <v>38</v>
+      </c>
+      <c r="GB2">
+        <v>38</v>
+      </c>
+      <c r="GC2">
+        <v>3420</v>
+      </c>
+      <c r="GD2">
+        <v>55</v>
+      </c>
+      <c r="GE2">
+        <v>1.45</v>
+      </c>
+      <c r="GF2">
+        <v>151</v>
+      </c>
+      <c r="GG2">
+        <v>98</v>
+      </c>
+      <c r="GH2">
+        <v>70.2</v>
+      </c>
+      <c r="GI2">
+        <v>21</v>
+      </c>
+      <c r="GJ2">
+        <v>5</v>
+      </c>
+      <c r="GK2">
+        <v>12</v>
+      </c>
+      <c r="GL2">
+        <v>12</v>
+      </c>
+      <c r="GM2">
+        <v>31.6</v>
+      </c>
+      <c r="GN2">
+        <v>10</v>
+      </c>
+      <c r="GO2">
+        <v>10</v>
+      </c>
+      <c r="GP2">
         <v>0</v>
       </c>
-      <c r="FE2">
+      <c r="GQ2">
         <v>0</v>
       </c>
-      <c r="FF2">
+      <c r="GR2">
+        <v>38</v>
+      </c>
+      <c r="GS2">
         <v>0</v>
       </c>
-      <c r="FG2">
+      <c r="GT2">
+        <v>7</v>
+      </c>
+      <c r="GU2">
+        <v>2</v>
+      </c>
+      <c r="GV2">
+        <v>50.2</v>
+      </c>
+      <c r="GW2">
+        <v>0.27</v>
+      </c>
+      <c r="GX2">
+        <v>-2.8</v>
+      </c>
+      <c r="GY2">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="GZ2">
+        <v>181</v>
+      </c>
+      <c r="HA2">
+        <v>385</v>
+      </c>
+      <c r="HB2">
+        <v>47</v>
+      </c>
+      <c r="HC2">
+        <v>1270</v>
+      </c>
+      <c r="HD2">
+        <v>174</v>
+      </c>
+      <c r="HE2">
+        <v>27.4</v>
+      </c>
+      <c r="HF2">
+        <v>30.4</v>
+      </c>
+      <c r="HG2">
+        <v>202</v>
+      </c>
+      <c r="HH2">
+        <v>18.3</v>
+      </c>
+      <c r="HI2">
+        <v>25</v>
+      </c>
+      <c r="HJ2">
+        <v>491</v>
+      </c>
+      <c r="HK2">
+        <v>13</v>
+      </c>
+      <c r="HL2">
+        <v>2.6</v>
+      </c>
+      <c r="HM2">
+        <v>22</v>
+      </c>
+      <c r="HN2">
+        <v>0.58</v>
+      </c>
+      <c r="HO2">
+        <v>13.9</v>
+      </c>
+      <c r="HP2">
+        <v>175</v>
+      </c>
+      <c r="HQ2">
+        <v>14</v>
+      </c>
+      <c r="HR2">
+        <v>34</v>
+      </c>
+      <c r="HS2">
+        <v>4.61</v>
+      </c>
+      <c r="HT2">
+        <v>0.1</v>
+      </c>
+      <c r="HU2">
+        <v>0.3</v>
+      </c>
+      <c r="HV2">
+        <v>0.1</v>
+      </c>
+      <c r="HW2">
+        <v>0.8</v>
+      </c>
+      <c r="HX2">
+        <v>2.3</v>
+      </c>
+      <c r="HY2">
+        <v>16972</v>
+      </c>
+      <c r="HZ2">
+        <v>20795</v>
+      </c>
+      <c r="IA2">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="IB2">
+        <v>304863</v>
+      </c>
+      <c r="IC2">
+        <v>108222</v>
+      </c>
+      <c r="ID2">
+        <v>7366</v>
+      </c>
+      <c r="IE2">
+        <v>8356</v>
+      </c>
+      <c r="IF2">
+        <v>88.2</v>
+      </c>
+      <c r="IG2">
+        <v>7099</v>
+      </c>
+      <c r="IH2">
+        <v>8110</v>
+      </c>
+      <c r="II2">
+        <v>87.5</v>
+      </c>
+      <c r="IJ2">
+        <v>2007</v>
+      </c>
+      <c r="IK2">
+        <v>3161</v>
+      </c>
+      <c r="IL2">
+        <v>63.5</v>
+      </c>
+      <c r="IM2">
+        <v>391</v>
+      </c>
+      <c r="IN2">
+        <v>1479</v>
+      </c>
+      <c r="IO2">
+        <v>398</v>
+      </c>
+      <c r="IP2">
+        <v>115</v>
+      </c>
+      <c r="IQ2">
+        <v>1688</v>
+      </c>
+      <c r="IR2">
+        <v>19069</v>
+      </c>
+      <c r="IS2">
+        <v>1639</v>
+      </c>
+      <c r="IT2">
+        <v>468</v>
+      </c>
+      <c r="IU2">
+        <v>25</v>
+      </c>
+      <c r="IV2">
+        <v>151</v>
+      </c>
+      <c r="IW2">
+        <v>744</v>
+      </c>
+      <c r="IX2">
+        <v>189</v>
+      </c>
+      <c r="IY2">
+        <v>97</v>
+      </c>
+      <c r="IZ2">
+        <v>63</v>
+      </c>
+      <c r="JA2">
+        <v>1</v>
+      </c>
+      <c r="JB2">
+        <v>653</v>
+      </c>
+      <c r="JC2">
+        <v>87</v>
+      </c>
+      <c r="JD2">
+        <v>346</v>
+      </c>
+      <c r="JE2">
+        <v>937</v>
+      </c>
+      <c r="JF2">
+        <v>24.66</v>
+      </c>
+      <c r="JG2">
+        <v>733</v>
+      </c>
+      <c r="JH2">
+        <v>53</v>
+      </c>
+      <c r="JI2">
+        <v>55</v>
+      </c>
+      <c r="JJ2">
+        <v>33</v>
+      </c>
+      <c r="JK2">
+        <v>103</v>
+      </c>
+      <c r="JL2">
+        <v>2.71</v>
+      </c>
+      <c r="JM2">
+        <v>75</v>
+      </c>
+      <c r="JN2">
+        <v>1</v>
+      </c>
+      <c r="JO2">
+        <v>9</v>
+      </c>
+      <c r="JP2">
+        <v>9</v>
+      </c>
+      <c r="JQ2">
+        <v>1</v>
+      </c>
+      <c r="JR2">
+        <v>595</v>
+      </c>
+      <c r="JS2">
+        <v>346</v>
+      </c>
+      <c r="JT2">
+        <v>284</v>
+      </c>
+      <c r="JU2">
+        <v>244</v>
+      </c>
+      <c r="JV2">
+        <v>67</v>
+      </c>
+      <c r="JW2">
+        <v>404</v>
+      </c>
+      <c r="JX2">
+        <v>92</v>
+      </c>
+      <c r="JY2">
+        <v>312</v>
+      </c>
+      <c r="JZ2">
+        <v>445</v>
+      </c>
+      <c r="KA2">
+        <v>649</v>
+      </c>
+      <c r="KB2">
+        <v>7</v>
+      </c>
+      <c r="KC2">
+        <v>24888</v>
+      </c>
+      <c r="KD2">
+        <v>2487</v>
+      </c>
+      <c r="KE2">
+        <v>7653</v>
+      </c>
+      <c r="KF2">
+        <v>11527</v>
+      </c>
+      <c r="KG2">
+        <v>5958</v>
+      </c>
+      <c r="KH2">
+        <v>883</v>
+      </c>
+      <c r="KI2">
+        <v>24878</v>
+      </c>
+      <c r="KJ2">
+        <v>14348</v>
+      </c>
+      <c r="KK2">
+        <v>785</v>
+      </c>
+      <c r="KL2">
+        <v>618</v>
+      </c>
+      <c r="KM2">
+        <v>171</v>
+      </c>
+      <c r="KN2">
+        <v>16794</v>
+      </c>
+      <c r="KO2">
+        <v>553</v>
+      </c>
+      <c r="KP2">
+        <v>304</v>
+      </c>
+      <c r="KQ2">
+        <v>3</v>
+      </c>
+      <c r="KR2">
+        <v>498</v>
+      </c>
+      <c r="KS2">
+        <v>427</v>
+      </c>
+      <c r="KT2">
+        <v>87</v>
+      </c>
+      <c r="KU2">
+        <v>8</v>
+      </c>
+      <c r="KV2">
+        <v>10</v>
+      </c>
+      <c r="KW2">
+        <v>2</v>
+      </c>
+      <c r="KX2">
+        <v>2132</v>
+      </c>
+      <c r="KY2">
+        <v>539</v>
+      </c>
+      <c r="KZ2">
+        <v>510</v>
+      </c>
+      <c r="LA2">
+        <v>51.4</v>
+      </c>
+      <c r="LB2">
+        <v>30</v>
+      </c>
+      <c r="LC2">
+        <v>46.9</v>
+      </c>
+      <c r="LD2">
+        <v>38</v>
+      </c>
+      <c r="LE2">
+        <v>418</v>
+      </c>
+      <c r="LF2">
+        <v>3420</v>
+      </c>
+      <c r="LG2">
+        <v>53</v>
+      </c>
+      <c r="LH2">
+        <v>33</v>
+      </c>
+      <c r="LI2">
+        <v>10</v>
+      </c>
+      <c r="LJ2">
+        <v>10</v>
+      </c>
+      <c r="LK2">
+        <v>87</v>
+      </c>
+      <c r="LL2">
+        <v>3</v>
+      </c>
+      <c r="LM2">
+        <v>1.39</v>
+      </c>
+      <c r="LN2">
+        <v>0.87</v>
+      </c>
+      <c r="LO2">
+        <v>2.26</v>
+      </c>
+      <c r="LP2">
+        <v>1.13</v>
+      </c>
+      <c r="LQ2">
+        <v>2</v>
+      </c>
+      <c r="LR2">
+        <v>47.3</v>
+      </c>
+      <c r="LS2">
+        <v>38.9</v>
+      </c>
+      <c r="LT2">
+        <v>1.24</v>
+      </c>
+      <c r="LU2">
+        <v>1.02</v>
+      </c>
+      <c r="LV2">
+        <v>38</v>
+      </c>
+      <c r="LW2">
+        <v>38</v>
+      </c>
+      <c r="LX2">
+        <v>3420</v>
+      </c>
+      <c r="LY2">
+        <v>61</v>
+      </c>
+      <c r="LZ2">
+        <v>1.61</v>
+      </c>
+      <c r="MA2">
+        <v>184</v>
+      </c>
+      <c r="MB2">
+        <v>122</v>
+      </c>
+      <c r="MC2">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="MD2">
+        <v>12</v>
+      </c>
+      <c r="ME2">
+        <v>5</v>
+      </c>
+      <c r="MF2">
+        <v>21</v>
+      </c>
+      <c r="MG2">
+        <v>6</v>
+      </c>
+      <c r="MH2">
+        <v>15.8</v>
+      </c>
+      <c r="MI2">
+        <v>10</v>
+      </c>
+      <c r="MJ2">
+        <v>6</v>
+      </c>
+      <c r="MK2">
+        <v>3</v>
+      </c>
+      <c r="ML2">
+        <v>1</v>
+      </c>
+      <c r="MM2">
+        <v>38</v>
+      </c>
+      <c r="MN2">
+        <v>4</v>
+      </c>
+      <c r="MO2">
+        <v>2</v>
+      </c>
+      <c r="MP2">
+        <v>2</v>
+      </c>
+      <c r="MQ2">
+        <v>57.9</v>
+      </c>
+      <c r="MR2">
+        <v>0.27</v>
+      </c>
+      <c r="MS2">
+        <v>-1.1</v>
+      </c>
+      <c r="MT2">
+        <v>-0.03</v>
+      </c>
+      <c r="MU2">
+        <v>163</v>
+      </c>
+      <c r="MV2">
+        <v>414</v>
+      </c>
+      <c r="MW2">
+        <v>39.4</v>
+      </c>
+      <c r="MX2">
+        <v>945</v>
+      </c>
+      <c r="MY2">
+        <v>204</v>
+      </c>
+      <c r="MZ2">
+        <v>31.2</v>
+      </c>
+      <c r="NA2">
+        <v>32.6</v>
+      </c>
+      <c r="NB2">
+        <v>277</v>
+      </c>
+      <c r="NC2">
+        <v>43</v>
+      </c>
+      <c r="ND2">
+        <v>38.1</v>
+      </c>
+      <c r="NE2">
+        <v>619</v>
+      </c>
+      <c r="NF2">
+        <v>20</v>
+      </c>
+      <c r="NG2">
+        <v>3.2</v>
+      </c>
+      <c r="NH2">
+        <v>37</v>
+      </c>
+      <c r="NI2">
+        <v>0.97</v>
+      </c>
+      <c r="NJ2">
+        <v>13.6</v>
+      </c>
+      <c r="NK2">
+        <v>141</v>
+      </c>
+      <c r="NL2">
+        <v>12</v>
+      </c>
+      <c r="NM2">
+        <v>36.1</v>
+      </c>
+      <c r="NN2">
+        <v>3.71</v>
+      </c>
+      <c r="NO2">
+        <v>0.11</v>
+      </c>
+      <c r="NP2">
+        <v>0.3</v>
+      </c>
+      <c r="NQ2">
+        <v>0.1</v>
+      </c>
+      <c r="NR2">
+        <v>5.7</v>
+      </c>
+      <c r="NS2">
+        <v>4.1</v>
+      </c>
+      <c r="NT2">
+        <v>14738</v>
+      </c>
+      <c r="NU2">
+        <v>18534</v>
+      </c>
+      <c r="NV2">
+        <v>79.5</v>
+      </c>
+      <c r="NW2">
+        <v>265774</v>
+      </c>
+      <c r="NX2">
+        <v>93729</v>
+      </c>
+      <c r="NY2">
+        <v>6493</v>
+      </c>
+      <c r="NZ2">
+        <v>7369</v>
+      </c>
+      <c r="OA2">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="OB2">
+        <v>6147</v>
+      </c>
+      <c r="OC2">
+        <v>7163</v>
+      </c>
+      <c r="OD2">
+        <v>85.8</v>
+      </c>
+      <c r="OE2">
+        <v>1723</v>
+      </c>
+      <c r="OF2">
+        <v>2959</v>
+      </c>
+      <c r="OG2">
+        <v>58.2</v>
+      </c>
+      <c r="OH2">
+        <v>303</v>
+      </c>
+      <c r="OI2">
+        <v>1117</v>
+      </c>
+      <c r="OJ2">
+        <v>244</v>
+      </c>
+      <c r="OK2">
+        <v>67</v>
+      </c>
+      <c r="OL2">
+        <v>1325</v>
+      </c>
+      <c r="OM2">
+        <v>16710</v>
+      </c>
+      <c r="ON2">
+        <v>1781</v>
+      </c>
+      <c r="OO2">
+        <v>559</v>
+      </c>
+      <c r="OP2">
+        <v>6</v>
+      </c>
+      <c r="OQ2">
+        <v>172</v>
+      </c>
+      <c r="OR2">
+        <v>628</v>
+      </c>
+      <c r="OS2">
+        <v>170</v>
+      </c>
+      <c r="OT2">
+        <v>68</v>
+      </c>
+      <c r="OU2">
+        <v>79</v>
+      </c>
+      <c r="OV2">
         <v>0</v>
       </c>
-      <c r="FH2">
+      <c r="OW2">
+        <v>666</v>
+      </c>
+      <c r="OX2">
+        <v>43</v>
+      </c>
+      <c r="OY2">
+        <v>363</v>
+      </c>
+      <c r="OZ2">
+        <v>706</v>
+      </c>
+      <c r="PA2">
+        <v>18.58</v>
+      </c>
+      <c r="PB2">
+        <v>487</v>
+      </c>
+      <c r="PC2">
+        <v>67</v>
+      </c>
+      <c r="PD2">
+        <v>41</v>
+      </c>
+      <c r="PE2">
+        <v>47</v>
+      </c>
+      <c r="PF2">
+        <v>97</v>
+      </c>
+      <c r="PG2">
+        <v>2.55</v>
+      </c>
+      <c r="PH2">
+        <v>58</v>
+      </c>
+      <c r="PI2">
+        <v>9</v>
+      </c>
+      <c r="PJ2">
+        <v>6</v>
+      </c>
+      <c r="PK2">
+        <v>11</v>
+      </c>
+      <c r="PL2">
+        <v>3</v>
+      </c>
+      <c r="PM2">
+        <v>560</v>
+      </c>
+      <c r="PN2">
+        <v>292</v>
+      </c>
+      <c r="PO2">
+        <v>270</v>
+      </c>
+      <c r="PP2">
+        <v>211</v>
+      </c>
+      <c r="PQ2">
+        <v>79</v>
+      </c>
+      <c r="PR2">
+        <v>420</v>
+      </c>
+      <c r="PS2">
+        <v>124</v>
+      </c>
+      <c r="PT2">
+        <v>296</v>
+      </c>
+      <c r="PU2">
+        <v>453</v>
+      </c>
+      <c r="PV2">
+        <v>781</v>
+      </c>
+      <c r="PW2">
+        <v>13</v>
+      </c>
+      <c r="PX2">
+        <v>22633</v>
+      </c>
+      <c r="PY2">
+        <v>2462</v>
+      </c>
+      <c r="PZ2">
+        <v>7359</v>
+      </c>
+      <c r="QA2">
+        <v>10690</v>
+      </c>
+      <c r="QB2">
+        <v>4827</v>
+      </c>
+      <c r="QC2">
+        <v>671</v>
+      </c>
+      <c r="QD2">
+        <v>22623</v>
+      </c>
+      <c r="QE2">
+        <v>12738</v>
+      </c>
+      <c r="QF2">
+        <v>715</v>
+      </c>
+      <c r="QG2">
+        <v>503</v>
+      </c>
+      <c r="QH2">
+        <v>137</v>
+      </c>
+      <c r="QI2">
+        <v>14643</v>
+      </c>
+      <c r="QJ2">
+        <v>585</v>
+      </c>
+      <c r="QK2">
+        <v>341</v>
+      </c>
+      <c r="QL2">
+        <v>1</v>
+      </c>
+      <c r="QM2">
+        <v>454</v>
+      </c>
+      <c r="QN2">
+        <v>480</v>
+      </c>
+      <c r="QO2">
+        <v>43</v>
+      </c>
+      <c r="QP2">
+        <v>10</v>
+      </c>
+      <c r="QQ2">
+        <v>10</v>
+      </c>
+      <c r="QR2">
+        <v>2</v>
+      </c>
+      <c r="QS2">
+        <v>2054</v>
+      </c>
+      <c r="QT2">
+        <v>510</v>
+      </c>
+      <c r="QU2">
+        <v>539</v>
+      </c>
+      <c r="QV2">
+        <v>48.6</v>
+      </c>
+      <c r="QW2" t="s">
+        <v>768</v>
+      </c>
+      <c r="QX2">
+        <v>30</v>
+      </c>
+      <c r="QY2">
+        <v>54.6</v>
+      </c>
+      <c r="QZ2">
+        <v>38</v>
+      </c>
+      <c r="RA2">
+        <v>418</v>
+      </c>
+      <c r="RB2">
+        <v>3420</v>
+      </c>
+      <c r="RC2">
+        <v>90</v>
+      </c>
+      <c r="RD2">
+        <v>65</v>
+      </c>
+      <c r="RE2">
+        <v>6</v>
+      </c>
+      <c r="RF2">
+        <v>7</v>
+      </c>
+      <c r="RG2">
+        <v>67</v>
+      </c>
+      <c r="RH2">
+        <v>3</v>
+      </c>
+      <c r="RI2">
+        <v>2.37</v>
+      </c>
+      <c r="RJ2">
+        <v>1.71</v>
+      </c>
+      <c r="RK2">
+        <v>4.08</v>
+      </c>
+      <c r="RL2">
+        <v>2.21</v>
+      </c>
+      <c r="RM2">
+        <v>3.92</v>
+      </c>
+      <c r="RN2">
+        <v>74.7</v>
+      </c>
+      <c r="RO2">
+        <v>69.3</v>
+      </c>
+      <c r="RP2">
+        <v>1.97</v>
+      </c>
+      <c r="RQ2">
+        <v>1.82</v>
+      </c>
+      <c r="RR2">
+        <v>38</v>
+      </c>
+      <c r="RS2">
+        <v>38</v>
+      </c>
+      <c r="RT2">
+        <v>3417</v>
+      </c>
+      <c r="RU2">
+        <v>47</v>
+      </c>
+      <c r="RV2">
+        <v>1.24</v>
+      </c>
+      <c r="RW2">
+        <v>112</v>
+      </c>
+      <c r="RX2">
+        <v>63</v>
+      </c>
+      <c r="RY2">
+        <v>62.5</v>
+      </c>
+      <c r="RZ2">
+        <v>23</v>
+      </c>
+      <c r="SA2">
+        <v>9</v>
+      </c>
+      <c r="SB2">
+        <v>6</v>
+      </c>
+      <c r="SC2">
+        <v>11</v>
+      </c>
+      <c r="SD2">
+        <v>28.9</v>
+      </c>
+      <c r="SE2">
+        <v>8</v>
+      </c>
+      <c r="SF2">
+        <v>5</v>
+      </c>
+      <c r="SG2">
+        <v>3</v>
+      </c>
+      <c r="SH2">
         <v>0</v>
       </c>
-      <c r="FI2">
+      <c r="SI2">
+        <v>38</v>
+      </c>
+      <c r="SJ2">
         <v>0</v>
       </c>
-      <c r="FJ2">
+      <c r="SK2">
+        <v>5</v>
+      </c>
+      <c r="SL2">
+        <v>1</v>
+      </c>
+      <c r="SM2">
+        <v>42.3</v>
+      </c>
+      <c r="SN2">
+        <v>0.31</v>
+      </c>
+      <c r="SO2">
+        <v>-3.7</v>
+      </c>
+      <c r="SP2">
+        <v>-0.1</v>
+      </c>
+      <c r="SQ2">
+        <v>132</v>
+      </c>
+      <c r="SR2">
+        <v>323</v>
+      </c>
+      <c r="SS2">
+        <v>40.9</v>
+      </c>
+      <c r="ST2">
+        <v>868</v>
+      </c>
+      <c r="SU2">
+        <v>161</v>
+      </c>
+      <c r="SV2">
+        <v>24.8</v>
+      </c>
+      <c r="SW2">
+        <v>31</v>
+      </c>
+      <c r="SX2">
+        <v>173</v>
+      </c>
+      <c r="SY2">
+        <v>62.4</v>
+      </c>
+      <c r="SZ2">
+        <v>47.7</v>
+      </c>
+      <c r="TA2">
+        <v>377</v>
+      </c>
+      <c r="TB2">
+        <v>14</v>
+      </c>
+      <c r="TC2">
+        <v>3.7</v>
+      </c>
+      <c r="TD2">
+        <v>66</v>
+      </c>
+      <c r="TE2">
+        <v>1.74</v>
+      </c>
+      <c r="TF2">
+        <v>16.9</v>
+      </c>
+      <c r="TG2">
+        <v>221</v>
+      </c>
+      <c r="TH2">
+        <v>28</v>
+      </c>
+      <c r="TI2">
+        <v>36</v>
+      </c>
+      <c r="TJ2">
+        <v>5.82</v>
+      </c>
+      <c r="TK2">
+        <v>0.14</v>
+      </c>
+      <c r="TL2">
+        <v>0.38</v>
+      </c>
+      <c r="TM2">
+        <v>0.12</v>
+      </c>
+      <c r="TN2">
+        <v>15.3</v>
+      </c>
+      <c r="TO2">
+        <v>14.7</v>
+      </c>
+      <c r="TP2">
+        <v>18066</v>
+      </c>
+      <c r="TQ2">
+        <v>22063</v>
+      </c>
+      <c r="TR2">
+        <v>81.90000000000001</v>
+      </c>
+      <c r="TS2">
+        <v>310229</v>
+      </c>
+      <c r="TT2">
+        <v>109918</v>
+      </c>
+      <c r="TU2">
+        <v>8542</v>
+      </c>
+      <c r="TV2">
+        <v>9641</v>
+      </c>
+      <c r="TW2">
+        <v>88.59999999999999</v>
+      </c>
+      <c r="TX2">
+        <v>7388</v>
+      </c>
+      <c r="TY2">
+        <v>8505</v>
+      </c>
+      <c r="TZ2">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="UA2">
+        <v>1686</v>
+      </c>
+      <c r="UB2">
+        <v>2744</v>
+      </c>
+      <c r="UC2">
+        <v>61.4</v>
+      </c>
+      <c r="UD2">
+        <v>487</v>
+      </c>
+      <c r="UE2">
+        <v>1635</v>
+      </c>
+      <c r="UF2">
+        <v>490</v>
+      </c>
+      <c r="UG2">
+        <v>85</v>
+      </c>
+      <c r="UH2">
+        <v>2077</v>
+      </c>
+      <c r="UI2">
+        <v>20351</v>
+      </c>
+      <c r="UJ2">
+        <v>1656</v>
+      </c>
+      <c r="UK2">
+        <v>508</v>
+      </c>
+      <c r="UL2">
+        <v>28</v>
+      </c>
+      <c r="UM2">
+        <v>181</v>
+      </c>
+      <c r="UN2">
+        <v>657</v>
+      </c>
+      <c r="UO2">
+        <v>201</v>
+      </c>
+      <c r="UP2">
+        <v>104</v>
+      </c>
+      <c r="UQ2">
+        <v>82</v>
+      </c>
+      <c r="UR2">
         <v>0</v>
       </c>
-      <c r="FK2">
-        <v>0</v>
-      </c>
-      <c r="FL2">
-        <v>0</v>
-      </c>
-      <c r="FM2">
-        <v>6.275</v>
-      </c>
-      <c r="FN2">
-        <v>0.7154544010627093</v>
-      </c>
-      <c r="FO2" t="s">
-        <v>812</v>
-      </c>
-      <c r="FP2">
-        <v>27</v>
-      </c>
-      <c r="FQ2">
-        <v>48.3</v>
-      </c>
-      <c r="FR2">
-        <v>20</v>
-      </c>
-      <c r="FS2">
-        <v>220</v>
-      </c>
-      <c r="FT2">
-        <v>1800</v>
-      </c>
-      <c r="FU2">
-        <v>23</v>
-      </c>
-      <c r="FV2">
-        <v>17</v>
-      </c>
-      <c r="FW2">
-        <v>4</v>
-      </c>
-      <c r="FX2">
+      <c r="US2">
+        <v>689</v>
+      </c>
+      <c r="UT2">
+        <v>56</v>
+      </c>
+      <c r="UU2">
+        <v>395</v>
+      </c>
+      <c r="UV2">
+        <v>1115</v>
+      </c>
+      <c r="UW2">
+        <v>29.34</v>
+      </c>
+      <c r="UX2">
+        <v>866</v>
+      </c>
+      <c r="UY2">
+        <v>68</v>
+      </c>
+      <c r="UZ2">
+        <v>61</v>
+      </c>
+      <c r="VA2">
+        <v>43</v>
+      </c>
+      <c r="VB2">
+        <v>162</v>
+      </c>
+      <c r="VC2">
+        <v>4.26</v>
+      </c>
+      <c r="VD2">
+        <v>127</v>
+      </c>
+      <c r="VE2">
+        <v>8</v>
+      </c>
+      <c r="VF2">
+        <v>9</v>
+      </c>
+      <c r="VG2">
         <v>5</v>
       </c>
-      <c r="FY2">
-        <v>50</v>
-      </c>
-      <c r="FZ2">
-        <v>2</v>
-      </c>
-      <c r="GA2">
-        <v>1.15</v>
-      </c>
-      <c r="GB2">
-        <v>0.85</v>
-      </c>
-      <c r="GC2">
-        <v>2</v>
-      </c>
-      <c r="GD2">
-        <v>0.95</v>
-      </c>
-      <c r="GE2">
-        <v>1.8</v>
-      </c>
-      <c r="GF2">
-        <v>25.9</v>
-      </c>
-      <c r="GG2">
-        <v>22</v>
-      </c>
-      <c r="GH2">
-        <v>1.29</v>
-      </c>
-      <c r="GI2">
-        <v>1.1</v>
-      </c>
-      <c r="GJ2">
-        <v>20</v>
-      </c>
-      <c r="GK2">
-        <v>20</v>
-      </c>
-      <c r="GL2">
-        <v>1800</v>
-      </c>
-      <c r="GM2">
-        <v>31</v>
-      </c>
-      <c r="GN2">
-        <v>1.55</v>
-      </c>
-      <c r="GO2">
-        <v>64</v>
-      </c>
-      <c r="GP2">
-        <v>33</v>
-      </c>
-      <c r="GQ2">
-        <v>57.8</v>
-      </c>
-      <c r="GR2">
-        <v>5</v>
-      </c>
-      <c r="GS2">
-        <v>5</v>
-      </c>
-      <c r="GT2">
-        <v>10</v>
-      </c>
-      <c r="GU2">
-        <v>5</v>
-      </c>
-      <c r="GV2">
-        <v>25</v>
-      </c>
-      <c r="GW2">
-        <v>4</v>
-      </c>
-      <c r="GX2">
-        <v>4</v>
-      </c>
-      <c r="GY2">
-        <v>0</v>
-      </c>
-      <c r="GZ2">
-        <v>0</v>
-      </c>
-      <c r="HA2">
-        <v>20</v>
-      </c>
-      <c r="HB2">
-        <v>0</v>
-      </c>
-      <c r="HC2">
+      <c r="VH2">
         <v>3</v>
       </c>
-      <c r="HD2">
-        <v>0</v>
-      </c>
-      <c r="HE2">
-        <v>26.1</v>
-      </c>
-      <c r="HF2">
-        <v>0.36</v>
-      </c>
-      <c r="HG2">
-        <v>-4.9</v>
-      </c>
-      <c r="HH2">
-        <v>-0.25</v>
-      </c>
-      <c r="HI2">
-        <v>119</v>
-      </c>
-      <c r="HJ2">
-        <v>279</v>
-      </c>
-      <c r="HK2">
-        <v>42.7</v>
-      </c>
-      <c r="HL2">
-        <v>712</v>
-      </c>
-      <c r="HM2">
-        <v>105</v>
-      </c>
-      <c r="HN2">
-        <v>30.9</v>
-      </c>
-      <c r="HO2">
-        <v>34.2</v>
-      </c>
-      <c r="HP2">
-        <v>183</v>
-      </c>
-      <c r="HQ2">
-        <v>32.2</v>
-      </c>
-      <c r="HR2">
-        <v>32.9</v>
-      </c>
-      <c r="HS2">
-        <v>264</v>
-      </c>
-      <c r="HT2">
-        <v>16</v>
-      </c>
-      <c r="HU2">
-        <v>6.1</v>
-      </c>
-      <c r="HV2">
-        <v>15</v>
-      </c>
-      <c r="HW2">
-        <v>0.75</v>
-      </c>
-      <c r="HX2">
-        <v>14</v>
-      </c>
-      <c r="HY2">
-        <v>87</v>
-      </c>
-      <c r="HZ2">
-        <v>10</v>
-      </c>
-      <c r="IA2">
-        <v>34.3</v>
-      </c>
-      <c r="IB2">
-        <v>4.35</v>
-      </c>
-      <c r="IC2">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="ID2">
-        <v>0.22</v>
-      </c>
-      <c r="IE2">
-        <v>0.09</v>
-      </c>
-      <c r="IF2">
-        <v>-2.9</v>
-      </c>
-      <c r="IG2">
-        <v>-3</v>
-      </c>
-      <c r="IH2">
-        <v>7498</v>
-      </c>
-      <c r="II2">
-        <v>9357</v>
-      </c>
-      <c r="IJ2">
-        <v>80.09999999999999</v>
-      </c>
-      <c r="IK2">
-        <v>141620</v>
-      </c>
-      <c r="IL2">
-        <v>52357</v>
-      </c>
-      <c r="IM2">
-        <v>3112</v>
-      </c>
-      <c r="IN2">
-        <v>3536</v>
-      </c>
-      <c r="IO2">
-        <v>88</v>
-      </c>
-      <c r="IP2">
-        <v>3108</v>
-      </c>
-      <c r="IQ2">
-        <v>3609</v>
-      </c>
-      <c r="IR2">
-        <v>86.09999999999999</v>
-      </c>
-      <c r="IS2">
-        <v>1089</v>
-      </c>
-      <c r="IT2">
-        <v>1721</v>
-      </c>
-      <c r="IU2">
-        <v>63.3</v>
-      </c>
-      <c r="IV2">
-        <v>205</v>
-      </c>
-      <c r="IW2">
-        <v>565</v>
-      </c>
-      <c r="IX2">
-        <v>171</v>
-      </c>
-      <c r="IY2">
-        <v>49</v>
-      </c>
-      <c r="IZ2">
-        <v>776</v>
-      </c>
-      <c r="JA2">
-        <v>8237</v>
-      </c>
-      <c r="JB2">
-        <v>1101</v>
-      </c>
-      <c r="JC2">
-        <v>313</v>
-      </c>
-      <c r="JD2">
-        <v>21</v>
-      </c>
-      <c r="JE2">
-        <v>112</v>
-      </c>
-      <c r="JF2">
-        <v>298</v>
-      </c>
-      <c r="JG2">
-        <v>87</v>
-      </c>
-      <c r="JH2">
-        <v>41</v>
-      </c>
-      <c r="JI2">
-        <v>23</v>
-      </c>
-      <c r="JJ2">
-        <v>0</v>
-      </c>
-      <c r="JK2">
-        <v>439</v>
-      </c>
-      <c r="JL2">
-        <v>19</v>
-      </c>
-      <c r="JM2">
-        <v>182</v>
-      </c>
-      <c r="JN2">
-        <v>461</v>
-      </c>
-      <c r="JO2">
-        <v>23.05</v>
-      </c>
-      <c r="JP2">
-        <v>368</v>
-      </c>
-      <c r="JQ2">
-        <v>25</v>
-      </c>
-      <c r="JR2">
-        <v>19</v>
-      </c>
-      <c r="JS2">
-        <v>24</v>
-      </c>
-      <c r="JT2">
-        <v>18</v>
-      </c>
-      <c r="JU2">
-        <v>41</v>
-      </c>
-      <c r="JV2">
-        <v>2.05</v>
-      </c>
-      <c r="JW2">
-        <v>31</v>
-      </c>
-      <c r="JX2">
-        <v>2</v>
-      </c>
-      <c r="JY2">
-        <v>2</v>
-      </c>
-      <c r="JZ2">
-        <v>3</v>
-      </c>
-      <c r="KA2">
-        <v>3</v>
-      </c>
-      <c r="KB2">
-        <v>0</v>
-      </c>
-      <c r="KC2">
-        <v>282</v>
-      </c>
-      <c r="KD2">
-        <v>151</v>
-      </c>
-      <c r="KE2">
-        <v>132</v>
-      </c>
-      <c r="KF2">
-        <v>113</v>
-      </c>
-      <c r="KG2">
-        <v>37</v>
-      </c>
-      <c r="KH2">
-        <v>116</v>
-      </c>
-      <c r="KI2">
-        <v>227</v>
-      </c>
-      <c r="KJ2">
-        <v>51.1</v>
-      </c>
-      <c r="KK2">
-        <v>111</v>
-      </c>
-      <c r="KL2">
-        <v>182</v>
-      </c>
-      <c r="KM2">
-        <v>55</v>
-      </c>
-      <c r="KN2">
-        <v>127</v>
-      </c>
-      <c r="KO2">
-        <v>148</v>
-      </c>
-      <c r="KP2">
-        <v>338</v>
-      </c>
-      <c r="KQ2">
-        <v>8</v>
-      </c>
-      <c r="KR2">
-        <v>11358</v>
-      </c>
-      <c r="KS2">
-        <v>1316</v>
-      </c>
-      <c r="KT2">
-        <v>3996</v>
-      </c>
-      <c r="KU2">
-        <v>4881</v>
-      </c>
-      <c r="KV2">
-        <v>2594</v>
-      </c>
-      <c r="KW2">
-        <v>397</v>
-      </c>
-      <c r="KX2">
-        <v>11353</v>
-      </c>
-      <c r="KY2">
-        <v>122</v>
-      </c>
-      <c r="KZ2">
-        <v>299</v>
-      </c>
-      <c r="LA2">
-        <v>40.8</v>
-      </c>
-      <c r="LB2">
-        <v>6477</v>
-      </c>
-      <c r="LC2">
-        <v>378</v>
-      </c>
-      <c r="LD2">
-        <v>244</v>
-      </c>
-      <c r="LE2">
-        <v>106</v>
-      </c>
-      <c r="LF2">
-        <v>7429</v>
-      </c>
-      <c r="LG2">
-        <v>273</v>
-      </c>
-      <c r="LH2">
-        <v>216</v>
-      </c>
-      <c r="LI2">
-        <v>1</v>
-      </c>
-      <c r="LJ2">
-        <v>207</v>
-      </c>
-      <c r="LK2">
-        <v>247</v>
-      </c>
-      <c r="LL2">
-        <v>19</v>
-      </c>
-      <c r="LM2">
-        <v>4</v>
-      </c>
-      <c r="LN2">
-        <v>4</v>
-      </c>
-      <c r="LO2">
-        <v>0</v>
-      </c>
-      <c r="LP2">
-        <v>909</v>
-      </c>
-      <c r="LQ2">
-        <v>183</v>
-      </c>
-      <c r="LR2">
-        <v>229</v>
-      </c>
-      <c r="LS2">
-        <v>44.4</v>
-      </c>
-      <c r="LT2">
-        <v>27</v>
-      </c>
-      <c r="LU2">
-        <v>51.8</v>
-      </c>
-      <c r="LV2">
-        <v>20</v>
-      </c>
-      <c r="LW2">
-        <v>220</v>
-      </c>
-      <c r="LX2">
-        <v>1800</v>
-      </c>
-      <c r="LY2">
-        <v>31</v>
-      </c>
-      <c r="LZ2">
-        <v>22</v>
-      </c>
-      <c r="MA2">
-        <v>4</v>
-      </c>
-      <c r="MB2">
-        <v>4</v>
-      </c>
-      <c r="MC2">
-        <v>46</v>
-      </c>
-      <c r="MD2">
-        <v>1</v>
-      </c>
-      <c r="ME2">
-        <v>1.55</v>
-      </c>
-      <c r="MF2">
-        <v>1.1</v>
-      </c>
-      <c r="MG2">
-        <v>2.65</v>
-      </c>
-      <c r="MH2">
-        <v>1.35</v>
-      </c>
-      <c r="MI2">
-        <v>2.45</v>
-      </c>
-      <c r="MJ2">
-        <v>27.3</v>
-      </c>
-      <c r="MK2">
-        <v>24.7</v>
-      </c>
-      <c r="ML2">
-        <v>1.36</v>
-      </c>
-      <c r="MM2">
-        <v>1.23</v>
-      </c>
-      <c r="MN2">
-        <v>20</v>
-      </c>
-      <c r="MO2">
-        <v>20</v>
-      </c>
-      <c r="MP2">
-        <v>1800</v>
-      </c>
-      <c r="MQ2">
-        <v>23</v>
-      </c>
-      <c r="MR2">
-        <v>1.15</v>
-      </c>
-      <c r="MS2">
+      <c r="VI2">
+        <v>606</v>
+      </c>
+      <c r="VJ2">
+        <v>343</v>
+      </c>
+      <c r="VK2">
+        <v>252</v>
+      </c>
+      <c r="VL2">
+        <v>256</v>
+      </c>
+      <c r="VM2">
+        <v>98</v>
+      </c>
+      <c r="VN2">
+        <v>421</v>
+      </c>
+      <c r="VO2">
         <v>92</v>
       </c>
-      <c r="MT2">
-        <v>68</v>
-      </c>
-      <c r="MU2">
-        <v>79.3</v>
-      </c>
-      <c r="MV2">
-        <v>10</v>
-      </c>
-      <c r="MW2">
-        <v>5</v>
-      </c>
-      <c r="MX2">
-        <v>5</v>
-      </c>
-      <c r="MY2">
-        <v>7</v>
-      </c>
-      <c r="MZ2">
-        <v>35</v>
-      </c>
-      <c r="NA2">
-        <v>5</v>
-      </c>
-      <c r="NB2">
-        <v>4</v>
-      </c>
-      <c r="NC2">
-        <v>1</v>
-      </c>
-      <c r="ND2">
-        <v>0</v>
-      </c>
-      <c r="NE2">
-        <v>20</v>
-      </c>
-      <c r="NF2">
-        <v>0</v>
-      </c>
-      <c r="NG2">
-        <v>3</v>
-      </c>
-      <c r="NH2">
-        <v>0</v>
-      </c>
-      <c r="NI2">
-        <v>25.7</v>
-      </c>
-      <c r="NJ2">
-        <v>0.23</v>
-      </c>
-      <c r="NK2">
-        <v>2.7</v>
-      </c>
-      <c r="NL2">
-        <v>0.13</v>
-      </c>
-      <c r="NM2">
-        <v>108</v>
-      </c>
-      <c r="NN2">
-        <v>251</v>
-      </c>
-      <c r="NO2">
-        <v>43</v>
-      </c>
-      <c r="NP2">
-        <v>616</v>
-      </c>
-      <c r="NQ2">
-        <v>105</v>
-      </c>
-      <c r="NR2">
-        <v>31.2</v>
-      </c>
-      <c r="NS2">
-        <v>31</v>
-      </c>
-      <c r="NT2">
-        <v>130</v>
-      </c>
-      <c r="NU2">
-        <v>45.4</v>
-      </c>
-      <c r="NV2">
-        <v>39.3</v>
-      </c>
-      <c r="NW2">
-        <v>234</v>
-      </c>
-      <c r="NX2">
-        <v>7</v>
-      </c>
-      <c r="NY2">
-        <v>3</v>
-      </c>
-      <c r="NZ2">
-        <v>17</v>
-      </c>
-      <c r="OA2">
-        <v>0.85</v>
-      </c>
-      <c r="OB2">
-        <v>15.3</v>
-      </c>
-      <c r="OC2">
-        <v>60</v>
-      </c>
-      <c r="OD2">
+      <c r="VP2">
+        <v>329</v>
+      </c>
+      <c r="VQ2">
+        <v>516</v>
+      </c>
+      <c r="VR2">
+        <v>484</v>
+      </c>
+      <c r="VS2">
         <v>11</v>
       </c>
-      <c r="OE2">
-        <v>25.2</v>
-      </c>
-      <c r="OF2">
-        <v>3</v>
-      </c>
-      <c r="OG2">
-        <v>0.11</v>
-      </c>
-      <c r="OH2">
-        <v>0.45</v>
-      </c>
-      <c r="OI2">
-        <v>0.11</v>
-      </c>
-      <c r="OJ2">
-        <v>3.7</v>
-      </c>
-      <c r="OK2">
-        <v>2.3</v>
-      </c>
-      <c r="OL2">
-        <v>8098</v>
-      </c>
-      <c r="OM2">
-        <v>10000</v>
-      </c>
-      <c r="ON2">
-        <v>81</v>
-      </c>
-      <c r="OO2">
-        <v>146437</v>
-      </c>
-      <c r="OP2">
-        <v>52729</v>
-      </c>
-      <c r="OQ2">
-        <v>3434</v>
-      </c>
-      <c r="OR2">
-        <v>3849</v>
-      </c>
-      <c r="OS2">
-        <v>89.2</v>
-      </c>
-      <c r="OT2">
-        <v>3557</v>
-      </c>
-      <c r="OU2">
-        <v>4039</v>
-      </c>
-      <c r="OV2">
-        <v>88.09999999999999</v>
-      </c>
-      <c r="OW2">
-        <v>885</v>
-      </c>
-      <c r="OX2">
-        <v>1542</v>
-      </c>
-      <c r="OY2">
-        <v>57.4</v>
-      </c>
-      <c r="OZ2">
-        <v>188</v>
-      </c>
-      <c r="PA2">
-        <v>586</v>
-      </c>
-      <c r="PB2">
-        <v>192</v>
-      </c>
-      <c r="PC2">
-        <v>58</v>
-      </c>
-      <c r="PD2">
-        <v>762</v>
-      </c>
-      <c r="PE2">
-        <v>9042</v>
-      </c>
-      <c r="PF2">
-        <v>891</v>
-      </c>
-      <c r="PG2">
-        <v>209</v>
-      </c>
-      <c r="PH2">
-        <v>28</v>
-      </c>
-      <c r="PI2">
-        <v>88</v>
-      </c>
-      <c r="PJ2">
-        <v>350</v>
-      </c>
-      <c r="PK2">
-        <v>86</v>
-      </c>
-      <c r="PL2">
-        <v>26</v>
-      </c>
-      <c r="PM2">
-        <v>39</v>
-      </c>
-      <c r="PN2">
-        <v>0</v>
-      </c>
-      <c r="PO2">
-        <v>398</v>
-      </c>
-      <c r="PP2">
-        <v>67</v>
-      </c>
-      <c r="PQ2">
-        <v>159</v>
-      </c>
-      <c r="PR2">
-        <v>433</v>
-      </c>
-      <c r="PS2">
-        <v>21.65</v>
-      </c>
-      <c r="PT2">
-        <v>335</v>
-      </c>
-      <c r="PU2">
-        <v>39</v>
-      </c>
-      <c r="PV2">
-        <v>13</v>
-      </c>
-      <c r="PW2">
-        <v>20</v>
-      </c>
-      <c r="PX2">
-        <v>17</v>
-      </c>
-      <c r="PY2">
-        <v>50</v>
-      </c>
-      <c r="PZ2">
-        <v>2.5</v>
-      </c>
-      <c r="QA2">
-        <v>39</v>
-      </c>
-      <c r="QB2">
-        <v>1</v>
-      </c>
-      <c r="QC2">
-        <v>3</v>
-      </c>
-      <c r="QD2">
-        <v>5</v>
-      </c>
-      <c r="QE2">
-        <v>2</v>
-      </c>
-      <c r="QF2">
-        <v>0</v>
-      </c>
-      <c r="QG2">
-        <v>355</v>
-      </c>
-      <c r="QH2">
-        <v>188</v>
-      </c>
-      <c r="QI2">
-        <v>171</v>
-      </c>
-      <c r="QJ2">
-        <v>141</v>
-      </c>
-      <c r="QK2">
-        <v>43</v>
-      </c>
-      <c r="QL2">
-        <v>139</v>
-      </c>
-      <c r="QM2">
-        <v>261</v>
-      </c>
-      <c r="QN2">
-        <v>53.3</v>
-      </c>
-      <c r="QO2">
-        <v>122</v>
-      </c>
-      <c r="QP2">
-        <v>230</v>
-      </c>
-      <c r="QQ2">
-        <v>71</v>
-      </c>
-      <c r="QR2">
-        <v>159</v>
-      </c>
-      <c r="QS2">
-        <v>175</v>
-      </c>
-      <c r="QT2">
-        <v>312</v>
-      </c>
-      <c r="QU2">
-        <v>6</v>
-      </c>
-      <c r="QV2">
-        <v>12034</v>
-      </c>
-      <c r="QW2">
-        <v>1328</v>
-      </c>
-      <c r="QX2">
-        <v>4127</v>
-      </c>
-      <c r="QY2">
-        <v>5222</v>
-      </c>
-      <c r="QZ2">
-        <v>2797</v>
-      </c>
-      <c r="RA2">
-        <v>440</v>
-      </c>
-      <c r="RB2">
-        <v>12030</v>
-      </c>
-      <c r="RC2">
-        <v>111</v>
-      </c>
-      <c r="RD2">
-        <v>259</v>
-      </c>
-      <c r="RE2">
-        <v>42.9</v>
-      </c>
-      <c r="RF2">
-        <v>6950</v>
-      </c>
-      <c r="RG2">
-        <v>366</v>
-      </c>
-      <c r="RH2">
-        <v>243</v>
-      </c>
-      <c r="RI2">
-        <v>83</v>
-      </c>
-      <c r="RJ2">
-        <v>8024</v>
-      </c>
-      <c r="RK2">
-        <v>272</v>
-      </c>
-      <c r="RL2">
-        <v>166</v>
-      </c>
-      <c r="RM2">
-        <v>1</v>
-      </c>
-      <c r="RN2">
-        <v>262</v>
-      </c>
-      <c r="RO2">
-        <v>190</v>
-      </c>
-      <c r="RP2">
-        <v>67</v>
-      </c>
-      <c r="RQ2">
-        <v>2</v>
-      </c>
-      <c r="RR2">
-        <v>5</v>
-      </c>
-      <c r="RS2">
-        <v>0</v>
-      </c>
-      <c r="RT2">
-        <v>1043</v>
-      </c>
-      <c r="RU2">
-        <v>229</v>
-      </c>
-      <c r="RV2">
-        <v>183</v>
-      </c>
-      <c r="RW2">
-        <v>55.6</v>
-      </c>
-      <c r="RX2" t="s">
-        <v>814</v>
-      </c>
-      <c r="RY2">
-        <v>24</v>
-      </c>
-      <c r="RZ2">
-        <v>49.1</v>
-      </c>
-      <c r="SA2">
-        <v>20</v>
-      </c>
-      <c r="SB2">
-        <v>220</v>
-      </c>
-      <c r="SC2">
-        <v>1800</v>
-      </c>
-      <c r="SD2">
-        <v>38</v>
-      </c>
-      <c r="SE2">
-        <v>27</v>
-      </c>
-      <c r="SF2">
-        <v>6</v>
-      </c>
-      <c r="SG2">
-        <v>8</v>
-      </c>
-      <c r="SH2">
-        <v>51</v>
-      </c>
-      <c r="SI2">
-        <v>1</v>
-      </c>
-      <c r="SJ2">
-        <v>1.9</v>
-      </c>
-      <c r="SK2">
-        <v>1.35</v>
-      </c>
-      <c r="SL2">
-        <v>3.25</v>
-      </c>
-      <c r="SM2">
-        <v>1.6</v>
-      </c>
-      <c r="SN2">
-        <v>2.95</v>
-      </c>
-      <c r="SO2">
-        <v>32.5</v>
-      </c>
-      <c r="SP2">
-        <v>26.1</v>
-      </c>
-      <c r="SQ2">
-        <v>1.62</v>
-      </c>
-      <c r="SR2">
-        <v>1.3</v>
-      </c>
-      <c r="SS2">
-        <v>20</v>
-      </c>
-      <c r="ST2">
-        <v>20</v>
-      </c>
-      <c r="SU2">
-        <v>1800</v>
-      </c>
-      <c r="SV2">
-        <v>23</v>
-      </c>
-      <c r="SW2">
-        <v>1.15</v>
-      </c>
-      <c r="SX2">
-        <v>74</v>
-      </c>
-      <c r="SY2">
-        <v>52</v>
-      </c>
-      <c r="SZ2">
-        <v>70.3</v>
-      </c>
-      <c r="TA2">
-        <v>11</v>
-      </c>
-      <c r="TB2">
-        <v>5</v>
-      </c>
-      <c r="TC2">
-        <v>4</v>
-      </c>
-      <c r="TD2">
-        <v>7</v>
-      </c>
-      <c r="TE2">
-        <v>35</v>
-      </c>
-      <c r="TF2">
-        <v>1</v>
-      </c>
-      <c r="TG2">
-        <v>1</v>
-      </c>
-      <c r="TH2">
-        <v>0</v>
-      </c>
-      <c r="TI2">
-        <v>0</v>
-      </c>
-      <c r="TJ2">
-        <v>20</v>
-      </c>
-      <c r="TK2">
-        <v>1</v>
-      </c>
-      <c r="TL2">
-        <v>3</v>
-      </c>
-      <c r="TM2">
-        <v>1</v>
-      </c>
-      <c r="TN2">
-        <v>18.9</v>
-      </c>
-      <c r="TO2">
-        <v>0.25</v>
-      </c>
-      <c r="TP2">
-        <v>-3.1</v>
-      </c>
-      <c r="TQ2">
-        <v>-0.15</v>
-      </c>
-      <c r="TR2">
-        <v>110</v>
-      </c>
-      <c r="TS2">
-        <v>249</v>
-      </c>
-      <c r="TT2">
-        <v>44.2</v>
-      </c>
-      <c r="TU2">
-        <v>521</v>
-      </c>
-      <c r="TV2">
-        <v>143</v>
-      </c>
-      <c r="TW2">
-        <v>28.8</v>
-      </c>
-      <c r="TX2">
-        <v>31.2</v>
-      </c>
-      <c r="TY2">
-        <v>153</v>
-      </c>
-      <c r="TZ2">
-        <v>64.7</v>
-      </c>
-      <c r="UA2">
-        <v>48.1</v>
-      </c>
-      <c r="UB2">
-        <v>247</v>
-      </c>
-      <c r="UC2">
-        <v>15</v>
-      </c>
-      <c r="UD2">
-        <v>6.1</v>
-      </c>
-      <c r="UE2">
-        <v>26</v>
-      </c>
-      <c r="UF2">
-        <v>1.3</v>
-      </c>
-      <c r="UG2">
-        <v>17.2</v>
-      </c>
-      <c r="UH2">
-        <v>85</v>
-      </c>
-      <c r="UI2">
-        <v>7</v>
-      </c>
-      <c r="UJ2">
-        <v>32.9</v>
-      </c>
-      <c r="UK2">
-        <v>4.25</v>
-      </c>
-      <c r="UL2">
-        <v>0.12</v>
-      </c>
-      <c r="UM2">
-        <v>0.38</v>
-      </c>
-      <c r="UN2">
-        <v>0.1</v>
-      </c>
-      <c r="UO2">
-        <v>5.5</v>
-      </c>
-      <c r="UP2">
-        <v>5.9</v>
-      </c>
-      <c r="UQ2">
-        <v>7683</v>
-      </c>
-      <c r="UR2">
-        <v>9811</v>
-      </c>
-      <c r="US2">
-        <v>78.3</v>
-      </c>
-      <c r="UT2">
-        <v>135397</v>
-      </c>
-      <c r="UU2">
-        <v>52544</v>
-      </c>
-      <c r="UV2">
-        <v>3554</v>
-      </c>
-      <c r="UW2">
-        <v>4090</v>
-      </c>
-      <c r="UX2">
-        <v>86.90000000000001</v>
-      </c>
-      <c r="UY2">
-        <v>3069</v>
-      </c>
-      <c r="UZ2">
-        <v>3670</v>
-      </c>
-      <c r="VA2">
-        <v>83.59999999999999</v>
-      </c>
-      <c r="VB2">
-        <v>829</v>
-      </c>
-      <c r="VC2">
-        <v>1487</v>
-      </c>
-      <c r="VD2">
-        <v>55.7</v>
-      </c>
-      <c r="VE2">
-        <v>219</v>
-      </c>
-      <c r="VF2">
-        <v>582</v>
-      </c>
-      <c r="VG2">
-        <v>213</v>
-      </c>
-      <c r="VH2">
-        <v>44</v>
-      </c>
-      <c r="VI2">
-        <v>858</v>
-      </c>
-      <c r="VJ2">
-        <v>8805</v>
-      </c>
-      <c r="VK2">
-        <v>978</v>
-      </c>
-      <c r="VL2">
-        <v>229</v>
-      </c>
-      <c r="VM2">
-        <v>25</v>
-      </c>
-      <c r="VN2">
-        <v>97</v>
-      </c>
-      <c r="VO2">
-        <v>309</v>
-      </c>
-      <c r="VP2">
-        <v>83</v>
-      </c>
-      <c r="VQ2">
-        <v>33</v>
-      </c>
-      <c r="VR2">
-        <v>31</v>
-      </c>
-      <c r="VS2">
-        <v>0</v>
-      </c>
       <c r="VT2">
-        <v>437</v>
+        <v>26392</v>
       </c>
       <c r="VU2">
-        <v>28</v>
+        <v>1779</v>
       </c>
       <c r="VV2">
-        <v>163</v>
+        <v>6640</v>
       </c>
       <c r="VW2">
-        <v>481</v>
+        <v>12068</v>
       </c>
       <c r="VX2">
-        <v>24.05</v>
+        <v>7924</v>
       </c>
       <c r="VY2">
-        <v>364</v>
+        <v>1147</v>
       </c>
       <c r="VZ2">
-        <v>39</v>
+        <v>26385</v>
       </c>
       <c r="WA2">
-        <v>23</v>
+        <v>15724</v>
       </c>
       <c r="WB2">
-        <v>27</v>
+        <v>874</v>
       </c>
       <c r="WC2">
-        <v>21</v>
+        <v>658</v>
       </c>
       <c r="WD2">
-        <v>69</v>
+        <v>256</v>
       </c>
       <c r="WE2">
-        <v>3.45</v>
+        <v>17945</v>
       </c>
       <c r="WF2">
-        <v>49</v>
+        <v>680</v>
       </c>
       <c r="WG2">
-        <v>4</v>
+        <v>406</v>
       </c>
       <c r="WH2">
         <v>1</v>
       </c>
       <c r="WI2">
+        <v>580</v>
+      </c>
+      <c r="WJ2">
+        <v>473</v>
+      </c>
+      <c r="WK2">
+        <v>56</v>
+      </c>
+      <c r="WL2">
+        <v>5</v>
+      </c>
+      <c r="WM2">
+        <v>8</v>
+      </c>
+      <c r="WN2">
+        <v>1</v>
+      </c>
+      <c r="WO2">
+        <v>2472</v>
+      </c>
+      <c r="WP2">
+        <v>633</v>
+      </c>
+      <c r="WQ2">
+        <v>506</v>
+      </c>
+      <c r="WR2">
+        <v>55.6</v>
+      </c>
+      <c r="WS2">
+        <v>30</v>
+      </c>
+      <c r="WT2">
+        <v>45.1</v>
+      </c>
+      <c r="WU2">
+        <v>38</v>
+      </c>
+      <c r="WV2">
+        <v>418</v>
+      </c>
+      <c r="WW2">
+        <v>3420</v>
+      </c>
+      <c r="WX2">
+        <v>46</v>
+      </c>
+      <c r="WY2">
+        <v>36</v>
+      </c>
+      <c r="WZ2">
+        <v>5</v>
+      </c>
+      <c r="XA2">
+        <v>8</v>
+      </c>
+      <c r="XB2">
+        <v>87</v>
+      </c>
+      <c r="XC2">
+        <v>4</v>
+      </c>
+      <c r="XD2">
+        <v>1.21</v>
+      </c>
+      <c r="XE2">
+        <v>0.95</v>
+      </c>
+      <c r="XF2">
+        <v>2.16</v>
+      </c>
+      <c r="XG2">
+        <v>1.08</v>
+      </c>
+      <c r="XH2">
+        <v>2.03</v>
+      </c>
+      <c r="XI2">
+        <v>41</v>
+      </c>
+      <c r="XJ2">
+        <v>34.7</v>
+      </c>
+      <c r="XK2">
+        <v>1.08</v>
+      </c>
+      <c r="XL2">
+        <v>0.91</v>
+      </c>
+      <c r="XM2">
+        <v>38</v>
+      </c>
+      <c r="XN2">
+        <v>38</v>
+      </c>
+      <c r="XO2">
+        <v>3420</v>
+      </c>
+      <c r="XP2">
+        <v>90</v>
+      </c>
+      <c r="XQ2">
+        <v>2.37</v>
+      </c>
+      <c r="XR2">
+        <v>228</v>
+      </c>
+      <c r="XS2">
+        <v>137</v>
+      </c>
+      <c r="XT2">
+        <v>63.2</v>
+      </c>
+      <c r="XU2">
+        <v>6</v>
+      </c>
+      <c r="XV2">
+        <v>9</v>
+      </c>
+      <c r="XW2">
+        <v>23</v>
+      </c>
+      <c r="XX2">
+        <v>5</v>
+      </c>
+      <c r="XY2">
+        <v>13.2</v>
+      </c>
+      <c r="XZ2">
         <v>7</v>
       </c>
-      <c r="WJ2">
-        <v>7</v>
-      </c>
-      <c r="WK2">
+      <c r="YA2">
+        <v>6</v>
+      </c>
+      <c r="YB2">
         <v>1</v>
       </c>
-      <c r="WL2">
-        <v>348</v>
-      </c>
-      <c r="WM2">
-        <v>197</v>
-      </c>
-      <c r="WN2">
-        <v>157</v>
-      </c>
-      <c r="WO2">
-        <v>147</v>
-      </c>
-      <c r="WP2">
-        <v>44</v>
-      </c>
-      <c r="WQ2">
-        <v>173</v>
-      </c>
-      <c r="WR2">
-        <v>311</v>
-      </c>
-      <c r="WS2">
-        <v>55.6</v>
-      </c>
-      <c r="WT2">
-        <v>138</v>
-      </c>
-      <c r="WU2">
-        <v>222</v>
-      </c>
-      <c r="WV2">
-        <v>45</v>
-      </c>
-      <c r="WW2">
-        <v>177</v>
-      </c>
-      <c r="WX2">
-        <v>230</v>
-      </c>
-      <c r="WY2">
-        <v>330</v>
-      </c>
-      <c r="WZ2">
-        <v>7</v>
-      </c>
-      <c r="XA2">
-        <v>12094</v>
-      </c>
-      <c r="XB2">
-        <v>1254</v>
-      </c>
-      <c r="XC2">
-        <v>3965</v>
-      </c>
-      <c r="XD2">
-        <v>5101</v>
-      </c>
-      <c r="XE2">
-        <v>3139</v>
-      </c>
-      <c r="XF2">
+      <c r="YC2">
+        <v>0</v>
+      </c>
+      <c r="YD2">
+        <v>38</v>
+      </c>
+      <c r="YE2">
+        <v>1</v>
+      </c>
+      <c r="YF2">
+        <v>6</v>
+      </c>
+      <c r="YG2">
+        <v>0</v>
+      </c>
+      <c r="YH2">
+        <v>76.8</v>
+      </c>
+      <c r="YI2">
+        <v>0.31</v>
+      </c>
+      <c r="YJ2">
+        <v>-13.2</v>
+      </c>
+      <c r="YK2">
+        <v>-0.35</v>
+      </c>
+      <c r="YL2">
+        <v>240</v>
+      </c>
+      <c r="YM2">
+        <v>673</v>
+      </c>
+      <c r="YN2">
+        <v>35.7</v>
+      </c>
+      <c r="YO2">
+        <v>1395</v>
+      </c>
+      <c r="YP2">
+        <v>170</v>
+      </c>
+      <c r="YQ2">
+        <v>37.8</v>
+      </c>
+      <c r="YR2">
+        <v>33.6</v>
+      </c>
+      <c r="YS2">
+        <v>312</v>
+      </c>
+      <c r="YT2">
+        <v>46.5</v>
+      </c>
+      <c r="YU2">
+        <v>36.8</v>
+      </c>
+      <c r="YV2">
         <v>497</v>
       </c>
-      <c r="XG2">
-        <v>12086</v>
-      </c>
-      <c r="XH2">
-        <v>122</v>
-      </c>
-      <c r="XI2">
-        <v>333</v>
-      </c>
-      <c r="XJ2">
-        <v>36.6</v>
-      </c>
-      <c r="XK2">
-        <v>6654</v>
-      </c>
-      <c r="XL2">
-        <v>348</v>
-      </c>
-      <c r="XM2">
-        <v>274</v>
-      </c>
-      <c r="XN2">
-        <v>110</v>
-      </c>
-      <c r="XO2">
-        <v>7625</v>
-      </c>
-      <c r="XP2">
-        <v>326</v>
-      </c>
-      <c r="XQ2">
-        <v>206</v>
-      </c>
-      <c r="XR2">
-        <v>1</v>
-      </c>
-      <c r="XS2">
-        <v>248</v>
-      </c>
-      <c r="XT2">
-        <v>207</v>
-      </c>
-      <c r="XU2">
-        <v>28</v>
-      </c>
-      <c r="XV2">
-        <v>6</v>
-      </c>
-      <c r="XW2">
-        <v>1</v>
-      </c>
-      <c r="XX2">
-        <v>1</v>
-      </c>
-      <c r="XY2">
-        <v>1175</v>
-      </c>
-      <c r="XZ2">
-        <v>303</v>
-      </c>
-      <c r="YA2">
-        <v>248</v>
-      </c>
-      <c r="YB2">
-        <v>55</v>
-      </c>
-      <c r="YC2">
-        <v>24</v>
-      </c>
-      <c r="YD2">
-        <v>51</v>
-      </c>
-      <c r="YE2">
-        <v>20</v>
-      </c>
-      <c r="YF2">
-        <v>220</v>
-      </c>
-      <c r="YG2">
-        <v>1800</v>
-      </c>
-      <c r="YH2">
-        <v>22</v>
-      </c>
-      <c r="YI2">
-        <v>16</v>
-      </c>
-      <c r="YJ2">
-        <v>1</v>
-      </c>
-      <c r="YK2">
-        <v>1</v>
-      </c>
-      <c r="YL2">
-        <v>45</v>
-      </c>
-      <c r="YM2">
-        <v>0</v>
-      </c>
-      <c r="YN2">
-        <v>1.1</v>
-      </c>
-      <c r="YO2">
-        <v>0.8</v>
-      </c>
-      <c r="YP2">
-        <v>1.9</v>
-      </c>
-      <c r="YQ2">
-        <v>1.05</v>
-      </c>
-      <c r="YR2">
-        <v>1.85</v>
-      </c>
-      <c r="YS2">
-        <v>21.3</v>
-      </c>
-      <c r="YT2">
-        <v>20.5</v>
-      </c>
-      <c r="YU2">
-        <v>1.06</v>
-      </c>
-      <c r="YV2">
-        <v>1.02</v>
-      </c>
       <c r="YW2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="YX2">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="YY2">
-        <v>1800</v>
+        <v>35</v>
       </c>
       <c r="YZ2">
-        <v>39</v>
+        <v>0.92</v>
       </c>
       <c r="ZA2">
-        <v>1.95</v>
+        <v>14.4</v>
       </c>
       <c r="ZB2">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="ZC2">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="ZD2">
-        <v>64.5</v>
+        <v>32.8</v>
       </c>
       <c r="ZE2">
-        <v>4</v>
+        <v>2.74</v>
       </c>
       <c r="ZF2">
-        <v>5</v>
+        <v>0.13</v>
       </c>
       <c r="ZG2">
-        <v>11</v>
+        <v>0.39</v>
       </c>
       <c r="ZH2">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="ZI2">
         <v>5</v>
       </c>
       <c r="ZJ2">
-        <v>8</v>
+        <v>6.3</v>
       </c>
       <c r="ZK2">
+        <v>14274</v>
+      </c>
+      <c r="ZL2">
+        <v>18377</v>
+      </c>
+      <c r="ZM2">
+        <v>77.7</v>
+      </c>
+      <c r="ZN2">
+        <v>251869</v>
+      </c>
+      <c r="ZO2">
+        <v>98214</v>
+      </c>
+      <c r="ZP2">
+        <v>6531</v>
+      </c>
+      <c r="ZQ2">
+        <v>7491</v>
+      </c>
+      <c r="ZR2">
+        <v>87.2</v>
+      </c>
+      <c r="ZS2">
+        <v>5707</v>
+      </c>
+      <c r="ZT2">
+        <v>6754</v>
+      </c>
+      <c r="ZU2">
+        <v>84.5</v>
+      </c>
+      <c r="ZV2">
+        <v>1605</v>
+      </c>
+      <c r="ZW2">
+        <v>3053</v>
+      </c>
+      <c r="ZX2">
+        <v>52.6</v>
+      </c>
+      <c r="ZY2">
+        <v>228</v>
+      </c>
+      <c r="ZZ2">
+        <v>885</v>
+      </c>
+      <c r="AAA2">
+        <v>201</v>
+      </c>
+      <c r="AAB2">
+        <v>43</v>
+      </c>
+      <c r="AAC2">
+        <v>1038</v>
+      </c>
+      <c r="AAD2">
+        <v>16502</v>
+      </c>
+      <c r="AAE2">
+        <v>1835</v>
+      </c>
+      <c r="AAF2">
+        <v>609</v>
+      </c>
+      <c r="AAG2">
+        <v>18</v>
+      </c>
+      <c r="AAH2">
+        <v>89</v>
+      </c>
+      <c r="AAI2">
+        <v>460</v>
+      </c>
+      <c r="AAJ2">
+        <v>120</v>
+      </c>
+      <c r="AAK2">
+        <v>48</v>
+      </c>
+      <c r="AAL2">
+        <v>53</v>
+      </c>
+      <c r="AAM2">
+        <v>0</v>
+      </c>
+      <c r="AAN2">
+        <v>640</v>
+      </c>
+      <c r="AAO2">
+        <v>40</v>
+      </c>
+      <c r="AAP2">
+        <v>351</v>
+      </c>
+      <c r="AAQ2">
+        <v>543</v>
+      </c>
+      <c r="AAR2">
+        <v>14.29</v>
+      </c>
+      <c r="AAS2">
+        <v>365</v>
+      </c>
+      <c r="AAT2">
+        <v>44</v>
+      </c>
+      <c r="AAU2">
+        <v>39</v>
+      </c>
+      <c r="AAV2">
+        <v>43</v>
+      </c>
+      <c r="AAW2">
+        <v>76</v>
+      </c>
+      <c r="AAX2">
+        <v>2</v>
+      </c>
+      <c r="AAY2">
+        <v>52</v>
+      </c>
+      <c r="AAZ2">
+        <v>4</v>
+      </c>
+      <c r="ABA2">
         <v>6</v>
       </c>
-      <c r="ZL2">
-        <v>2</v>
-      </c>
-      <c r="ZM2">
+      <c r="ABB2">
+        <v>5</v>
+      </c>
+      <c r="ABC2">
         <v>0</v>
       </c>
-      <c r="ZN2">
-        <v>20</v>
-      </c>
-      <c r="ZO2">
+      <c r="ABD2">
+        <v>716</v>
+      </c>
+      <c r="ABE2">
+        <v>407</v>
+      </c>
+      <c r="ABF2">
+        <v>418</v>
+      </c>
+      <c r="ABG2">
+        <v>243</v>
+      </c>
+      <c r="ABH2">
+        <v>55</v>
+      </c>
+      <c r="ABI2">
+        <v>494</v>
+      </c>
+      <c r="ABJ2">
+        <v>151</v>
+      </c>
+      <c r="ABK2">
+        <v>343</v>
+      </c>
+      <c r="ABL2">
+        <v>528</v>
+      </c>
+      <c r="ABM2">
+        <v>717</v>
+      </c>
+      <c r="ABN2">
+        <v>15</v>
+      </c>
+      <c r="ABO2">
+        <v>22821</v>
+      </c>
+      <c r="ABP2">
+        <v>3113</v>
+      </c>
+      <c r="ABQ2">
+        <v>9294</v>
+      </c>
+      <c r="ABR2">
+        <v>9985</v>
+      </c>
+      <c r="ABS2">
+        <v>3778</v>
+      </c>
+      <c r="ABT2">
+        <v>515</v>
+      </c>
+      <c r="ABU2">
+        <v>22813</v>
+      </c>
+      <c r="ABV2">
+        <v>12053</v>
+      </c>
+      <c r="ABW2">
+        <v>549</v>
+      </c>
+      <c r="ABX2">
+        <v>387</v>
+      </c>
+      <c r="ABY2">
+        <v>109</v>
+      </c>
+      <c r="ABZ2">
+        <v>14104</v>
+      </c>
+      <c r="ACA2">
+        <v>646</v>
+      </c>
+      <c r="ACB2">
+        <v>341</v>
+      </c>
+      <c r="ACC2">
+        <v>3</v>
+      </c>
+      <c r="ACD2">
+        <v>504</v>
+      </c>
+      <c r="ACE2">
+        <v>548</v>
+      </c>
+      <c r="ACF2">
+        <v>40</v>
+      </c>
+      <c r="ACG2">
+        <v>5</v>
+      </c>
+      <c r="ACH2">
+        <v>7</v>
+      </c>
+      <c r="ACI2">
         <v>0</v>
       </c>
-      <c r="ZP2">
-        <v>2</v>
-      </c>
-      <c r="ZQ2">
-        <v>1</v>
-      </c>
-      <c r="ZR2">
-        <v>33.6</v>
-      </c>
-      <c r="ZS2">
-        <v>0.28</v>
-      </c>
-      <c r="ZT2">
-        <v>-4.4</v>
-      </c>
-      <c r="ZU2">
-        <v>-0.22</v>
-      </c>
-      <c r="ZV2">
-        <v>101</v>
-      </c>
-      <c r="ZW2">
-        <v>312</v>
-      </c>
-      <c r="ZX2">
-        <v>32.4</v>
-      </c>
-      <c r="ZY2">
-        <v>705</v>
-      </c>
-      <c r="ZZ2">
-        <v>96</v>
-      </c>
-      <c r="AAA2">
-        <v>36.5</v>
-      </c>
-      <c r="AAB2">
-        <v>34.9</v>
-      </c>
-      <c r="AAC2">
-        <v>141</v>
-      </c>
-      <c r="AAD2">
-        <v>39</v>
-      </c>
-      <c r="AAE2">
-        <v>37.5</v>
-      </c>
-      <c r="AAF2">
-        <v>239</v>
-      </c>
-      <c r="AAG2">
-        <v>10</v>
-      </c>
-      <c r="AAH2">
-        <v>4.2</v>
-      </c>
-      <c r="AAI2">
-        <v>26</v>
-      </c>
-      <c r="AAJ2">
-        <v>1.3</v>
-      </c>
-      <c r="AAK2">
-        <v>15.5</v>
-      </c>
-      <c r="AAL2">
-        <v>73</v>
-      </c>
-      <c r="AAM2">
-        <v>6</v>
-      </c>
-      <c r="AAN2">
-        <v>30.2</v>
-      </c>
-      <c r="AAO2">
-        <v>3.65</v>
-      </c>
-      <c r="AAP2">
-        <v>0.09</v>
-      </c>
-      <c r="AAQ2">
-        <v>0.29</v>
-      </c>
-      <c r="AAR2">
-        <v>0.09</v>
-      </c>
-      <c r="AAS2">
-        <v>0.7</v>
-      </c>
-      <c r="AAT2">
-        <v>0.5</v>
-      </c>
-      <c r="AAU2">
-        <v>7944</v>
-      </c>
-      <c r="AAV2">
-        <v>10147</v>
-      </c>
-      <c r="AAW2">
-        <v>78.3</v>
-      </c>
-      <c r="AAX2">
-        <v>140518</v>
-      </c>
-      <c r="AAY2">
-        <v>52356</v>
-      </c>
-      <c r="AAZ2">
-        <v>3527</v>
-      </c>
-      <c r="ABA2">
-        <v>4009</v>
-      </c>
-      <c r="ABB2">
-        <v>88</v>
-      </c>
-      <c r="ABC2">
-        <v>3258</v>
-      </c>
-      <c r="ABD2">
-        <v>3865</v>
-      </c>
-      <c r="ABE2">
-        <v>84.3</v>
-      </c>
-      <c r="ABF2">
-        <v>884</v>
-      </c>
-      <c r="ABG2">
-        <v>1624</v>
-      </c>
-      <c r="ABH2">
-        <v>54.4</v>
-      </c>
-      <c r="ABI2">
-        <v>182</v>
-      </c>
-      <c r="ABJ2">
-        <v>570</v>
-      </c>
-      <c r="ABK2">
-        <v>152</v>
-      </c>
-      <c r="ABL2">
-        <v>41</v>
-      </c>
-      <c r="ABM2">
-        <v>688</v>
-      </c>
-      <c r="ABN2">
-        <v>9080</v>
-      </c>
-      <c r="ABO2">
-        <v>1041</v>
-      </c>
-      <c r="ABP2">
-        <v>269</v>
-      </c>
-      <c r="ABQ2">
-        <v>16</v>
-      </c>
-      <c r="ABR2">
-        <v>60</v>
-      </c>
-      <c r="ABS2">
-        <v>324</v>
-      </c>
-      <c r="ABT2">
-        <v>87</v>
-      </c>
-      <c r="ABU2">
-        <v>19</v>
-      </c>
-      <c r="ABV2">
-        <v>38</v>
-      </c>
-      <c r="ABW2">
-        <v>0</v>
-      </c>
-      <c r="ABX2">
-        <v>462</v>
-      </c>
-      <c r="ABY2">
-        <v>26</v>
-      </c>
-      <c r="ABZ2">
-        <v>192</v>
-      </c>
-      <c r="ACA2">
-        <v>424</v>
-      </c>
-      <c r="ACB2">
-        <v>21.2</v>
-      </c>
-      <c r="ACC2">
-        <v>325</v>
-      </c>
-      <c r="ACD2">
-        <v>36</v>
-      </c>
-      <c r="ACE2">
-        <v>16</v>
-      </c>
-      <c r="ACF2">
-        <v>21</v>
-      </c>
-      <c r="ACG2">
-        <v>19</v>
-      </c>
-      <c r="ACH2">
-        <v>40</v>
-      </c>
-      <c r="ACI2">
-        <v>2</v>
-      </c>
       <c r="ACJ2">
-        <v>30</v>
+        <v>2251</v>
       </c>
       <c r="ACK2">
-        <v>2</v>
+        <v>506</v>
       </c>
       <c r="ACL2">
-        <v>3</v>
+        <v>633</v>
       </c>
       <c r="ACM2">
-        <v>2</v>
-      </c>
-      <c r="ACN2">
-        <v>3</v>
-      </c>
-      <c r="ACO2">
-        <v>0</v>
-      </c>
-      <c r="ACP2">
-        <v>368</v>
-      </c>
-      <c r="ACQ2">
-        <v>220</v>
-      </c>
-      <c r="ACR2">
-        <v>200</v>
-      </c>
-      <c r="ACS2">
-        <v>126</v>
-      </c>
-      <c r="ACT2">
-        <v>42</v>
-      </c>
-      <c r="ACU2">
-        <v>162</v>
-      </c>
-      <c r="ACV2">
-        <v>284</v>
-      </c>
-      <c r="ACW2">
-        <v>57</v>
-      </c>
-      <c r="ACX2">
-        <v>122</v>
-      </c>
-      <c r="ACY2">
-        <v>222</v>
-      </c>
-      <c r="ACZ2">
-        <v>75</v>
-      </c>
-      <c r="ADA2">
-        <v>147</v>
-      </c>
-      <c r="ADB2">
-        <v>196</v>
-      </c>
-      <c r="ADC2">
-        <v>324</v>
-      </c>
-      <c r="ADD2">
-        <v>4</v>
-      </c>
-      <c r="ADE2">
-        <v>12444</v>
-      </c>
-      <c r="ADF2">
-        <v>1351</v>
-      </c>
-      <c r="ADG2">
-        <v>4299</v>
-      </c>
-      <c r="ADH2">
-        <v>5533</v>
-      </c>
-      <c r="ADI2">
-        <v>2748</v>
-      </c>
-      <c r="ADJ2">
-        <v>397</v>
-      </c>
-      <c r="ADK2">
-        <v>12443</v>
-      </c>
-      <c r="ADL2">
-        <v>138</v>
-      </c>
-      <c r="ADM2">
-        <v>350</v>
-      </c>
-      <c r="ADN2">
-        <v>39.4</v>
-      </c>
-      <c r="ADO2">
-        <v>6961</v>
-      </c>
-      <c r="ADP2">
-        <v>317</v>
-      </c>
-      <c r="ADQ2">
-        <v>239</v>
-      </c>
-      <c r="ADR2">
-        <v>81</v>
-      </c>
-      <c r="ADS2">
-        <v>7831</v>
-      </c>
-      <c r="ADT2">
-        <v>356</v>
-      </c>
-      <c r="ADU2">
-        <v>175</v>
-      </c>
-      <c r="ADV2">
-        <v>0</v>
-      </c>
-      <c r="ADW2">
-        <v>220</v>
-      </c>
-      <c r="ADX2">
-        <v>232</v>
-      </c>
-      <c r="ADY2">
-        <v>26</v>
-      </c>
-      <c r="ADZ2">
-        <v>1</v>
-      </c>
-      <c r="AEA2">
-        <v>8</v>
-      </c>
-      <c r="AEB2">
-        <v>1</v>
-      </c>
-      <c r="AEC2">
-        <v>1214</v>
-      </c>
-      <c r="AED2">
-        <v>248</v>
-      </c>
-      <c r="AEE2">
-        <v>303</v>
-      </c>
-      <c r="AEF2">
-        <v>45</v>
+        <v>44.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Matchdays 32 and 33 + notebook for Lineup simulation
</commit_message>
<xml_diff>
--- a/tmp/playermatchdata.xlsx
+++ b/tmp/playermatchdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="770">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -2311,13 +2311,16 @@
     <t>opp_vs_team_aerials_won_pct</t>
   </si>
   <si>
-    <t>Immobile</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Lazio</t>
+    <t>Frattesi</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Sassuolo</t>
+  </si>
+  <si>
+    <t>23-115</t>
   </si>
   <si>
     <t>Atalanta</t>
@@ -4989,10 +4992,10 @@
         <v>765</v>
       </c>
       <c r="B2">
-        <v>452</v>
+        <v>274</v>
       </c>
       <c r="C2">
-        <v>785</v>
+        <v>2848</v>
       </c>
       <c r="D2" t="s">
         <v>766</v>
@@ -5004,88 +5007,88 @@
         <v>765</v>
       </c>
       <c r="H2">
-        <v>250</v>
-      </c>
-      <c r="I2">
-        <v>30</v>
+        <v>192</v>
+      </c>
+      <c r="I2" t="s">
+        <v>768</v>
       </c>
       <c r="J2">
-        <v>1990</v>
+        <v>1999</v>
       </c>
       <c r="K2">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L2">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="M2">
-        <v>2849</v>
+        <v>1816</v>
       </c>
       <c r="N2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="O2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.63</v>
+        <v>0.25</v>
       </c>
       <c r="U2">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>0.82</v>
+        <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.51</v>
+        <v>0.25</v>
       </c>
       <c r="X2">
-        <v>0.6899999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="Y2">
-        <v>19.8</v>
+        <v>4.8</v>
       </c>
       <c r="Z2">
-        <v>13.6</v>
+        <v>4.8</v>
       </c>
       <c r="AA2">
-        <v>0.63</v>
+        <v>0.24</v>
       </c>
       <c r="AB2">
-        <v>0.43</v>
+        <v>0.24</v>
       </c>
       <c r="AC2">
         <v>0</v>
       </c>
       <c r="AD2">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>39.3</v>
+        <v>45</v>
       </c>
       <c r="AG2">
-        <v>1.39</v>
+        <v>0.89</v>
       </c>
       <c r="AH2">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="AI2">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="AJ2">
         <v>0.12</v>
@@ -5094,250 +5097,250 @@
         <v>0.2</v>
       </c>
       <c r="AL2">
-        <v>2.4</v>
+        <v>0.2</v>
       </c>
       <c r="AM2">
-        <v>651</v>
+        <v>509</v>
       </c>
       <c r="AN2">
-        <v>897</v>
+        <v>648</v>
       </c>
       <c r="AO2">
-        <v>72.59999999999999</v>
+        <v>78.5</v>
       </c>
       <c r="AP2">
-        <v>8700</v>
+        <v>8833</v>
       </c>
       <c r="AQ2">
-        <v>1781</v>
+        <v>2393</v>
       </c>
       <c r="AR2">
-        <v>393</v>
+        <v>239</v>
       </c>
       <c r="AS2">
-        <v>488</v>
+        <v>289</v>
       </c>
       <c r="AT2">
-        <v>80.5</v>
+        <v>82.7</v>
       </c>
       <c r="AU2">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="AV2">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="AW2">
-        <v>72.40000000000001</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="AX2">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="AY2">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="AZ2">
-        <v>63.1</v>
+        <v>67</v>
       </c>
       <c r="BA2">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="BB2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="BC2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="BD2">
         <v>1</v>
       </c>
       <c r="BE2">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BF2">
-        <v>867</v>
+        <v>631</v>
       </c>
       <c r="BG2">
+        <v>17</v>
+      </c>
+      <c r="BH2">
+        <v>13</v>
+      </c>
+      <c r="BI2">
+        <v>4</v>
+      </c>
+      <c r="BJ2">
+        <v>15</v>
+      </c>
+      <c r="BK2">
+        <v>10</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>4</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>14</v>
+      </c>
+      <c r="BS2">
+        <v>61</v>
+      </c>
+      <c r="BT2">
+        <v>3.02</v>
+      </c>
+      <c r="BU2">
+        <v>49</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>4</v>
+      </c>
+      <c r="BX2">
+        <v>3</v>
+      </c>
+      <c r="BY2">
+        <v>4</v>
+      </c>
+      <c r="BZ2">
+        <v>0.2</v>
+      </c>
+      <c r="CA2">
+        <v>4</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+      <c r="CE2">
+        <v>0</v>
+      </c>
+      <c r="CF2">
+        <v>42</v>
+      </c>
+      <c r="CG2">
+        <v>19</v>
+      </c>
+      <c r="CH2">
+        <v>14</v>
+      </c>
+      <c r="CI2">
+        <v>22</v>
+      </c>
+      <c r="CJ2">
+        <v>6</v>
+      </c>
+      <c r="CK2">
+        <v>17</v>
+      </c>
+      <c r="CL2">
+        <v>3</v>
+      </c>
+      <c r="CM2">
+        <v>14</v>
+      </c>
+      <c r="CN2">
+        <v>8</v>
+      </c>
+      <c r="CO2">
         <v>27</v>
       </c>
-      <c r="BH2">
-        <v>3</v>
-      </c>
-      <c r="BI2">
-        <v>3</v>
-      </c>
-      <c r="BJ2">
-        <v>3</v>
-      </c>
-      <c r="BK2">
-        <v>18</v>
-      </c>
-      <c r="BL2">
-        <v>6</v>
-      </c>
-      <c r="BM2">
-        <v>4</v>
-      </c>
-      <c r="BN2">
-        <v>1</v>
-      </c>
-      <c r="BO2">
-        <v>0</v>
-      </c>
-      <c r="BP2">
-        <v>10</v>
-      </c>
-      <c r="BQ2">
-        <v>3</v>
-      </c>
-      <c r="BR2">
-        <v>31</v>
-      </c>
-      <c r="BS2">
-        <v>118</v>
-      </c>
-      <c r="BT2">
-        <v>3.73</v>
-      </c>
-      <c r="BU2">
-        <v>86</v>
-      </c>
-      <c r="BV2">
-        <v>0</v>
-      </c>
-      <c r="BW2">
+      <c r="CP2">
+        <v>0</v>
+      </c>
+      <c r="CQ2">
+        <v>898</v>
+      </c>
+      <c r="CR2">
+        <v>43</v>
+      </c>
+      <c r="CS2">
+        <v>182</v>
+      </c>
+      <c r="CT2">
+        <v>455</v>
+      </c>
+      <c r="CU2">
+        <v>276</v>
+      </c>
+      <c r="CV2">
+        <v>60</v>
+      </c>
+      <c r="CW2">
+        <v>898</v>
+      </c>
+      <c r="CX2">
+        <v>505</v>
+      </c>
+      <c r="CY2">
+        <v>47</v>
+      </c>
+      <c r="CZ2">
+        <v>37</v>
+      </c>
+      <c r="DA2">
         <v>14</v>
       </c>
-      <c r="BX2">
-        <v>8</v>
-      </c>
-      <c r="BY2">
-        <v>15</v>
-      </c>
-      <c r="BZ2">
-        <v>0.47</v>
-      </c>
-      <c r="CA2">
-        <v>8</v>
-      </c>
-      <c r="CB2">
-        <v>0</v>
-      </c>
-      <c r="CC2">
-        <v>2</v>
-      </c>
-      <c r="CD2">
-        <v>4</v>
-      </c>
-      <c r="CE2">
-        <v>0</v>
-      </c>
-      <c r="CF2">
-        <v>14</v>
-      </c>
-      <c r="CG2">
-        <v>13</v>
-      </c>
-      <c r="CH2">
-        <v>4</v>
-      </c>
-      <c r="CI2">
-        <v>6</v>
-      </c>
-      <c r="CJ2">
-        <v>4</v>
-      </c>
-      <c r="CK2">
-        <v>13</v>
-      </c>
-      <c r="CL2">
-        <v>1</v>
-      </c>
-      <c r="CM2">
+      <c r="DB2">
+        <v>607</v>
+      </c>
+      <c r="DC2">
+        <v>34</v>
+      </c>
+      <c r="DD2">
+        <v>28</v>
+      </c>
+      <c r="DE2">
+        <v>0</v>
+      </c>
+      <c r="DF2">
+        <v>28</v>
+      </c>
+      <c r="DG2">
+        <v>38</v>
+      </c>
+      <c r="DH2">
+        <v>0</v>
+      </c>
+      <c r="DI2">
+        <v>0</v>
+      </c>
+      <c r="DJ2">
+        <v>0</v>
+      </c>
+      <c r="DK2">
+        <v>0</v>
+      </c>
+      <c r="DL2">
+        <v>103</v>
+      </c>
+      <c r="DM2">
+        <v>17</v>
+      </c>
+      <c r="DN2">
         <v>12</v>
       </c>
-      <c r="CN2">
-        <v>6</v>
-      </c>
-      <c r="CO2">
-        <v>9</v>
-      </c>
-      <c r="CP2">
-        <v>0</v>
-      </c>
-      <c r="CQ2">
-        <v>1218</v>
-      </c>
-      <c r="CR2">
-        <v>10</v>
-      </c>
-      <c r="CS2">
-        <v>94</v>
-      </c>
-      <c r="CT2">
-        <v>443</v>
-      </c>
-      <c r="CU2">
-        <v>692</v>
-      </c>
-      <c r="CV2">
-        <v>207</v>
-      </c>
-      <c r="CW2">
-        <v>1210</v>
-      </c>
-      <c r="CX2">
-        <v>700</v>
-      </c>
-      <c r="CY2">
-        <v>74</v>
-      </c>
-      <c r="CZ2">
-        <v>43</v>
-      </c>
-      <c r="DA2">
-        <v>38</v>
-      </c>
-      <c r="DB2">
-        <v>968</v>
-      </c>
-      <c r="DC2">
-        <v>71</v>
-      </c>
-      <c r="DD2">
-        <v>34</v>
-      </c>
-      <c r="DE2">
-        <v>0</v>
-      </c>
-      <c r="DF2">
-        <v>37</v>
-      </c>
-      <c r="DG2">
-        <v>44</v>
-      </c>
-      <c r="DH2">
-        <v>30</v>
-      </c>
-      <c r="DI2">
-        <v>3</v>
-      </c>
-      <c r="DJ2">
-        <v>0</v>
-      </c>
-      <c r="DK2">
-        <v>0</v>
-      </c>
-      <c r="DL2">
-        <v>79</v>
-      </c>
-      <c r="DM2">
-        <v>26</v>
-      </c>
-      <c r="DN2">
-        <v>54</v>
-      </c>
       <c r="DO2">
-        <v>32.5</v>
+        <v>58.6</v>
       </c>
       <c r="DP2">
         <v>0</v>
@@ -5460,1828 +5463,1828 @@
         <v>0</v>
       </c>
       <c r="FD2">
-        <v>6.228571428571429</v>
+        <v>6.318181818181818</v>
       </c>
       <c r="FE2">
-        <v>0.9361231385946214</v>
+        <v>0.6997638326518479</v>
       </c>
       <c r="FF2" t="s">
         <v>767</v>
       </c>
       <c r="FG2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="FH2">
-        <v>53</v>
+        <v>48.7</v>
       </c>
       <c r="FI2">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="FJ2">
-        <v>418</v>
+        <v>242</v>
       </c>
       <c r="FK2">
-        <v>3420</v>
+        <v>1980</v>
       </c>
       <c r="FL2">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="FM2">
+        <v>18</v>
+      </c>
+      <c r="FN2">
+        <v>4</v>
+      </c>
+      <c r="FO2">
+        <v>5</v>
+      </c>
+      <c r="FP2">
+        <v>57</v>
+      </c>
+      <c r="FQ2">
+        <v>2</v>
+      </c>
+      <c r="FR2">
+        <v>1.14</v>
+      </c>
+      <c r="FS2">
+        <v>0.82</v>
+      </c>
+      <c r="FT2">
+        <v>1.95</v>
+      </c>
+      <c r="FU2">
+        <v>0.95</v>
+      </c>
+      <c r="FV2">
+        <v>1.77</v>
+      </c>
+      <c r="FW2">
+        <v>28.1</v>
+      </c>
+      <c r="FX2">
+        <v>24.2</v>
+      </c>
+      <c r="FY2">
+        <v>1.28</v>
+      </c>
+      <c r="FZ2">
+        <v>1.1</v>
+      </c>
+      <c r="GA2">
+        <v>22</v>
+      </c>
+      <c r="GB2">
+        <v>22</v>
+      </c>
+      <c r="GC2">
+        <v>1980</v>
+      </c>
+      <c r="GD2">
+        <v>33</v>
+      </c>
+      <c r="GE2">
+        <v>1.5</v>
+      </c>
+      <c r="GF2">
+        <v>73</v>
+      </c>
+      <c r="GG2">
         <v>40</v>
       </c>
-      <c r="FN2">
+      <c r="GH2">
+        <v>60.3</v>
+      </c>
+      <c r="GI2">
         <v>6</v>
       </c>
-      <c r="FO2">
+      <c r="GJ2">
+        <v>6</v>
+      </c>
+      <c r="GK2">
         <v>10</v>
       </c>
-      <c r="FP2">
-        <v>107</v>
-      </c>
-      <c r="FQ2">
-        <v>5</v>
-      </c>
-      <c r="FR2">
-        <v>1.55</v>
-      </c>
-      <c r="FS2">
+      <c r="GL2">
+        <v>6</v>
+      </c>
+      <c r="GM2">
+        <v>27.3</v>
+      </c>
+      <c r="GN2">
+        <v>4</v>
+      </c>
+      <c r="GO2">
+        <v>4</v>
+      </c>
+      <c r="GP2">
+        <v>0</v>
+      </c>
+      <c r="GQ2">
+        <v>0</v>
+      </c>
+      <c r="GR2">
+        <v>22</v>
+      </c>
+      <c r="GS2">
+        <v>0</v>
+      </c>
+      <c r="GT2">
+        <v>3</v>
+      </c>
+      <c r="GU2">
+        <v>0</v>
+      </c>
+      <c r="GV2">
+        <v>27.7</v>
+      </c>
+      <c r="GW2">
+        <v>0.34</v>
+      </c>
+      <c r="GX2">
+        <v>-5.3</v>
+      </c>
+      <c r="GY2">
+        <v>-0.24</v>
+      </c>
+      <c r="GZ2">
+        <v>122</v>
+      </c>
+      <c r="HA2">
+        <v>295</v>
+      </c>
+      <c r="HB2">
+        <v>41.4</v>
+      </c>
+      <c r="HC2">
+        <v>772</v>
+      </c>
+      <c r="HD2">
+        <v>118</v>
+      </c>
+      <c r="HE2">
+        <v>29.8</v>
+      </c>
+      <c r="HF2">
+        <v>33.8</v>
+      </c>
+      <c r="HG2">
+        <v>195</v>
+      </c>
+      <c r="HH2">
+        <v>33.3</v>
+      </c>
+      <c r="HI2">
+        <v>33.7</v>
+      </c>
+      <c r="HJ2">
+        <v>304</v>
+      </c>
+      <c r="HK2">
+        <v>19</v>
+      </c>
+      <c r="HL2">
+        <v>6.3</v>
+      </c>
+      <c r="HM2">
+        <v>23</v>
+      </c>
+      <c r="HN2">
         <v>1.05</v>
       </c>
-      <c r="FT2">
-        <v>2.61</v>
-      </c>
-      <c r="FU2">
-        <v>1.39</v>
-      </c>
-      <c r="FV2">
-        <v>2.45</v>
-      </c>
-      <c r="FW2">
-        <v>58.2</v>
-      </c>
-      <c r="FX2">
-        <v>50.7</v>
-      </c>
-      <c r="FY2">
-        <v>1.53</v>
-      </c>
-      <c r="FZ2">
-        <v>1.33</v>
-      </c>
-      <c r="GA2">
-        <v>38</v>
-      </c>
-      <c r="GB2">
-        <v>38</v>
-      </c>
-      <c r="GC2">
-        <v>3420</v>
-      </c>
-      <c r="GD2">
-        <v>55</v>
-      </c>
-      <c r="GE2">
-        <v>1.45</v>
-      </c>
-      <c r="GF2">
+      <c r="HO2">
+        <v>14.5</v>
+      </c>
+      <c r="HP2">
+        <v>96</v>
+      </c>
+      <c r="HQ2">
+        <v>12</v>
+      </c>
+      <c r="HR2">
+        <v>34.5</v>
+      </c>
+      <c r="HS2">
+        <v>4.36</v>
+      </c>
+      <c r="HT2">
+        <v>0.08</v>
+      </c>
+      <c r="HU2">
+        <v>0.22</v>
+      </c>
+      <c r="HV2">
+        <v>0.09</v>
+      </c>
+      <c r="HW2">
+        <v>-3.1</v>
+      </c>
+      <c r="HX2">
+        <v>-3.2</v>
+      </c>
+      <c r="HY2">
+        <v>8389</v>
+      </c>
+      <c r="HZ2">
+        <v>10407</v>
+      </c>
+      <c r="IA2">
+        <v>80.59999999999999</v>
+      </c>
+      <c r="IB2">
+        <v>158263</v>
+      </c>
+      <c r="IC2">
+        <v>57659</v>
+      </c>
+      <c r="ID2">
+        <v>3486</v>
+      </c>
+      <c r="IE2">
+        <v>3939</v>
+      </c>
+      <c r="IF2">
+        <v>88.5</v>
+      </c>
+      <c r="IG2">
+        <v>3507</v>
+      </c>
+      <c r="IH2">
+        <v>4057</v>
+      </c>
+      <c r="II2">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="IJ2">
+        <v>1196</v>
+      </c>
+      <c r="IK2">
+        <v>1889</v>
+      </c>
+      <c r="IL2">
+        <v>63.3</v>
+      </c>
+      <c r="IM2">
+        <v>223</v>
+      </c>
+      <c r="IN2">
+        <v>611</v>
+      </c>
+      <c r="IO2">
+        <v>185</v>
+      </c>
+      <c r="IP2">
+        <v>52</v>
+      </c>
+      <c r="IQ2">
+        <v>854</v>
+      </c>
+      <c r="IR2">
+        <v>9196</v>
+      </c>
+      <c r="IS2">
+        <v>1192</v>
+      </c>
+      <c r="IT2">
+        <v>341</v>
+      </c>
+      <c r="IU2">
+        <v>21</v>
+      </c>
+      <c r="IV2">
+        <v>124</v>
+      </c>
+      <c r="IW2">
+        <v>334</v>
+      </c>
+      <c r="IX2">
+        <v>96</v>
+      </c>
+      <c r="IY2">
+        <v>44</v>
+      </c>
+      <c r="IZ2">
+        <v>27</v>
+      </c>
+      <c r="JA2">
+        <v>0</v>
+      </c>
+      <c r="JB2">
+        <v>472</v>
+      </c>
+      <c r="JC2">
+        <v>19</v>
+      </c>
+      <c r="JD2">
+        <v>197</v>
+      </c>
+      <c r="JE2">
+        <v>504</v>
+      </c>
+      <c r="JF2">
+        <v>22.91</v>
+      </c>
+      <c r="JG2">
+        <v>404</v>
+      </c>
+      <c r="JH2">
+        <v>27</v>
+      </c>
+      <c r="JI2">
+        <v>24</v>
+      </c>
+      <c r="JJ2">
+        <v>21</v>
+      </c>
+      <c r="JK2">
+        <v>45</v>
+      </c>
+      <c r="JL2">
+        <v>2.05</v>
+      </c>
+      <c r="JM2">
+        <v>35</v>
+      </c>
+      <c r="JN2">
+        <v>2</v>
+      </c>
+      <c r="JO2">
+        <v>3</v>
+      </c>
+      <c r="JP2">
+        <v>3</v>
+      </c>
+      <c r="JQ2">
+        <v>0</v>
+      </c>
+      <c r="JR2">
+        <v>311</v>
+      </c>
+      <c r="JS2">
+        <v>169</v>
+      </c>
+      <c r="JT2">
         <v>151</v>
       </c>
-      <c r="GG2">
-        <v>98</v>
-      </c>
-      <c r="GH2">
-        <v>70.2</v>
-      </c>
-      <c r="GI2">
-        <v>21</v>
-      </c>
-      <c r="GJ2">
-        <v>5</v>
-      </c>
-      <c r="GK2">
-        <v>12</v>
-      </c>
-      <c r="GL2">
-        <v>12</v>
-      </c>
-      <c r="GM2">
-        <v>31.6</v>
-      </c>
-      <c r="GN2">
-        <v>10</v>
-      </c>
-      <c r="GO2">
-        <v>10</v>
-      </c>
-      <c r="GP2">
-        <v>0</v>
-      </c>
-      <c r="GQ2">
-        <v>0</v>
-      </c>
-      <c r="GR2">
-        <v>38</v>
-      </c>
-      <c r="GS2">
-        <v>0</v>
-      </c>
-      <c r="GT2">
-        <v>7</v>
-      </c>
-      <c r="GU2">
-        <v>2</v>
-      </c>
-      <c r="GV2">
-        <v>50.2</v>
-      </c>
-      <c r="GW2">
-        <v>0.27</v>
-      </c>
-      <c r="GX2">
-        <v>-2.8</v>
-      </c>
-      <c r="GY2">
-        <v>-0.07000000000000001</v>
-      </c>
-      <c r="GZ2">
-        <v>181</v>
-      </c>
-      <c r="HA2">
-        <v>385</v>
-      </c>
-      <c r="HB2">
-        <v>47</v>
-      </c>
-      <c r="HC2">
-        <v>1270</v>
-      </c>
-      <c r="HD2">
-        <v>174</v>
-      </c>
-      <c r="HE2">
-        <v>27.4</v>
-      </c>
-      <c r="HF2">
-        <v>30.4</v>
-      </c>
-      <c r="HG2">
-        <v>202</v>
-      </c>
-      <c r="HH2">
-        <v>18.3</v>
-      </c>
-      <c r="HI2">
-        <v>25</v>
-      </c>
-      <c r="HJ2">
-        <v>491</v>
-      </c>
-      <c r="HK2">
-        <v>13</v>
-      </c>
-      <c r="HL2">
-        <v>2.6</v>
-      </c>
-      <c r="HM2">
+      <c r="JU2">
+        <v>119</v>
+      </c>
+      <c r="JV2">
+        <v>41</v>
+      </c>
+      <c r="JW2">
+        <v>199</v>
+      </c>
+      <c r="JX2">
+        <v>61</v>
+      </c>
+      <c r="JY2">
+        <v>138</v>
+      </c>
+      <c r="JZ2">
+        <v>160</v>
+      </c>
+      <c r="KA2">
+        <v>390</v>
+      </c>
+      <c r="KB2">
+        <v>8</v>
+      </c>
+      <c r="KC2">
+        <v>12625</v>
+      </c>
+      <c r="KD2">
+        <v>1458</v>
+      </c>
+      <c r="KE2">
+        <v>4412</v>
+      </c>
+      <c r="KF2">
+        <v>5491</v>
+      </c>
+      <c r="KG2">
+        <v>2846</v>
+      </c>
+      <c r="KH2">
+        <v>425</v>
+      </c>
+      <c r="KI2">
+        <v>12620</v>
+      </c>
+      <c r="KJ2">
+        <v>7280</v>
+      </c>
+      <c r="KK2">
+        <v>415</v>
+      </c>
+      <c r="KL2">
+        <v>279</v>
+      </c>
+      <c r="KM2">
+        <v>110</v>
+      </c>
+      <c r="KN2">
+        <v>8311</v>
+      </c>
+      <c r="KO2">
+        <v>298</v>
+      </c>
+      <c r="KP2">
+        <v>228</v>
+      </c>
+      <c r="KQ2">
+        <v>1</v>
+      </c>
+      <c r="KR2">
+        <v>227</v>
+      </c>
+      <c r="KS2">
+        <v>269</v>
+      </c>
+      <c r="KT2">
+        <v>19</v>
+      </c>
+      <c r="KU2">
+        <v>4</v>
+      </c>
+      <c r="KV2">
+        <v>4</v>
+      </c>
+      <c r="KW2">
+        <v>0</v>
+      </c>
+      <c r="KX2">
+        <v>994</v>
+      </c>
+      <c r="KY2">
+        <v>206</v>
+      </c>
+      <c r="KZ2">
+        <v>256</v>
+      </c>
+      <c r="LA2">
+        <v>44.6</v>
+      </c>
+      <c r="LB2">
+        <v>29</v>
+      </c>
+      <c r="LC2">
+        <v>51.3</v>
+      </c>
+      <c r="LD2">
         <v>22</v>
       </c>
-      <c r="HN2">
-        <v>0.58</v>
-      </c>
-      <c r="HO2">
-        <v>13.9</v>
-      </c>
-      <c r="HP2">
-        <v>175</v>
-      </c>
-      <c r="HQ2">
-        <v>14</v>
-      </c>
-      <c r="HR2">
-        <v>34</v>
-      </c>
-      <c r="HS2">
-        <v>4.61</v>
-      </c>
-      <c r="HT2">
-        <v>0.1</v>
-      </c>
-      <c r="HU2">
-        <v>0.3</v>
-      </c>
-      <c r="HV2">
-        <v>0.1</v>
-      </c>
-      <c r="HW2">
-        <v>0.8</v>
-      </c>
-      <c r="HX2">
-        <v>2.3</v>
-      </c>
-      <c r="HY2">
-        <v>16972</v>
-      </c>
-      <c r="HZ2">
-        <v>20795</v>
-      </c>
-      <c r="IA2">
-        <v>81.59999999999999</v>
-      </c>
-      <c r="IB2">
-        <v>304863</v>
-      </c>
-      <c r="IC2">
-        <v>108222</v>
-      </c>
-      <c r="ID2">
-        <v>7366</v>
-      </c>
-      <c r="IE2">
-        <v>8356</v>
-      </c>
-      <c r="IF2">
-        <v>88.2</v>
-      </c>
-      <c r="IG2">
-        <v>7099</v>
-      </c>
-      <c r="IH2">
-        <v>8110</v>
-      </c>
-      <c r="II2">
-        <v>87.5</v>
-      </c>
-      <c r="IJ2">
-        <v>2007</v>
-      </c>
-      <c r="IK2">
-        <v>3161</v>
-      </c>
-      <c r="IL2">
-        <v>63.5</v>
-      </c>
-      <c r="IM2">
-        <v>391</v>
-      </c>
-      <c r="IN2">
-        <v>1479</v>
-      </c>
-      <c r="IO2">
-        <v>398</v>
-      </c>
-      <c r="IP2">
-        <v>115</v>
-      </c>
-      <c r="IQ2">
-        <v>1688</v>
-      </c>
-      <c r="IR2">
-        <v>19069</v>
-      </c>
-      <c r="IS2">
-        <v>1639</v>
-      </c>
-      <c r="IT2">
-        <v>468</v>
-      </c>
-      <c r="IU2">
-        <v>25</v>
-      </c>
-      <c r="IV2">
-        <v>151</v>
-      </c>
-      <c r="IW2">
-        <v>744</v>
-      </c>
-      <c r="IX2">
-        <v>189</v>
-      </c>
-      <c r="IY2">
-        <v>97</v>
-      </c>
-      <c r="IZ2">
-        <v>63</v>
-      </c>
-      <c r="JA2">
-        <v>1</v>
-      </c>
-      <c r="JB2">
-        <v>653</v>
-      </c>
-      <c r="JC2">
-        <v>87</v>
-      </c>
-      <c r="JD2">
-        <v>346</v>
-      </c>
-      <c r="JE2">
-        <v>937</v>
-      </c>
-      <c r="JF2">
-        <v>24.66</v>
-      </c>
-      <c r="JG2">
-        <v>733</v>
-      </c>
-      <c r="JH2">
-        <v>53</v>
-      </c>
-      <c r="JI2">
-        <v>55</v>
-      </c>
-      <c r="JJ2">
+      <c r="LE2">
+        <v>242</v>
+      </c>
+      <c r="LF2">
+        <v>1980</v>
+      </c>
+      <c r="LG2">
         <v>33</v>
       </c>
-      <c r="JK2">
-        <v>103</v>
-      </c>
-      <c r="JL2">
-        <v>2.71</v>
-      </c>
-      <c r="JM2">
-        <v>75</v>
-      </c>
-      <c r="JN2">
-        <v>1</v>
-      </c>
-      <c r="JO2">
-        <v>9</v>
-      </c>
-      <c r="JP2">
-        <v>9</v>
-      </c>
-      <c r="JQ2">
-        <v>1</v>
-      </c>
-      <c r="JR2">
-        <v>595</v>
-      </c>
-      <c r="JS2">
-        <v>346</v>
-      </c>
-      <c r="JT2">
-        <v>284</v>
-      </c>
-      <c r="JU2">
-        <v>244</v>
-      </c>
-      <c r="JV2">
-        <v>67</v>
-      </c>
-      <c r="JW2">
-        <v>404</v>
-      </c>
-      <c r="JX2">
-        <v>92</v>
-      </c>
-      <c r="JY2">
-        <v>312</v>
-      </c>
-      <c r="JZ2">
-        <v>445</v>
-      </c>
-      <c r="KA2">
-        <v>649</v>
-      </c>
-      <c r="KB2">
-        <v>7</v>
-      </c>
-      <c r="KC2">
-        <v>24888</v>
-      </c>
-      <c r="KD2">
-        <v>2487</v>
-      </c>
-      <c r="KE2">
-        <v>7653</v>
-      </c>
-      <c r="KF2">
-        <v>11527</v>
-      </c>
-      <c r="KG2">
-        <v>5958</v>
-      </c>
-      <c r="KH2">
-        <v>883</v>
-      </c>
-      <c r="KI2">
-        <v>24878</v>
-      </c>
-      <c r="KJ2">
-        <v>14348</v>
-      </c>
-      <c r="KK2">
-        <v>785</v>
-      </c>
-      <c r="KL2">
-        <v>618</v>
-      </c>
-      <c r="KM2">
-        <v>171</v>
-      </c>
-      <c r="KN2">
-        <v>16794</v>
-      </c>
-      <c r="KO2">
-        <v>553</v>
-      </c>
-      <c r="KP2">
-        <v>304</v>
-      </c>
-      <c r="KQ2">
-        <v>3</v>
-      </c>
-      <c r="KR2">
-        <v>498</v>
-      </c>
-      <c r="KS2">
-        <v>427</v>
-      </c>
-      <c r="KT2">
-        <v>87</v>
-      </c>
-      <c r="KU2">
-        <v>8</v>
-      </c>
-      <c r="KV2">
-        <v>10</v>
-      </c>
-      <c r="KW2">
-        <v>2</v>
-      </c>
-      <c r="KX2">
-        <v>2132</v>
-      </c>
-      <c r="KY2">
-        <v>539</v>
-      </c>
-      <c r="KZ2">
-        <v>510</v>
-      </c>
-      <c r="LA2">
-        <v>51.4</v>
-      </c>
-      <c r="LB2">
-        <v>30</v>
-      </c>
-      <c r="LC2">
-        <v>46.9</v>
-      </c>
-      <c r="LD2">
-        <v>38</v>
-      </c>
-      <c r="LE2">
-        <v>418</v>
-      </c>
-      <c r="LF2">
-        <v>3420</v>
-      </c>
-      <c r="LG2">
-        <v>53</v>
-      </c>
       <c r="LH2">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="LI2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="LJ2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="LK2">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="LL2">
         <v>3</v>
       </c>
       <c r="LM2">
-        <v>1.39</v>
+        <v>1.5</v>
       </c>
       <c r="LN2">
-        <v>0.87</v>
+        <v>1.09</v>
       </c>
       <c r="LO2">
-        <v>2.26</v>
+        <v>2.59</v>
       </c>
       <c r="LP2">
-        <v>1.13</v>
+        <v>1.32</v>
       </c>
       <c r="LQ2">
-        <v>2</v>
+        <v>2.41</v>
       </c>
       <c r="LR2">
-        <v>47.3</v>
+        <v>29.4</v>
       </c>
       <c r="LS2">
-        <v>38.9</v>
+        <v>26.8</v>
       </c>
       <c r="LT2">
-        <v>1.24</v>
+        <v>1.34</v>
       </c>
       <c r="LU2">
-        <v>1.02</v>
+        <v>1.22</v>
       </c>
       <c r="LV2">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="LW2">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="LX2">
-        <v>3420</v>
+        <v>1980</v>
       </c>
       <c r="LY2">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="LZ2">
-        <v>1.61</v>
+        <v>1.18</v>
       </c>
       <c r="MA2">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="MB2">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="MC2">
-        <v>70.09999999999999</v>
+        <v>78.2</v>
       </c>
       <c r="MD2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="ME2">
+        <v>6</v>
+      </c>
+      <c r="MF2">
+        <v>6</v>
+      </c>
+      <c r="MG2">
+        <v>7</v>
+      </c>
+      <c r="MH2">
+        <v>31.8</v>
+      </c>
+      <c r="MI2">
         <v>5</v>
       </c>
-      <c r="MF2">
-        <v>21</v>
-      </c>
-      <c r="MG2">
-        <v>6</v>
-      </c>
-      <c r="MH2">
-        <v>15.8</v>
-      </c>
-      <c r="MI2">
-        <v>10</v>
-      </c>
       <c r="MJ2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="MK2">
+        <v>1</v>
+      </c>
+      <c r="ML2">
+        <v>0</v>
+      </c>
+      <c r="MM2">
+        <v>22</v>
+      </c>
+      <c r="MN2">
+        <v>0</v>
+      </c>
+      <c r="MO2">
         <v>3</v>
       </c>
-      <c r="ML2">
+      <c r="MP2">
         <v>1</v>
       </c>
-      <c r="MM2">
-        <v>38</v>
-      </c>
-      <c r="MN2">
-        <v>4</v>
-      </c>
-      <c r="MO2">
-        <v>2</v>
-      </c>
-      <c r="MP2">
-        <v>2</v>
-      </c>
       <c r="MQ2">
-        <v>57.9</v>
+        <v>27.4</v>
       </c>
       <c r="MR2">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="MS2">
-        <v>-1.1</v>
+        <v>2.4</v>
       </c>
       <c r="MT2">
-        <v>-0.03</v>
+        <v>0.11</v>
       </c>
       <c r="MU2">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="MV2">
-        <v>414</v>
+        <v>266</v>
       </c>
       <c r="MW2">
-        <v>39.4</v>
+        <v>41.7</v>
       </c>
       <c r="MX2">
-        <v>945</v>
+        <v>668</v>
       </c>
       <c r="MY2">
-        <v>204</v>
+        <v>118</v>
       </c>
       <c r="MZ2">
-        <v>31.2</v>
+        <v>30.4</v>
       </c>
       <c r="NA2">
-        <v>32.6</v>
+        <v>30.7</v>
       </c>
       <c r="NB2">
-        <v>277</v>
+        <v>147</v>
       </c>
       <c r="NC2">
-        <v>43</v>
+        <v>42.9</v>
       </c>
       <c r="ND2">
         <v>38.1</v>
       </c>
       <c r="NE2">
-        <v>619</v>
+        <v>265</v>
       </c>
       <c r="NF2">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="NG2">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="NH2">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="NI2">
-        <v>0.97</v>
+        <v>0.77</v>
       </c>
       <c r="NJ2">
-        <v>13.6</v>
+        <v>14.9</v>
       </c>
       <c r="NK2">
-        <v>141</v>
+        <v>69</v>
       </c>
       <c r="NL2">
         <v>12</v>
       </c>
       <c r="NM2">
-        <v>36.1</v>
+        <v>26.3</v>
       </c>
       <c r="NN2">
-        <v>3.71</v>
+        <v>3.14</v>
       </c>
       <c r="NO2">
         <v>0.11</v>
       </c>
       <c r="NP2">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
       <c r="NQ2">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="NR2">
-        <v>5.7</v>
+        <v>3.6</v>
       </c>
       <c r="NS2">
-        <v>4.1</v>
+        <v>2.2</v>
       </c>
       <c r="NT2">
-        <v>14738</v>
+        <v>8861</v>
       </c>
       <c r="NU2">
-        <v>18534</v>
+        <v>10937</v>
       </c>
       <c r="NV2">
-        <v>79.5</v>
+        <v>81</v>
       </c>
       <c r="NW2">
-        <v>265774</v>
+        <v>160290</v>
       </c>
       <c r="NX2">
-        <v>93729</v>
+        <v>57754</v>
       </c>
       <c r="NY2">
-        <v>6493</v>
+        <v>3781</v>
       </c>
       <c r="NZ2">
-        <v>7369</v>
+        <v>4229</v>
       </c>
       <c r="OA2">
-        <v>88.09999999999999</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="OB2">
-        <v>6147</v>
+        <v>3872</v>
       </c>
       <c r="OC2">
-        <v>7163</v>
+        <v>4404</v>
       </c>
       <c r="OD2">
-        <v>85.8</v>
+        <v>87.90000000000001</v>
       </c>
       <c r="OE2">
-        <v>1723</v>
+        <v>973</v>
       </c>
       <c r="OF2">
-        <v>2959</v>
+        <v>1694</v>
       </c>
       <c r="OG2">
-        <v>58.2</v>
+        <v>57.4</v>
       </c>
       <c r="OH2">
-        <v>303</v>
+        <v>206</v>
       </c>
       <c r="OI2">
-        <v>1117</v>
+        <v>647</v>
       </c>
       <c r="OJ2">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="OK2">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="OL2">
-        <v>1325</v>
+        <v>836</v>
       </c>
       <c r="OM2">
-        <v>16710</v>
+        <v>9880</v>
       </c>
       <c r="ON2">
-        <v>1781</v>
+        <v>985</v>
       </c>
       <c r="OO2">
-        <v>559</v>
+        <v>228</v>
       </c>
       <c r="OP2">
+        <v>29</v>
+      </c>
+      <c r="OQ2">
+        <v>96</v>
+      </c>
+      <c r="OR2">
+        <v>399</v>
+      </c>
+      <c r="OS2">
+        <v>103</v>
+      </c>
+      <c r="OT2">
+        <v>37</v>
+      </c>
+      <c r="OU2">
+        <v>43</v>
+      </c>
+      <c r="OV2">
+        <v>0</v>
+      </c>
+      <c r="OW2">
+        <v>434</v>
+      </c>
+      <c r="OX2">
+        <v>72</v>
+      </c>
+      <c r="OY2">
+        <v>172</v>
+      </c>
+      <c r="OZ2">
+        <v>473</v>
+      </c>
+      <c r="PA2">
+        <v>21.5</v>
+      </c>
+      <c r="PB2">
+        <v>361</v>
+      </c>
+      <c r="PC2">
+        <v>46</v>
+      </c>
+      <c r="PD2">
+        <v>23</v>
+      </c>
+      <c r="PE2">
+        <v>19</v>
+      </c>
+      <c r="PF2">
+        <v>53</v>
+      </c>
+      <c r="PG2">
+        <v>2.41</v>
+      </c>
+      <c r="PH2">
+        <v>41</v>
+      </c>
+      <c r="PI2">
+        <v>2</v>
+      </c>
+      <c r="PJ2">
+        <v>5</v>
+      </c>
+      <c r="PK2">
+        <v>2</v>
+      </c>
+      <c r="PL2">
+        <v>0</v>
+      </c>
+      <c r="PM2">
+        <v>389</v>
+      </c>
+      <c r="PN2">
+        <v>211</v>
+      </c>
+      <c r="PO2">
+        <v>189</v>
+      </c>
+      <c r="PP2">
+        <v>153</v>
+      </c>
+      <c r="PQ2">
+        <v>47</v>
+      </c>
+      <c r="PR2">
+        <v>249</v>
+      </c>
+      <c r="PS2">
+        <v>77</v>
+      </c>
+      <c r="PT2">
+        <v>172</v>
+      </c>
+      <c r="PU2">
+        <v>189</v>
+      </c>
+      <c r="PV2">
+        <v>343</v>
+      </c>
+      <c r="PW2">
         <v>6</v>
       </c>
-      <c r="OQ2">
-        <v>172</v>
-      </c>
-      <c r="OR2">
-        <v>628</v>
-      </c>
-      <c r="OS2">
-        <v>170</v>
-      </c>
-      <c r="OT2">
-        <v>68</v>
-      </c>
-      <c r="OU2">
-        <v>79</v>
-      </c>
-      <c r="OV2">
-        <v>0</v>
-      </c>
-      <c r="OW2">
-        <v>666</v>
-      </c>
-      <c r="OX2">
-        <v>43</v>
-      </c>
-      <c r="OY2">
-        <v>363</v>
-      </c>
-      <c r="OZ2">
-        <v>706</v>
-      </c>
-      <c r="PA2">
-        <v>18.58</v>
-      </c>
-      <c r="PB2">
-        <v>487</v>
-      </c>
-      <c r="PC2">
-        <v>67</v>
-      </c>
-      <c r="PD2">
-        <v>41</v>
-      </c>
-      <c r="PE2">
-        <v>47</v>
-      </c>
-      <c r="PF2">
-        <v>97</v>
-      </c>
-      <c r="PG2">
-        <v>2.55</v>
-      </c>
-      <c r="PH2">
-        <v>58</v>
-      </c>
-      <c r="PI2">
-        <v>9</v>
-      </c>
-      <c r="PJ2">
-        <v>6</v>
-      </c>
-      <c r="PK2">
-        <v>11</v>
-      </c>
-      <c r="PL2">
-        <v>3</v>
-      </c>
-      <c r="PM2">
-        <v>560</v>
-      </c>
-      <c r="PN2">
-        <v>292</v>
-      </c>
-      <c r="PO2">
-        <v>270</v>
-      </c>
-      <c r="PP2">
-        <v>211</v>
-      </c>
-      <c r="PQ2">
-        <v>79</v>
-      </c>
-      <c r="PR2">
-        <v>420</v>
-      </c>
-      <c r="PS2">
-        <v>124</v>
-      </c>
-      <c r="PT2">
-        <v>296</v>
-      </c>
-      <c r="PU2">
-        <v>453</v>
-      </c>
-      <c r="PV2">
-        <v>781</v>
-      </c>
-      <c r="PW2">
-        <v>13</v>
-      </c>
       <c r="PX2">
-        <v>22633</v>
+        <v>13180</v>
       </c>
       <c r="PY2">
-        <v>2462</v>
+        <v>1463</v>
       </c>
       <c r="PZ2">
-        <v>7359</v>
+        <v>4526</v>
       </c>
       <c r="QA2">
-        <v>10690</v>
+        <v>5725</v>
       </c>
       <c r="QB2">
-        <v>4827</v>
+        <v>3048</v>
       </c>
       <c r="QC2">
-        <v>671</v>
+        <v>491</v>
       </c>
       <c r="QD2">
-        <v>22623</v>
+        <v>13176</v>
       </c>
       <c r="QE2">
-        <v>12738</v>
+        <v>7651</v>
       </c>
       <c r="QF2">
-        <v>715</v>
+        <v>399</v>
       </c>
       <c r="QG2">
-        <v>503</v>
+        <v>261</v>
       </c>
       <c r="QH2">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="QI2">
-        <v>14643</v>
+        <v>8777</v>
       </c>
       <c r="QJ2">
-        <v>585</v>
+        <v>307</v>
       </c>
       <c r="QK2">
-        <v>341</v>
+        <v>180</v>
       </c>
       <c r="QL2">
         <v>1</v>
       </c>
       <c r="QM2">
-        <v>454</v>
+        <v>287</v>
       </c>
       <c r="QN2">
-        <v>480</v>
+        <v>206</v>
       </c>
       <c r="QO2">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="QP2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="QQ2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="QR2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="QS2">
-        <v>2054</v>
+        <v>1131</v>
       </c>
       <c r="QT2">
-        <v>510</v>
+        <v>256</v>
       </c>
       <c r="QU2">
-        <v>539</v>
+        <v>206</v>
       </c>
       <c r="QV2">
+        <v>55.4</v>
+      </c>
+      <c r="QW2" t="s">
+        <v>769</v>
+      </c>
+      <c r="QX2">
+        <v>24</v>
+      </c>
+      <c r="QY2">
         <v>48.6</v>
       </c>
-      <c r="QW2" t="s">
-        <v>768</v>
-      </c>
-      <c r="QX2">
-        <v>30</v>
-      </c>
-      <c r="QY2">
-        <v>54.6</v>
-      </c>
       <c r="QZ2">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="RA2">
-        <v>418</v>
+        <v>242</v>
       </c>
       <c r="RB2">
-        <v>3420</v>
+        <v>1980</v>
       </c>
       <c r="RC2">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="RD2">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="RE2">
         <v>6</v>
       </c>
       <c r="RF2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="RG2">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="RH2">
         <v>3</v>
       </c>
       <c r="RI2">
-        <v>2.37</v>
+        <v>1.82</v>
       </c>
       <c r="RJ2">
-        <v>1.71</v>
+        <v>1.27</v>
       </c>
       <c r="RK2">
-        <v>4.08</v>
+        <v>3.09</v>
       </c>
       <c r="RL2">
-        <v>2.21</v>
+        <v>1.55</v>
       </c>
       <c r="RM2">
-        <v>3.92</v>
+        <v>2.82</v>
       </c>
       <c r="RN2">
-        <v>74.7</v>
+        <v>36</v>
       </c>
       <c r="RO2">
-        <v>69.3</v>
+        <v>29.5</v>
       </c>
       <c r="RP2">
-        <v>1.97</v>
+        <v>1.63</v>
       </c>
       <c r="RQ2">
-        <v>1.82</v>
+        <v>1.34</v>
       </c>
       <c r="RR2">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="RS2">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="RT2">
-        <v>3417</v>
+        <v>1980</v>
       </c>
       <c r="RU2">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="RV2">
-        <v>1.24</v>
+        <v>1.09</v>
       </c>
       <c r="RW2">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="RX2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="RY2">
-        <v>62.5</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="RZ2">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="SA2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="SB2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="SC2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="SD2">
-        <v>28.9</v>
+        <v>36.4</v>
       </c>
       <c r="SE2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="SF2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="SG2">
+        <v>0</v>
+      </c>
+      <c r="SH2">
+        <v>0</v>
+      </c>
+      <c r="SI2">
+        <v>22</v>
+      </c>
+      <c r="SJ2">
+        <v>1</v>
+      </c>
+      <c r="SK2">
         <v>3</v>
-      </c>
-      <c r="SH2">
-        <v>0</v>
-      </c>
-      <c r="SI2">
-        <v>38</v>
-      </c>
-      <c r="SJ2">
-        <v>0</v>
-      </c>
-      <c r="SK2">
-        <v>5</v>
       </c>
       <c r="SL2">
         <v>1</v>
       </c>
       <c r="SM2">
-        <v>42.3</v>
+        <v>20.7</v>
       </c>
       <c r="SN2">
-        <v>0.31</v>
+        <v>0.23</v>
       </c>
       <c r="SO2">
-        <v>-3.7</v>
+        <v>-2.3</v>
       </c>
       <c r="SP2">
         <v>-0.1</v>
       </c>
       <c r="SQ2">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="SR2">
-        <v>323</v>
+        <v>278</v>
       </c>
       <c r="SS2">
-        <v>40.9</v>
+        <v>42.8</v>
       </c>
       <c r="ST2">
-        <v>868</v>
+        <v>578</v>
       </c>
       <c r="SU2">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="SV2">
-        <v>24.8</v>
+        <v>29.9</v>
       </c>
       <c r="SW2">
+        <v>31.4</v>
+      </c>
+      <c r="SX2">
+        <v>162</v>
+      </c>
+      <c r="SY2">
+        <v>64.8</v>
+      </c>
+      <c r="SZ2">
+        <v>48.3</v>
+      </c>
+      <c r="TA2">
+        <v>272</v>
+      </c>
+      <c r="TB2">
+        <v>17</v>
+      </c>
+      <c r="TC2">
+        <v>6.3</v>
+      </c>
+      <c r="TD2">
+        <v>28</v>
+      </c>
+      <c r="TE2">
+        <v>1.27</v>
+      </c>
+      <c r="TF2">
+        <v>17</v>
+      </c>
+      <c r="TG2">
+        <v>97</v>
+      </c>
+      <c r="TH2">
+        <v>8</v>
+      </c>
+      <c r="TI2">
+        <v>33.7</v>
+      </c>
+      <c r="TJ2">
+        <v>4.41</v>
+      </c>
+      <c r="TK2">
+        <v>0.12</v>
+      </c>
+      <c r="TL2">
+        <v>0.35</v>
+      </c>
+      <c r="TM2">
+        <v>0.1</v>
+      </c>
+      <c r="TN2">
+        <v>4</v>
+      </c>
+      <c r="TO2">
+        <v>4.5</v>
+      </c>
+      <c r="TP2">
+        <v>8446</v>
+      </c>
+      <c r="TQ2">
+        <v>10790</v>
+      </c>
+      <c r="TR2">
+        <v>78.3</v>
+      </c>
+      <c r="TS2">
+        <v>147926</v>
+      </c>
+      <c r="TT2">
+        <v>57069</v>
+      </c>
+      <c r="TU2">
+        <v>3951</v>
+      </c>
+      <c r="TV2">
+        <v>4537</v>
+      </c>
+      <c r="TW2">
+        <v>87.09999999999999</v>
+      </c>
+      <c r="TX2">
+        <v>3347</v>
+      </c>
+      <c r="TY2">
+        <v>4007</v>
+      </c>
+      <c r="TZ2">
+        <v>83.5</v>
+      </c>
+      <c r="UA2">
+        <v>893</v>
+      </c>
+      <c r="UB2">
+        <v>1622</v>
+      </c>
+      <c r="UC2">
+        <v>55.1</v>
+      </c>
+      <c r="UD2">
+        <v>243</v>
+      </c>
+      <c r="UE2">
+        <v>631</v>
+      </c>
+      <c r="UF2">
+        <v>227</v>
+      </c>
+      <c r="UG2">
+        <v>47</v>
+      </c>
+      <c r="UH2">
+        <v>932</v>
+      </c>
+      <c r="UI2">
+        <v>9688</v>
+      </c>
+      <c r="UJ2">
+        <v>1072</v>
+      </c>
+      <c r="UK2">
+        <v>252</v>
+      </c>
+      <c r="UL2">
+        <v>25</v>
+      </c>
+      <c r="UM2">
+        <v>100</v>
+      </c>
+      <c r="UN2">
+        <v>344</v>
+      </c>
+      <c r="UO2">
+        <v>97</v>
+      </c>
+      <c r="UP2">
+        <v>40</v>
+      </c>
+      <c r="UQ2">
+        <v>36</v>
+      </c>
+      <c r="UR2">
+        <v>0</v>
+      </c>
+      <c r="US2">
+        <v>482</v>
+      </c>
+      <c r="UT2">
+        <v>30</v>
+      </c>
+      <c r="UU2">
+        <v>181</v>
+      </c>
+      <c r="UV2">
+        <v>535</v>
+      </c>
+      <c r="UW2">
+        <v>24.32</v>
+      </c>
+      <c r="UX2">
+        <v>400</v>
+      </c>
+      <c r="UY2">
+        <v>43</v>
+      </c>
+      <c r="UZ2">
         <v>31</v>
       </c>
-      <c r="SX2">
-        <v>173</v>
-      </c>
-      <c r="SY2">
-        <v>62.4</v>
-      </c>
-      <c r="SZ2">
-        <v>47.7</v>
-      </c>
-      <c r="TA2">
-        <v>377</v>
-      </c>
-      <c r="TB2">
-        <v>14</v>
-      </c>
-      <c r="TC2">
-        <v>3.7</v>
-      </c>
-      <c r="TD2">
-        <v>66</v>
-      </c>
-      <c r="TE2">
-        <v>1.74</v>
-      </c>
-      <c r="TF2">
-        <v>16.9</v>
-      </c>
-      <c r="TG2">
-        <v>221</v>
-      </c>
-      <c r="TH2">
-        <v>28</v>
-      </c>
-      <c r="TI2">
-        <v>36</v>
-      </c>
-      <c r="TJ2">
-        <v>5.82</v>
-      </c>
-      <c r="TK2">
-        <v>0.14</v>
-      </c>
-      <c r="TL2">
-        <v>0.38</v>
-      </c>
-      <c r="TM2">
-        <v>0.12</v>
-      </c>
-      <c r="TN2">
-        <v>15.3</v>
-      </c>
-      <c r="TO2">
-        <v>14.7</v>
-      </c>
-      <c r="TP2">
-        <v>18066</v>
-      </c>
-      <c r="TQ2">
-        <v>22063</v>
-      </c>
-      <c r="TR2">
-        <v>81.90000000000001</v>
-      </c>
-      <c r="TS2">
-        <v>310229</v>
-      </c>
-      <c r="TT2">
-        <v>109918</v>
-      </c>
-      <c r="TU2">
-        <v>8542</v>
-      </c>
-      <c r="TV2">
-        <v>9641</v>
-      </c>
-      <c r="TW2">
-        <v>88.59999999999999</v>
-      </c>
-      <c r="TX2">
-        <v>7388</v>
-      </c>
-      <c r="TY2">
-        <v>8505</v>
-      </c>
-      <c r="TZ2">
-        <v>86.90000000000001</v>
-      </c>
-      <c r="UA2">
-        <v>1686</v>
-      </c>
-      <c r="UB2">
-        <v>2744</v>
-      </c>
-      <c r="UC2">
-        <v>61.4</v>
-      </c>
-      <c r="UD2">
-        <v>487</v>
-      </c>
-      <c r="UE2">
-        <v>1635</v>
-      </c>
-      <c r="UF2">
-        <v>490</v>
-      </c>
-      <c r="UG2">
-        <v>85</v>
-      </c>
-      <c r="UH2">
-        <v>2077</v>
-      </c>
-      <c r="UI2">
-        <v>20351</v>
-      </c>
-      <c r="UJ2">
-        <v>1656</v>
-      </c>
-      <c r="UK2">
-        <v>508</v>
-      </c>
-      <c r="UL2">
-        <v>28</v>
-      </c>
-      <c r="UM2">
-        <v>181</v>
-      </c>
-      <c r="UN2">
-        <v>657</v>
-      </c>
-      <c r="UO2">
-        <v>201</v>
-      </c>
-      <c r="UP2">
-        <v>104</v>
-      </c>
-      <c r="UQ2">
-        <v>82</v>
-      </c>
-      <c r="UR2">
-        <v>0</v>
-      </c>
-      <c r="US2">
-        <v>689</v>
-      </c>
-      <c r="UT2">
-        <v>56</v>
-      </c>
-      <c r="UU2">
-        <v>395</v>
-      </c>
-      <c r="UV2">
-        <v>1115</v>
-      </c>
-      <c r="UW2">
-        <v>29.34</v>
-      </c>
-      <c r="UX2">
-        <v>866</v>
-      </c>
-      <c r="UY2">
-        <v>68</v>
-      </c>
-      <c r="UZ2">
-        <v>61</v>
-      </c>
       <c r="VA2">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="VB2">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="VC2">
-        <v>4.26</v>
+        <v>3.32</v>
       </c>
       <c r="VD2">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="VE2">
+        <v>4</v>
+      </c>
+      <c r="VF2">
+        <v>7</v>
+      </c>
+      <c r="VG2">
+        <v>7</v>
+      </c>
+      <c r="VH2">
+        <v>1</v>
+      </c>
+      <c r="VI2">
+        <v>373</v>
+      </c>
+      <c r="VJ2">
+        <v>210</v>
+      </c>
+      <c r="VK2">
+        <v>171</v>
+      </c>
+      <c r="VL2">
+        <v>158</v>
+      </c>
+      <c r="VM2">
+        <v>44</v>
+      </c>
+      <c r="VN2">
+        <v>252</v>
+      </c>
+      <c r="VO2">
+        <v>55</v>
+      </c>
+      <c r="VP2">
+        <v>197</v>
+      </c>
+      <c r="VQ2">
+        <v>249</v>
+      </c>
+      <c r="VR2">
+        <v>374</v>
+      </c>
+      <c r="VS2">
         <v>8</v>
       </c>
-      <c r="VF2">
-        <v>9</v>
-      </c>
-      <c r="VG2">
-        <v>5</v>
-      </c>
-      <c r="VH2">
-        <v>3</v>
-      </c>
-      <c r="VI2">
-        <v>606</v>
-      </c>
-      <c r="VJ2">
-        <v>343</v>
-      </c>
-      <c r="VK2">
-        <v>252</v>
-      </c>
-      <c r="VL2">
-        <v>256</v>
-      </c>
-      <c r="VM2">
-        <v>98</v>
-      </c>
-      <c r="VN2">
-        <v>421</v>
-      </c>
-      <c r="VO2">
-        <v>92</v>
-      </c>
-      <c r="VP2">
-        <v>329</v>
-      </c>
-      <c r="VQ2">
-        <v>516</v>
-      </c>
-      <c r="VR2">
-        <v>484</v>
-      </c>
-      <c r="VS2">
-        <v>11</v>
-      </c>
       <c r="VT2">
-        <v>26392</v>
+        <v>13308</v>
       </c>
       <c r="VU2">
-        <v>1779</v>
+        <v>1401</v>
       </c>
       <c r="VV2">
-        <v>6640</v>
+        <v>4403</v>
       </c>
       <c r="VW2">
-        <v>12068</v>
+        <v>5595</v>
       </c>
       <c r="VX2">
-        <v>7924</v>
+        <v>3432</v>
       </c>
       <c r="VY2">
-        <v>1147</v>
+        <v>544</v>
       </c>
       <c r="VZ2">
-        <v>26385</v>
+        <v>13300</v>
       </c>
       <c r="WA2">
-        <v>15724</v>
+        <v>7345</v>
       </c>
       <c r="WB2">
-        <v>874</v>
+        <v>385</v>
       </c>
       <c r="WC2">
-        <v>658</v>
+        <v>300</v>
       </c>
       <c r="WD2">
-        <v>256</v>
+        <v>126</v>
       </c>
       <c r="WE2">
-        <v>17945</v>
+        <v>8382</v>
       </c>
       <c r="WF2">
-        <v>680</v>
+        <v>352</v>
       </c>
       <c r="WG2">
-        <v>406</v>
+        <v>226</v>
       </c>
       <c r="WH2">
         <v>1</v>
       </c>
       <c r="WI2">
-        <v>580</v>
+        <v>275</v>
       </c>
       <c r="WJ2">
-        <v>473</v>
+        <v>229</v>
       </c>
       <c r="WK2">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="WL2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="WM2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="WN2">
         <v>1</v>
       </c>
       <c r="WO2">
-        <v>2472</v>
+        <v>1296</v>
       </c>
       <c r="WP2">
-        <v>633</v>
+        <v>328</v>
       </c>
       <c r="WQ2">
-        <v>506</v>
+        <v>273</v>
       </c>
       <c r="WR2">
-        <v>55.6</v>
+        <v>54.6</v>
       </c>
       <c r="WS2">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="WT2">
-        <v>45.1</v>
+        <v>51.4</v>
       </c>
       <c r="WU2">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="WV2">
-        <v>418</v>
+        <v>242</v>
       </c>
       <c r="WW2">
-        <v>3420</v>
+        <v>1980</v>
       </c>
       <c r="WX2">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="WY2">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="WZ2">
+        <v>1</v>
+      </c>
+      <c r="XA2">
+        <v>1</v>
+      </c>
+      <c r="XB2">
+        <v>51</v>
+      </c>
+      <c r="XC2">
+        <v>0</v>
+      </c>
+      <c r="XD2">
+        <v>1.05</v>
+      </c>
+      <c r="XE2">
+        <v>0.77</v>
+      </c>
+      <c r="XF2">
+        <v>1.82</v>
+      </c>
+      <c r="XG2">
+        <v>1</v>
+      </c>
+      <c r="XH2">
+        <v>1.77</v>
+      </c>
+      <c r="XI2">
+        <v>23.4</v>
+      </c>
+      <c r="XJ2">
+        <v>22.6</v>
+      </c>
+      <c r="XK2">
+        <v>1.07</v>
+      </c>
+      <c r="XL2">
+        <v>1.03</v>
+      </c>
+      <c r="XM2">
+        <v>22</v>
+      </c>
+      <c r="XN2">
+        <v>22</v>
+      </c>
+      <c r="XO2">
+        <v>1980</v>
+      </c>
+      <c r="XP2">
+        <v>41</v>
+      </c>
+      <c r="XQ2">
+        <v>1.86</v>
+      </c>
+      <c r="XR2">
+        <v>105</v>
+      </c>
+      <c r="XS2">
+        <v>63</v>
+      </c>
+      <c r="XT2">
+        <v>66.7</v>
+      </c>
+      <c r="XU2">
         <v>5</v>
       </c>
-      <c r="XA2">
+      <c r="XV2">
+        <v>5</v>
+      </c>
+      <c r="XW2">
+        <v>12</v>
+      </c>
+      <c r="XX2">
+        <v>2</v>
+      </c>
+      <c r="XY2">
+        <v>9.1</v>
+      </c>
+      <c r="XZ2">
         <v>8</v>
-      </c>
-      <c r="XB2">
-        <v>87</v>
-      </c>
-      <c r="XC2">
-        <v>4</v>
-      </c>
-      <c r="XD2">
-        <v>1.21</v>
-      </c>
-      <c r="XE2">
-        <v>0.95</v>
-      </c>
-      <c r="XF2">
-        <v>2.16</v>
-      </c>
-      <c r="XG2">
-        <v>1.08</v>
-      </c>
-      <c r="XH2">
-        <v>2.03</v>
-      </c>
-      <c r="XI2">
-        <v>41</v>
-      </c>
-      <c r="XJ2">
-        <v>34.7</v>
-      </c>
-      <c r="XK2">
-        <v>1.08</v>
-      </c>
-      <c r="XL2">
-        <v>0.91</v>
-      </c>
-      <c r="XM2">
-        <v>38</v>
-      </c>
-      <c r="XN2">
-        <v>38</v>
-      </c>
-      <c r="XO2">
-        <v>3420</v>
-      </c>
-      <c r="XP2">
-        <v>90</v>
-      </c>
-      <c r="XQ2">
-        <v>2.37</v>
-      </c>
-      <c r="XR2">
-        <v>228</v>
-      </c>
-      <c r="XS2">
-        <v>137</v>
-      </c>
-      <c r="XT2">
-        <v>63.2</v>
-      </c>
-      <c r="XU2">
-        <v>6</v>
-      </c>
-      <c r="XV2">
-        <v>9</v>
-      </c>
-      <c r="XW2">
-        <v>23</v>
-      </c>
-      <c r="XX2">
-        <v>5</v>
-      </c>
-      <c r="XY2">
-        <v>13.2</v>
-      </c>
-      <c r="XZ2">
-        <v>7</v>
       </c>
       <c r="YA2">
         <v>6</v>
       </c>
       <c r="YB2">
+        <v>2</v>
+      </c>
+      <c r="YC2">
+        <v>0</v>
+      </c>
+      <c r="YD2">
+        <v>22</v>
+      </c>
+      <c r="YE2">
+        <v>0</v>
+      </c>
+      <c r="YF2">
+        <v>2</v>
+      </c>
+      <c r="YG2">
         <v>1</v>
       </c>
-      <c r="YC2">
-        <v>0</v>
-      </c>
-      <c r="YD2">
+      <c r="YH2">
+        <v>37.4</v>
+      </c>
+      <c r="YI2">
+        <v>0.28</v>
+      </c>
+      <c r="YJ2">
+        <v>-2.6</v>
+      </c>
+      <c r="YK2">
+        <v>-0.12</v>
+      </c>
+      <c r="YL2">
+        <v>111</v>
+      </c>
+      <c r="YM2">
+        <v>332</v>
+      </c>
+      <c r="YN2">
+        <v>33.4</v>
+      </c>
+      <c r="YO2">
+        <v>775</v>
+      </c>
+      <c r="YP2">
+        <v>105</v>
+      </c>
+      <c r="YQ2">
+        <v>35.2</v>
+      </c>
+      <c r="YR2">
+        <v>34.5</v>
+      </c>
+      <c r="YS2">
+        <v>149</v>
+      </c>
+      <c r="YT2">
+        <v>39.6</v>
+      </c>
+      <c r="YU2">
         <v>38</v>
       </c>
-      <c r="YE2">
+      <c r="YV2">
+        <v>269</v>
+      </c>
+      <c r="YW2">
+        <v>13</v>
+      </c>
+      <c r="YX2">
+        <v>4.8</v>
+      </c>
+      <c r="YY2">
+        <v>34</v>
+      </c>
+      <c r="YZ2">
+        <v>1.55</v>
+      </c>
+      <c r="ZA2">
+        <v>15.9</v>
+      </c>
+      <c r="ZB2">
+        <v>86</v>
+      </c>
+      <c r="ZC2">
+        <v>9</v>
+      </c>
+      <c r="ZD2">
+        <v>31.5</v>
+      </c>
+      <c r="ZE2">
+        <v>3.91</v>
+      </c>
+      <c r="ZF2">
+        <v>0.08</v>
+      </c>
+      <c r="ZG2">
+        <v>0.26</v>
+      </c>
+      <c r="ZH2">
+        <v>0.08</v>
+      </c>
+      <c r="ZI2">
+        <v>-0.4</v>
+      </c>
+      <c r="ZJ2">
+        <v>-0.6</v>
+      </c>
+      <c r="ZK2">
+        <v>8987</v>
+      </c>
+      <c r="ZL2">
+        <v>11411</v>
+      </c>
+      <c r="ZM2">
+        <v>78.8</v>
+      </c>
+      <c r="ZN2">
+        <v>158900</v>
+      </c>
+      <c r="ZO2">
+        <v>58611</v>
+      </c>
+      <c r="ZP2">
+        <v>3979</v>
+      </c>
+      <c r="ZQ2">
+        <v>4515</v>
+      </c>
+      <c r="ZR2">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="ZS2">
+        <v>3706</v>
+      </c>
+      <c r="ZT2">
+        <v>4382</v>
+      </c>
+      <c r="ZU2">
+        <v>84.59999999999999</v>
+      </c>
+      <c r="ZV2">
+        <v>991</v>
+      </c>
+      <c r="ZW2">
+        <v>1788</v>
+      </c>
+      <c r="ZX2">
+        <v>55.4</v>
+      </c>
+      <c r="ZY2">
+        <v>204</v>
+      </c>
+      <c r="ZZ2">
+        <v>648</v>
+      </c>
+      <c r="AAA2">
+        <v>166</v>
+      </c>
+      <c r="AAB2">
+        <v>42</v>
+      </c>
+      <c r="AAC2">
+        <v>786</v>
+      </c>
+      <c r="AAD2">
+        <v>10248</v>
+      </c>
+      <c r="AAE2">
+        <v>1137</v>
+      </c>
+      <c r="AAF2">
+        <v>295</v>
+      </c>
+      <c r="AAG2">
+        <v>17</v>
+      </c>
+      <c r="AAH2">
+        <v>67</v>
+      </c>
+      <c r="AAI2">
+        <v>351</v>
+      </c>
+      <c r="AAJ2">
+        <v>94</v>
+      </c>
+      <c r="AAK2">
+        <v>22</v>
+      </c>
+      <c r="AAL2">
+        <v>42</v>
+      </c>
+      <c r="AAM2">
+        <v>0</v>
+      </c>
+      <c r="AAN2">
+        <v>506</v>
+      </c>
+      <c r="AAO2">
+        <v>26</v>
+      </c>
+      <c r="AAP2">
+        <v>212</v>
+      </c>
+      <c r="AAQ2">
+        <v>479</v>
+      </c>
+      <c r="AAR2">
+        <v>21.77</v>
+      </c>
+      <c r="AAS2">
+        <v>371</v>
+      </c>
+      <c r="AAT2">
+        <v>37</v>
+      </c>
+      <c r="AAU2">
+        <v>22</v>
+      </c>
+      <c r="AAV2">
+        <v>23</v>
+      </c>
+      <c r="AAW2">
+        <v>42</v>
+      </c>
+      <c r="AAX2">
+        <v>1.91</v>
+      </c>
+      <c r="AAY2">
+        <v>32</v>
+      </c>
+      <c r="AAZ2">
+        <v>2</v>
+      </c>
+      <c r="ABA2">
+        <v>2</v>
+      </c>
+      <c r="ABB2">
+        <v>3</v>
+      </c>
+      <c r="ABC2">
+        <v>0</v>
+      </c>
+      <c r="ABD2">
+        <v>403</v>
+      </c>
+      <c r="ABE2">
+        <v>243</v>
+      </c>
+      <c r="ABF2">
+        <v>220</v>
+      </c>
+      <c r="ABG2">
+        <v>136</v>
+      </c>
+      <c r="ABH2">
+        <v>47</v>
+      </c>
+      <c r="ABI2">
+        <v>247</v>
+      </c>
+      <c r="ABJ2">
+        <v>83</v>
+      </c>
+      <c r="ABK2">
+        <v>164</v>
+      </c>
+      <c r="ABL2">
+        <v>211</v>
+      </c>
+      <c r="ABM2">
+        <v>361</v>
+      </c>
+      <c r="ABN2">
+        <v>4</v>
+      </c>
+      <c r="ABO2">
+        <v>13928</v>
+      </c>
+      <c r="ABP2">
+        <v>1487</v>
+      </c>
+      <c r="ABQ2">
+        <v>4726</v>
+      </c>
+      <c r="ABR2">
+        <v>6271</v>
+      </c>
+      <c r="ABS2">
+        <v>3076</v>
+      </c>
+      <c r="ABT2">
+        <v>428</v>
+      </c>
+      <c r="ABU2">
+        <v>13927</v>
+      </c>
+      <c r="ABV2">
+        <v>7906</v>
+      </c>
+      <c r="ABW2">
+        <v>362</v>
+      </c>
+      <c r="ABX2">
+        <v>281</v>
+      </c>
+      <c r="ABY2">
+        <v>84</v>
+      </c>
+      <c r="ABZ2">
+        <v>8868</v>
+      </c>
+      <c r="ACA2">
+        <v>375</v>
+      </c>
+      <c r="ACB2">
+        <v>186</v>
+      </c>
+      <c r="ACC2">
+        <v>0</v>
+      </c>
+      <c r="ACD2">
+        <v>244</v>
+      </c>
+      <c r="ACE2">
+        <v>256</v>
+      </c>
+      <c r="ACF2">
+        <v>26</v>
+      </c>
+      <c r="ACG2">
         <v>1</v>
       </c>
-      <c r="YF2">
-        <v>6</v>
-      </c>
-      <c r="YG2">
-        <v>0</v>
-      </c>
-      <c r="YH2">
-        <v>76.8</v>
-      </c>
-      <c r="YI2">
-        <v>0.31</v>
-      </c>
-      <c r="YJ2">
-        <v>-13.2</v>
-      </c>
-      <c r="YK2">
-        <v>-0.35</v>
-      </c>
-      <c r="YL2">
-        <v>240</v>
-      </c>
-      <c r="YM2">
-        <v>673</v>
-      </c>
-      <c r="YN2">
-        <v>35.7</v>
-      </c>
-      <c r="YO2">
-        <v>1395</v>
-      </c>
-      <c r="YP2">
-        <v>170</v>
-      </c>
-      <c r="YQ2">
-        <v>37.8</v>
-      </c>
-      <c r="YR2">
-        <v>33.6</v>
-      </c>
-      <c r="YS2">
-        <v>312</v>
-      </c>
-      <c r="YT2">
-        <v>46.5</v>
-      </c>
-      <c r="YU2">
-        <v>36.8</v>
-      </c>
-      <c r="YV2">
-        <v>497</v>
-      </c>
-      <c r="YW2">
-        <v>10</v>
-      </c>
-      <c r="YX2">
-        <v>2</v>
-      </c>
-      <c r="YY2">
-        <v>35</v>
-      </c>
-      <c r="YZ2">
-        <v>0.92</v>
-      </c>
-      <c r="ZA2">
-        <v>14.4</v>
-      </c>
-      <c r="ZB2">
-        <v>104</v>
-      </c>
-      <c r="ZC2">
-        <v>14</v>
-      </c>
-      <c r="ZD2">
-        <v>32.8</v>
-      </c>
-      <c r="ZE2">
-        <v>2.74</v>
-      </c>
-      <c r="ZF2">
-        <v>0.13</v>
-      </c>
-      <c r="ZG2">
-        <v>0.39</v>
-      </c>
-      <c r="ZH2">
-        <v>0.11</v>
-      </c>
-      <c r="ZI2">
-        <v>5</v>
-      </c>
-      <c r="ZJ2">
-        <v>6.3</v>
-      </c>
-      <c r="ZK2">
-        <v>14274</v>
-      </c>
-      <c r="ZL2">
-        <v>18377</v>
-      </c>
-      <c r="ZM2">
-        <v>77.7</v>
-      </c>
-      <c r="ZN2">
-        <v>251869</v>
-      </c>
-      <c r="ZO2">
-        <v>98214</v>
-      </c>
-      <c r="ZP2">
-        <v>6531</v>
-      </c>
-      <c r="ZQ2">
-        <v>7491</v>
-      </c>
-      <c r="ZR2">
-        <v>87.2</v>
-      </c>
-      <c r="ZS2">
-        <v>5707</v>
-      </c>
-      <c r="ZT2">
-        <v>6754</v>
-      </c>
-      <c r="ZU2">
-        <v>84.5</v>
-      </c>
-      <c r="ZV2">
-        <v>1605</v>
-      </c>
-      <c r="ZW2">
-        <v>3053</v>
-      </c>
-      <c r="ZX2">
-        <v>52.6</v>
-      </c>
-      <c r="ZY2">
-        <v>228</v>
-      </c>
-      <c r="ZZ2">
-        <v>885</v>
-      </c>
-      <c r="AAA2">
-        <v>201</v>
-      </c>
-      <c r="AAB2">
-        <v>43</v>
-      </c>
-      <c r="AAC2">
-        <v>1038</v>
-      </c>
-      <c r="AAD2">
-        <v>16502</v>
-      </c>
-      <c r="AAE2">
-        <v>1835</v>
-      </c>
-      <c r="AAF2">
-        <v>609</v>
-      </c>
-      <c r="AAG2">
-        <v>18</v>
-      </c>
-      <c r="AAH2">
-        <v>89</v>
-      </c>
-      <c r="AAI2">
-        <v>460</v>
-      </c>
-      <c r="AAJ2">
-        <v>120</v>
-      </c>
-      <c r="AAK2">
-        <v>48</v>
-      </c>
-      <c r="AAL2">
-        <v>53</v>
-      </c>
-      <c r="AAM2">
-        <v>0</v>
-      </c>
-      <c r="AAN2">
-        <v>640</v>
-      </c>
-      <c r="AAO2">
-        <v>40</v>
-      </c>
-      <c r="AAP2">
-        <v>351</v>
-      </c>
-      <c r="AAQ2">
-        <v>543</v>
-      </c>
-      <c r="AAR2">
-        <v>14.29</v>
-      </c>
-      <c r="AAS2">
-        <v>365</v>
-      </c>
-      <c r="AAT2">
-        <v>44</v>
-      </c>
-      <c r="AAU2">
-        <v>39</v>
-      </c>
-      <c r="AAV2">
-        <v>43</v>
-      </c>
-      <c r="AAW2">
-        <v>76</v>
-      </c>
-      <c r="AAX2">
-        <v>2</v>
-      </c>
-      <c r="AAY2">
-        <v>52</v>
-      </c>
-      <c r="AAZ2">
-        <v>4</v>
-      </c>
-      <c r="ABA2">
-        <v>6</v>
-      </c>
-      <c r="ABB2">
-        <v>5</v>
-      </c>
-      <c r="ABC2">
-        <v>0</v>
-      </c>
-      <c r="ABD2">
-        <v>716</v>
-      </c>
-      <c r="ABE2">
-        <v>407</v>
-      </c>
-      <c r="ABF2">
-        <v>418</v>
-      </c>
-      <c r="ABG2">
-        <v>243</v>
-      </c>
-      <c r="ABH2">
-        <v>55</v>
-      </c>
-      <c r="ABI2">
-        <v>494</v>
-      </c>
-      <c r="ABJ2">
-        <v>151</v>
-      </c>
-      <c r="ABK2">
-        <v>343</v>
-      </c>
-      <c r="ABL2">
-        <v>528</v>
-      </c>
-      <c r="ABM2">
-        <v>717</v>
-      </c>
-      <c r="ABN2">
-        <v>15</v>
-      </c>
-      <c r="ABO2">
-        <v>22821</v>
-      </c>
-      <c r="ABP2">
-        <v>3113</v>
-      </c>
-      <c r="ABQ2">
-        <v>9294</v>
-      </c>
-      <c r="ABR2">
-        <v>9985</v>
-      </c>
-      <c r="ABS2">
-        <v>3778</v>
-      </c>
-      <c r="ABT2">
-        <v>515</v>
-      </c>
-      <c r="ABU2">
-        <v>22813</v>
-      </c>
-      <c r="ABV2">
-        <v>12053</v>
-      </c>
-      <c r="ABW2">
-        <v>549</v>
-      </c>
-      <c r="ABX2">
-        <v>387</v>
-      </c>
-      <c r="ABY2">
-        <v>109</v>
-      </c>
-      <c r="ABZ2">
-        <v>14104</v>
-      </c>
-      <c r="ACA2">
-        <v>646</v>
-      </c>
-      <c r="ACB2">
-        <v>341</v>
-      </c>
-      <c r="ACC2">
-        <v>3</v>
-      </c>
-      <c r="ACD2">
-        <v>504</v>
-      </c>
-      <c r="ACE2">
-        <v>548</v>
-      </c>
-      <c r="ACF2">
-        <v>40</v>
-      </c>
-      <c r="ACG2">
-        <v>5</v>
-      </c>
       <c r="ACH2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="ACI2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ACJ2">
-        <v>2251</v>
+        <v>1335</v>
       </c>
       <c r="ACK2">
-        <v>506</v>
+        <v>273</v>
       </c>
       <c r="ACL2">
-        <v>633</v>
+        <v>328</v>
       </c>
       <c r="ACM2">
-        <v>44.4</v>
+        <v>45.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code updated for Serie A 2023/2024
- Reorganization of data folders
- Code adapted for the new Serie A season, also considering only a small number of league games has been played
- Stats from other leagues are considered for players at their first Serie A season (rookies), for now without any adaptation based on league difficulty
- Minor fixes
</commit_message>
<xml_diff>
--- a/tmp/playermatchdata.xlsx
+++ b/tmp/playermatchdata.xlsx
@@ -2311,16 +2311,16 @@
     <t>opp_vs_team_aerials_won_pct</t>
   </si>
   <si>
-    <t>Frattesi</t>
+    <t>Barella</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>Sassuolo</t>
-  </si>
-  <si>
-    <t>23-185</t>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>26-214</t>
   </si>
   <si>
     <t>Atalanta</t>
@@ -4992,10 +4992,10 @@
         <v>765</v>
       </c>
       <c r="B2">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C2">
-        <v>2848</v>
+        <v>1870</v>
       </c>
       <c r="D2" t="s">
         <v>766</v>
@@ -5007,319 +5007,319 @@
         <v>765</v>
       </c>
       <c r="H2">
-        <v>202</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>768</v>
       </c>
       <c r="J2">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="K2">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="L2">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="M2">
-        <v>2454</v>
+        <v>218</v>
       </c>
       <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0.1</v>
+      </c>
+      <c r="Z2">
+        <v>0.1</v>
+      </c>
+      <c r="AA2">
+        <v>0.06</v>
+      </c>
+      <c r="AB2">
+        <v>0.06</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>25</v>
+      </c>
+      <c r="AG2">
+        <v>0.41</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0.03</v>
+      </c>
+      <c r="AK2">
+        <v>-0.1</v>
+      </c>
+      <c r="AL2">
+        <v>-0.1</v>
+      </c>
+      <c r="AM2">
+        <v>142</v>
+      </c>
+      <c r="AN2">
+        <v>165</v>
+      </c>
+      <c r="AO2">
+        <v>86.09999999999999</v>
+      </c>
+      <c r="AP2">
+        <v>2515</v>
+      </c>
+      <c r="AQ2">
+        <v>872</v>
+      </c>
+      <c r="AR2">
+        <v>68</v>
+      </c>
+      <c r="AS2">
+        <v>75</v>
+      </c>
+      <c r="AT2">
+        <v>90.7</v>
+      </c>
+      <c r="AU2">
+        <v>52</v>
+      </c>
+      <c r="AV2">
+        <v>60</v>
+      </c>
+      <c r="AW2">
+        <v>86.7</v>
+      </c>
+      <c r="AX2">
+        <v>16</v>
+      </c>
+      <c r="AY2">
+        <v>24</v>
+      </c>
+      <c r="AZ2">
+        <v>66.7</v>
+      </c>
+      <c r="BA2">
+        <v>5</v>
+      </c>
+      <c r="BB2">
+        <v>24</v>
+      </c>
+      <c r="BC2">
+        <v>11</v>
+      </c>
+      <c r="BD2">
+        <v>2</v>
+      </c>
+      <c r="BE2">
+        <v>32</v>
+      </c>
+      <c r="BF2">
+        <v>160</v>
+      </c>
+      <c r="BG2">
+        <v>5</v>
+      </c>
+      <c r="BH2">
+        <v>3</v>
+      </c>
+      <c r="BI2">
+        <v>2</v>
+      </c>
+      <c r="BJ2">
+        <v>5</v>
+      </c>
+      <c r="BK2">
+        <v>3</v>
+      </c>
+      <c r="BL2">
+        <v>1</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>1</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>1</v>
+      </c>
+      <c r="BS2">
+        <v>11</v>
+      </c>
+      <c r="BT2">
+        <v>4.54</v>
+      </c>
+      <c r="BU2">
+        <v>11</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>1</v>
+      </c>
+      <c r="BZ2">
+        <v>0.41</v>
+      </c>
+      <c r="CA2">
+        <v>1</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+      <c r="CE2">
+        <v>0</v>
+      </c>
+      <c r="CF2">
         <v>6</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
+      <c r="CG2">
+        <v>2</v>
+      </c>
+      <c r="CH2">
+        <v>2</v>
+      </c>
+      <c r="CI2">
         <v>4</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0.22</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0.22</v>
-      </c>
-      <c r="W2">
-        <v>0.22</v>
-      </c>
-      <c r="X2">
-        <v>0.22</v>
-      </c>
-      <c r="Y2">
-        <v>5.9</v>
-      </c>
-      <c r="Z2">
-        <v>5.9</v>
-      </c>
-      <c r="AA2">
-        <v>0.22</v>
-      </c>
-      <c r="AB2">
-        <v>0.22</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>21</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>39.6</v>
-      </c>
-      <c r="AG2">
-        <v>0.77</v>
-      </c>
-      <c r="AH2">
-        <v>0.11</v>
-      </c>
-      <c r="AI2">
-        <v>0.29</v>
-      </c>
-      <c r="AJ2">
-        <v>0.11</v>
-      </c>
-      <c r="AK2">
-        <v>0.1</v>
-      </c>
-      <c r="AL2">
-        <v>0.1</v>
-      </c>
-      <c r="AM2">
-        <v>680</v>
-      </c>
-      <c r="AN2">
-        <v>877</v>
-      </c>
-      <c r="AO2">
-        <v>77.5</v>
-      </c>
-      <c r="AP2">
-        <v>11542</v>
-      </c>
-      <c r="AQ2">
-        <v>3193</v>
-      </c>
-      <c r="AR2">
-        <v>331</v>
-      </c>
-      <c r="AS2">
-        <v>401</v>
-      </c>
-      <c r="AT2">
-        <v>82.5</v>
-      </c>
-      <c r="AU2">
-        <v>252</v>
-      </c>
-      <c r="AV2">
-        <v>309</v>
-      </c>
-      <c r="AW2">
-        <v>81.59999999999999</v>
-      </c>
-      <c r="AX2">
-        <v>71</v>
-      </c>
-      <c r="AY2">
-        <v>106</v>
-      </c>
-      <c r="AZ2">
-        <v>67</v>
-      </c>
-      <c r="BA2">
-        <v>25</v>
-      </c>
-      <c r="BB2">
-        <v>68</v>
-      </c>
-      <c r="BC2">
-        <v>18</v>
-      </c>
-      <c r="BD2">
+      <c r="CJ2">
+        <v>0</v>
+      </c>
+      <c r="CK2">
         <v>1</v>
       </c>
-      <c r="BE2">
-        <v>114</v>
-      </c>
-      <c r="BF2">
-        <v>853</v>
-      </c>
-      <c r="BG2">
-        <v>23</v>
-      </c>
-      <c r="BH2">
-        <v>17</v>
-      </c>
-      <c r="BI2">
-        <v>4</v>
-      </c>
-      <c r="BJ2">
-        <v>17</v>
-      </c>
-      <c r="BK2">
-        <v>19</v>
-      </c>
-      <c r="BL2">
-        <v>0</v>
-      </c>
-      <c r="BM2">
-        <v>0</v>
-      </c>
-      <c r="BN2">
-        <v>0</v>
-      </c>
-      <c r="BO2">
-        <v>0</v>
-      </c>
-      <c r="BP2">
+      <c r="CL2">
+        <v>0</v>
+      </c>
+      <c r="CM2">
+        <v>1</v>
+      </c>
+      <c r="CN2">
+        <v>0</v>
+      </c>
+      <c r="CO2">
+        <v>0</v>
+      </c>
+      <c r="CP2">
+        <v>0</v>
+      </c>
+      <c r="CQ2">
+        <v>183</v>
+      </c>
+      <c r="CR2">
+        <v>3</v>
+      </c>
+      <c r="CS2">
+        <v>22</v>
+      </c>
+      <c r="CT2">
+        <v>112</v>
+      </c>
+      <c r="CU2">
+        <v>51</v>
+      </c>
+      <c r="CV2">
+        <v>1</v>
+      </c>
+      <c r="CW2">
+        <v>183</v>
+      </c>
+      <c r="CX2">
+        <v>121</v>
+      </c>
+      <c r="CY2">
+        <v>7</v>
+      </c>
+      <c r="CZ2">
         <v>6</v>
       </c>
-      <c r="BQ2">
+      <c r="DA2">
+        <v>0</v>
+      </c>
+      <c r="DB2">
+        <v>149</v>
+      </c>
+      <c r="DC2">
+        <v>0</v>
+      </c>
+      <c r="DD2">
+        <v>0</v>
+      </c>
+      <c r="DE2">
+        <v>0</v>
+      </c>
+      <c r="DF2">
         <v>1</v>
       </c>
-      <c r="BR2">
-        <v>25</v>
-      </c>
-      <c r="BS2">
-        <v>72</v>
-      </c>
-      <c r="BT2">
-        <v>2.64</v>
-      </c>
-      <c r="BU2">
-        <v>55</v>
-      </c>
-      <c r="BV2">
-        <v>0</v>
-      </c>
-      <c r="BW2">
-        <v>5</v>
-      </c>
-      <c r="BX2">
-        <v>5</v>
-      </c>
-      <c r="BY2">
-        <v>4</v>
-      </c>
-      <c r="BZ2">
-        <v>0.15</v>
-      </c>
-      <c r="CA2">
-        <v>4</v>
-      </c>
-      <c r="CB2">
-        <v>0</v>
-      </c>
-      <c r="CC2">
-        <v>0</v>
-      </c>
-      <c r="CD2">
-        <v>0</v>
-      </c>
-      <c r="CE2">
-        <v>0</v>
-      </c>
-      <c r="CF2">
-        <v>53</v>
-      </c>
-      <c r="CG2">
-        <v>29</v>
-      </c>
-      <c r="CH2">
-        <v>19</v>
-      </c>
-      <c r="CI2">
-        <v>27</v>
-      </c>
-      <c r="CJ2">
-        <v>7</v>
-      </c>
-      <c r="CK2">
-        <v>19</v>
-      </c>
-      <c r="CL2">
+      <c r="DG2">
         <v>3</v>
       </c>
-      <c r="CM2">
-        <v>16</v>
-      </c>
-      <c r="CN2">
-        <v>12</v>
-      </c>
-      <c r="CO2">
-        <v>39</v>
-      </c>
-      <c r="CP2">
-        <v>0</v>
-      </c>
-      <c r="CQ2">
-        <v>1210</v>
-      </c>
-      <c r="CR2">
-        <v>60</v>
-      </c>
-      <c r="CS2">
-        <v>249</v>
-      </c>
-      <c r="CT2">
-        <v>594</v>
-      </c>
-      <c r="CU2">
-        <v>387</v>
-      </c>
-      <c r="CV2">
-        <v>90</v>
-      </c>
-      <c r="CW2">
-        <v>1210</v>
-      </c>
-      <c r="CX2">
-        <v>682</v>
-      </c>
-      <c r="CY2">
-        <v>65</v>
-      </c>
-      <c r="CZ2">
-        <v>49</v>
-      </c>
-      <c r="DA2">
-        <v>19</v>
-      </c>
-      <c r="DB2">
-        <v>839</v>
-      </c>
-      <c r="DC2">
-        <v>48</v>
-      </c>
-      <c r="DD2">
-        <v>35</v>
-      </c>
-      <c r="DE2">
-        <v>0</v>
-      </c>
-      <c r="DF2">
-        <v>36</v>
-      </c>
-      <c r="DG2">
-        <v>48</v>
-      </c>
       <c r="DH2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DI2">
         <v>0</v>
@@ -5331,16 +5331,16 @@
         <v>0</v>
       </c>
       <c r="DL2">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="DM2">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="DN2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="DO2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="DP2">
         <v>0</v>
@@ -5463,1828 +5463,1828 @@
         <v>0</v>
       </c>
       <c r="FD2">
-        <v>6.290322580645161</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="FE2">
-        <v>0.6321263852343686</v>
+        <v>0.2357022603955158</v>
       </c>
       <c r="FF2" t="s">
         <v>767</v>
       </c>
       <c r="FG2">
+        <v>18</v>
+      </c>
+      <c r="FH2">
+        <v>51.3</v>
+      </c>
+      <c r="FI2">
+        <v>3</v>
+      </c>
+      <c r="FJ2">
+        <v>33</v>
+      </c>
+      <c r="FK2">
+        <v>270</v>
+      </c>
+      <c r="FL2">
+        <v>8</v>
+      </c>
+      <c r="FM2">
+        <v>7</v>
+      </c>
+      <c r="FN2">
+        <v>1</v>
+      </c>
+      <c r="FO2">
+        <v>1</v>
+      </c>
+      <c r="FP2">
+        <v>3</v>
+      </c>
+      <c r="FQ2">
+        <v>0</v>
+      </c>
+      <c r="FR2">
+        <v>2.67</v>
+      </c>
+      <c r="FS2">
+        <v>2.33</v>
+      </c>
+      <c r="FT2">
+        <v>5</v>
+      </c>
+      <c r="FU2">
+        <v>2.33</v>
+      </c>
+      <c r="FV2">
+        <v>4.67</v>
+      </c>
+      <c r="FW2">
+        <v>7.3</v>
+      </c>
+      <c r="FX2">
+        <v>6.5</v>
+      </c>
+      <c r="FY2">
+        <v>2.42</v>
+      </c>
+      <c r="FZ2">
+        <v>2.17</v>
+      </c>
+      <c r="GA2">
+        <v>3</v>
+      </c>
+      <c r="GB2">
+        <v>3</v>
+      </c>
+      <c r="GC2">
+        <v>270</v>
+      </c>
+      <c r="GD2">
+        <v>0</v>
+      </c>
+      <c r="GE2">
+        <v>0</v>
+      </c>
+      <c r="GF2">
+        <v>6</v>
+      </c>
+      <c r="GG2">
+        <v>6</v>
+      </c>
+      <c r="GH2">
+        <v>100</v>
+      </c>
+      <c r="GI2">
+        <v>3</v>
+      </c>
+      <c r="GJ2">
+        <v>0</v>
+      </c>
+      <c r="GK2">
+        <v>0</v>
+      </c>
+      <c r="GL2">
+        <v>3</v>
+      </c>
+      <c r="GM2">
+        <v>100</v>
+      </c>
+      <c r="GN2">
+        <v>0</v>
+      </c>
+      <c r="GO2">
+        <v>0</v>
+      </c>
+      <c r="GP2">
+        <v>0</v>
+      </c>
+      <c r="GQ2">
+        <v>0</v>
+      </c>
+      <c r="GR2">
+        <v>3</v>
+      </c>
+      <c r="GS2">
+        <v>0</v>
+      </c>
+      <c r="GT2">
+        <v>0</v>
+      </c>
+      <c r="GU2">
+        <v>0</v>
+      </c>
+      <c r="GV2">
+        <v>1.2</v>
+      </c>
+      <c r="GW2">
+        <v>0.21</v>
+      </c>
+      <c r="GX2">
+        <v>1.2</v>
+      </c>
+      <c r="GY2">
+        <v>0.41</v>
+      </c>
+      <c r="GZ2">
+        <v>19</v>
+      </c>
+      <c r="HA2">
+        <v>32</v>
+      </c>
+      <c r="HB2">
+        <v>59.4</v>
+      </c>
+      <c r="HC2">
+        <v>81</v>
+      </c>
+      <c r="HD2">
+        <v>12</v>
+      </c>
+      <c r="HE2">
+        <v>33.3</v>
+      </c>
+      <c r="HF2">
+        <v>31.4</v>
+      </c>
+      <c r="HG2">
+        <v>21</v>
+      </c>
+      <c r="HH2">
+        <v>23.8</v>
+      </c>
+      <c r="HI2">
+        <v>31</v>
+      </c>
+      <c r="HJ2">
+        <v>35</v>
+      </c>
+      <c r="HK2">
+        <v>1</v>
+      </c>
+      <c r="HL2">
+        <v>2.9</v>
+      </c>
+      <c r="HM2">
+        <v>0</v>
+      </c>
+      <c r="HN2">
+        <v>0</v>
+      </c>
+      <c r="HO2">
+        <v>6.8</v>
+      </c>
+      <c r="HP2">
+        <v>16</v>
+      </c>
+      <c r="HQ2">
+        <v>2</v>
+      </c>
+      <c r="HR2">
+        <v>27.1</v>
+      </c>
+      <c r="HS2">
+        <v>5.33</v>
+      </c>
+      <c r="HT2">
+        <v>0.12</v>
+      </c>
+      <c r="HU2">
+        <v>0.44</v>
+      </c>
+      <c r="HV2">
+        <v>0.11</v>
+      </c>
+      <c r="HW2">
+        <v>0.7</v>
+      </c>
+      <c r="HX2">
+        <v>0.5</v>
+      </c>
+      <c r="HY2">
+        <v>1367</v>
+      </c>
+      <c r="HZ2">
+        <v>1610</v>
+      </c>
+      <c r="IA2">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="IB2">
+        <v>24158</v>
+      </c>
+      <c r="IC2">
+        <v>8292</v>
+      </c>
+      <c r="ID2">
+        <v>613</v>
+      </c>
+      <c r="IE2">
+        <v>670</v>
+      </c>
+      <c r="IF2">
+        <v>91.5</v>
+      </c>
+      <c r="IG2">
+        <v>551</v>
+      </c>
+      <c r="IH2">
+        <v>619</v>
+      </c>
+      <c r="II2">
+        <v>89</v>
+      </c>
+      <c r="IJ2">
+        <v>146</v>
+      </c>
+      <c r="IK2">
+        <v>229</v>
+      </c>
+      <c r="IL2">
+        <v>63.8</v>
+      </c>
+      <c r="IM2">
+        <v>44</v>
+      </c>
+      <c r="IN2">
+        <v>109</v>
+      </c>
+      <c r="IO2">
+        <v>38</v>
+      </c>
+      <c r="IP2">
+        <v>12</v>
+      </c>
+      <c r="IQ2">
+        <v>146</v>
+      </c>
+      <c r="IR2">
+        <v>1497</v>
+      </c>
+      <c r="IS2">
+        <v>110</v>
+      </c>
+      <c r="IT2">
+        <v>33</v>
+      </c>
+      <c r="IU2">
+        <v>10</v>
+      </c>
+      <c r="IV2">
         <v>29</v>
       </c>
-      <c r="FH2">
-        <v>48.9</v>
-      </c>
-      <c r="FI2">
+      <c r="IW2">
+        <v>58</v>
+      </c>
+      <c r="IX2">
+        <v>16</v>
+      </c>
+      <c r="IY2">
+        <v>2</v>
+      </c>
+      <c r="IZ2">
+        <v>12</v>
+      </c>
+      <c r="JA2">
+        <v>0</v>
+      </c>
+      <c r="JB2">
+        <v>37</v>
+      </c>
+      <c r="JC2">
+        <v>3</v>
+      </c>
+      <c r="JD2">
+        <v>17</v>
+      </c>
+      <c r="JE2">
+        <v>108</v>
+      </c>
+      <c r="JF2">
+        <v>36</v>
+      </c>
+      <c r="JG2">
+        <v>83</v>
+      </c>
+      <c r="JH2">
+        <v>9</v>
+      </c>
+      <c r="JI2">
+        <v>7</v>
+      </c>
+      <c r="JJ2">
+        <v>6</v>
+      </c>
+      <c r="JK2">
+        <v>15</v>
+      </c>
+      <c r="JL2">
+        <v>5</v>
+      </c>
+      <c r="JM2">
+        <v>12</v>
+      </c>
+      <c r="JN2">
+        <v>0</v>
+      </c>
+      <c r="JO2">
+        <v>1</v>
+      </c>
+      <c r="JP2">
+        <v>1</v>
+      </c>
+      <c r="JQ2">
+        <v>1</v>
+      </c>
+      <c r="JR2">
+        <v>61</v>
+      </c>
+      <c r="JS2">
+        <v>38</v>
+      </c>
+      <c r="JT2">
+        <v>34</v>
+      </c>
+      <c r="JU2">
+        <v>19</v>
+      </c>
+      <c r="JV2">
+        <v>8</v>
+      </c>
+      <c r="JW2">
+        <v>33</v>
+      </c>
+      <c r="JX2">
+        <v>12</v>
+      </c>
+      <c r="JY2">
+        <v>21</v>
+      </c>
+      <c r="JZ2">
+        <v>20</v>
+      </c>
+      <c r="KA2">
+        <v>46</v>
+      </c>
+      <c r="KB2">
+        <v>0</v>
+      </c>
+      <c r="KC2">
+        <v>1917</v>
+      </c>
+      <c r="KD2">
+        <v>172</v>
+      </c>
+      <c r="KE2">
+        <v>557</v>
+      </c>
+      <c r="KF2">
+        <v>878</v>
+      </c>
+      <c r="KG2">
+        <v>502</v>
+      </c>
+      <c r="KH2">
+        <v>100</v>
+      </c>
+      <c r="KI2">
+        <v>1916</v>
+      </c>
+      <c r="KJ2">
+        <v>1242</v>
+      </c>
+      <c r="KK2">
+        <v>62</v>
+      </c>
+      <c r="KL2">
+        <v>45</v>
+      </c>
+      <c r="KM2">
+        <v>17</v>
+      </c>
+      <c r="KN2">
+        <v>1354</v>
+      </c>
+      <c r="KO2">
+        <v>30</v>
+      </c>
+      <c r="KP2">
+        <v>13</v>
+      </c>
+      <c r="KQ2">
+        <v>0</v>
+      </c>
+      <c r="KR2">
         <v>31</v>
       </c>
-      <c r="FJ2">
-        <v>341</v>
-      </c>
-      <c r="FK2">
-        <v>2790</v>
-      </c>
-      <c r="FL2">
-        <v>37</v>
-      </c>
-      <c r="FM2">
+      <c r="KS2">
+        <v>33</v>
+      </c>
+      <c r="KT2">
+        <v>3</v>
+      </c>
+      <c r="KU2">
+        <v>1</v>
+      </c>
+      <c r="KV2">
+        <v>0</v>
+      </c>
+      <c r="KW2">
+        <v>0</v>
+      </c>
+      <c r="KX2">
+        <v>156</v>
+      </c>
+      <c r="KY2">
+        <v>36</v>
+      </c>
+      <c r="KZ2">
         <v>24</v>
       </c>
-      <c r="FN2">
+      <c r="LA2">
+        <v>60</v>
+      </c>
+      <c r="LB2">
+        <v>18</v>
+      </c>
+      <c r="LC2">
+        <v>48.7</v>
+      </c>
+      <c r="LD2">
+        <v>3</v>
+      </c>
+      <c r="LE2">
+        <v>33</v>
+      </c>
+      <c r="LF2">
+        <v>270</v>
+      </c>
+      <c r="LG2">
+        <v>0</v>
+      </c>
+      <c r="LH2">
+        <v>0</v>
+      </c>
+      <c r="LI2">
+        <v>0</v>
+      </c>
+      <c r="LJ2">
+        <v>0</v>
+      </c>
+      <c r="LK2">
+        <v>3</v>
+      </c>
+      <c r="LL2">
+        <v>0</v>
+      </c>
+      <c r="LM2">
+        <v>0</v>
+      </c>
+      <c r="LN2">
+        <v>0</v>
+      </c>
+      <c r="LO2">
+        <v>0</v>
+      </c>
+      <c r="LP2">
+        <v>0</v>
+      </c>
+      <c r="LQ2">
+        <v>0</v>
+      </c>
+      <c r="LR2">
+        <v>1.8</v>
+      </c>
+      <c r="LS2">
+        <v>1.8</v>
+      </c>
+      <c r="LT2">
+        <v>0.6</v>
+      </c>
+      <c r="LU2">
+        <v>0.6</v>
+      </c>
+      <c r="LV2">
+        <v>3</v>
+      </c>
+      <c r="LW2">
+        <v>3</v>
+      </c>
+      <c r="LX2">
+        <v>270</v>
+      </c>
+      <c r="LY2">
+        <v>8</v>
+      </c>
+      <c r="LZ2">
+        <v>2.67</v>
+      </c>
+      <c r="MA2">
+        <v>17</v>
+      </c>
+      <c r="MB2">
+        <v>9</v>
+      </c>
+      <c r="MC2">
+        <v>58.8</v>
+      </c>
+      <c r="MD2">
+        <v>0</v>
+      </c>
+      <c r="ME2">
+        <v>0</v>
+      </c>
+      <c r="MF2">
+        <v>3</v>
+      </c>
+      <c r="MG2">
+        <v>0</v>
+      </c>
+      <c r="MH2">
+        <v>0</v>
+      </c>
+      <c r="MI2">
+        <v>1</v>
+      </c>
+      <c r="MJ2">
+        <v>1</v>
+      </c>
+      <c r="MK2">
+        <v>0</v>
+      </c>
+      <c r="ML2">
+        <v>0</v>
+      </c>
+      <c r="MM2">
+        <v>3</v>
+      </c>
+      <c r="MN2">
+        <v>0</v>
+      </c>
+      <c r="MO2">
+        <v>0</v>
+      </c>
+      <c r="MP2">
+        <v>0</v>
+      </c>
+      <c r="MQ2">
+        <v>5.3</v>
+      </c>
+      <c r="MR2">
+        <v>0.26</v>
+      </c>
+      <c r="MS2">
+        <v>-2.7</v>
+      </c>
+      <c r="MT2">
+        <v>-0.89</v>
+      </c>
+      <c r="MU2">
+        <v>14</v>
+      </c>
+      <c r="MV2">
+        <v>39</v>
+      </c>
+      <c r="MW2">
+        <v>35.9</v>
+      </c>
+      <c r="MX2">
+        <v>84</v>
+      </c>
+      <c r="MY2">
+        <v>15</v>
+      </c>
+      <c r="MZ2">
+        <v>31</v>
+      </c>
+      <c r="NA2">
+        <v>33.2</v>
+      </c>
+      <c r="NB2">
+        <v>24</v>
+      </c>
+      <c r="NC2">
+        <v>54.2</v>
+      </c>
+      <c r="ND2">
+        <v>46.9</v>
+      </c>
+      <c r="NE2">
+        <v>45</v>
+      </c>
+      <c r="NF2">
+        <v>0</v>
+      </c>
+      <c r="NG2">
+        <v>0</v>
+      </c>
+      <c r="NH2">
+        <v>4</v>
+      </c>
+      <c r="NI2">
+        <v>1.33</v>
+      </c>
+      <c r="NJ2">
+        <v>16.5</v>
+      </c>
+      <c r="NK2">
         <v>6</v>
       </c>
-      <c r="FO2">
+      <c r="NL2">
+        <v>0</v>
+      </c>
+      <c r="NM2">
+        <v>20</v>
+      </c>
+      <c r="NN2">
+        <v>2</v>
+      </c>
+      <c r="NO2">
+        <v>0</v>
+      </c>
+      <c r="NP2">
+        <v>0</v>
+      </c>
+      <c r="NQ2">
+        <v>0.06</v>
+      </c>
+      <c r="NR2">
+        <v>-1.8</v>
+      </c>
+      <c r="NS2">
+        <v>-1.8</v>
+      </c>
+      <c r="NT2">
+        <v>1261</v>
+      </c>
+      <c r="NU2">
+        <v>1502</v>
+      </c>
+      <c r="NV2">
+        <v>84</v>
+      </c>
+      <c r="NW2">
+        <v>24183</v>
+      </c>
+      <c r="NX2">
+        <v>7787</v>
+      </c>
+      <c r="NY2">
+        <v>501</v>
+      </c>
+      <c r="NZ2">
+        <v>558</v>
+      </c>
+      <c r="OA2">
+        <v>89.8</v>
+      </c>
+      <c r="OB2">
+        <v>552</v>
+      </c>
+      <c r="OC2">
+        <v>622</v>
+      </c>
+      <c r="OD2">
+        <v>88.7</v>
+      </c>
+      <c r="OE2">
+        <v>177</v>
+      </c>
+      <c r="OF2">
+        <v>246</v>
+      </c>
+      <c r="OG2">
+        <v>72</v>
+      </c>
+      <c r="OH2">
+        <v>22</v>
+      </c>
+      <c r="OI2">
+        <v>89</v>
+      </c>
+      <c r="OJ2">
+        <v>26</v>
+      </c>
+      <c r="OK2">
+        <v>8</v>
+      </c>
+      <c r="OL2">
+        <v>112</v>
+      </c>
+      <c r="OM2">
+        <v>1362</v>
+      </c>
+      <c r="ON2">
+        <v>137</v>
+      </c>
+      <c r="OO2">
+        <v>34</v>
+      </c>
+      <c r="OP2">
+        <v>1</v>
+      </c>
+      <c r="OQ2">
+        <v>21</v>
+      </c>
+      <c r="OR2">
+        <v>51</v>
+      </c>
+      <c r="OS2">
+        <v>8</v>
+      </c>
+      <c r="OT2">
+        <v>0</v>
+      </c>
+      <c r="OU2">
         <v>7</v>
       </c>
-      <c r="FP2">
-        <v>71</v>
-      </c>
-      <c r="FQ2">
+      <c r="OV2">
+        <v>0</v>
+      </c>
+      <c r="OW2">
+        <v>51</v>
+      </c>
+      <c r="OX2">
+        <v>3</v>
+      </c>
+      <c r="OY2">
+        <v>30</v>
+      </c>
+      <c r="OZ2">
+        <v>52</v>
+      </c>
+      <c r="PA2">
+        <v>17.33</v>
+      </c>
+      <c r="PB2">
+        <v>44</v>
+      </c>
+      <c r="PC2">
+        <v>0</v>
+      </c>
+      <c r="PD2">
+        <v>1</v>
+      </c>
+      <c r="PE2">
         <v>2</v>
       </c>
-      <c r="FR2">
-        <v>1.19</v>
-      </c>
-      <c r="FS2">
-        <v>0.77</v>
-      </c>
-      <c r="FT2">
-        <v>1.97</v>
-      </c>
-      <c r="FU2">
+      <c r="PF2">
+        <v>0</v>
+      </c>
+      <c r="PG2">
+        <v>0</v>
+      </c>
+      <c r="PH2">
+        <v>0</v>
+      </c>
+      <c r="PI2">
+        <v>0</v>
+      </c>
+      <c r="PJ2">
+        <v>0</v>
+      </c>
+      <c r="PK2">
+        <v>0</v>
+      </c>
+      <c r="PL2">
+        <v>0</v>
+      </c>
+      <c r="PM2">
+        <v>28</v>
+      </c>
+      <c r="PN2">
+        <v>17</v>
+      </c>
+      <c r="PO2">
+        <v>18</v>
+      </c>
+      <c r="PP2">
+        <v>7</v>
+      </c>
+      <c r="PQ2">
+        <v>3</v>
+      </c>
+      <c r="PR2">
+        <v>28</v>
+      </c>
+      <c r="PS2">
+        <v>14</v>
+      </c>
+      <c r="PT2">
+        <v>14</v>
+      </c>
+      <c r="PU2">
+        <v>26</v>
+      </c>
+      <c r="PV2">
+        <v>62</v>
+      </c>
+      <c r="PW2">
         <v>1</v>
       </c>
-      <c r="FV2">
-        <v>1.77</v>
-      </c>
-      <c r="FW2">
-        <v>40.7</v>
-      </c>
-      <c r="FX2">
-        <v>35.3</v>
-      </c>
-      <c r="FY2">
-        <v>1.31</v>
-      </c>
-      <c r="FZ2">
-        <v>1.14</v>
-      </c>
-      <c r="GA2">
-        <v>31</v>
-      </c>
-      <c r="GB2">
-        <v>31</v>
-      </c>
-      <c r="GC2">
-        <v>2790</v>
-      </c>
-      <c r="GD2">
+      <c r="PX2">
+        <v>1788</v>
+      </c>
+      <c r="PY2">
+        <v>214</v>
+      </c>
+      <c r="PZ2">
+        <v>593</v>
+      </c>
+      <c r="QA2">
+        <v>813</v>
+      </c>
+      <c r="QB2">
+        <v>395</v>
+      </c>
+      <c r="QC2">
+        <v>54</v>
+      </c>
+      <c r="QD2">
+        <v>1788</v>
+      </c>
+      <c r="QE2">
+        <v>1158</v>
+      </c>
+      <c r="QF2">
+        <v>62</v>
+      </c>
+      <c r="QG2">
         <v>46</v>
       </c>
-      <c r="GE2">
-        <v>1.48</v>
-      </c>
-      <c r="GF2">
-        <v>102</v>
-      </c>
-      <c r="GG2">
-        <v>56</v>
-      </c>
-      <c r="GH2">
-        <v>58.8</v>
-      </c>
-      <c r="GI2">
-        <v>11</v>
-      </c>
-      <c r="GJ2">
-        <v>7</v>
-      </c>
-      <c r="GK2">
-        <v>13</v>
-      </c>
-      <c r="GL2">
-        <v>9</v>
-      </c>
-      <c r="GM2">
-        <v>29</v>
-      </c>
-      <c r="GN2">
-        <v>4</v>
-      </c>
-      <c r="GO2">
-        <v>4</v>
-      </c>
-      <c r="GP2">
-        <v>0</v>
-      </c>
-      <c r="GQ2">
-        <v>0</v>
-      </c>
-      <c r="GR2">
-        <v>31</v>
-      </c>
-      <c r="GS2">
-        <v>0</v>
-      </c>
-      <c r="GT2">
-        <v>5</v>
-      </c>
-      <c r="GU2">
-        <v>0</v>
-      </c>
-      <c r="GV2">
-        <v>34.3</v>
-      </c>
-      <c r="GW2">
-        <v>0.31</v>
-      </c>
-      <c r="GX2">
-        <v>-11.7</v>
-      </c>
-      <c r="GY2">
-        <v>-0.38</v>
-      </c>
-      <c r="GZ2">
-        <v>162</v>
-      </c>
-      <c r="HA2">
-        <v>398</v>
-      </c>
-      <c r="HB2">
-        <v>40.7</v>
-      </c>
-      <c r="HC2">
-        <v>1007</v>
-      </c>
-      <c r="HD2">
-        <v>164</v>
-      </c>
-      <c r="HE2">
-        <v>31</v>
-      </c>
-      <c r="HF2">
-        <v>33.9</v>
-      </c>
-      <c r="HG2">
-        <v>265</v>
-      </c>
-      <c r="HH2">
-        <v>32.5</v>
-      </c>
-      <c r="HI2">
-        <v>33.1</v>
-      </c>
-      <c r="HJ2">
-        <v>437</v>
-      </c>
-      <c r="HK2">
+      <c r="QH2">
+        <v>12</v>
+      </c>
+      <c r="QI2">
+        <v>1249</v>
+      </c>
+      <c r="QJ2">
+        <v>35</v>
+      </c>
+      <c r="QK2">
         <v>26</v>
       </c>
-      <c r="HL2">
-        <v>5.9</v>
-      </c>
-      <c r="HM2">
-        <v>26</v>
-      </c>
-      <c r="HN2">
-        <v>0.84</v>
-      </c>
-      <c r="HO2">
-        <v>13.9</v>
-      </c>
-      <c r="HP2">
-        <v>137</v>
-      </c>
-      <c r="HQ2">
-        <v>19</v>
-      </c>
-      <c r="HR2">
-        <v>34.9</v>
-      </c>
-      <c r="HS2">
-        <v>4.42</v>
-      </c>
-      <c r="HT2">
-        <v>0.08</v>
-      </c>
-      <c r="HU2">
-        <v>0.23</v>
-      </c>
-      <c r="HV2">
-        <v>0.09</v>
-      </c>
-      <c r="HW2">
-        <v>-3.7</v>
-      </c>
-      <c r="HX2">
-        <v>-4.3</v>
-      </c>
-      <c r="HY2">
-        <v>11782</v>
-      </c>
-      <c r="HZ2">
-        <v>14710</v>
-      </c>
-      <c r="IA2">
-        <v>80.09999999999999</v>
-      </c>
-      <c r="IB2">
-        <v>217288</v>
-      </c>
-      <c r="IC2">
-        <v>81006</v>
-      </c>
-      <c r="ID2">
-        <v>5070</v>
-      </c>
-      <c r="IE2">
-        <v>5772</v>
-      </c>
-      <c r="IF2">
-        <v>87.8</v>
-      </c>
-      <c r="IG2">
-        <v>4900</v>
-      </c>
-      <c r="IH2">
-        <v>5686</v>
-      </c>
-      <c r="II2">
-        <v>86.2</v>
-      </c>
-      <c r="IJ2">
-        <v>1523</v>
-      </c>
-      <c r="IK2">
-        <v>2491</v>
-      </c>
-      <c r="IL2">
-        <v>61.1</v>
-      </c>
-      <c r="IM2">
-        <v>308</v>
-      </c>
-      <c r="IN2">
-        <v>885</v>
-      </c>
-      <c r="IO2">
-        <v>256</v>
-      </c>
-      <c r="IP2">
-        <v>69</v>
-      </c>
-      <c r="IQ2">
-        <v>1230</v>
-      </c>
-      <c r="IR2">
-        <v>13008</v>
-      </c>
-      <c r="IS2">
-        <v>1676</v>
-      </c>
-      <c r="IT2">
-        <v>451</v>
-      </c>
-      <c r="IU2">
-        <v>26</v>
-      </c>
-      <c r="IV2">
-        <v>158</v>
-      </c>
-      <c r="IW2">
-        <v>502</v>
-      </c>
-      <c r="IX2">
-        <v>147</v>
-      </c>
-      <c r="IY2">
-        <v>63</v>
-      </c>
-      <c r="IZ2">
-        <v>42</v>
-      </c>
-      <c r="JA2">
-        <v>0</v>
-      </c>
-      <c r="JB2">
-        <v>685</v>
-      </c>
-      <c r="JC2">
-        <v>26</v>
-      </c>
-      <c r="JD2">
-        <v>296</v>
-      </c>
-      <c r="JE2">
-        <v>711</v>
-      </c>
-      <c r="JF2">
-        <v>22.94</v>
-      </c>
-      <c r="JG2">
-        <v>548</v>
-      </c>
-      <c r="JH2">
-        <v>46</v>
-      </c>
-      <c r="JI2">
-        <v>35</v>
-      </c>
-      <c r="JJ2">
+      <c r="QL2">
+        <v>0</v>
+      </c>
+      <c r="QM2">
+        <v>34</v>
+      </c>
+      <c r="QN2">
         <v>30</v>
       </c>
-      <c r="JK2">
-        <v>65</v>
-      </c>
-      <c r="JL2">
-        <v>2.1</v>
-      </c>
-      <c r="JM2">
-        <v>43</v>
-      </c>
-      <c r="JN2">
+      <c r="QO2">
         <v>3</v>
       </c>
-      <c r="JO2">
-        <v>9</v>
-      </c>
-      <c r="JP2">
-        <v>6</v>
-      </c>
-      <c r="JQ2">
-        <v>0</v>
-      </c>
-      <c r="JR2">
-        <v>427</v>
-      </c>
-      <c r="JS2">
-        <v>237</v>
-      </c>
-      <c r="JT2">
-        <v>203</v>
-      </c>
-      <c r="JU2">
-        <v>159</v>
-      </c>
-      <c r="JV2">
-        <v>65</v>
-      </c>
-      <c r="JW2">
-        <v>306</v>
-      </c>
-      <c r="JX2">
-        <v>100</v>
-      </c>
-      <c r="JY2">
-        <v>206</v>
-      </c>
-      <c r="JZ2">
-        <v>235</v>
-      </c>
-      <c r="KA2">
-        <v>575</v>
-      </c>
-      <c r="KB2">
-        <v>13</v>
-      </c>
-      <c r="KC2">
-        <v>17897</v>
-      </c>
-      <c r="KD2">
-        <v>2035</v>
-      </c>
-      <c r="KE2">
-        <v>6181</v>
-      </c>
-      <c r="KF2">
-        <v>7729</v>
-      </c>
-      <c r="KG2">
-        <v>4166</v>
-      </c>
-      <c r="KH2">
-        <v>645</v>
-      </c>
-      <c r="KI2">
-        <v>17890</v>
-      </c>
-      <c r="KJ2">
-        <v>10295</v>
-      </c>
-      <c r="KK2">
-        <v>605</v>
-      </c>
-      <c r="KL2">
-        <v>406</v>
-      </c>
-      <c r="KM2">
-        <v>166</v>
-      </c>
-      <c r="KN2">
-        <v>11666</v>
-      </c>
-      <c r="KO2">
-        <v>446</v>
-      </c>
-      <c r="KP2">
-        <v>310</v>
-      </c>
-      <c r="KQ2">
+      <c r="QP2">
+        <v>0</v>
+      </c>
+      <c r="QQ2">
         <v>1</v>
       </c>
-      <c r="KR2">
-        <v>336</v>
-      </c>
-      <c r="KS2">
-        <v>355</v>
-      </c>
-      <c r="KT2">
-        <v>26</v>
-      </c>
-      <c r="KU2">
-        <v>5</v>
-      </c>
-      <c r="KV2">
-        <v>4</v>
-      </c>
-      <c r="KW2">
-        <v>0</v>
-      </c>
-      <c r="KX2">
-        <v>1456</v>
-      </c>
-      <c r="KY2">
-        <v>329</v>
-      </c>
-      <c r="KZ2">
-        <v>385</v>
-      </c>
-      <c r="LA2">
-        <v>46.1</v>
-      </c>
-      <c r="LB2">
-        <v>29</v>
-      </c>
-      <c r="LC2">
-        <v>51.1</v>
-      </c>
-      <c r="LD2">
-        <v>31</v>
-      </c>
-      <c r="LE2">
-        <v>341</v>
-      </c>
-      <c r="LF2">
-        <v>2790</v>
-      </c>
-      <c r="LG2">
-        <v>46</v>
-      </c>
-      <c r="LH2">
-        <v>35</v>
-      </c>
-      <c r="LI2">
-        <v>4</v>
-      </c>
-      <c r="LJ2">
-        <v>4</v>
-      </c>
-      <c r="LK2">
-        <v>69</v>
-      </c>
-      <c r="LL2">
-        <v>4</v>
-      </c>
-      <c r="LM2">
-        <v>1.48</v>
-      </c>
-      <c r="LN2">
-        <v>1.13</v>
-      </c>
-      <c r="LO2">
-        <v>2.61</v>
-      </c>
-      <c r="LP2">
-        <v>1.35</v>
-      </c>
-      <c r="LQ2">
-        <v>2.48</v>
-      </c>
-      <c r="LR2">
-        <v>40.2</v>
-      </c>
-      <c r="LS2">
-        <v>37.6</v>
-      </c>
-      <c r="LT2">
-        <v>1.3</v>
-      </c>
-      <c r="LU2">
-        <v>1.21</v>
-      </c>
-      <c r="LV2">
-        <v>31</v>
-      </c>
-      <c r="LW2">
-        <v>31</v>
-      </c>
-      <c r="LX2">
-        <v>2790</v>
-      </c>
-      <c r="LY2">
-        <v>38</v>
-      </c>
-      <c r="LZ2">
-        <v>1.23</v>
-      </c>
-      <c r="MA2">
-        <v>144</v>
-      </c>
-      <c r="MB2">
-        <v>106</v>
-      </c>
-      <c r="MC2">
-        <v>77.8</v>
-      </c>
-      <c r="MD2">
-        <v>13</v>
-      </c>
-      <c r="ME2">
-        <v>7</v>
-      </c>
-      <c r="MF2">
-        <v>11</v>
-      </c>
-      <c r="MG2">
-        <v>9</v>
-      </c>
-      <c r="MH2">
-        <v>29</v>
-      </c>
-      <c r="MI2">
-        <v>7</v>
-      </c>
-      <c r="MJ2">
-        <v>6</v>
-      </c>
-      <c r="MK2">
-        <v>1</v>
-      </c>
-      <c r="ML2">
-        <v>0</v>
-      </c>
-      <c r="MM2">
-        <v>31</v>
-      </c>
-      <c r="MN2">
-        <v>1</v>
-      </c>
-      <c r="MO2">
-        <v>5</v>
-      </c>
-      <c r="MP2">
-        <v>1</v>
-      </c>
-      <c r="MQ2">
-        <v>38.9</v>
-      </c>
-      <c r="MR2">
-        <v>0.23</v>
-      </c>
-      <c r="MS2">
-        <v>1.9</v>
-      </c>
-      <c r="MT2">
-        <v>0.06</v>
-      </c>
-      <c r="MU2">
-        <v>164</v>
-      </c>
-      <c r="MV2">
-        <v>411</v>
-      </c>
-      <c r="MW2">
-        <v>39.9</v>
-      </c>
-      <c r="MX2">
-        <v>928</v>
-      </c>
-      <c r="MY2">
-        <v>161</v>
-      </c>
-      <c r="MZ2">
-        <v>33.2</v>
-      </c>
-      <c r="NA2">
-        <v>32.1</v>
-      </c>
-      <c r="NB2">
-        <v>220</v>
-      </c>
-      <c r="NC2">
-        <v>46.8</v>
-      </c>
-      <c r="ND2">
-        <v>39.7</v>
-      </c>
-      <c r="NE2">
-        <v>384</v>
-      </c>
-      <c r="NF2">
-        <v>17</v>
-      </c>
-      <c r="NG2">
-        <v>4.4</v>
-      </c>
-      <c r="NH2">
-        <v>23</v>
-      </c>
-      <c r="NI2">
-        <v>0.74</v>
-      </c>
-      <c r="NJ2">
-        <v>13.9</v>
-      </c>
-      <c r="NK2">
-        <v>98</v>
-      </c>
-      <c r="NL2">
-        <v>13</v>
-      </c>
-      <c r="NM2">
-        <v>25.3</v>
-      </c>
-      <c r="NN2">
-        <v>3.16</v>
-      </c>
-      <c r="NO2">
-        <v>0.11</v>
-      </c>
-      <c r="NP2">
-        <v>0.43</v>
-      </c>
-      <c r="NQ2">
-        <v>0.1</v>
-      </c>
-      <c r="NR2">
-        <v>5.8</v>
-      </c>
-      <c r="NS2">
-        <v>4.4</v>
-      </c>
-      <c r="NT2">
-        <v>12383</v>
-      </c>
-      <c r="NU2">
-        <v>15407</v>
-      </c>
-      <c r="NV2">
-        <v>80.40000000000001</v>
-      </c>
-      <c r="NW2">
-        <v>224055</v>
-      </c>
-      <c r="NX2">
-        <v>80728</v>
-      </c>
-      <c r="NY2">
-        <v>5387</v>
-      </c>
-      <c r="NZ2">
-        <v>6031</v>
-      </c>
-      <c r="OA2">
-        <v>89.3</v>
-      </c>
-      <c r="OB2">
-        <v>5317</v>
-      </c>
-      <c r="OC2">
-        <v>6109</v>
-      </c>
-      <c r="OD2">
-        <v>87</v>
-      </c>
-      <c r="OE2">
-        <v>1358</v>
-      </c>
-      <c r="OF2">
-        <v>2419</v>
-      </c>
-      <c r="OG2">
-        <v>56.1</v>
-      </c>
-      <c r="OH2">
-        <v>304</v>
-      </c>
-      <c r="OI2">
-        <v>885</v>
-      </c>
-      <c r="OJ2">
-        <v>276</v>
-      </c>
-      <c r="OK2">
-        <v>91</v>
-      </c>
-      <c r="OL2">
-        <v>1128</v>
-      </c>
-      <c r="OM2">
-        <v>13870</v>
-      </c>
-      <c r="ON2">
-        <v>1443</v>
-      </c>
-      <c r="OO2">
-        <v>342</v>
-      </c>
-      <c r="OP2">
-        <v>41</v>
-      </c>
-      <c r="OQ2">
-        <v>139</v>
-      </c>
-      <c r="OR2">
-        <v>579</v>
-      </c>
-      <c r="OS2">
-        <v>151</v>
-      </c>
-      <c r="OT2">
-        <v>66</v>
-      </c>
-      <c r="OU2">
-        <v>51</v>
-      </c>
-      <c r="OV2">
-        <v>0</v>
-      </c>
-      <c r="OW2">
-        <v>628</v>
-      </c>
-      <c r="OX2">
-        <v>94</v>
-      </c>
-      <c r="OY2">
-        <v>261</v>
-      </c>
-      <c r="OZ2">
-        <v>684</v>
-      </c>
-      <c r="PA2">
-        <v>22.06</v>
-      </c>
-      <c r="PB2">
-        <v>503</v>
-      </c>
-      <c r="PC2">
-        <v>74</v>
-      </c>
-      <c r="PD2">
-        <v>34</v>
-      </c>
-      <c r="PE2">
-        <v>25</v>
-      </c>
-      <c r="PF2">
-        <v>73</v>
-      </c>
-      <c r="PG2">
-        <v>2.35</v>
-      </c>
-      <c r="PH2">
-        <v>54</v>
-      </c>
-      <c r="PI2">
-        <v>4</v>
-      </c>
-      <c r="PJ2">
-        <v>7</v>
-      </c>
-      <c r="PK2">
-        <v>2</v>
-      </c>
-      <c r="PL2">
-        <v>0</v>
-      </c>
-      <c r="PM2">
-        <v>545</v>
-      </c>
-      <c r="PN2">
-        <v>309</v>
-      </c>
-      <c r="PO2">
-        <v>269</v>
-      </c>
-      <c r="PP2">
-        <v>216</v>
-      </c>
-      <c r="PQ2">
-        <v>60</v>
-      </c>
-      <c r="PR2">
-        <v>355</v>
-      </c>
-      <c r="PS2">
-        <v>100</v>
-      </c>
-      <c r="PT2">
-        <v>255</v>
-      </c>
-      <c r="PU2">
-        <v>251</v>
-      </c>
-      <c r="PV2">
-        <v>514</v>
-      </c>
-      <c r="PW2">
-        <v>9</v>
-      </c>
-      <c r="PX2">
-        <v>18652</v>
-      </c>
-      <c r="PY2">
-        <v>2079</v>
-      </c>
-      <c r="PZ2">
-        <v>6432</v>
-      </c>
-      <c r="QA2">
-        <v>8155</v>
-      </c>
-      <c r="QB2">
-        <v>4232</v>
-      </c>
-      <c r="QC2">
-        <v>690</v>
-      </c>
-      <c r="QD2">
-        <v>18648</v>
-      </c>
-      <c r="QE2">
-        <v>10730</v>
-      </c>
-      <c r="QF2">
-        <v>553</v>
-      </c>
-      <c r="QG2">
-        <v>368</v>
-      </c>
-      <c r="QH2">
-        <v>140</v>
-      </c>
-      <c r="QI2">
-        <v>12266</v>
-      </c>
-      <c r="QJ2">
-        <v>454</v>
-      </c>
-      <c r="QK2">
-        <v>246</v>
-      </c>
-      <c r="QL2">
-        <v>1</v>
-      </c>
-      <c r="QM2">
-        <v>384</v>
-      </c>
-      <c r="QN2">
-        <v>307</v>
-      </c>
-      <c r="QO2">
-        <v>94</v>
-      </c>
-      <c r="QP2">
-        <v>2</v>
-      </c>
-      <c r="QQ2">
-        <v>7</v>
-      </c>
       <c r="QR2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="QS2">
-        <v>1611</v>
+        <v>128</v>
       </c>
       <c r="QT2">
-        <v>385</v>
+        <v>24</v>
       </c>
       <c r="QU2">
-        <v>329</v>
+        <v>36</v>
       </c>
       <c r="QV2">
-        <v>53.9</v>
+        <v>40</v>
       </c>
       <c r="QW2" t="s">
         <v>769</v>
       </c>
       <c r="QX2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="QY2">
-        <v>50</v>
+        <v>51.7</v>
       </c>
       <c r="QZ2">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="RA2">
-        <v>341</v>
+        <v>33</v>
       </c>
       <c r="RB2">
-        <v>2790</v>
+        <v>270</v>
       </c>
       <c r="RC2">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="RD2">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="RE2">
+        <v>0</v>
+      </c>
+      <c r="RF2">
+        <v>0</v>
+      </c>
+      <c r="RG2">
+        <v>2</v>
+      </c>
+      <c r="RH2">
+        <v>0</v>
+      </c>
+      <c r="RI2">
+        <v>2</v>
+      </c>
+      <c r="RJ2">
+        <v>2</v>
+      </c>
+      <c r="RK2">
+        <v>4</v>
+      </c>
+      <c r="RL2">
+        <v>2</v>
+      </c>
+      <c r="RM2">
+        <v>4</v>
+      </c>
+      <c r="RN2">
+        <v>4.2</v>
+      </c>
+      <c r="RO2">
+        <v>4.2</v>
+      </c>
+      <c r="RP2">
+        <v>1.41</v>
+      </c>
+      <c r="RQ2">
+        <v>1.41</v>
+      </c>
+      <c r="RR2">
+        <v>3</v>
+      </c>
+      <c r="RS2">
+        <v>3</v>
+      </c>
+      <c r="RT2">
+        <v>270</v>
+      </c>
+      <c r="RU2">
+        <v>2</v>
+      </c>
+      <c r="RV2">
+        <v>0.67</v>
+      </c>
+      <c r="RW2">
+        <v>10</v>
+      </c>
+      <c r="RX2">
+        <v>8</v>
+      </c>
+      <c r="RY2">
+        <v>80</v>
+      </c>
+      <c r="RZ2">
+        <v>2</v>
+      </c>
+      <c r="SA2">
+        <v>0</v>
+      </c>
+      <c r="SB2">
+        <v>1</v>
+      </c>
+      <c r="SC2">
+        <v>2</v>
+      </c>
+      <c r="SD2">
+        <v>66.7</v>
+      </c>
+      <c r="SE2">
+        <v>0</v>
+      </c>
+      <c r="SF2">
+        <v>0</v>
+      </c>
+      <c r="SG2">
+        <v>0</v>
+      </c>
+      <c r="SH2">
+        <v>0</v>
+      </c>
+      <c r="SI2">
+        <v>3</v>
+      </c>
+      <c r="SJ2">
+        <v>0</v>
+      </c>
+      <c r="SK2">
+        <v>1</v>
+      </c>
+      <c r="SL2">
+        <v>0</v>
+      </c>
+      <c r="SM2">
+        <v>2.1</v>
+      </c>
+      <c r="SN2">
+        <v>0.21</v>
+      </c>
+      <c r="SO2">
+        <v>0.1</v>
+      </c>
+      <c r="SP2">
+        <v>0.04</v>
+      </c>
+      <c r="SQ2">
+        <v>11</v>
+      </c>
+      <c r="SR2">
+        <v>34</v>
+      </c>
+      <c r="SS2">
+        <v>32.4</v>
+      </c>
+      <c r="ST2">
+        <v>88</v>
+      </c>
+      <c r="SU2">
+        <v>18</v>
+      </c>
+      <c r="SV2">
+        <v>27.3</v>
+      </c>
+      <c r="SW2">
+        <v>29.3</v>
+      </c>
+      <c r="SX2">
+        <v>18</v>
+      </c>
+      <c r="SY2">
+        <v>55.6</v>
+      </c>
+      <c r="SZ2">
+        <v>46.1</v>
+      </c>
+      <c r="TA2">
+        <v>28</v>
+      </c>
+      <c r="TB2">
+        <v>2</v>
+      </c>
+      <c r="TC2">
+        <v>7.1</v>
+      </c>
+      <c r="TD2">
+        <v>8</v>
+      </c>
+      <c r="TE2">
+        <v>2.67</v>
+      </c>
+      <c r="TF2">
+        <v>22</v>
+      </c>
+      <c r="TG2">
+        <v>18</v>
+      </c>
+      <c r="TH2">
+        <v>0</v>
+      </c>
+      <c r="TI2">
+        <v>34.6</v>
+      </c>
+      <c r="TJ2">
         <v>6</v>
       </c>
-      <c r="RF2">
-        <v>8</v>
-      </c>
-      <c r="RG2">
-        <v>76</v>
-      </c>
-      <c r="RH2">
-        <v>3</v>
-      </c>
-      <c r="RI2">
-        <v>1.61</v>
-      </c>
-      <c r="RJ2">
-        <v>1.03</v>
-      </c>
-      <c r="RK2">
-        <v>2.65</v>
-      </c>
-      <c r="RL2">
-        <v>1.42</v>
-      </c>
-      <c r="RM2">
-        <v>2.45</v>
-      </c>
-      <c r="RN2">
-        <v>47.6</v>
-      </c>
-      <c r="RO2">
-        <v>41.1</v>
-      </c>
-      <c r="RP2">
-        <v>1.53</v>
-      </c>
-      <c r="RQ2">
-        <v>1.33</v>
-      </c>
-      <c r="RR2">
-        <v>31</v>
-      </c>
-      <c r="RS2">
-        <v>31</v>
-      </c>
-      <c r="RT2">
-        <v>2790</v>
-      </c>
-      <c r="RU2">
-        <v>36</v>
-      </c>
-      <c r="RV2">
-        <v>1.16</v>
-      </c>
-      <c r="RW2">
-        <v>119</v>
-      </c>
-      <c r="RX2">
-        <v>85</v>
-      </c>
-      <c r="RY2">
-        <v>72.3</v>
-      </c>
-      <c r="RZ2">
-        <v>15</v>
-      </c>
-      <c r="SA2">
-        <v>7</v>
-      </c>
-      <c r="SB2">
-        <v>9</v>
-      </c>
-      <c r="SC2">
-        <v>9</v>
-      </c>
-      <c r="SD2">
-        <v>29</v>
-      </c>
-      <c r="SE2">
-        <v>3</v>
-      </c>
-      <c r="SF2">
-        <v>3</v>
-      </c>
-      <c r="SG2">
-        <v>0</v>
-      </c>
-      <c r="SH2">
-        <v>0</v>
-      </c>
-      <c r="SI2">
-        <v>31</v>
-      </c>
-      <c r="SJ2">
-        <v>1</v>
-      </c>
-      <c r="SK2">
-        <v>5</v>
-      </c>
-      <c r="SL2">
-        <v>2</v>
-      </c>
-      <c r="SM2">
-        <v>30.3</v>
-      </c>
-      <c r="SN2">
-        <v>0.23</v>
-      </c>
-      <c r="SO2">
-        <v>-3.7</v>
-      </c>
-      <c r="SP2">
-        <v>-0.12</v>
-      </c>
-      <c r="SQ2">
-        <v>147</v>
-      </c>
-      <c r="SR2">
-        <v>373</v>
-      </c>
-      <c r="SS2">
-        <v>39.4</v>
-      </c>
-      <c r="ST2">
-        <v>744</v>
-      </c>
-      <c r="SU2">
-        <v>203</v>
-      </c>
-      <c r="SV2">
-        <v>29.4</v>
-      </c>
-      <c r="SW2">
-        <v>31.3</v>
-      </c>
-      <c r="SX2">
-        <v>231</v>
-      </c>
-      <c r="SY2">
-        <v>66.7</v>
-      </c>
-      <c r="SZ2">
-        <v>50.1</v>
-      </c>
-      <c r="TA2">
-        <v>373</v>
-      </c>
-      <c r="TB2">
-        <v>27</v>
-      </c>
-      <c r="TC2">
-        <v>7.2</v>
-      </c>
-      <c r="TD2">
-        <v>38</v>
-      </c>
-      <c r="TE2">
-        <v>1.23</v>
-      </c>
-      <c r="TF2">
-        <v>16.1</v>
-      </c>
-      <c r="TG2">
-        <v>135</v>
-      </c>
-      <c r="TH2">
-        <v>12</v>
-      </c>
-      <c r="TI2">
-        <v>33.7</v>
-      </c>
-      <c r="TJ2">
-        <v>4.35</v>
-      </c>
       <c r="TK2">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="TL2">
         <v>0.33</v>
       </c>
       <c r="TM2">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="TN2">
-        <v>2.4</v>
+        <v>1.8</v>
       </c>
       <c r="TO2">
-        <v>2.9</v>
+        <v>1.8</v>
       </c>
       <c r="TP2">
-        <v>12448</v>
+        <v>1395</v>
       </c>
       <c r="TQ2">
-        <v>15837</v>
+        <v>1694</v>
       </c>
       <c r="TR2">
-        <v>78.59999999999999</v>
+        <v>82.3</v>
       </c>
       <c r="TS2">
-        <v>215503</v>
+        <v>24117</v>
       </c>
       <c r="TT2">
-        <v>80416</v>
+        <v>8315</v>
       </c>
       <c r="TU2">
-        <v>5938</v>
+        <v>631</v>
       </c>
       <c r="TV2">
-        <v>6772</v>
+        <v>715</v>
       </c>
       <c r="TW2">
-        <v>87.7</v>
+        <v>88.3</v>
       </c>
       <c r="TX2">
-        <v>4908</v>
+        <v>599</v>
       </c>
       <c r="TY2">
-        <v>5842</v>
+        <v>672</v>
       </c>
       <c r="TZ2">
-        <v>84</v>
+        <v>89.09999999999999</v>
       </c>
       <c r="UA2">
-        <v>1245</v>
+        <v>132</v>
       </c>
       <c r="UB2">
-        <v>2293</v>
+        <v>220</v>
       </c>
       <c r="UC2">
-        <v>54.3</v>
+        <v>60</v>
       </c>
       <c r="UD2">
-        <v>324</v>
+        <v>41</v>
       </c>
       <c r="UE2">
-        <v>947</v>
+        <v>93</v>
       </c>
       <c r="UF2">
-        <v>319</v>
+        <v>36</v>
       </c>
       <c r="UG2">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="UH2">
-        <v>1360</v>
+        <v>164</v>
       </c>
       <c r="UI2">
-        <v>14215</v>
+        <v>1554</v>
       </c>
       <c r="UJ2">
-        <v>1578</v>
+        <v>133</v>
       </c>
       <c r="UK2">
-        <v>355</v>
+        <v>30</v>
       </c>
       <c r="UL2">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="UM2">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="UN2">
-        <v>535</v>
+        <v>81</v>
       </c>
       <c r="UO2">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="UP2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="UQ2">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="UR2">
         <v>0</v>
       </c>
       <c r="US2">
-        <v>741</v>
+        <v>59</v>
       </c>
       <c r="UT2">
+        <v>7</v>
+      </c>
+      <c r="UU2">
+        <v>28</v>
+      </c>
+      <c r="UV2">
+        <v>97</v>
+      </c>
+      <c r="UW2">
+        <v>32.33</v>
+      </c>
+      <c r="UX2">
+        <v>79</v>
+      </c>
+      <c r="UY2">
+        <v>7</v>
+      </c>
+      <c r="UZ2">
+        <v>4</v>
+      </c>
+      <c r="VA2">
+        <v>0</v>
+      </c>
+      <c r="VB2">
+        <v>11</v>
+      </c>
+      <c r="VC2">
+        <v>3.67</v>
+      </c>
+      <c r="VD2">
+        <v>9</v>
+      </c>
+      <c r="VE2">
+        <v>1</v>
+      </c>
+      <c r="VF2">
+        <v>1</v>
+      </c>
+      <c r="VG2">
+        <v>0</v>
+      </c>
+      <c r="VH2">
+        <v>0</v>
+      </c>
+      <c r="VI2">
+        <v>43</v>
+      </c>
+      <c r="VJ2">
+        <v>22</v>
+      </c>
+      <c r="VK2">
+        <v>19</v>
+      </c>
+      <c r="VL2">
+        <v>17</v>
+      </c>
+      <c r="VM2">
+        <v>7</v>
+      </c>
+      <c r="VN2">
+        <v>39</v>
+      </c>
+      <c r="VO2">
+        <v>8</v>
+      </c>
+      <c r="VP2">
+        <v>31</v>
+      </c>
+      <c r="VQ2">
+        <v>27</v>
+      </c>
+      <c r="VR2">
+        <v>35</v>
+      </c>
+      <c r="VS2">
+        <v>0</v>
+      </c>
+      <c r="VT2">
+        <v>1993</v>
+      </c>
+      <c r="VU2">
+        <v>146</v>
+      </c>
+      <c r="VV2">
+        <v>555</v>
+      </c>
+      <c r="VW2">
+        <v>841</v>
+      </c>
+      <c r="VX2">
+        <v>618</v>
+      </c>
+      <c r="VY2">
+        <v>89</v>
+      </c>
+      <c r="VZ2">
+        <v>1993</v>
+      </c>
+      <c r="WA2">
+        <v>1282</v>
+      </c>
+      <c r="WB2">
+        <v>73</v>
+      </c>
+      <c r="WC2">
+        <v>56</v>
+      </c>
+      <c r="WD2">
+        <v>20</v>
+      </c>
+      <c r="WE2">
+        <v>1379</v>
+      </c>
+      <c r="WF2">
+        <v>38</v>
+      </c>
+      <c r="WG2">
+        <v>26</v>
+      </c>
+      <c r="WH2">
+        <v>0</v>
+      </c>
+      <c r="WI2">
+        <v>34</v>
+      </c>
+      <c r="WJ2">
+        <v>27</v>
+      </c>
+      <c r="WK2">
+        <v>7</v>
+      </c>
+      <c r="WL2">
+        <v>0</v>
+      </c>
+      <c r="WM2">
+        <v>0</v>
+      </c>
+      <c r="WN2">
+        <v>0</v>
+      </c>
+      <c r="WO2">
+        <v>172</v>
+      </c>
+      <c r="WP2">
+        <v>42</v>
+      </c>
+      <c r="WQ2">
         <v>44</v>
       </c>
-      <c r="UU2">
-        <v>301</v>
-      </c>
-      <c r="UV2">
-        <v>741</v>
-      </c>
-      <c r="UW2">
-        <v>23.9</v>
-      </c>
-      <c r="UX2">
-        <v>552</v>
-      </c>
-      <c r="UY2">
-        <v>59</v>
-      </c>
-      <c r="UZ2">
-        <v>39</v>
-      </c>
-      <c r="VA2">
-        <v>29</v>
-      </c>
-      <c r="VB2">
-        <v>90</v>
-      </c>
-      <c r="VC2">
-        <v>2.9</v>
-      </c>
-      <c r="VD2">
-        <v>68</v>
-      </c>
-      <c r="VE2">
+      <c r="WR2">
+        <v>48.8</v>
+      </c>
+      <c r="WS2">
+        <v>20</v>
+      </c>
+      <c r="WT2">
+        <v>48.3</v>
+      </c>
+      <c r="WU2">
+        <v>3</v>
+      </c>
+      <c r="WV2">
+        <v>33</v>
+      </c>
+      <c r="WW2">
+        <v>270</v>
+      </c>
+      <c r="WX2">
+        <v>2</v>
+      </c>
+      <c r="WY2">
+        <v>2</v>
+      </c>
+      <c r="WZ2">
+        <v>0</v>
+      </c>
+      <c r="XA2">
+        <v>0</v>
+      </c>
+      <c r="XB2">
         <v>4</v>
       </c>
-      <c r="VF2">
+      <c r="XC2">
+        <v>0</v>
+      </c>
+      <c r="XD2">
+        <v>0.67</v>
+      </c>
+      <c r="XE2">
+        <v>0.67</v>
+      </c>
+      <c r="XF2">
+        <v>1.33</v>
+      </c>
+      <c r="XG2">
+        <v>0.67</v>
+      </c>
+      <c r="XH2">
+        <v>1.33</v>
+      </c>
+      <c r="XI2">
+        <v>1.5</v>
+      </c>
+      <c r="XJ2">
+        <v>1.5</v>
+      </c>
+      <c r="XK2">
+        <v>0.51</v>
+      </c>
+      <c r="XL2">
+        <v>0.51</v>
+      </c>
+      <c r="XM2">
+        <v>3</v>
+      </c>
+      <c r="XN2">
+        <v>3</v>
+      </c>
+      <c r="XO2">
+        <v>270</v>
+      </c>
+      <c r="XP2">
+        <v>6</v>
+      </c>
+      <c r="XQ2">
+        <v>2</v>
+      </c>
+      <c r="XR2">
+        <v>18</v>
+      </c>
+      <c r="XS2">
+        <v>12</v>
+      </c>
+      <c r="XT2">
+        <v>66.7</v>
+      </c>
+      <c r="XU2">
+        <v>1</v>
+      </c>
+      <c r="XV2">
+        <v>0</v>
+      </c>
+      <c r="XW2">
+        <v>2</v>
+      </c>
+      <c r="XX2">
+        <v>0</v>
+      </c>
+      <c r="XY2">
+        <v>0</v>
+      </c>
+      <c r="XZ2">
+        <v>0</v>
+      </c>
+      <c r="YA2">
+        <v>0</v>
+      </c>
+      <c r="YB2">
+        <v>0</v>
+      </c>
+      <c r="YC2">
+        <v>0</v>
+      </c>
+      <c r="YD2">
+        <v>3</v>
+      </c>
+      <c r="YE2">
+        <v>0</v>
+      </c>
+      <c r="YF2">
+        <v>2</v>
+      </c>
+      <c r="YG2">
+        <v>0</v>
+      </c>
+      <c r="YH2">
+        <v>3.5</v>
+      </c>
+      <c r="YI2">
+        <v>0.19</v>
+      </c>
+      <c r="YJ2">
+        <v>-2.5</v>
+      </c>
+      <c r="YK2">
+        <v>-0.83</v>
+      </c>
+      <c r="YL2">
+        <v>6</v>
+      </c>
+      <c r="YM2">
+        <v>36</v>
+      </c>
+      <c r="YN2">
+        <v>16.7</v>
+      </c>
+      <c r="YO2">
+        <v>126</v>
+      </c>
+      <c r="YP2">
+        <v>10</v>
+      </c>
+      <c r="YQ2">
+        <v>25.4</v>
+      </c>
+      <c r="YR2">
+        <v>31.3</v>
+      </c>
+      <c r="YS2">
+        <v>20</v>
+      </c>
+      <c r="YT2">
+        <v>20</v>
+      </c>
+      <c r="YU2">
+        <v>26.4</v>
+      </c>
+      <c r="YV2">
+        <v>54</v>
+      </c>
+      <c r="YW2">
+        <v>1</v>
+      </c>
+      <c r="YX2">
+        <v>1.9</v>
+      </c>
+      <c r="YY2">
+        <v>2</v>
+      </c>
+      <c r="YZ2">
+        <v>0.67</v>
+      </c>
+      <c r="ZA2">
+        <v>21</v>
+      </c>
+      <c r="ZB2">
+        <v>10</v>
+      </c>
+      <c r="ZC2">
+        <v>1</v>
+      </c>
+      <c r="ZD2">
+        <v>31.3</v>
+      </c>
+      <c r="ZE2">
+        <v>3.33</v>
+      </c>
+      <c r="ZF2">
+        <v>0.06</v>
+      </c>
+      <c r="ZG2">
+        <v>0.2</v>
+      </c>
+      <c r="ZH2">
+        <v>0.05</v>
+      </c>
+      <c r="ZI2">
+        <v>0.5</v>
+      </c>
+      <c r="ZJ2">
+        <v>0.5</v>
+      </c>
+      <c r="ZK2">
+        <v>1305</v>
+      </c>
+      <c r="ZL2">
+        <v>1593</v>
+      </c>
+      <c r="ZM2">
+        <v>81.90000000000001</v>
+      </c>
+      <c r="ZN2">
+        <v>21713</v>
+      </c>
+      <c r="ZO2">
+        <v>7532</v>
+      </c>
+      <c r="ZP2">
+        <v>634</v>
+      </c>
+      <c r="ZQ2">
+        <v>687</v>
+      </c>
+      <c r="ZR2">
+        <v>92.3</v>
+      </c>
+      <c r="ZS2">
+        <v>524</v>
+      </c>
+      <c r="ZT2">
+        <v>593</v>
+      </c>
+      <c r="ZU2">
+        <v>88.40000000000001</v>
+      </c>
+      <c r="ZV2">
+        <v>112</v>
+      </c>
+      <c r="ZW2">
+        <v>227</v>
+      </c>
+      <c r="ZX2">
+        <v>49.3</v>
+      </c>
+      <c r="ZY2">
+        <v>26</v>
+      </c>
+      <c r="ZZ2">
+        <v>91</v>
+      </c>
+      <c r="AAA2">
+        <v>17</v>
+      </c>
+      <c r="AAB2">
+        <v>5</v>
+      </c>
+      <c r="AAC2">
+        <v>85</v>
+      </c>
+      <c r="AAD2">
+        <v>1442</v>
+      </c>
+      <c r="AAE2">
+        <v>149</v>
+      </c>
+      <c r="AAF2">
+        <v>40</v>
+      </c>
+      <c r="AAG2">
+        <v>3</v>
+      </c>
+      <c r="AAH2">
+        <v>6</v>
+      </c>
+      <c r="AAI2">
+        <v>36</v>
+      </c>
+      <c r="AAJ2">
+        <v>13</v>
+      </c>
+      <c r="AAK2">
         <v>8</v>
       </c>
-      <c r="VG2">
-        <v>7</v>
-      </c>
-      <c r="VH2">
+      <c r="AAL2">
+        <v>4</v>
+      </c>
+      <c r="AAM2">
+        <v>0</v>
+      </c>
+      <c r="AAN2">
+        <v>55</v>
+      </c>
+      <c r="AAO2">
+        <v>2</v>
+      </c>
+      <c r="AAP2">
+        <v>37</v>
+      </c>
+      <c r="AAQ2">
+        <v>55</v>
+      </c>
+      <c r="AAR2">
+        <v>18.33</v>
+      </c>
+      <c r="AAS2">
+        <v>44</v>
+      </c>
+      <c r="AAT2">
+        <v>6</v>
+      </c>
+      <c r="AAU2">
         <v>1</v>
       </c>
-      <c r="VI2">
-        <v>520</v>
-      </c>
-      <c r="VJ2">
-        <v>301</v>
-      </c>
-      <c r="VK2">
-        <v>246</v>
-      </c>
-      <c r="VL2">
-        <v>217</v>
-      </c>
-      <c r="VM2">
-        <v>57</v>
-      </c>
-      <c r="VN2">
-        <v>379</v>
-      </c>
-      <c r="VO2">
-        <v>80</v>
-      </c>
-      <c r="VP2">
-        <v>299</v>
-      </c>
-      <c r="VQ2">
-        <v>346</v>
-      </c>
-      <c r="VR2">
-        <v>517</v>
-      </c>
-      <c r="VS2">
-        <v>9</v>
-      </c>
-      <c r="VT2">
-        <v>19422</v>
-      </c>
-      <c r="VU2">
-        <v>1867</v>
-      </c>
-      <c r="VV2">
-        <v>6140</v>
-      </c>
-      <c r="VW2">
-        <v>8290</v>
-      </c>
-      <c r="VX2">
-        <v>5178</v>
-      </c>
-      <c r="VY2">
-        <v>773</v>
-      </c>
-      <c r="VZ2">
-        <v>19414</v>
-      </c>
-      <c r="WA2">
-        <v>10767</v>
-      </c>
-      <c r="WB2">
-        <v>564</v>
-      </c>
-      <c r="WC2">
-        <v>455</v>
-      </c>
-      <c r="WD2">
-        <v>174</v>
-      </c>
-      <c r="WE2">
-        <v>12365</v>
-      </c>
-      <c r="WF2">
-        <v>514</v>
-      </c>
-      <c r="WG2">
-        <v>315</v>
-      </c>
-      <c r="WH2">
+      <c r="AAV2">
         <v>1</v>
       </c>
-      <c r="WI2">
-        <v>381</v>
-      </c>
-      <c r="WJ2">
-        <v>320</v>
-      </c>
-      <c r="WK2">
+      <c r="AAW2">
+        <v>3</v>
+      </c>
+      <c r="AAX2">
+        <v>1</v>
+      </c>
+      <c r="AAY2">
+        <v>0</v>
+      </c>
+      <c r="AAZ2">
+        <v>2</v>
+      </c>
+      <c r="ABA2">
+        <v>0</v>
+      </c>
+      <c r="ABB2">
+        <v>0</v>
+      </c>
+      <c r="ABC2">
+        <v>1</v>
+      </c>
+      <c r="ABD2">
+        <v>43</v>
+      </c>
+      <c r="ABE2">
+        <v>23</v>
+      </c>
+      <c r="ABF2">
+        <v>21</v>
+      </c>
+      <c r="ABG2">
+        <v>20</v>
+      </c>
+      <c r="ABH2">
+        <v>2</v>
+      </c>
+      <c r="ABI2">
+        <v>35</v>
+      </c>
+      <c r="ABJ2">
+        <v>13</v>
+      </c>
+      <c r="ABK2">
+        <v>22</v>
+      </c>
+      <c r="ABL2">
+        <v>34</v>
+      </c>
+      <c r="ABM2">
+        <v>62</v>
+      </c>
+      <c r="ABN2">
+        <v>1</v>
+      </c>
+      <c r="ABO2">
+        <v>1904</v>
+      </c>
+      <c r="ABP2">
+        <v>267</v>
+      </c>
+      <c r="ABQ2">
+        <v>746</v>
+      </c>
+      <c r="ABR2">
+        <v>831</v>
+      </c>
+      <c r="ABS2">
+        <v>344</v>
+      </c>
+      <c r="ABT2">
+        <v>42</v>
+      </c>
+      <c r="ABU2">
+        <v>1904</v>
+      </c>
+      <c r="ABV2">
+        <v>1108</v>
+      </c>
+      <c r="ABW2">
+        <v>52</v>
+      </c>
+      <c r="ABX2">
+        <v>33</v>
+      </c>
+      <c r="ABY2">
+        <v>10</v>
+      </c>
+      <c r="ABZ2">
+        <v>1287</v>
+      </c>
+      <c r="ACA2">
+        <v>36</v>
+      </c>
+      <c r="ACB2">
+        <v>25</v>
+      </c>
+      <c r="ACC2">
+        <v>0</v>
+      </c>
+      <c r="ACD2">
+        <v>28</v>
+      </c>
+      <c r="ACE2">
+        <v>33</v>
+      </c>
+      <c r="ACF2">
+        <v>2</v>
+      </c>
+      <c r="ACG2">
+        <v>0</v>
+      </c>
+      <c r="ACH2">
+        <v>0</v>
+      </c>
+      <c r="ACI2">
+        <v>0</v>
+      </c>
+      <c r="ACJ2">
+        <v>157</v>
+      </c>
+      <c r="ACK2">
         <v>44</v>
       </c>
-      <c r="WL2">
-        <v>6</v>
-      </c>
-      <c r="WM2">
-        <v>3</v>
-      </c>
-      <c r="WN2">
-        <v>2</v>
-      </c>
-      <c r="WO2">
-        <v>1840</v>
-      </c>
-      <c r="WP2">
-        <v>472</v>
-      </c>
-      <c r="WQ2">
-        <v>389</v>
-      </c>
-      <c r="WR2">
-        <v>54.8</v>
-      </c>
-      <c r="WS2">
-        <v>25</v>
-      </c>
-      <c r="WT2">
-        <v>50</v>
-      </c>
-      <c r="WU2">
-        <v>31</v>
-      </c>
-      <c r="WV2">
-        <v>341</v>
-      </c>
-      <c r="WW2">
-        <v>2790</v>
-      </c>
-      <c r="WX2">
-        <v>34</v>
-      </c>
-      <c r="WY2">
-        <v>26</v>
-      </c>
-      <c r="WZ2">
-        <v>3</v>
-      </c>
-      <c r="XA2">
-        <v>3</v>
-      </c>
-      <c r="XB2">
-        <v>70</v>
-      </c>
-      <c r="XC2">
-        <v>0</v>
-      </c>
-      <c r="XD2">
-        <v>1.1</v>
-      </c>
-      <c r="XE2">
-        <v>0.84</v>
-      </c>
-      <c r="XF2">
-        <v>1.94</v>
-      </c>
-      <c r="XG2">
-        <v>1</v>
-      </c>
-      <c r="XH2">
-        <v>1.84</v>
-      </c>
-      <c r="XI2">
-        <v>33.7</v>
-      </c>
-      <c r="XJ2">
-        <v>31.4</v>
-      </c>
-      <c r="XK2">
-        <v>1.09</v>
-      </c>
-      <c r="XL2">
-        <v>1.01</v>
-      </c>
-      <c r="XM2">
-        <v>31</v>
-      </c>
-      <c r="XN2">
-        <v>31</v>
-      </c>
-      <c r="XO2">
-        <v>2790</v>
-      </c>
-      <c r="XP2">
-        <v>51</v>
-      </c>
-      <c r="XQ2">
-        <v>1.65</v>
-      </c>
-      <c r="XR2">
-        <v>143</v>
-      </c>
-      <c r="XS2">
-        <v>91</v>
-      </c>
-      <c r="XT2">
-        <v>68.5</v>
-      </c>
-      <c r="XU2">
-        <v>9</v>
-      </c>
-      <c r="XV2">
-        <v>7</v>
-      </c>
-      <c r="XW2">
-        <v>15</v>
-      </c>
-      <c r="XX2">
-        <v>6</v>
-      </c>
-      <c r="XY2">
-        <v>19.4</v>
-      </c>
-      <c r="XZ2">
-        <v>8</v>
-      </c>
-      <c r="YA2">
-        <v>6</v>
-      </c>
-      <c r="YB2">
-        <v>2</v>
-      </c>
-      <c r="YC2">
-        <v>0</v>
-      </c>
-      <c r="YD2">
-        <v>31</v>
-      </c>
-      <c r="YE2">
-        <v>0</v>
-      </c>
-      <c r="YF2">
-        <v>3</v>
-      </c>
-      <c r="YG2">
-        <v>1</v>
-      </c>
-      <c r="YH2">
-        <v>48.5</v>
-      </c>
-      <c r="YI2">
-        <v>0.29</v>
-      </c>
-      <c r="YJ2">
-        <v>-1.5</v>
-      </c>
-      <c r="YK2">
-        <v>-0.05</v>
-      </c>
-      <c r="YL2">
-        <v>170</v>
-      </c>
-      <c r="YM2">
-        <v>503</v>
-      </c>
-      <c r="YN2">
-        <v>33.8</v>
-      </c>
-      <c r="YO2">
-        <v>1042</v>
-      </c>
-      <c r="YP2">
-        <v>140</v>
-      </c>
-      <c r="YQ2">
-        <v>38.8</v>
-      </c>
-      <c r="YR2">
-        <v>35.7</v>
-      </c>
-      <c r="YS2">
-        <v>229</v>
-      </c>
-      <c r="YT2">
-        <v>43.2</v>
-      </c>
-      <c r="YU2">
-        <v>39.5</v>
-      </c>
-      <c r="YV2">
-        <v>411</v>
-      </c>
-      <c r="YW2">
-        <v>15</v>
-      </c>
-      <c r="YX2">
-        <v>3.6</v>
-      </c>
-      <c r="YY2">
-        <v>43</v>
-      </c>
-      <c r="YZ2">
-        <v>1.39</v>
-      </c>
-      <c r="ZA2">
-        <v>16</v>
-      </c>
-      <c r="ZB2">
-        <v>116</v>
-      </c>
-      <c r="ZC2">
-        <v>15</v>
-      </c>
-      <c r="ZD2">
-        <v>30.9</v>
-      </c>
-      <c r="ZE2">
-        <v>3.74</v>
-      </c>
-      <c r="ZF2">
-        <v>0.08</v>
-      </c>
-      <c r="ZG2">
-        <v>0.27</v>
-      </c>
-      <c r="ZH2">
-        <v>0.08</v>
-      </c>
-      <c r="ZI2">
-        <v>0.3</v>
-      </c>
-      <c r="ZJ2">
-        <v>-0.4</v>
-      </c>
-      <c r="ZK2">
-        <v>12385</v>
-      </c>
-      <c r="ZL2">
-        <v>15785</v>
-      </c>
-      <c r="ZM2">
-        <v>78.5</v>
-      </c>
-      <c r="ZN2">
-        <v>218820</v>
-      </c>
-      <c r="ZO2">
-        <v>81779</v>
-      </c>
-      <c r="ZP2">
-        <v>5599</v>
-      </c>
-      <c r="ZQ2">
-        <v>6353</v>
-      </c>
-      <c r="ZR2">
-        <v>88.09999999999999</v>
-      </c>
-      <c r="ZS2">
-        <v>5015</v>
-      </c>
-      <c r="ZT2">
-        <v>5929</v>
-      </c>
-      <c r="ZU2">
-        <v>84.59999999999999</v>
-      </c>
-      <c r="ZV2">
-        <v>1370</v>
-      </c>
-      <c r="ZW2">
-        <v>2504</v>
-      </c>
-      <c r="ZX2">
-        <v>54.7</v>
-      </c>
-      <c r="ZY2">
-        <v>283</v>
-      </c>
-      <c r="ZZ2">
-        <v>907</v>
-      </c>
-      <c r="AAA2">
-        <v>220</v>
-      </c>
-      <c r="AAB2">
-        <v>64</v>
-      </c>
-      <c r="AAC2">
-        <v>1080</v>
-      </c>
-      <c r="AAD2">
-        <v>14173</v>
-      </c>
-      <c r="AAE2">
-        <v>1572</v>
-      </c>
-      <c r="AAF2">
-        <v>406</v>
-      </c>
-      <c r="AAG2">
-        <v>25</v>
-      </c>
-      <c r="AAH2">
-        <v>95</v>
-      </c>
-      <c r="AAI2">
-        <v>485</v>
-      </c>
-      <c r="AAJ2">
-        <v>123</v>
-      </c>
-      <c r="AAK2">
-        <v>32</v>
-      </c>
-      <c r="AAL2">
-        <v>54</v>
-      </c>
-      <c r="AAM2">
-        <v>0</v>
-      </c>
-      <c r="AAN2">
-        <v>698</v>
-      </c>
-      <c r="AAO2">
-        <v>40</v>
-      </c>
-      <c r="AAP2">
-        <v>324</v>
-      </c>
-      <c r="AAQ2">
-        <v>660</v>
-      </c>
-      <c r="AAR2">
-        <v>21.29</v>
-      </c>
-      <c r="AAS2">
-        <v>496</v>
-      </c>
-      <c r="AAT2">
-        <v>53</v>
-      </c>
-      <c r="AAU2">
-        <v>31</v>
-      </c>
-      <c r="AAV2">
-        <v>34</v>
-      </c>
-      <c r="AAW2">
-        <v>60</v>
-      </c>
-      <c r="AAX2">
-        <v>1.94</v>
-      </c>
-      <c r="AAY2">
-        <v>45</v>
-      </c>
-      <c r="AAZ2">
-        <v>4</v>
-      </c>
-      <c r="ABA2">
-        <v>3</v>
-      </c>
-      <c r="ABB2">
-        <v>3</v>
-      </c>
-      <c r="ABC2">
-        <v>0</v>
-      </c>
-      <c r="ABD2">
-        <v>607</v>
-      </c>
-      <c r="ABE2">
-        <v>377</v>
-      </c>
-      <c r="ABF2">
-        <v>335</v>
-      </c>
-      <c r="ABG2">
-        <v>208</v>
-      </c>
-      <c r="ABH2">
-        <v>64</v>
-      </c>
-      <c r="ABI2">
-        <v>377</v>
-      </c>
-      <c r="ABJ2">
-        <v>108</v>
-      </c>
-      <c r="ABK2">
-        <v>269</v>
-      </c>
-      <c r="ABL2">
-        <v>299</v>
-      </c>
-      <c r="ABM2">
-        <v>576</v>
-      </c>
-      <c r="ABN2">
-        <v>7</v>
-      </c>
-      <c r="ABO2">
-        <v>19456</v>
-      </c>
-      <c r="ABP2">
-        <v>2106</v>
-      </c>
-      <c r="ABQ2">
-        <v>6629</v>
-      </c>
-      <c r="ABR2">
-        <v>8776</v>
-      </c>
-      <c r="ABS2">
-        <v>4256</v>
-      </c>
-      <c r="ABT2">
-        <v>576</v>
-      </c>
-      <c r="ABU2">
-        <v>19453</v>
-      </c>
-      <c r="ABV2">
-        <v>11179</v>
-      </c>
-      <c r="ABW2">
-        <v>502</v>
-      </c>
-      <c r="ABX2">
-        <v>394</v>
-      </c>
-      <c r="ABY2">
-        <v>114</v>
-      </c>
-      <c r="ABZ2">
-        <v>12239</v>
-      </c>
-      <c r="ACA2">
-        <v>531</v>
-      </c>
-      <c r="ACB2">
-        <v>266</v>
-      </c>
-      <c r="ACC2">
-        <v>0</v>
-      </c>
-      <c r="ACD2">
-        <v>338</v>
-      </c>
-      <c r="ACE2">
-        <v>356</v>
-      </c>
-      <c r="ACF2">
-        <v>40</v>
-      </c>
-      <c r="ACG2">
-        <v>1</v>
-      </c>
-      <c r="ACH2">
-        <v>8</v>
-      </c>
-      <c r="ACI2">
-        <v>1</v>
-      </c>
-      <c r="ACJ2">
-        <v>1865</v>
-      </c>
-      <c r="ACK2">
-        <v>389</v>
-      </c>
       <c r="ACL2">
-        <v>472</v>
+        <v>42</v>
       </c>
       <c r="ACM2">
-        <v>45.2</v>
+        <v>51.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Serie A 23/24 matchday 5
</commit_message>
<xml_diff>
--- a/tmp/playermatchdata.xlsx
+++ b/tmp/playermatchdata.xlsx
@@ -2320,7 +2320,7 @@
     <t>Inter</t>
   </si>
   <si>
-    <t>26-214</t>
+    <t>26-226</t>
   </si>
   <si>
     <t>Atalanta</t>
@@ -4992,7 +4992,7 @@
         <v>765</v>
       </c>
       <c r="B2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C2">
         <v>1870</v>
@@ -5007,7 +5007,7 @@
         <v>765</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
         <v>768</v>
@@ -5016,13 +5016,13 @@
         <v>1997</v>
       </c>
       <c r="K2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M2">
-        <v>218</v>
+        <v>281</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -5064,10 +5064,10 @@
         <v>0.1</v>
       </c>
       <c r="AA2">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="AB2">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -5082,7 +5082,7 @@
         <v>25</v>
       </c>
       <c r="AG2">
-        <v>0.41</v>
+        <v>0.32</v>
       </c>
       <c r="AH2">
         <v>0</v>
@@ -5100,52 +5100,52 @@
         <v>-0.1</v>
       </c>
       <c r="AM2">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="AN2">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="AO2">
-        <v>86.09999999999999</v>
+        <v>86.2</v>
       </c>
       <c r="AP2">
-        <v>2515</v>
+        <v>2848</v>
       </c>
       <c r="AQ2">
-        <v>872</v>
+        <v>1017</v>
       </c>
       <c r="AR2">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="AS2">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="AT2">
-        <v>90.7</v>
+        <v>91.2</v>
       </c>
       <c r="AU2">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AV2">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AW2">
-        <v>86.7</v>
+        <v>85.90000000000001</v>
       </c>
       <c r="AX2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AY2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AZ2">
-        <v>66.7</v>
+        <v>69.2</v>
       </c>
       <c r="BA2">
         <v>5</v>
       </c>
       <c r="BB2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BC2">
         <v>11</v>
@@ -5154,10 +5154,10 @@
         <v>2</v>
       </c>
       <c r="BE2">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="BF2">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="BG2">
         <v>5</v>
@@ -5169,7 +5169,7 @@
         <v>2</v>
       </c>
       <c r="BJ2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="BK2">
         <v>3</v>
@@ -5193,16 +5193,16 @@
         <v>0</v>
       </c>
       <c r="BR2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BS2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BT2">
-        <v>4.54</v>
+        <v>3.84</v>
       </c>
       <c r="BU2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BV2">
         <v>0</v>
@@ -5217,7 +5217,7 @@
         <v>1</v>
       </c>
       <c r="BZ2">
-        <v>0.41</v>
+        <v>0.32</v>
       </c>
       <c r="CA2">
         <v>1</v>
@@ -5235,29 +5235,29 @@
         <v>0</v>
       </c>
       <c r="CF2">
+        <v>10</v>
+      </c>
+      <c r="CG2">
+        <v>5</v>
+      </c>
+      <c r="CH2">
+        <v>4</v>
+      </c>
+      <c r="CI2">
         <v>6</v>
       </c>
-      <c r="CG2">
+      <c r="CJ2">
+        <v>0</v>
+      </c>
+      <c r="CK2">
         <v>2</v>
       </c>
-      <c r="CH2">
+      <c r="CL2">
+        <v>0</v>
+      </c>
+      <c r="CM2">
         <v>2</v>
       </c>
-      <c r="CI2">
-        <v>4</v>
-      </c>
-      <c r="CJ2">
-        <v>0</v>
-      </c>
-      <c r="CK2">
-        <v>1</v>
-      </c>
-      <c r="CL2">
-        <v>0</v>
-      </c>
-      <c r="CM2">
-        <v>1</v>
-      </c>
       <c r="CN2">
         <v>0</v>
       </c>
@@ -5268,28 +5268,28 @@
         <v>0</v>
       </c>
       <c r="CQ2">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="CR2">
         <v>3</v>
       </c>
       <c r="CS2">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="CT2">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="CU2">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="CV2">
         <v>1</v>
       </c>
       <c r="CW2">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="CX2">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="CY2">
         <v>7</v>
@@ -5301,10 +5301,10 @@
         <v>0</v>
       </c>
       <c r="DB2">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="DC2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DD2">
         <v>0</v>
@@ -5313,7 +5313,7 @@
         <v>0</v>
       </c>
       <c r="DF2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="DG2">
         <v>3</v>
@@ -5334,7 +5334,7 @@
         <v>11</v>
       </c>
       <c r="DM2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DN2">
         <v>0</v>
@@ -5463,100 +5463,100 @@
         <v>0</v>
       </c>
       <c r="FD2">
-        <v>6.333333333333333</v>
+        <v>6.375</v>
       </c>
       <c r="FE2">
-        <v>0.2357022603955158</v>
+        <v>0.2165063509461096</v>
       </c>
       <c r="FF2" t="s">
         <v>767</v>
       </c>
       <c r="FG2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="FH2">
-        <v>51.3</v>
+        <v>48.8</v>
       </c>
       <c r="FI2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="FJ2">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="FK2">
-        <v>270</v>
+        <v>360</v>
       </c>
       <c r="FL2">
+        <v>13</v>
+      </c>
+      <c r="FM2">
+        <v>11</v>
+      </c>
+      <c r="FN2">
+        <v>2</v>
+      </c>
+      <c r="FO2">
+        <v>2</v>
+      </c>
+      <c r="FP2">
+        <v>5</v>
+      </c>
+      <c r="FQ2">
+        <v>0</v>
+      </c>
+      <c r="FR2">
+        <v>3.25</v>
+      </c>
+      <c r="FS2">
+        <v>2.75</v>
+      </c>
+      <c r="FT2">
+        <v>6</v>
+      </c>
+      <c r="FU2">
+        <v>2.75</v>
+      </c>
+      <c r="FV2">
+        <v>5.5</v>
+      </c>
+      <c r="FW2">
+        <v>9.9</v>
+      </c>
+      <c r="FX2">
+        <v>8.4</v>
+      </c>
+      <c r="FY2">
+        <v>2.47</v>
+      </c>
+      <c r="FZ2">
+        <v>2.09</v>
+      </c>
+      <c r="GA2">
+        <v>4</v>
+      </c>
+      <c r="GB2">
+        <v>4</v>
+      </c>
+      <c r="GC2">
+        <v>360</v>
+      </c>
+      <c r="GD2">
+        <v>1</v>
+      </c>
+      <c r="GE2">
+        <v>0.25</v>
+      </c>
+      <c r="GF2">
         <v>8</v>
       </c>
-      <c r="FM2">
+      <c r="GG2">
         <v>7</v>
       </c>
-      <c r="FN2">
-        <v>1</v>
-      </c>
-      <c r="FO2">
-        <v>1</v>
-      </c>
-      <c r="FP2">
-        <v>3</v>
-      </c>
-      <c r="FQ2">
-        <v>0</v>
-      </c>
-      <c r="FR2">
-        <v>2.67</v>
-      </c>
-      <c r="FS2">
-        <v>2.33</v>
-      </c>
-      <c r="FT2">
-        <v>5</v>
-      </c>
-      <c r="FU2">
-        <v>2.33</v>
-      </c>
-      <c r="FV2">
-        <v>4.67</v>
-      </c>
-      <c r="FW2">
-        <v>7.3</v>
-      </c>
-      <c r="FX2">
-        <v>6.5</v>
-      </c>
-      <c r="FY2">
-        <v>2.42</v>
-      </c>
-      <c r="FZ2">
-        <v>2.17</v>
-      </c>
-      <c r="GA2">
-        <v>3</v>
-      </c>
-      <c r="GB2">
-        <v>3</v>
-      </c>
-      <c r="GC2">
-        <v>270</v>
-      </c>
-      <c r="GD2">
-        <v>0</v>
-      </c>
-      <c r="GE2">
-        <v>0</v>
-      </c>
-      <c r="GF2">
-        <v>6</v>
-      </c>
-      <c r="GG2">
-        <v>6</v>
-      </c>
       <c r="GH2">
-        <v>100</v>
+        <v>87.5</v>
       </c>
       <c r="GI2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="GJ2">
         <v>0</v>
@@ -5568,241 +5568,241 @@
         <v>3</v>
       </c>
       <c r="GM2">
+        <v>75</v>
+      </c>
+      <c r="GN2">
+        <v>0</v>
+      </c>
+      <c r="GO2">
+        <v>0</v>
+      </c>
+      <c r="GP2">
+        <v>0</v>
+      </c>
+      <c r="GQ2">
+        <v>0</v>
+      </c>
+      <c r="GR2">
+        <v>4</v>
+      </c>
+      <c r="GS2">
+        <v>0</v>
+      </c>
+      <c r="GT2">
+        <v>0</v>
+      </c>
+      <c r="GU2">
+        <v>0</v>
+      </c>
+      <c r="GV2">
+        <v>1.6</v>
+      </c>
+      <c r="GW2">
+        <v>0.2</v>
+      </c>
+      <c r="GX2">
+        <v>0.6</v>
+      </c>
+      <c r="GY2">
+        <v>0.16</v>
+      </c>
+      <c r="GZ2">
+        <v>24</v>
+      </c>
+      <c r="HA2">
+        <v>41</v>
+      </c>
+      <c r="HB2">
+        <v>58.5</v>
+      </c>
+      <c r="HC2">
+        <v>112</v>
+      </c>
+      <c r="HD2">
+        <v>19</v>
+      </c>
+      <c r="HE2">
+        <v>31.3</v>
+      </c>
+      <c r="HF2">
+        <v>30.8</v>
+      </c>
+      <c r="HG2">
+        <v>29</v>
+      </c>
+      <c r="HH2">
+        <v>20.7</v>
+      </c>
+      <c r="HI2">
+        <v>28.3</v>
+      </c>
+      <c r="HJ2">
+        <v>41</v>
+      </c>
+      <c r="HK2">
+        <v>2</v>
+      </c>
+      <c r="HL2">
+        <v>4.9</v>
+      </c>
+      <c r="HM2">
+        <v>0</v>
+      </c>
+      <c r="HN2">
+        <v>0</v>
+      </c>
+      <c r="HO2">
+        <v>6.5</v>
+      </c>
+      <c r="HP2">
+        <v>22</v>
+      </c>
+      <c r="HQ2">
+        <v>3</v>
+      </c>
+      <c r="HR2">
+        <v>30.6</v>
+      </c>
+      <c r="HS2">
+        <v>5.5</v>
+      </c>
+      <c r="HT2">
+        <v>0.15</v>
+      </c>
+      <c r="HU2">
+        <v>0.5</v>
+      </c>
+      <c r="HV2">
+        <v>0.12</v>
+      </c>
+      <c r="HW2">
+        <v>3.1</v>
+      </c>
+      <c r="HX2">
+        <v>2.6</v>
+      </c>
+      <c r="HY2">
+        <v>1672</v>
+      </c>
+      <c r="HZ2">
+        <v>1987</v>
+      </c>
+      <c r="IA2">
+        <v>84.09999999999999</v>
+      </c>
+      <c r="IB2">
+        <v>29759</v>
+      </c>
+      <c r="IC2">
+        <v>10606</v>
+      </c>
+      <c r="ID2">
+        <v>741</v>
+      </c>
+      <c r="IE2">
+        <v>813</v>
+      </c>
+      <c r="IF2">
+        <v>91.09999999999999</v>
+      </c>
+      <c r="IG2">
+        <v>671</v>
+      </c>
+      <c r="IH2">
+        <v>755</v>
+      </c>
+      <c r="II2">
+        <v>88.90000000000001</v>
+      </c>
+      <c r="IJ2">
+        <v>186</v>
+      </c>
+      <c r="IK2">
+        <v>294</v>
+      </c>
+      <c r="IL2">
+        <v>63.3</v>
+      </c>
+      <c r="IM2">
+        <v>54</v>
+      </c>
+      <c r="IN2">
+        <v>133</v>
+      </c>
+      <c r="IO2">
+        <v>44</v>
+      </c>
+      <c r="IP2">
+        <v>15</v>
+      </c>
+      <c r="IQ2">
+        <v>173</v>
+      </c>
+      <c r="IR2">
+        <v>1827</v>
+      </c>
+      <c r="IS2">
+        <v>155</v>
+      </c>
+      <c r="IT2">
+        <v>46</v>
+      </c>
+      <c r="IU2">
+        <v>11</v>
+      </c>
+      <c r="IV2">
+        <v>36</v>
+      </c>
+      <c r="IW2">
+        <v>70</v>
+      </c>
+      <c r="IX2">
+        <v>21</v>
+      </c>
+      <c r="IY2">
+        <v>5</v>
+      </c>
+      <c r="IZ2">
+        <v>13</v>
+      </c>
+      <c r="JA2">
+        <v>0</v>
+      </c>
+      <c r="JB2">
+        <v>53</v>
+      </c>
+      <c r="JC2">
+        <v>5</v>
+      </c>
+      <c r="JD2">
+        <v>27</v>
+      </c>
+      <c r="JE2">
+        <v>133</v>
+      </c>
+      <c r="JF2">
+        <v>33.25</v>
+      </c>
+      <c r="JG2">
         <v>100</v>
       </c>
-      <c r="GN2">
-        <v>0</v>
-      </c>
-      <c r="GO2">
-        <v>0</v>
-      </c>
-      <c r="GP2">
-        <v>0</v>
-      </c>
-      <c r="GQ2">
-        <v>0</v>
-      </c>
-      <c r="GR2">
-        <v>3</v>
-      </c>
-      <c r="GS2">
-        <v>0</v>
-      </c>
-      <c r="GT2">
-        <v>0</v>
-      </c>
-      <c r="GU2">
-        <v>0</v>
-      </c>
-      <c r="GV2">
-        <v>1.2</v>
-      </c>
-      <c r="GW2">
-        <v>0.21</v>
-      </c>
-      <c r="GX2">
-        <v>1.2</v>
-      </c>
-      <c r="GY2">
-        <v>0.41</v>
-      </c>
-      <c r="GZ2">
+      <c r="JH2">
+        <v>12</v>
+      </c>
+      <c r="JI2">
+        <v>8</v>
+      </c>
+      <c r="JJ2">
+        <v>8</v>
+      </c>
+      <c r="JK2">
+        <v>23</v>
+      </c>
+      <c r="JL2">
+        <v>5.75</v>
+      </c>
+      <c r="JM2">
         <v>19</v>
-      </c>
-      <c r="HA2">
-        <v>32</v>
-      </c>
-      <c r="HB2">
-        <v>59.4</v>
-      </c>
-      <c r="HC2">
-        <v>81</v>
-      </c>
-      <c r="HD2">
-        <v>12</v>
-      </c>
-      <c r="HE2">
-        <v>33.3</v>
-      </c>
-      <c r="HF2">
-        <v>31.4</v>
-      </c>
-      <c r="HG2">
-        <v>21</v>
-      </c>
-      <c r="HH2">
-        <v>23.8</v>
-      </c>
-      <c r="HI2">
-        <v>31</v>
-      </c>
-      <c r="HJ2">
-        <v>35</v>
-      </c>
-      <c r="HK2">
-        <v>1</v>
-      </c>
-      <c r="HL2">
-        <v>2.9</v>
-      </c>
-      <c r="HM2">
-        <v>0</v>
-      </c>
-      <c r="HN2">
-        <v>0</v>
-      </c>
-      <c r="HO2">
-        <v>6.8</v>
-      </c>
-      <c r="HP2">
-        <v>16</v>
-      </c>
-      <c r="HQ2">
-        <v>2</v>
-      </c>
-      <c r="HR2">
-        <v>27.1</v>
-      </c>
-      <c r="HS2">
-        <v>5.33</v>
-      </c>
-      <c r="HT2">
-        <v>0.12</v>
-      </c>
-      <c r="HU2">
-        <v>0.44</v>
-      </c>
-      <c r="HV2">
-        <v>0.11</v>
-      </c>
-      <c r="HW2">
-        <v>0.7</v>
-      </c>
-      <c r="HX2">
-        <v>0.5</v>
-      </c>
-      <c r="HY2">
-        <v>1367</v>
-      </c>
-      <c r="HZ2">
-        <v>1610</v>
-      </c>
-      <c r="IA2">
-        <v>84.90000000000001</v>
-      </c>
-      <c r="IB2">
-        <v>24158</v>
-      </c>
-      <c r="IC2">
-        <v>8292</v>
-      </c>
-      <c r="ID2">
-        <v>613</v>
-      </c>
-      <c r="IE2">
-        <v>670</v>
-      </c>
-      <c r="IF2">
-        <v>91.5</v>
-      </c>
-      <c r="IG2">
-        <v>551</v>
-      </c>
-      <c r="IH2">
-        <v>619</v>
-      </c>
-      <c r="II2">
-        <v>89</v>
-      </c>
-      <c r="IJ2">
-        <v>146</v>
-      </c>
-      <c r="IK2">
-        <v>229</v>
-      </c>
-      <c r="IL2">
-        <v>63.8</v>
-      </c>
-      <c r="IM2">
-        <v>44</v>
-      </c>
-      <c r="IN2">
-        <v>109</v>
-      </c>
-      <c r="IO2">
-        <v>38</v>
-      </c>
-      <c r="IP2">
-        <v>12</v>
-      </c>
-      <c r="IQ2">
-        <v>146</v>
-      </c>
-      <c r="IR2">
-        <v>1497</v>
-      </c>
-      <c r="IS2">
-        <v>110</v>
-      </c>
-      <c r="IT2">
-        <v>33</v>
-      </c>
-      <c r="IU2">
-        <v>10</v>
-      </c>
-      <c r="IV2">
-        <v>29</v>
-      </c>
-      <c r="IW2">
-        <v>58</v>
-      </c>
-      <c r="IX2">
-        <v>16</v>
-      </c>
-      <c r="IY2">
-        <v>2</v>
-      </c>
-      <c r="IZ2">
-        <v>12</v>
-      </c>
-      <c r="JA2">
-        <v>0</v>
-      </c>
-      <c r="JB2">
-        <v>37</v>
-      </c>
-      <c r="JC2">
-        <v>3</v>
-      </c>
-      <c r="JD2">
-        <v>17</v>
-      </c>
-      <c r="JE2">
-        <v>108</v>
-      </c>
-      <c r="JF2">
-        <v>36</v>
-      </c>
-      <c r="JG2">
-        <v>83</v>
-      </c>
-      <c r="JH2">
-        <v>9</v>
-      </c>
-      <c r="JI2">
-        <v>7</v>
-      </c>
-      <c r="JJ2">
-        <v>6</v>
-      </c>
-      <c r="JK2">
-        <v>15</v>
-      </c>
-      <c r="JL2">
-        <v>5</v>
-      </c>
-      <c r="JM2">
-        <v>12</v>
       </c>
       <c r="JN2">
         <v>0</v>
@@ -5811,286 +5811,286 @@
         <v>1</v>
       </c>
       <c r="JP2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JQ2">
         <v>1</v>
       </c>
       <c r="JR2">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="JS2">
+        <v>45</v>
+      </c>
+      <c r="JT2">
         <v>38</v>
       </c>
-      <c r="JT2">
-        <v>34</v>
-      </c>
       <c r="JU2">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="JV2">
         <v>8</v>
       </c>
       <c r="JW2">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="JX2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="JY2">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="JZ2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="KA2">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="KB2">
         <v>0</v>
       </c>
       <c r="KC2">
-        <v>1917</v>
+        <v>2381</v>
       </c>
       <c r="KD2">
-        <v>172</v>
+        <v>239</v>
       </c>
       <c r="KE2">
-        <v>557</v>
+        <v>729</v>
       </c>
       <c r="KF2">
-        <v>878</v>
+        <v>1068</v>
       </c>
       <c r="KG2">
-        <v>502</v>
+        <v>607</v>
       </c>
       <c r="KH2">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="KI2">
-        <v>1916</v>
+        <v>2379</v>
       </c>
       <c r="KJ2">
-        <v>1242</v>
+        <v>1549</v>
       </c>
       <c r="KK2">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="KL2">
+        <v>54</v>
+      </c>
+      <c r="KM2">
+        <v>22</v>
+      </c>
+      <c r="KN2">
+        <v>1657</v>
+      </c>
+      <c r="KO2">
+        <v>40</v>
+      </c>
+      <c r="KP2">
+        <v>17</v>
+      </c>
+      <c r="KQ2">
+        <v>0</v>
+      </c>
+      <c r="KR2">
+        <v>47</v>
+      </c>
+      <c r="KS2">
         <v>45</v>
       </c>
-      <c r="KM2">
-        <v>17</v>
-      </c>
-      <c r="KN2">
-        <v>1354</v>
-      </c>
-      <c r="KO2">
+      <c r="KT2">
+        <v>5</v>
+      </c>
+      <c r="KU2">
+        <v>2</v>
+      </c>
+      <c r="KV2">
+        <v>0</v>
+      </c>
+      <c r="KW2">
+        <v>0</v>
+      </c>
+      <c r="KX2">
+        <v>187</v>
+      </c>
+      <c r="KY2">
+        <v>44</v>
+      </c>
+      <c r="KZ2">
         <v>30</v>
       </c>
-      <c r="KP2">
+      <c r="LA2">
+        <v>59.5</v>
+      </c>
+      <c r="LB2">
+        <v>19</v>
+      </c>
+      <c r="LC2">
+        <v>51.3</v>
+      </c>
+      <c r="LD2">
+        <v>4</v>
+      </c>
+      <c r="LE2">
+        <v>44</v>
+      </c>
+      <c r="LF2">
+        <v>360</v>
+      </c>
+      <c r="LG2">
+        <v>1</v>
+      </c>
+      <c r="LH2">
+        <v>1</v>
+      </c>
+      <c r="LI2">
+        <v>0</v>
+      </c>
+      <c r="LJ2">
+        <v>0</v>
+      </c>
+      <c r="LK2">
+        <v>5</v>
+      </c>
+      <c r="LL2">
+        <v>0</v>
+      </c>
+      <c r="LM2">
+        <v>0.25</v>
+      </c>
+      <c r="LN2">
+        <v>0.25</v>
+      </c>
+      <c r="LO2">
+        <v>0.5</v>
+      </c>
+      <c r="LP2">
+        <v>0.25</v>
+      </c>
+      <c r="LQ2">
+        <v>0.5</v>
+      </c>
+      <c r="LR2">
+        <v>2.9</v>
+      </c>
+      <c r="LS2">
+        <v>2.9</v>
+      </c>
+      <c r="LT2">
+        <v>0.71</v>
+      </c>
+      <c r="LU2">
+        <v>0.71</v>
+      </c>
+      <c r="LV2">
+        <v>4</v>
+      </c>
+      <c r="LW2">
+        <v>4</v>
+      </c>
+      <c r="LX2">
+        <v>360</v>
+      </c>
+      <c r="LY2">
         <v>13</v>
       </c>
-      <c r="KQ2">
-        <v>0</v>
-      </c>
-      <c r="KR2">
-        <v>31</v>
-      </c>
-      <c r="KS2">
-        <v>33</v>
-      </c>
-      <c r="KT2">
-        <v>3</v>
-      </c>
-      <c r="KU2">
-        <v>1</v>
-      </c>
-      <c r="KV2">
-        <v>0</v>
-      </c>
-      <c r="KW2">
-        <v>0</v>
-      </c>
-      <c r="KX2">
-        <v>156</v>
-      </c>
-      <c r="KY2">
-        <v>36</v>
-      </c>
-      <c r="KZ2">
+      <c r="LZ2">
+        <v>3.25</v>
+      </c>
+      <c r="MA2">
         <v>24</v>
       </c>
-      <c r="LA2">
-        <v>60</v>
-      </c>
-      <c r="LB2">
+      <c r="MB2">
+        <v>11</v>
+      </c>
+      <c r="MC2">
+        <v>54.2</v>
+      </c>
+      <c r="MD2">
+        <v>0</v>
+      </c>
+      <c r="ME2">
+        <v>0</v>
+      </c>
+      <c r="MF2">
+        <v>4</v>
+      </c>
+      <c r="MG2">
+        <v>0</v>
+      </c>
+      <c r="MH2">
+        <v>0</v>
+      </c>
+      <c r="MI2">
+        <v>2</v>
+      </c>
+      <c r="MJ2">
+        <v>2</v>
+      </c>
+      <c r="MK2">
+        <v>0</v>
+      </c>
+      <c r="ML2">
+        <v>0</v>
+      </c>
+      <c r="MM2">
+        <v>4</v>
+      </c>
+      <c r="MN2">
+        <v>0</v>
+      </c>
+      <c r="MO2">
+        <v>0</v>
+      </c>
+      <c r="MP2">
+        <v>0</v>
+      </c>
+      <c r="MQ2">
+        <v>9.1</v>
+      </c>
+      <c r="MR2">
+        <v>0.31</v>
+      </c>
+      <c r="MS2">
+        <v>-3.9</v>
+      </c>
+      <c r="MT2">
+        <v>-0.96</v>
+      </c>
+      <c r="MU2">
+        <v>15</v>
+      </c>
+      <c r="MV2">
+        <v>40</v>
+      </c>
+      <c r="MW2">
+        <v>37.5</v>
+      </c>
+      <c r="MX2">
+        <v>112</v>
+      </c>
+      <c r="MY2">
         <v>18</v>
       </c>
-      <c r="LC2">
-        <v>48.7</v>
-      </c>
-      <c r="LD2">
-        <v>3</v>
-      </c>
-      <c r="LE2">
-        <v>33</v>
-      </c>
-      <c r="LF2">
-        <v>270</v>
-      </c>
-      <c r="LG2">
-        <v>0</v>
-      </c>
-      <c r="LH2">
-        <v>0</v>
-      </c>
-      <c r="LI2">
-        <v>0</v>
-      </c>
-      <c r="LJ2">
-        <v>0</v>
-      </c>
-      <c r="LK2">
-        <v>3</v>
-      </c>
-      <c r="LL2">
-        <v>0</v>
-      </c>
-      <c r="LM2">
-        <v>0</v>
-      </c>
-      <c r="LN2">
-        <v>0</v>
-      </c>
-      <c r="LO2">
-        <v>0</v>
-      </c>
-      <c r="LP2">
-        <v>0</v>
-      </c>
-      <c r="LQ2">
-        <v>0</v>
-      </c>
-      <c r="LR2">
-        <v>1.8</v>
-      </c>
-      <c r="LS2">
-        <v>1.8</v>
-      </c>
-      <c r="LT2">
-        <v>0.6</v>
-      </c>
-      <c r="LU2">
-        <v>0.6</v>
-      </c>
-      <c r="LV2">
-        <v>3</v>
-      </c>
-      <c r="LW2">
-        <v>3</v>
-      </c>
-      <c r="LX2">
-        <v>270</v>
-      </c>
-      <c r="LY2">
-        <v>8</v>
-      </c>
-      <c r="LZ2">
-        <v>2.67</v>
-      </c>
-      <c r="MA2">
-        <v>17</v>
-      </c>
-      <c r="MB2">
-        <v>9</v>
-      </c>
-      <c r="MC2">
-        <v>58.8</v>
-      </c>
-      <c r="MD2">
-        <v>0</v>
-      </c>
-      <c r="ME2">
-        <v>0</v>
-      </c>
-      <c r="MF2">
-        <v>3</v>
-      </c>
-      <c r="MG2">
-        <v>0</v>
-      </c>
-      <c r="MH2">
-        <v>0</v>
-      </c>
-      <c r="MI2">
-        <v>1</v>
-      </c>
-      <c r="MJ2">
-        <v>1</v>
-      </c>
-      <c r="MK2">
-        <v>0</v>
-      </c>
-      <c r="ML2">
-        <v>0</v>
-      </c>
-      <c r="MM2">
-        <v>3</v>
-      </c>
-      <c r="MN2">
-        <v>0</v>
-      </c>
-      <c r="MO2">
-        <v>0</v>
-      </c>
-      <c r="MP2">
-        <v>0</v>
-      </c>
-      <c r="MQ2">
-        <v>5.3</v>
-      </c>
-      <c r="MR2">
-        <v>0.26</v>
-      </c>
-      <c r="MS2">
-        <v>-2.7</v>
-      </c>
-      <c r="MT2">
-        <v>-0.89</v>
-      </c>
-      <c r="MU2">
-        <v>14</v>
-      </c>
-      <c r="MV2">
-        <v>39</v>
-      </c>
-      <c r="MW2">
-        <v>35.9</v>
-      </c>
-      <c r="MX2">
-        <v>84</v>
-      </c>
-      <c r="MY2">
-        <v>15</v>
-      </c>
       <c r="MZ2">
-        <v>31</v>
+        <v>23.2</v>
       </c>
       <c r="NA2">
-        <v>33.2</v>
+        <v>30.3</v>
       </c>
       <c r="NB2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="NC2">
-        <v>54.2</v>
+        <v>51.9</v>
       </c>
       <c r="ND2">
-        <v>46.9</v>
+        <v>45.3</v>
       </c>
       <c r="NE2">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="NF2">
         <v>0</v>
@@ -6102,112 +6102,112 @@
         <v>4</v>
       </c>
       <c r="NI2">
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="NJ2">
-        <v>16.5</v>
+        <v>14.9</v>
       </c>
       <c r="NK2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="NL2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NM2">
-        <v>20</v>
+        <v>20.5</v>
       </c>
       <c r="NN2">
         <v>2</v>
       </c>
       <c r="NO2">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="NP2">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="NQ2">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="NR2">
-        <v>-1.8</v>
+        <v>-1.9</v>
       </c>
       <c r="NS2">
-        <v>-1.8</v>
+        <v>-1.9</v>
       </c>
       <c r="NT2">
-        <v>1261</v>
+        <v>1754</v>
       </c>
       <c r="NU2">
-        <v>1502</v>
+        <v>2055</v>
       </c>
       <c r="NV2">
-        <v>84</v>
+        <v>85.40000000000001</v>
       </c>
       <c r="NW2">
-        <v>24183</v>
+        <v>32260</v>
       </c>
       <c r="NX2">
-        <v>7787</v>
+        <v>10313</v>
       </c>
       <c r="NY2">
-        <v>501</v>
+        <v>738</v>
       </c>
       <c r="NZ2">
-        <v>558</v>
+        <v>816</v>
       </c>
       <c r="OA2">
-        <v>89.8</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="OB2">
-        <v>552</v>
+        <v>759</v>
       </c>
       <c r="OC2">
-        <v>622</v>
+        <v>841</v>
       </c>
       <c r="OD2">
-        <v>88.7</v>
+        <v>90.2</v>
       </c>
       <c r="OE2">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="OF2">
-        <v>246</v>
+        <v>290</v>
       </c>
       <c r="OG2">
-        <v>72</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="OH2">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="OI2">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="OJ2">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="OK2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="OL2">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="OM2">
-        <v>1362</v>
+        <v>1872</v>
       </c>
       <c r="ON2">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="OO2">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="OP2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="OQ2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="OR2">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="OS2">
         <v>8</v>
@@ -6222,25 +6222,25 @@
         <v>0</v>
       </c>
       <c r="OW2">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="OX2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="OY2">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="OZ2">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="PA2">
-        <v>17.33</v>
+        <v>17.25</v>
       </c>
       <c r="PB2">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="PC2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PD2">
         <v>1</v>
@@ -6249,13 +6249,13 @@
         <v>2</v>
       </c>
       <c r="PF2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="PG2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="PH2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="PI2">
         <v>0</v>
@@ -6270,136 +6270,136 @@
         <v>0</v>
       </c>
       <c r="PM2">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="PN2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="PO2">
+        <v>21</v>
+      </c>
+      <c r="PP2">
+        <v>10</v>
+      </c>
+      <c r="PQ2">
+        <v>5</v>
+      </c>
+      <c r="PR2">
+        <v>41</v>
+      </c>
+      <c r="PS2">
         <v>18</v>
       </c>
-      <c r="PP2">
-        <v>7</v>
-      </c>
-      <c r="PQ2">
-        <v>3</v>
-      </c>
-      <c r="PR2">
-        <v>28</v>
-      </c>
-      <c r="PS2">
-        <v>14</v>
-      </c>
       <c r="PT2">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="PU2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="PV2">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="PW2">
         <v>1</v>
       </c>
       <c r="PX2">
-        <v>1788</v>
+        <v>2432</v>
       </c>
       <c r="PY2">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="PZ2">
-        <v>593</v>
+        <v>746</v>
       </c>
       <c r="QA2">
-        <v>813</v>
+        <v>1156</v>
       </c>
       <c r="QB2">
-        <v>395</v>
+        <v>546</v>
       </c>
       <c r="QC2">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="QD2">
-        <v>1788</v>
+        <v>2432</v>
       </c>
       <c r="QE2">
-        <v>1158</v>
+        <v>1630</v>
       </c>
       <c r="QF2">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="QG2">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="QH2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="QI2">
-        <v>1249</v>
+        <v>1733</v>
       </c>
       <c r="QJ2">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="QK2">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="QL2">
         <v>0</v>
       </c>
       <c r="QM2">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="QN2">
+        <v>44</v>
+      </c>
+      <c r="QO2">
+        <v>5</v>
+      </c>
+      <c r="QP2">
+        <v>0</v>
+      </c>
+      <c r="QQ2">
+        <v>2</v>
+      </c>
+      <c r="QR2">
+        <v>0</v>
+      </c>
+      <c r="QS2">
+        <v>163</v>
+      </c>
+      <c r="QT2">
         <v>30</v>
       </c>
-      <c r="QO2">
-        <v>3</v>
-      </c>
-      <c r="QP2">
-        <v>0</v>
-      </c>
-      <c r="QQ2">
-        <v>1</v>
-      </c>
-      <c r="QR2">
-        <v>0</v>
-      </c>
-      <c r="QS2">
-        <v>128</v>
-      </c>
-      <c r="QT2">
-        <v>24</v>
-      </c>
       <c r="QU2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="QV2">
-        <v>40</v>
+        <v>40.5</v>
       </c>
       <c r="QW2" t="s">
         <v>769</v>
       </c>
       <c r="QX2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="QY2">
-        <v>51.7</v>
+        <v>49.5</v>
       </c>
       <c r="QZ2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="RA2">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="RB2">
-        <v>270</v>
+        <v>360</v>
       </c>
       <c r="RC2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="RD2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="RE2">
         <v>0</v>
@@ -6408,7 +6408,7 @@
         <v>0</v>
       </c>
       <c r="RG2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="RH2">
         <v>0</v>
@@ -6429,40 +6429,40 @@
         <v>4</v>
       </c>
       <c r="RN2">
-        <v>4.2</v>
+        <v>4.9</v>
       </c>
       <c r="RO2">
-        <v>4.2</v>
+        <v>4.9</v>
       </c>
       <c r="RP2">
-        <v>1.41</v>
+        <v>1.23</v>
       </c>
       <c r="RQ2">
-        <v>1.41</v>
+        <v>1.23</v>
       </c>
       <c r="RR2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="RS2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="RT2">
-        <v>270</v>
+        <v>360</v>
       </c>
       <c r="RU2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="RV2">
-        <v>0.67</v>
+        <v>1.25</v>
       </c>
       <c r="RW2">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="RX2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="RY2">
-        <v>80</v>
+        <v>72.2</v>
       </c>
       <c r="RZ2">
         <v>2</v>
@@ -6471,13 +6471,13 @@
         <v>0</v>
       </c>
       <c r="SB2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="SC2">
         <v>2</v>
       </c>
       <c r="SD2">
-        <v>66.7</v>
+        <v>50</v>
       </c>
       <c r="SE2">
         <v>0</v>
@@ -6492,7 +6492,7 @@
         <v>0</v>
       </c>
       <c r="SI2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="SJ2">
         <v>0</v>
@@ -6504,214 +6504,214 @@
         <v>0</v>
       </c>
       <c r="SM2">
-        <v>2.1</v>
+        <v>4.1</v>
       </c>
       <c r="SN2">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="SO2">
-        <v>0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="SP2">
-        <v>0.04</v>
+        <v>-0.24</v>
       </c>
       <c r="SQ2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="SR2">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="SS2">
-        <v>32.4</v>
+        <v>28.6</v>
       </c>
       <c r="ST2">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="SU2">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="SV2">
-        <v>27.3</v>
+        <v>29.3</v>
       </c>
       <c r="SW2">
-        <v>29.3</v>
+        <v>31.1</v>
       </c>
       <c r="SX2">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="SY2">
-        <v>55.6</v>
+        <v>62.5</v>
       </c>
       <c r="SZ2">
-        <v>46.1</v>
+        <v>51.9</v>
       </c>
       <c r="TA2">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="TB2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="TC2">
-        <v>7.1</v>
+        <v>7.3</v>
       </c>
       <c r="TD2">
         <v>8</v>
       </c>
       <c r="TE2">
-        <v>2.67</v>
+        <v>2</v>
       </c>
       <c r="TF2">
+        <v>21.2</v>
+      </c>
+      <c r="TG2">
         <v>22</v>
       </c>
-      <c r="TG2">
-        <v>18</v>
-      </c>
       <c r="TH2">
         <v>0</v>
       </c>
       <c r="TI2">
-        <v>34.6</v>
+        <v>34.9</v>
       </c>
       <c r="TJ2">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="TK2">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="TL2">
-        <v>0.33</v>
+        <v>0.36</v>
       </c>
       <c r="TM2">
         <v>0.08</v>
       </c>
       <c r="TN2">
-        <v>1.8</v>
+        <v>3.1</v>
       </c>
       <c r="TO2">
-        <v>1.8</v>
+        <v>3.1</v>
       </c>
       <c r="TP2">
-        <v>1395</v>
+        <v>1710</v>
       </c>
       <c r="TQ2">
-        <v>1694</v>
+        <v>2117</v>
       </c>
       <c r="TR2">
-        <v>82.3</v>
+        <v>80.8</v>
       </c>
       <c r="TS2">
-        <v>24117</v>
+        <v>29680</v>
       </c>
       <c r="TT2">
-        <v>8315</v>
+        <v>10551</v>
       </c>
       <c r="TU2">
-        <v>631</v>
+        <v>769</v>
       </c>
       <c r="TV2">
-        <v>715</v>
+        <v>880</v>
       </c>
       <c r="TW2">
-        <v>88.3</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="TX2">
-        <v>599</v>
+        <v>733</v>
       </c>
       <c r="TY2">
-        <v>672</v>
+        <v>825</v>
       </c>
       <c r="TZ2">
-        <v>89.09999999999999</v>
+        <v>88.8</v>
       </c>
       <c r="UA2">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="UB2">
-        <v>220</v>
+        <v>291</v>
       </c>
       <c r="UC2">
-        <v>60</v>
+        <v>56.4</v>
       </c>
       <c r="UD2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="UE2">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="UF2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="UG2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="UH2">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="UI2">
-        <v>1554</v>
+        <v>1927</v>
       </c>
       <c r="UJ2">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="UK2">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="UL2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="UM2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="UN2">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="UO2">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="UP2">
         <v>8</v>
       </c>
       <c r="UQ2">
+        <v>13</v>
+      </c>
+      <c r="UR2">
+        <v>0</v>
+      </c>
+      <c r="US2">
+        <v>85</v>
+      </c>
+      <c r="UT2">
         <v>9</v>
       </c>
-      <c r="UR2">
-        <v>0</v>
-      </c>
-      <c r="US2">
-        <v>59</v>
-      </c>
-      <c r="UT2">
-        <v>7</v>
-      </c>
       <c r="UU2">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="UV2">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="UW2">
-        <v>32.33</v>
+        <v>28.5</v>
       </c>
       <c r="UX2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="UY2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="UZ2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="VA2">
         <v>0</v>
       </c>
       <c r="VB2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="VC2">
-        <v>3.67</v>
+        <v>3.75</v>
       </c>
       <c r="VD2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="VE2">
         <v>1</v>
@@ -6726,199 +6726,199 @@
         <v>0</v>
       </c>
       <c r="VI2">
+        <v>70</v>
+      </c>
+      <c r="VJ2">
+        <v>39</v>
+      </c>
+      <c r="VK2">
+        <v>37</v>
+      </c>
+      <c r="VL2">
+        <v>24</v>
+      </c>
+      <c r="VM2">
+        <v>9</v>
+      </c>
+      <c r="VN2">
+        <v>52</v>
+      </c>
+      <c r="VO2">
+        <v>11</v>
+      </c>
+      <c r="VP2">
+        <v>41</v>
+      </c>
+      <c r="VQ2">
         <v>43</v>
       </c>
-      <c r="VJ2">
-        <v>22</v>
-      </c>
-      <c r="VK2">
-        <v>19</v>
-      </c>
-      <c r="VL2">
-        <v>17</v>
-      </c>
-      <c r="VM2">
-        <v>7</v>
-      </c>
-      <c r="VN2">
+      <c r="VR2">
+        <v>59</v>
+      </c>
+      <c r="VS2">
+        <v>1</v>
+      </c>
+      <c r="VT2">
+        <v>2541</v>
+      </c>
+      <c r="VU2">
+        <v>214</v>
+      </c>
+      <c r="VV2">
+        <v>777</v>
+      </c>
+      <c r="VW2">
+        <v>1068</v>
+      </c>
+      <c r="VX2">
+        <v>723</v>
+      </c>
+      <c r="VY2">
+        <v>104</v>
+      </c>
+      <c r="VZ2">
+        <v>2541</v>
+      </c>
+      <c r="WA2">
+        <v>1603</v>
+      </c>
+      <c r="WB2">
+        <v>92</v>
+      </c>
+      <c r="WC2">
+        <v>65</v>
+      </c>
+      <c r="WD2">
+        <v>24</v>
+      </c>
+      <c r="WE2">
+        <v>1694</v>
+      </c>
+      <c r="WF2">
+        <v>51</v>
+      </c>
+      <c r="WG2">
         <v>39</v>
       </c>
-      <c r="VO2">
+      <c r="WH2">
+        <v>0</v>
+      </c>
+      <c r="WI2">
+        <v>48</v>
+      </c>
+      <c r="WJ2">
+        <v>34</v>
+      </c>
+      <c r="WK2">
+        <v>9</v>
+      </c>
+      <c r="WL2">
+        <v>0</v>
+      </c>
+      <c r="WM2">
+        <v>0</v>
+      </c>
+      <c r="WN2">
+        <v>0</v>
+      </c>
+      <c r="WO2">
+        <v>232</v>
+      </c>
+      <c r="WP2">
+        <v>60</v>
+      </c>
+      <c r="WQ2">
+        <v>65</v>
+      </c>
+      <c r="WR2">
+        <v>48</v>
+      </c>
+      <c r="WS2">
+        <v>23</v>
+      </c>
+      <c r="WT2">
+        <v>50.5</v>
+      </c>
+      <c r="WU2">
+        <v>4</v>
+      </c>
+      <c r="WV2">
+        <v>44</v>
+      </c>
+      <c r="WW2">
+        <v>360</v>
+      </c>
+      <c r="WX2">
+        <v>5</v>
+      </c>
+      <c r="WY2">
+        <v>4</v>
+      </c>
+      <c r="WZ2">
+        <v>0</v>
+      </c>
+      <c r="XA2">
+        <v>0</v>
+      </c>
+      <c r="XB2">
+        <v>5</v>
+      </c>
+      <c r="XC2">
+        <v>0</v>
+      </c>
+      <c r="XD2">
+        <v>1.25</v>
+      </c>
+      <c r="XE2">
+        <v>1</v>
+      </c>
+      <c r="XF2">
+        <v>2.25</v>
+      </c>
+      <c r="XG2">
+        <v>1.25</v>
+      </c>
+      <c r="XH2">
+        <v>2.25</v>
+      </c>
+      <c r="XI2">
+        <v>2.6</v>
+      </c>
+      <c r="XJ2">
+        <v>2.6</v>
+      </c>
+      <c r="XK2">
+        <v>0.66</v>
+      </c>
+      <c r="XL2">
+        <v>0.66</v>
+      </c>
+      <c r="XM2">
+        <v>4</v>
+      </c>
+      <c r="XN2">
+        <v>4</v>
+      </c>
+      <c r="XO2">
+        <v>360</v>
+      </c>
+      <c r="XP2">
         <v>8</v>
-      </c>
-      <c r="VP2">
-        <v>31</v>
-      </c>
-      <c r="VQ2">
-        <v>27</v>
-      </c>
-      <c r="VR2">
-        <v>35</v>
-      </c>
-      <c r="VS2">
-        <v>0</v>
-      </c>
-      <c r="VT2">
-        <v>1993</v>
-      </c>
-      <c r="VU2">
-        <v>146</v>
-      </c>
-      <c r="VV2">
-        <v>555</v>
-      </c>
-      <c r="VW2">
-        <v>841</v>
-      </c>
-      <c r="VX2">
-        <v>618</v>
-      </c>
-      <c r="VY2">
-        <v>89</v>
-      </c>
-      <c r="VZ2">
-        <v>1993</v>
-      </c>
-      <c r="WA2">
-        <v>1282</v>
-      </c>
-      <c r="WB2">
-        <v>73</v>
-      </c>
-      <c r="WC2">
-        <v>56</v>
-      </c>
-      <c r="WD2">
-        <v>20</v>
-      </c>
-      <c r="WE2">
-        <v>1379</v>
-      </c>
-      <c r="WF2">
-        <v>38</v>
-      </c>
-      <c r="WG2">
-        <v>26</v>
-      </c>
-      <c r="WH2">
-        <v>0</v>
-      </c>
-      <c r="WI2">
-        <v>34</v>
-      </c>
-      <c r="WJ2">
-        <v>27</v>
-      </c>
-      <c r="WK2">
-        <v>7</v>
-      </c>
-      <c r="WL2">
-        <v>0</v>
-      </c>
-      <c r="WM2">
-        <v>0</v>
-      </c>
-      <c r="WN2">
-        <v>0</v>
-      </c>
-      <c r="WO2">
-        <v>172</v>
-      </c>
-      <c r="WP2">
-        <v>42</v>
-      </c>
-      <c r="WQ2">
-        <v>44</v>
-      </c>
-      <c r="WR2">
-        <v>48.8</v>
-      </c>
-      <c r="WS2">
-        <v>20</v>
-      </c>
-      <c r="WT2">
-        <v>48.3</v>
-      </c>
-      <c r="WU2">
-        <v>3</v>
-      </c>
-      <c r="WV2">
-        <v>33</v>
-      </c>
-      <c r="WW2">
-        <v>270</v>
-      </c>
-      <c r="WX2">
-        <v>2</v>
-      </c>
-      <c r="WY2">
-        <v>2</v>
-      </c>
-      <c r="WZ2">
-        <v>0</v>
-      </c>
-      <c r="XA2">
-        <v>0</v>
-      </c>
-      <c r="XB2">
-        <v>4</v>
-      </c>
-      <c r="XC2">
-        <v>0</v>
-      </c>
-      <c r="XD2">
-        <v>0.67</v>
-      </c>
-      <c r="XE2">
-        <v>0.67</v>
-      </c>
-      <c r="XF2">
-        <v>1.33</v>
-      </c>
-      <c r="XG2">
-        <v>0.67</v>
-      </c>
-      <c r="XH2">
-        <v>1.33</v>
-      </c>
-      <c r="XI2">
-        <v>1.5</v>
-      </c>
-      <c r="XJ2">
-        <v>1.5</v>
-      </c>
-      <c r="XK2">
-        <v>0.51</v>
-      </c>
-      <c r="XL2">
-        <v>0.51</v>
-      </c>
-      <c r="XM2">
-        <v>3</v>
-      </c>
-      <c r="XN2">
-        <v>3</v>
-      </c>
-      <c r="XO2">
-        <v>270</v>
-      </c>
-      <c r="XP2">
-        <v>6</v>
       </c>
       <c r="XQ2">
         <v>2</v>
       </c>
       <c r="XR2">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="XS2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="XT2">
-        <v>66.7</v>
+        <v>63.6</v>
       </c>
       <c r="XU2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="XV2">
         <v>0</v>
@@ -6945,7 +6945,7 @@
         <v>0</v>
       </c>
       <c r="YD2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="YE2">
         <v>0</v>
@@ -6957,40 +6957,40 @@
         <v>0</v>
       </c>
       <c r="YH2">
-        <v>3.5</v>
+        <v>4.3</v>
       </c>
       <c r="YI2">
         <v>0.19</v>
       </c>
       <c r="YJ2">
-        <v>-2.5</v>
+        <v>-3.7</v>
       </c>
       <c r="YK2">
-        <v>-0.83</v>
+        <v>-0.93</v>
       </c>
       <c r="YL2">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="YM2">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="YN2">
-        <v>16.7</v>
+        <v>31.4</v>
       </c>
       <c r="YO2">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="YP2">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="YQ2">
-        <v>25.4</v>
+        <v>28</v>
       </c>
       <c r="YR2">
-        <v>31.3</v>
+        <v>32.6</v>
       </c>
       <c r="YS2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="YT2">
         <v>20</v>
@@ -6999,175 +6999,175 @@
         <v>26.4</v>
       </c>
       <c r="YV2">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="YW2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="YX2">
-        <v>1.9</v>
+        <v>3.4</v>
       </c>
       <c r="YY2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="YZ2">
-        <v>0.67</v>
+        <v>0.75</v>
       </c>
       <c r="ZA2">
-        <v>21</v>
+        <v>17.5</v>
       </c>
       <c r="ZB2">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="ZC2">
         <v>1</v>
       </c>
       <c r="ZD2">
-        <v>31.3</v>
+        <v>38.3</v>
       </c>
       <c r="ZE2">
-        <v>3.33</v>
+        <v>4.5</v>
       </c>
       <c r="ZF2">
+        <v>0.11</v>
+      </c>
+      <c r="ZG2">
+        <v>0.28</v>
+      </c>
+      <c r="ZH2">
         <v>0.06</v>
       </c>
-      <c r="ZG2">
-        <v>0.2</v>
-      </c>
-      <c r="ZH2">
-        <v>0.05</v>
-      </c>
       <c r="ZI2">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
       <c r="ZJ2">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
       <c r="ZK2">
-        <v>1305</v>
+        <v>1761</v>
       </c>
       <c r="ZL2">
-        <v>1593</v>
+        <v>2153</v>
       </c>
       <c r="ZM2">
-        <v>81.90000000000001</v>
+        <v>81.8</v>
       </c>
       <c r="ZN2">
-        <v>21713</v>
+        <v>30316</v>
       </c>
       <c r="ZO2">
-        <v>7532</v>
+        <v>10955</v>
       </c>
       <c r="ZP2">
-        <v>634</v>
+        <v>818</v>
       </c>
       <c r="ZQ2">
-        <v>687</v>
+        <v>897</v>
       </c>
       <c r="ZR2">
-        <v>92.3</v>
+        <v>91.2</v>
       </c>
       <c r="ZS2">
-        <v>524</v>
+        <v>726</v>
       </c>
       <c r="ZT2">
-        <v>593</v>
+        <v>831</v>
       </c>
       <c r="ZU2">
-        <v>88.40000000000001</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="ZV2">
-        <v>112</v>
+        <v>170</v>
       </c>
       <c r="ZW2">
-        <v>227</v>
+        <v>312</v>
       </c>
       <c r="ZX2">
-        <v>49.3</v>
+        <v>54.5</v>
       </c>
       <c r="ZY2">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="ZZ2">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="AAA2">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="AAB2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AAC2">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="AAD2">
-        <v>1442</v>
+        <v>1947</v>
       </c>
       <c r="AAE2">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="AAF2">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AAG2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AAH2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AAI2">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="AAJ2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AAK2">
         <v>8</v>
       </c>
       <c r="AAL2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AAM2">
         <v>0</v>
       </c>
       <c r="AAN2">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="AAO2">
         <v>2</v>
       </c>
       <c r="AAP2">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="AAQ2">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="AAR2">
-        <v>18.33</v>
+        <v>21</v>
       </c>
       <c r="AAS2">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="AAT2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AAU2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AAV2">
         <v>1</v>
       </c>
       <c r="AAW2">
+        <v>9</v>
+      </c>
+      <c r="AAX2">
+        <v>2.25</v>
+      </c>
+      <c r="AAY2">
+        <v>4</v>
+      </c>
+      <c r="AAZ2">
         <v>3</v>
-      </c>
-      <c r="AAX2">
-        <v>1</v>
-      </c>
-      <c r="AAY2">
-        <v>0</v>
-      </c>
-      <c r="AAZ2">
-        <v>2</v>
       </c>
       <c r="ABA2">
         <v>0</v>
@@ -7179,88 +7179,88 @@
         <v>1</v>
       </c>
       <c r="ABD2">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="ABE2">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="ABF2">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="ABG2">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="ABH2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="ABI2">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="ABJ2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="ABK2">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="ABL2">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="ABM2">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="ABN2">
         <v>1</v>
       </c>
       <c r="ABO2">
-        <v>1904</v>
+        <v>2584</v>
       </c>
       <c r="ABP2">
-        <v>267</v>
+        <v>323</v>
       </c>
       <c r="ABQ2">
-        <v>746</v>
+        <v>916</v>
       </c>
       <c r="ABR2">
-        <v>831</v>
+        <v>1144</v>
       </c>
       <c r="ABS2">
-        <v>344</v>
+        <v>548</v>
       </c>
       <c r="ABT2">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="ABU2">
-        <v>1904</v>
+        <v>2584</v>
       </c>
       <c r="ABV2">
-        <v>1108</v>
+        <v>1536</v>
       </c>
       <c r="ABW2">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="ABX2">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="ABY2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="ABZ2">
-        <v>1287</v>
+        <v>1736</v>
       </c>
       <c r="ACA2">
+        <v>58</v>
+      </c>
+      <c r="ACB2">
+        <v>38</v>
+      </c>
+      <c r="ACC2">
+        <v>0</v>
+      </c>
+      <c r="ACD2">
         <v>36</v>
       </c>
-      <c r="ACB2">
-        <v>25</v>
-      </c>
-      <c r="ACC2">
-        <v>0</v>
-      </c>
-      <c r="ACD2">
-        <v>28</v>
-      </c>
       <c r="ACE2">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="ACF2">
         <v>2</v>
@@ -7275,16 +7275,16 @@
         <v>0</v>
       </c>
       <c r="ACJ2">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="ACK2">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="ACL2">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="ACM2">
-        <v>51.2</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>